<commit_message>
cache code segments to up speed
</commit_message>
<xml_diff>
--- a/index_bbg_rating_live.xlsx
+++ b/index_bbg_rating_live.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kaimin Khaw\Desktop\Credit Rating Model Website\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kaimin Khaw\Desktop\credit-rating-deploy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BABA80CB-647A-439B-B3EA-C825A41E9B86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F68CB52C-E6FC-48D4-8661-C49279E1A100}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2A12413E-A5EC-426E-A187-DE07F52921C3}"/>
   </bookViews>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="353">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="354">
   <si>
     <t>Turkey</t>
   </si>
@@ -1107,6 +1107,9 @@
   </si>
   <si>
     <t>Ba3u</t>
+  </si>
+  <si>
+    <t>CCC+u</t>
   </si>
 </sst>
 </file>
@@ -1192,1531 +1195,1531 @@
   <volType type="realTimeData">
     <main first="bofaddin.rtdserver">
       <tp t="s">
-        <v>#N/A Requesting Data...4227691815</v>
+        <v>#N/A Requesting Data...4084940804</v>
         <stp/>
         <stp>BDP|13719527809048657439</stp>
         <tr r="E3" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3733088635</v>
+        <v>#N/A Requesting Data...3818166150</v>
         <stp/>
         <stp>BDP|12363409739849183621</stp>
         <tr r="G98" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3737949734</v>
+        <v>#N/A Requesting Data...3936637966</v>
         <stp/>
         <stp>BDP|17606584297068117917</stp>
         <tr r="G105" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3764575264</v>
+        <v>#N/A Requesting Data...3582039849</v>
         <stp/>
         <stp>BDP|12825277506793769973</stp>
         <tr r="F22" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4282393552</v>
+        <v>#N/A Requesting Data...4167090013</v>
         <stp/>
         <stp>BDP|13615906068526188051</stp>
         <tr r="G101" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4017714521</v>
+        <v>#N/A Requesting Data...4215472552</v>
         <stp/>
         <stp>BDP|10912677687245148127</stp>
         <tr r="G106" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4243346383</v>
+        <v>#N/A Requesting Data...4071996823</v>
         <stp/>
         <stp>BDP|16221541486007837625</stp>
         <tr r="G58" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3783025260</v>
+        <v>#N/A Requesting Data...4114476026</v>
         <stp/>
         <stp>BDP|14989839765876665645</stp>
         <tr r="C81" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4262949459</v>
+        <v>#N/A Requesting Data...3668815360</v>
         <stp/>
         <stp>BDP|16792452589360294083</stp>
         <tr r="E11" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4100645631</v>
+        <v>#N/A Requesting Data...3955049544</v>
         <stp/>
         <stp>BDP|16409240184993364568</stp>
         <tr r="E54" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4075820073</v>
+        <v>#N/A Requesting Data...4066999936</v>
         <stp/>
         <stp>BDP|12376141866138693768</stp>
         <tr r="C88" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4253209962</v>
+        <v>#N/A Requesting Data...3799792905</v>
         <stp/>
         <stp>BDP|13146963289471890960</stp>
         <tr r="C18" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3777528810</v>
+        <v>#N/A Requesting Data...3914697931</v>
         <stp/>
         <stp>BDP|10167725043130019931</stp>
         <tr r="C110" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4218785455</v>
+        <v>#N/A Requesting Data...3655857831</v>
         <stp/>
         <stp>BDP|10589422899161895655</stp>
         <tr r="G76" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3751752877</v>
+        <v>#N/A Requesting Data...4026033311</v>
         <stp/>
         <stp>BDP|15228795190517586693</stp>
         <tr r="E84" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3736941159</v>
+        <v>#N/A Requesting Data...3942019898</v>
         <stp/>
         <stp>BDP|10096201946458505444</stp>
         <tr r="G97" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3850213225</v>
+        <v>#N/A Requesting Data...3814219693</v>
         <stp/>
         <stp>BDP|18253401034836307331</stp>
         <tr r="F99" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3890558287</v>
+        <v>#N/A Requesting Data...4003975361</v>
         <stp/>
         <stp>BDP|10867273920449518201</stp>
         <tr r="G71" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4167359658</v>
+        <v>#N/A Requesting Data...4030248805</v>
         <stp/>
         <stp>BDP|14811872563886412749</stp>
         <tr r="E114" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3833765817</v>
+        <v>#N/A Requesting Data...4173553565</v>
         <stp/>
         <stp>BDP|15237334583701669483</stp>
         <tr r="C112" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3933547051</v>
+        <v>#N/A Requesting Data...4248521151</v>
         <stp/>
         <stp>BDP|14006145231309322495</stp>
         <tr r="C65" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4184004273</v>
+        <v>#N/A Requesting Data...3973396673</v>
         <stp/>
         <stp>BDP|14761213634019822741</stp>
         <tr r="G2" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3968361472</v>
+        <v>#N/A Requesting Data...3769923197</v>
         <stp/>
         <stp>BDP|15399231330039360601</stp>
         <tr r="E42" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4288193974</v>
+        <v>#N/A Requesting Data...4134176344</v>
         <stp/>
         <stp>BDP|11120752607359953480</stp>
         <tr r="G61" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4165279835</v>
+        <v>#N/A Requesting Data...3745060468</v>
         <stp/>
         <stp>BDP|15939978441203902037</stp>
         <tr r="C26" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3811437682</v>
+        <v>#N/A Requesting Data...3782108872</v>
         <stp/>
         <stp>BDP|18066043829836356791</stp>
         <tr r="G78" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3893527000</v>
+        <v>#N/A Requesting Data...4066827677</v>
         <stp/>
         <stp>BDP|14168806967588813989</stp>
         <tr r="F77" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4022855054</v>
+        <v>#N/A Requesting Data...4102979142</v>
         <stp/>
         <stp>BDP|18397803367339867766</stp>
         <tr r="F101" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3948946971</v>
+        <v>#N/A Requesting Data...3770151263</v>
         <stp/>
         <stp>BDP|15895803206017416271</stp>
         <tr r="C33" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4108245256</v>
+        <v>#N/A Requesting Data...4083708151</v>
         <stp/>
         <stp>BDP|14908732543227691836</stp>
         <tr r="E94" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3738156500</v>
+        <v>#N/A Requesting Data...3911993897</v>
         <stp/>
         <stp>BDP|12957817799052931996</stp>
         <tr r="E120" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3761098180</v>
+        <v>#N/A Requesting Data...4025837358</v>
         <stp/>
         <stp>BDP|16275205432289392600</stp>
         <tr r="E101" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3808593621</v>
+        <v>#N/A Requesting Data...3869758937</v>
         <stp/>
         <stp>BDP|10407655300028223605</stp>
         <tr r="F47" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4263536074</v>
+        <v>#N/A Requesting Data...3856786581</v>
         <stp/>
         <stp>BDP|14031612538318230186</stp>
         <tr r="C136" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3986672357</v>
+        <v>#N/A Requesting Data...3726006503</v>
         <stp/>
         <stp>BDP|13840587393604095357</stp>
         <tr r="G3" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4195458193</v>
+        <v>#N/A Requesting Data...3948414322</v>
         <stp/>
         <stp>BDP|18397555740376217727</stp>
         <tr r="F17" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4108661925</v>
+        <v>#N/A Requesting Data...3843665062</v>
         <stp/>
         <stp>BDP|15886108592084595196</stp>
         <tr r="F19" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4243628040</v>
+        <v>#N/A Requesting Data...4090535034</v>
         <stp/>
         <stp>BDP|12574943311804341655</stp>
         <tr r="C58" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3812640614</v>
+        <v>#N/A Requesting Data...4056868476</v>
         <stp/>
         <stp>BDP|15276164033266227932</stp>
         <tr r="C121" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3869506602</v>
+        <v>#N/A Requesting Data...3726393719</v>
         <stp/>
         <stp>BDP|11413915902765857449</stp>
         <tr r="C135" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3886856078</v>
+        <v>#N/A Requesting Data...3798936595</v>
         <stp/>
         <stp>BDP|10888161880627674738</stp>
         <tr r="G74" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3846734972</v>
+        <v>#N/A Requesting Data...3926614609</v>
         <stp/>
         <stp>BDP|18252264749434830399</stp>
         <tr r="E91" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3959601374</v>
+        <v>#N/A Requesting Data...3672628817</v>
         <stp/>
         <stp>BDP|16230814927561165496</stp>
         <tr r="C25" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4231068649</v>
+        <v>#N/A Requesting Data...4216089997</v>
         <stp/>
         <stp>BDP|11669407615485914850</stp>
         <tr r="E28" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4022903900</v>
+        <v>#N/A Requesting Data...3830389832</v>
         <stp/>
         <stp>BDP|15385895124225473341</stp>
         <tr r="F89" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4266712483</v>
+        <v>#N/A Requesting Data...3942830157</v>
         <stp/>
         <stp>BDP|16215575297831427265</stp>
         <tr r="G19" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3771324683</v>
+        <v>#N/A Requesting Data...4272428885</v>
         <stp/>
         <stp>BDP|15664489079057139842</stp>
         <tr r="C50" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3927268721</v>
+        <v>#N/A Requesting Data...3789272974</v>
         <stp/>
         <stp>BDP|13556466380534139208</stp>
         <tr r="C63" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3899143931</v>
+        <v>#N/A Requesting Data...4182875044</v>
         <stp/>
         <stp>BDP|12426034393664290636</stp>
         <tr r="G70" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3779264909</v>
+        <v>#N/A Requesting Data...3949420847</v>
         <stp/>
         <stp>BDP|11206974657257798316</stp>
         <tr r="G5" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4241777285</v>
+        <v>#N/A Requesting Data...4158614471</v>
         <stp/>
         <stp>BDP|15687672872765725835</stp>
         <tr r="G133" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4031930174</v>
+        <v>#N/A Requesting Data...3859021594</v>
         <stp/>
         <stp>BDP|10646340980557108540</stp>
         <tr r="G83" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4110519496</v>
+        <v>#N/A Requesting Data...4043172443</v>
         <stp/>
         <stp>BDP|13932387258969800286</stp>
         <tr r="G30" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4091701990</v>
+        <v>#N/A Requesting Data...3842083138</v>
         <stp/>
         <stp>BDP|14685689793557045247</stp>
         <tr r="G11" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3993879272</v>
+        <v>#N/A Requesting Data...3853686362</v>
         <stp/>
         <stp>BDP|11792528289940283264</stp>
         <tr r="G39" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4058552394</v>
+        <v>#N/A Requesting Data...3925565773</v>
         <stp/>
         <stp>BDP|14038814629908297802</stp>
         <tr r="E14" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3834009252</v>
+        <v>#N/A Requesting Data...3819747339</v>
         <stp/>
         <stp>BDP|17960836852555549100</stp>
         <tr r="F79" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3843559115</v>
+        <v>#N/A Requesting Data...4288117455</v>
         <stp/>
         <stp>BDP|12258786923690042954</stp>
         <tr r="G82" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3928161871</v>
+        <v>#N/A Requesting Data...4291596956</v>
         <stp/>
         <stp>BDP|11831892951331348329</stp>
         <tr r="C35" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3835945645</v>
+        <v>#N/A Requesting Data...4217312828</v>
         <stp/>
         <stp>BDP|12634554786653062247</stp>
         <tr r="F34" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3957965183</v>
+        <v>#N/A Requesting Data...4054871828</v>
         <stp/>
         <stp>BDP|10304787173197381988</stp>
         <tr r="G53" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4113818026</v>
+        <v>#N/A Requesting Data...3843648100</v>
         <stp/>
         <stp>BDP|15772343051115104818</stp>
         <tr r="C127" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3864892852</v>
+        <v>#N/A Requesting Data...3980979718</v>
         <stp/>
         <stp>BDP|13619322587163510542</stp>
         <tr r="C45" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4287084935</v>
+        <v>#N/A Requesting Data...4063486971</v>
         <stp/>
         <stp>BDP|13709828003397613269</stp>
         <tr r="C54" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4027971775</v>
+        <v>#N/A Requesting Data...4136110991</v>
         <stp/>
         <stp>BDP|11596891797659679653</stp>
         <tr r="C89" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3998637234</v>
+        <v>#N/A Requesting Data...3836849735</v>
         <stp/>
         <stp>BDP|18339290641951108002</stp>
         <tr r="E17" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4191398456</v>
+        <v>#N/A Requesting Data...4257494646</v>
         <stp/>
         <stp>BDP|10418265688390464525</stp>
         <tr r="E18" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4265645951</v>
+        <v>#N/A Requesting Data...4086890445</v>
         <stp/>
         <stp>BDP|14859691791600738447</stp>
         <tr r="F45" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3905307487</v>
+        <v>#N/A Requesting Data...3789630501</v>
         <stp/>
         <stp>BDP|18255708956124343152</stp>
         <tr r="E26" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4102181453</v>
+        <v>#N/A Requesting Data...4242777602</v>
         <stp/>
         <stp>BDP|16855823919014233436</stp>
         <tr r="F30" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3967288727</v>
+        <v>#N/A Requesting Data...4055919642</v>
         <stp/>
         <stp>BDP|12821872971201299383</stp>
         <tr r="G124" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4194894409</v>
+        <v>#N/A Requesting Data...3715815420</v>
         <stp/>
         <stp>BDP|11466185903217969815</stp>
         <tr r="F33" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4242983788</v>
+        <v>#N/A Requesting Data...3739842703</v>
         <stp/>
         <stp>BDP|13711300257260836914</stp>
         <tr r="C102" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4156121969</v>
+        <v>#N/A Requesting Data...3813514650</v>
         <stp/>
         <stp>BDP|11622318103537999967</stp>
         <tr r="F15" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3983687119</v>
+        <v>#N/A Requesting Data...4108278260</v>
         <stp/>
         <stp>BDP|10597445640754361898</stp>
         <tr r="F50" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4050855709</v>
+        <v>#N/A Requesting Data...4015507631</v>
         <stp/>
         <stp>BDP|13987588094432951117</stp>
         <tr r="E127" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3929679802</v>
+        <v>#N/A Requesting Data...4004672391</v>
         <stp/>
         <stp>BDP|11655961067423868102</stp>
         <tr r="G104" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4037770250</v>
+        <v>#N/A Requesting Data...3855903510</v>
         <stp/>
         <stp>BDP|12468839190466923900</stp>
         <tr r="C20" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4050592134</v>
+        <v>#N/A Requesting Data...3763639943</v>
         <stp/>
         <stp>BDP|18411047804853597705</stp>
         <tr r="C67" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4087341723</v>
+        <v>#N/A Requesting Data...3874574207</v>
         <stp/>
         <stp>BDP|18331339124097518219</stp>
         <tr r="F66" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3835009002</v>
+        <v>#N/A Requesting Data...3735618464</v>
         <stp/>
         <stp>BDP|14983531083496973331</stp>
         <tr r="G132" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3905658838</v>
+        <v>#N/A Requesting Data...4252362543</v>
         <stp/>
         <stp>BDP|14115869171127460078</stp>
         <tr r="G37" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3970793098</v>
+        <v>#N/A Requesting Data...3712586628</v>
         <stp/>
         <stp>BDP|16963038037211063893</stp>
         <tr r="C13" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4073280365</v>
+        <v>#N/A Requesting Data...3862194290</v>
         <stp/>
         <stp>BDP|13900268704084418991</stp>
         <tr r="E37" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4253239281</v>
+        <v>#N/A Requesting Data...3937501614</v>
         <stp/>
         <stp>BDP|16311230542528118454</stp>
         <tr r="E9" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4042263989</v>
+        <v>#N/A Requesting Data...4068844929</v>
         <stp/>
         <stp>BDP|12403550728001134908</stp>
         <tr r="G38" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4260310572</v>
+        <v>#N/A Requesting Data...3849263416</v>
         <stp/>
         <stp>BDP|10528694388950747396</stp>
         <tr r="F80" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4077740579</v>
+        <v>#N/A Requesting Data...4225330012</v>
         <stp/>
         <stp>BDP|17962073596443790028</stp>
         <tr r="F23" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4238171738</v>
+        <v>#N/A Requesting Data...4214888431</v>
         <stp/>
         <stp>BDP|11322749828038387103</stp>
         <tr r="E122" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3913385953</v>
+        <v>#N/A Requesting Data...4157874441</v>
         <stp/>
         <stp>BDP|14872467854648029062</stp>
         <tr r="C75" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4040415744</v>
+        <v>#N/A Requesting Data...4003540637</v>
         <stp/>
         <stp>BDP|14951668809329151689</stp>
         <tr r="E56" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4123786034</v>
+        <v>#N/A Requesting Data...3949838596</v>
         <stp/>
         <stp>BDP|14211231849266296941</stp>
         <tr r="G103" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4129163512</v>
+        <v>#N/A Requesting Data...4217759461</v>
         <stp/>
         <stp>BDP|15282935006718574931</stp>
         <tr r="E92" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3832506130</v>
+        <v>#N/A Requesting Data...4288776602</v>
         <stp/>
         <stp>BDP|16389940868391785591</stp>
         <tr r="C120" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4085072805</v>
+        <v>#N/A Requesting Data...3782460224</v>
         <stp/>
         <stp>BDP|10830300668358540045</stp>
         <tr r="C115" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3916244869</v>
+        <v>#N/A Requesting Data...4038101368</v>
         <stp/>
         <stp>BDP|15417892931237679498</stp>
         <tr r="F8" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4232952533</v>
+        <v>#N/A Requesting Data...3720466309</v>
         <stp/>
         <stp>BDP|13776760394691002167</stp>
         <tr r="C4" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3941683127</v>
+        <v>#N/A Requesting Data...4255608986</v>
         <stp/>
         <stp>BDP|12950924085148446689</stp>
         <tr r="E121" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4033629673</v>
+        <v>#N/A Requesting Data...4103173843</v>
         <stp/>
         <stp>BDP|11202744698684518690</stp>
         <tr r="G111" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4081769740</v>
+        <v>#N/A Requesting Data...4134471993</v>
         <stp/>
         <stp>BDP|11005719894013994183</stp>
         <tr r="C3" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4118285208</v>
+        <v>#N/A Requesting Data...4010740088</v>
         <stp/>
         <stp>BDP|17061881470574956177</stp>
         <tr r="C69" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4256014887</v>
+        <v>#N/A Requesting Data...4232809097</v>
         <stp/>
         <stp>BDP|10195299258766033392</stp>
         <tr r="E90" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3957196912</v>
+        <v>#N/A Requesting Data...4239449222</v>
         <stp/>
         <stp>BDP|17559180385128709479</stp>
         <tr r="E15" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3847560974</v>
+        <v>#N/A Requesting Data...4184478731</v>
         <stp/>
         <stp>BDP|10477087317801173223</stp>
         <tr r="F125" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4231065098</v>
+        <v>#N/A Requesting Data...3885165547</v>
         <stp/>
         <stp>BDP|10431478218456128129</stp>
         <tr r="G32" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3900016541</v>
+        <v>#N/A Requesting Data...3719541900</v>
         <stp/>
         <stp>BDP|12817533695869473568</stp>
         <tr r="C82" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3889730343</v>
+        <v>#N/A Requesting Data...4028779754</v>
         <stp/>
         <stp>BDP|16722436137983528090</stp>
         <tr r="F127" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4287622696</v>
+        <v>#N/A Requesting Data...3866216667</v>
         <stp/>
         <stp>BDP|14949322880769358496</stp>
         <tr r="G16" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3941200501</v>
+        <v>#N/A Requesting Data...3845850965</v>
         <stp/>
         <stp>BDP|12620594347341901004</stp>
         <tr r="C76" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3969657936</v>
+        <v>#N/A Requesting Data...3994768203</v>
         <stp/>
         <stp>BDP|12047021516217693612</stp>
         <tr r="E126" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3889017418</v>
+        <v>#N/A Requesting Data...3965853537</v>
         <stp/>
         <stp>BDP|13612225533853005354</stp>
         <tr r="F102" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3928173110</v>
+        <v>#N/A Requesting Data...3923948554</v>
         <stp/>
         <stp>BDP|11536436753390219250</stp>
         <tr r="F129" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3932850521</v>
+        <v>#N/A Requesting Data...3888980933</v>
         <stp/>
         <stp>BDP|12946334758336119017</stp>
         <tr r="E72" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4153443894</v>
+        <v>#N/A Requesting Data...3972359311</v>
         <stp/>
         <stp>BDP|17733998071078953332</stp>
         <tr r="C23" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4085602482</v>
+        <v>#N/A Requesting Data...4128145364</v>
         <stp/>
         <stp>BDP|16362559715466602618</stp>
         <tr r="F68" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3954158766</v>
+        <v>#N/A Requesting Data...3923441085</v>
         <stp/>
         <stp>BDP|16070475881909673177</stp>
         <tr r="E112" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3930013742</v>
+        <v>#N/A Requesting Data...3821166789</v>
         <stp/>
         <stp>BDP|17590878194950224438</stp>
         <tr r="G87" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3972086725</v>
+        <v>#N/A Requesting Data...3736919126</v>
         <stp/>
         <stp>BDP|12427007793358727164</stp>
         <tr r="F100" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4123554973</v>
+        <v>#N/A Requesting Data...4192301686</v>
         <stp/>
         <stp>BDP|15601293270144483737</stp>
         <tr r="G15" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3904818320</v>
+        <v>#N/A Requesting Data...4142318778</v>
         <stp/>
         <stp>BDP|13723200346810339697</stp>
         <tr r="C38" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4165086327</v>
+        <v>#N/A Requesting Data...3780791477</v>
         <stp/>
         <stp>BDP|18086118189074176643</stp>
         <tr r="E88" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3991717687</v>
+        <v>#N/A Requesting Data...3850562052</v>
         <stp/>
         <stp>BDP|15679917748483251829</stp>
         <tr r="E6" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4127485883</v>
+        <v>#N/A Requesting Data...3811928410</v>
         <stp/>
         <stp>BDP|13421293548936861023</stp>
         <tr r="G66" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4113806937</v>
+        <v>#N/A Requesting Data...4055253438</v>
         <stp/>
         <stp>BDP|10594946509929542325</stp>
         <tr r="F5" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3930831896</v>
+        <v>#N/A Requesting Data...3916528819</v>
         <stp/>
         <stp>BDP|10668212108445960480</stp>
         <tr r="G57" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3976938694</v>
+        <v>#N/A Requesting Data...3981055296</v>
         <stp/>
         <stp>BDP|10103273213286136651</stp>
         <tr r="C6" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3902718926</v>
+        <v>#N/A Requesting Data...4029407828</v>
         <stp/>
         <stp>BDP|11259721862376480554</stp>
         <tr r="G69" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4218818791</v>
+        <v>#N/A Requesting Data...4084600666</v>
         <stp/>
         <stp>BDP|14885566279524266176</stp>
         <tr r="E30" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4186346132</v>
+        <v>#N/A Requesting Data...3782025563</v>
         <stp/>
         <stp>BDP|14519079130534129014</stp>
         <tr r="C49" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4065824291</v>
+        <v>#N/A Requesting Data...4157772126</v>
         <stp/>
         <stp>BDP|14873136635550817546</stp>
         <tr r="G130" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4088152712</v>
+        <v>#N/A Requesting Data...3906845388</v>
         <stp/>
         <stp>BDP|16641457892301341972</stp>
         <tr r="F130" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4274243353</v>
+        <v>#N/A Requesting Data...3820605786</v>
         <stp/>
         <stp>BDP|13231746637163726724</stp>
         <tr r="E7" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3896191177</v>
+        <v>#N/A Requesting Data...3769824919</v>
         <stp/>
         <stp>BDP|12945735048800380256</stp>
         <tr r="G118" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3990604420</v>
+        <v>#N/A Requesting Data...4135619376</v>
         <stp/>
         <stp>BDP|11265248170961260631</stp>
         <tr r="E47" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4020404293</v>
+        <v>#N/A Requesting Data...4015549366</v>
         <stp/>
         <stp>BDP|16351851074029385080</stp>
         <tr r="G35" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4100063599</v>
+        <v>#N/A Requesting Data...4289574953</v>
         <stp/>
         <stp>BDP|11944358991052271970</stp>
         <tr r="C103" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4279570101</v>
+        <v>#N/A Requesting Data...4274985090</v>
         <stp/>
         <stp>BDP|18410981990650283866</stp>
         <tr r="C99" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4059907230</v>
+        <v>#N/A Requesting Data...3925195095</v>
         <stp/>
         <stp>BDP|14383773052580838655</stp>
         <tr r="F104" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4192247115</v>
+        <v>#N/A Requesting Data...3970206489</v>
         <stp/>
         <stp>BDP|10871340643964419300</stp>
         <tr r="F95" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4284885116</v>
+        <v>#N/A Requesting Data...3962101529</v>
         <stp/>
         <stp>BDP|14690280185656044816</stp>
         <tr r="C94" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4067566648</v>
+        <v>#N/A Requesting Data...4009385647</v>
         <stp/>
         <stp>BDP|18305693996456795112</stp>
         <tr r="G80" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4007242924</v>
+        <v>#N/A Requesting Data...3903956740</v>
         <stp/>
         <stp>BDP|16273225567973824127</stp>
         <tr r="C79" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4294052762</v>
+        <v>#N/A Requesting Data...3910445700</v>
         <stp/>
         <stp>BDP|13313129291618997350</stp>
         <tr r="C43" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4240072798</v>
+        <v>#N/A Requesting Data...4002531030</v>
         <stp/>
         <stp>BDP|15444947284180871401</stp>
         <tr r="G27" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4185090690</v>
+        <v>#N/A Requesting Data...4183457531</v>
         <stp/>
         <stp>BDP|12935317504846234704</stp>
         <tr r="F98" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4114958799</v>
+        <v>#N/A Requesting Data...4293866495</v>
         <stp/>
         <stp>BDP|13057895365605005829</stp>
         <tr r="C138" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3972123535</v>
+        <v>#N/A Requesting Data...4233928023</v>
         <stp/>
         <stp>BDP|16160321537943284588</stp>
         <tr r="E76" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4257103329</v>
+        <v>#N/A Requesting Data...4063682295</v>
         <stp/>
         <stp>BDP|10621599828921836610</stp>
         <tr r="C12" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3922467468</v>
+        <v>#N/A Requesting Data...3982100701</v>
         <stp/>
         <stp>BDP|14881076967673386157</stp>
         <tr r="F122" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4014903222</v>
+        <v>#N/A Requesting Data...3958830716</v>
         <stp/>
         <stp>BDP|17321553610055816607</stp>
         <tr r="F96" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4128819473</v>
+        <v>#N/A Requesting Data...3831490489</v>
         <stp/>
         <stp>BDP|12793555755147383546</stp>
         <tr r="F42" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4255052446</v>
+        <v>#N/A Requesting Data...4008837764</v>
         <stp/>
         <stp>BDP|10194327202093986081</stp>
         <tr r="F132" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4242746142</v>
+        <v>#N/A Requesting Data...3882152658</v>
         <stp/>
         <stp>BDP|12798194599768683232</stp>
         <tr r="C42" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4064067269</v>
+        <v>#N/A Requesting Data...3789432313</v>
         <stp/>
         <stp>BDP|15675203172551734114</stp>
         <tr r="F12" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4129813957</v>
+        <v>#N/A Requesting Data...4181608202</v>
         <stp/>
         <stp>BDP|17779010845097021465</stp>
         <tr r="G23" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4081433913</v>
+        <v>#N/A Requesting Data...3827215005</v>
         <stp/>
         <stp>BDP|14698661432127374654</stp>
         <tr r="E53" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4126009736</v>
+        <v>#N/A Requesting Data...3937527172</v>
         <stp/>
         <stp>BDP|16055018629402477686</stp>
         <tr r="F18" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4035416018</v>
+        <v>#N/A Requesting Data...4273072254</v>
         <stp/>
         <stp>BDP|14191015466523343124</stp>
         <tr r="G42" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4228284077</v>
+        <v>#N/A Requesting Data...4179056873</v>
         <stp/>
         <stp>BDP|16690545673604064064</stp>
         <tr r="G6" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4124942242</v>
+        <v>#N/A Requesting Data...3950885477</v>
         <stp/>
         <stp>BDP|11057556593645206836</stp>
         <tr r="E116" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4175858335</v>
+        <v>#N/A Requesting Data...4064659021</v>
         <stp/>
         <stp>BDP|14753168038796700174</stp>
         <tr r="E131" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4263517485</v>
+        <v>#N/A Requesting Data...4049160098</v>
         <stp/>
         <stp>BDP|18400936140157917378</stp>
         <tr r="G108" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4182109787</v>
+        <v>#N/A Requesting Data...4255801130</v>
         <stp/>
         <stp>BDP|11308062409311166143</stp>
         <tr r="F138" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3992807509</v>
+        <v>#N/A Requesting Data...4119105963</v>
         <stp/>
         <stp>BDP|14929251921187622207</stp>
         <tr r="G120" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4289059774</v>
+        <v>#N/A Requesting Data...3868926601</v>
         <stp/>
         <stp>BDP|13312546151322475095</stp>
         <tr r="C117" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3956531848</v>
+        <v>#N/A Requesting Data...3797662668</v>
         <stp/>
         <stp>BDP|10370784365528062849</stp>
         <tr r="G51" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4281801057</v>
+        <v>#N/A Requesting Data...4195869048</v>
         <stp/>
         <stp>BDP|17808503947101138629</stp>
         <tr r="F128" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4272631882</v>
+        <v>#N/A Requesting Data...4262530422</v>
         <stp/>
         <stp>BDP|17640270888515662931</stp>
         <tr r="E20" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4045847174</v>
+        <v>#N/A Requesting Data...4174920295</v>
         <stp/>
         <stp>BDP|17853766030844520642</stp>
         <tr r="F65" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4040905348</v>
+        <v>#N/A Requesting Data...4175396313</v>
         <stp/>
         <stp>BDP|17345319339237647129</stp>
         <tr r="C10" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4158270106</v>
+        <v>#N/A Requesting Data...3913439302</v>
         <stp/>
         <stp>BDP|18428163184190295050</stp>
         <tr r="C48" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4079934245</v>
+        <v>#N/A Requesting Data...3996076963</v>
         <stp/>
         <stp>BDP|11469771160883398201</stp>
         <tr r="G20" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3957353800</v>
+        <v>#N/A Requesting Data...4110630158</v>
         <stp/>
         <stp>BDP|12945229628891094206</stp>
         <tr r="F36" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4194213604</v>
+        <v>#N/A Requesting Data...4236264309</v>
         <stp/>
         <stp>BDP|13088969316699575369</stp>
         <tr r="G17" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4231022491</v>
+        <v>#N/A Requesting Data...4146450232</v>
         <stp/>
         <stp>BDP|14386928546318260068</stp>
         <tr r="C78" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4101612964</v>
+        <v>#N/A Requesting Data...4277446044</v>
         <stp/>
         <stp>BDP|16250000632946565269</stp>
         <tr r="F32" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4017258711</v>
+        <v>#N/A Requesting Data...4268161809</v>
         <stp/>
         <stp>BDP|10062445544650347114</stp>
         <tr r="E69" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4127085648</v>
+        <v>#N/A Requesting Data...4243878473</v>
         <stp/>
         <stp>BDP|18056984346180923430</stp>
         <tr r="F67" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4262175570</v>
+        <v>#N/A Requesting Data...3961603607</v>
         <stp/>
         <stp>BDP|13607419850307697457</stp>
         <tr r="G55" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3985749101</v>
+        <v>#N/A Requesting Data...3840721055</v>
         <stp/>
         <stp>BDP|17151526894293450943</stp>
         <tr r="E34" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4233209853</v>
+        <v>#N/A Requesting Data...4109307142</v>
         <stp/>
         <stp>BDP|14769233272840536059</stp>
         <tr r="F48" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4202553697</v>
+        <v>#N/A Requesting Data...4245254799</v>
         <stp/>
         <stp>BDP|16347078018142331376</stp>
         <tr r="E59" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3949877321</v>
+        <v>#N/A Requesting Data...3984816695</v>
         <stp/>
         <stp>BDP|12157937398585487157</stp>
         <tr r="F69" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4114902819</v>
+        <v>#N/A Requesting Data...3964908911</v>
         <stp/>
         <stp>BDP|10450024654077121490</stp>
         <tr r="G29" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4193700368</v>
+        <v>#N/A Requesting Data...3843968508</v>
         <stp/>
         <stp>BDP|12405274734177384298</stp>
         <tr r="G109" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4221015412</v>
+        <v>#N/A Requesting Data...4287409680</v>
         <stp/>
         <stp>BDP|11693290023110245727</stp>
         <tr r="F93" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4138215748</v>
+        <v>#N/A Requesting Data...3972799483</v>
         <stp/>
         <stp>BDP|16857915317939051104</stp>
         <tr r="E4" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4195968958</v>
+        <v>#N/A Requesting Data...4127353415</v>
         <stp/>
         <stp>BDP|13092630751014311204</stp>
         <tr r="C29" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4284270694</v>
+        <v>#N/A Requesting Data...3882015561</v>
         <stp/>
         <stp>BDP|16560165422091315234</stp>
         <tr r="E74" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4132006698</v>
+        <v>#N/A Requesting Data...3880459477</v>
         <stp/>
         <stp>BDP|15578620992514708823</stp>
         <tr r="C74" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4193165411</v>
+        <v>#N/A Requesting Data...4106623690</v>
         <stp/>
         <stp>BDP|16311826266949112751</stp>
         <tr r="E137" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4047358762</v>
+        <v>#N/A Requesting Data...3892413226</v>
         <stp/>
         <stp>BDP|12423551309476829732</stp>
         <tr r="E29" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4194333025</v>
+        <v>#N/A Requesting Data...3903370690</v>
         <stp/>
         <stp>BDP|15334425393507822980</stp>
         <tr r="C71" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4082668081</v>
+        <v>#N/A Requesting Data...4172102319</v>
         <stp/>
         <stp>BDP|14187404668490888034</stp>
         <tr r="E115" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3990398278</v>
+        <v>#N/A Requesting Data...4207626703</v>
         <stp/>
         <stp>BDP|14038301256494491076</stp>
         <tr r="E12" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4264781593</v>
+        <v>#N/A Requesting Data...3988065021</v>
         <stp/>
         <stp>BDP|12212063840830333025</stp>
         <tr r="E132" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4141909181</v>
+        <v>#N/A Requesting Data...4011930538</v>
         <stp/>
         <stp>BDP|12411228970299104833</stp>
         <tr r="E40" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4093718663</v>
+        <v>#N/A Requesting Data...4246691729</v>
         <stp/>
         <stp>BDP|11324255971734653659</stp>
         <tr r="G93" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4284629359</v>
+        <v>#N/A Requesting Data...3945092227</v>
         <stp/>
         <stp>BDP|15080702944965265524</stp>
         <tr r="E5" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4210730656</v>
+        <v>#N/A Requesting Data...4110323298</v>
         <stp/>
         <stp>BDP|12709330545317601409</stp>
         <tr r="F78" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4231383906</v>
+        <v>#N/A Requesting Data...3980255103</v>
         <stp/>
         <stp>BDP|17558583635766924170</stp>
         <tr r="C139" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4027542372</v>
+        <v>#N/A Requesting Data...4224113963</v>
         <stp/>
         <stp>BDP|14043797868641345244</stp>
         <tr r="G127" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4166872417</v>
+        <v>#N/A Requesting Data...3942705804</v>
         <stp/>
         <stp>BDP|11097146762171726091</stp>
         <tr r="C125" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4216510144</v>
+        <v>#N/A Requesting Data...4235245989</v>
         <stp/>
         <stp>BDP|10083242995488903402</stp>
         <tr r="E22" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4174251786</v>
+        <v>#N/A Requesting Data...4100293387</v>
         <stp/>
         <stp>BDP|14104003677163905777</stp>
         <tr r="G89" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4259669742</v>
+        <v>#N/A Requesting Data...4143639241</v>
         <stp/>
         <stp>BDP|10493155251505330684</stp>
         <tr r="F113" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4099404140</v>
+        <v>#N/A Requesting Data...4075777882</v>
         <stp/>
         <stp>BDP|17307159600861837050</stp>
         <tr r="C28" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3988490173</v>
+        <v>#N/A Requesting Data...4086712737</v>
         <stp/>
         <stp>BDP|11974207352247436657</stp>
         <tr r="G84" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4217257414</v>
+        <v>#N/A Requesting Data...3922265052</v>
         <stp/>
         <stp>BDP|12417029733397010193</stp>
         <tr r="G129" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4055521959</v>
+        <v>#N/A Requesting Data...4272931456</v>
         <stp/>
         <stp>BDP|13696428749777505366</stp>
         <tr r="C128" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4217838683</v>
+        <v>#N/A Requesting Data...4288303824</v>
         <stp/>
         <stp>BDP|10265435339313984301</stp>
         <tr r="F136" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4209840863</v>
+        <v>#N/A Requesting Data...4079119593</v>
         <stp/>
         <stp>BDP|16742662035804692035</stp>
         <tr r="E24" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4216836040</v>
+        <v>#N/A Requesting Data...4093720398</v>
         <stp/>
         <stp>BDP|13311072247345018521</stp>
         <tr r="E129" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4012304579</v>
+        <v>#N/A Requesting Data...4192760549</v>
         <stp/>
         <stp>BDP|14635385909938704819</stp>
         <tr r="E106" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4237096382</v>
+        <v>#N/A Requesting Data...4179204759</v>
         <stp/>
         <stp>BDP|17965266240553639582</stp>
         <tr r="E10" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4293441329</v>
+        <v>#N/A Requesting Data...4097899956</v>
         <stp/>
         <stp>BDP|14559650107303581628</stp>
         <tr r="C72" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4002301313</v>
+        <v>#N/A Requesting Data...4047406248</v>
         <stp/>
         <stp>BDP|12078771150016496119</stp>
         <tr r="G102" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4151271904</v>
+        <v>#N/A Requesting Data...4290665076</v>
         <stp/>
         <stp>BDP|13437131854538783812</stp>
         <tr r="G22" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4274515865</v>
+        <v>#N/A Requesting Data...4283773006</v>
         <stp/>
         <stp>BDP|11816803688615161347</stp>
         <tr r="E51" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4230726052</v>
+        <v>#N/A Requesting Data...3900232939</v>
         <stp/>
         <stp>BDP|11136233214231371414</stp>
         <tr r="G139" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4242646261</v>
+        <v>#N/A Requesting Data...4135146810</v>
         <stp/>
         <stp>BDP|16387121100332435221</stp>
         <tr r="G96" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4161361902</v>
+        <v>#N/A Requesting Data...4088537188</v>
         <stp/>
         <stp>BDP|10044993787394494110</stp>
         <tr r="C113" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4165806239</v>
+        <v>#N/A Requesting Data...4043925487</v>
         <stp/>
         <stp>BDP|16851432539276999316</stp>
         <tr r="E44" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4246690164</v>
+        <v>#N/A Requesting Data...4102075933</v>
         <stp/>
         <stp>BDP|17514330731974993734</stp>
         <tr r="E65" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4007502134</v>
+        <v>#N/A Requesting Data...3903739618</v>
         <stp/>
         <stp>BDP|13397290692205579908</stp>
         <tr r="G128" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4137598091</v>
+        <v>#N/A Requesting Data...3912652524</v>
         <stp/>
         <stp>BDP|11770519860203890508</stp>
         <tr r="F106" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4099615291</v>
+        <v>#N/A Requesting Data...4136430582</v>
         <stp/>
         <stp>BDP|11828615722360397168</stp>
         <tr r="E71" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4209741732</v>
+        <v>#N/A Requesting Data...4147888412</v>
         <stp/>
         <stp>BDP|12429929188915695292</stp>
         <tr r="F109" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4132559050</v>
+        <v>#N/A Requesting Data...3898002279</v>
         <stp/>
         <stp>BDP|14807781952773549162</stp>
         <tr r="G33" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4226379380</v>
+        <v>#N/A Requesting Data...3910882585</v>
         <stp/>
         <stp>BDP|14141528956866623622</stp>
         <tr r="C134" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4052807459</v>
+        <v>#N/A Requesting Data...4218229505</v>
         <stp/>
         <stp>BDP|11925450918217650729</stp>
         <tr r="F86" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4139041670</v>
+        <v>#N/A Requesting Data...3997814971</v>
         <stp/>
         <stp>BDP|10075353521710450506</stp>
         <tr r="C109" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4086706456</v>
+        <v>#N/A Requesting Data...4156746288</v>
         <stp/>
         <stp>BDP|14507687284196916837</stp>
         <tr r="F6" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4029425110</v>
+        <v>#N/A Requesting Data...4062077742</v>
         <stp/>
         <stp>BDP|17592946715913980887</stp>
         <tr r="F7" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4127270361</v>
+        <v>#N/A Requesting Data...3936975363</v>
         <stp/>
         <stp>BDP|12670343566891576248</stp>
         <tr r="G36" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4144698312</v>
+        <v>#N/A Requesting Data...4268450078</v>
         <stp/>
         <stp>BDP|16059776447550017157</stp>
         <tr r="F63" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4028457140</v>
+        <v>#N/A Requesting Data...3897561636</v>
         <stp/>
         <stp>BDP|13709786759646324310</stp>
         <tr r="F46" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4068850106</v>
+        <v>#N/A Requesting Data...4016344473</v>
         <stp/>
         <stp>BDP|17680007951225535344</stp>
         <tr r="C93" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4037043523</v>
+        <v>#N/A Requesting Data...4147190011</v>
         <stp/>
         <stp>BDP|14249466628496635139</stp>
         <tr r="F26" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4253743191</v>
+        <v>#N/A Requesting Data...4220379217</v>
         <stp/>
         <stp>BDP|12616286245214000526</stp>
         <tr r="C114" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4238672586</v>
+        <v>#N/A Requesting Data...4117358004</v>
         <stp/>
         <stp>BDP|13229487552560837780</stp>
         <tr r="E139" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4180457815</v>
+        <v>#N/A Requesting Data...4114908813</v>
         <stp/>
         <stp>BDP|18412208651713792994</stp>
         <tr r="F118" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4138484527</v>
+        <v>#N/A Requesting Data...3914998288</v>
         <stp/>
         <stp>BDP|16919456577607807790</stp>
         <tr r="G56" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4110595061</v>
+        <v>#N/A Requesting Data...4240735050</v>
         <stp/>
         <stp>BDP|14958917677776306912</stp>
         <tr r="E124" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4116639937</v>
+        <v>#N/A Requesting Data...4106643057</v>
         <stp/>
         <stp>BDP|16906362551851442479</stp>
         <tr r="F14" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4207883705</v>
+        <v>#N/A Requesting Data...4041295239</v>
         <stp/>
         <stp>BDP|13303498173634341154</stp>
         <tr r="G72" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4268401968</v>
+        <v>#N/A Requesting Data...4126853206</v>
         <stp/>
         <stp>BDP|11394026073756494578</stp>
         <tr r="F4" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4167730100</v>
+        <v>#N/A Requesting Data...4044536328</v>
         <stp/>
         <stp>BDP|12821707660430898618</stp>
         <tr r="C40" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4189953527</v>
+        <v>#N/A Requesting Data...4093385864</v>
         <stp/>
         <stp>BDP|12207042919767891145</stp>
         <tr r="G131" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4126317930</v>
+        <v>#N/A Requesting Data...4148270083</v>
         <stp/>
         <stp>BDP|17617562141366516571</stp>
         <tr r="F24" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4059576820</v>
+        <v>#N/A Requesting Data...4186174723</v>
         <stp/>
         <stp>BDP|13776066979946925741</stp>
         <tr r="C90" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4059919298</v>
+        <v>#N/A Requesting Data...3953853568</v>
         <stp/>
         <stp>BDP|15429465971742273156</stp>
         <tr r="E67" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4291921622</v>
+        <v>#N/A Requesting Data...4168485936</v>
         <stp/>
         <stp>BDP|13319017160191784122</stp>
         <tr r="E43" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4165406142</v>
+        <v>#N/A Requesting Data...4244600025</v>
         <stp/>
         <stp>BDP|17197570677470339052</stp>
         <tr r="E33" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4224246976</v>
+        <v>#N/A Requesting Data...4260703250</v>
         <stp/>
         <stp>BDP|18198100188843948773</stp>
         <tr r="G60" s="1"/>
@@ -2724,1783 +2727,1783 @@
     </main>
     <main first="bofaddin.rtdserver">
       <tp t="s">
-        <v>#N/A Requesting Data...4104479652</v>
+        <v>#N/A Requesting Data...3923079893</v>
         <stp/>
         <stp>BDP|3930904544763426134</stp>
         <tr r="C55" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4188784700</v>
+        <v>#N/A Requesting Data...4095691644</v>
         <stp/>
         <stp>BDP|7103625188072362707</stp>
         <tr r="E98" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4234510974</v>
+        <v>#N/A Requesting Data...4246259143</v>
         <stp/>
         <stp>BDP|9365312653090978315</stp>
         <tr r="G136" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4163678681</v>
+        <v>#N/A Requesting Data...3977594600</v>
         <stp/>
         <stp>BDP|6412151529379694002</stp>
         <tr r="F110" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4153113622</v>
+        <v>#N/A Requesting Data...4051958392</v>
         <stp/>
         <stp>BDP|6245426297947871034</stp>
         <tr r="C80" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4209262050</v>
+        <v>#N/A Requesting Data...4253564460</v>
         <stp/>
         <stp>BDP|2350385774053258906</stp>
         <tr r="F72" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4211106883</v>
+        <v>#N/A Requesting Data...4004663020</v>
         <stp/>
         <stp>BDP|8530657130876609747</stp>
         <tr r="C44" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4255001518</v>
+        <v>#N/A Requesting Data...4265411192</v>
         <stp/>
         <stp>BDP|7198979431090342164</stp>
         <tr r="E50" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4105484428</v>
+        <v>#N/A Requesting Data...4198570260</v>
         <stp/>
         <stp>BDP|9075300299347332881</stp>
         <tr r="G79" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4123999987</v>
+        <v>#N/A Requesting Data...3971912727</v>
         <stp/>
         <stp>BDP|5029740995104753357</stp>
         <tr r="C111" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4067661789</v>
+        <v>#N/A Requesting Data...4141519438</v>
         <stp/>
         <stp>BDP|8128743572863334748</stp>
         <tr r="C47" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4254312088</v>
+        <v>#N/A Requesting Data...4042984356</v>
         <stp/>
         <stp>BDP|6339719327836450907</stp>
         <tr r="C98" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4151322747</v>
+        <v>#N/A Requesting Data...4237773302</v>
         <stp/>
         <stp>BDP|4200580269163222863</stp>
         <tr r="E25" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4100164363</v>
+        <v>#N/A Requesting Data...4029251741</v>
         <stp/>
         <stp>BDP|5989352249668473659</stp>
         <tr r="G50" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4266260763</v>
+        <v>#N/A Requesting Data...4278589162</v>
         <stp/>
         <stp>BDP|2484433252649720677</stp>
         <tr r="G68" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4286797811</v>
+        <v>#N/A Requesting Data...3964639861</v>
         <stp/>
         <stp>BDP|6249870436562567333</stp>
         <tr r="E49" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4176065030</v>
+        <v>#N/A Requesting Data...4052716193</v>
         <stp/>
         <stp>BDP|9572192910556051262</stp>
         <tr r="E134" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4178429609</v>
+        <v>#N/A Requesting Data...4157966939</v>
         <stp/>
         <stp>BDP|7540551159163224910</stp>
         <tr r="F51" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4217296302</v>
+        <v>#N/A Requesting Data...4291924839</v>
         <stp/>
         <stp>BDP|8451204331587951367</stp>
         <tr r="F52" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4096274765</v>
+        <v>#N/A Requesting Data...4163563999</v>
         <stp/>
         <stp>BDP|3109256470563958869</stp>
         <tr r="C52" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4253722583</v>
+        <v>#N/A Requesting Data...4262880956</v>
         <stp/>
         <stp>BDP|3590543194827878545</stp>
         <tr r="F59" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4197063792</v>
+        <v>#N/A Requesting Data...4206181717</v>
         <stp/>
         <stp>BDP|3009997314886390075</stp>
         <tr r="G100" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4094495558</v>
+        <v>#N/A Requesting Data...4287833446</v>
         <stp/>
         <stp>BDP|4777106988391072114</stp>
         <tr r="F103" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4115864580</v>
+        <v>#N/A Requesting Data...3977810480</v>
         <stp/>
         <stp>BDP|4303401897634933024</stp>
         <tr r="E93" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4141601550</v>
+        <v>#N/A Requesting Data...3985851484</v>
         <stp/>
         <stp>BDP|9055938583773500695</stp>
         <tr r="C34" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4250799344</v>
+        <v>#N/A Requesting Data...4288560979</v>
         <stp/>
         <stp>BDP|1573317174439842142</stp>
         <tr r="E133" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4227499424</v>
+        <v>#N/A Requesting Data...4219555876</v>
         <stp/>
         <stp>BDP|7180318607099335068</stp>
         <tr r="C9" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4202570645</v>
+        <v>#N/A Requesting Data...4171464529</v>
         <stp/>
         <stp>BDP|8371873502449565411</stp>
         <tr r="C62" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4229343704</v>
+        <v>#N/A Requesting Data...3997055861</v>
         <stp/>
         <stp>BDP|9300723062997279226</stp>
         <tr r="C124" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4202617703</v>
+        <v>#N/A Requesting Data...3973618511</v>
         <stp/>
         <stp>BDP|5492561896244379063</stp>
         <tr r="F70" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4222162846</v>
+        <v>#N/A Requesting Data...4258716274</v>
         <stp/>
         <stp>BDP|8460669760190400504</stp>
         <tr r="C27" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4228961193</v>
+        <v>#N/A Requesting Data...3999859084</v>
         <stp/>
         <stp>BDP|7634975275120208406</stp>
         <tr r="C31" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4237518174</v>
+        <v>#N/A Requesting Data...4066268547</v>
         <stp/>
         <stp>BDP|4040591290066838371</stp>
         <tr r="E13" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4213626079</v>
+        <v>#N/A Requesting Data...4293769777</v>
         <stp/>
         <stp>BDP|9247766641156585153</stp>
         <tr r="G94" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4242260332</v>
+        <v>#N/A Requesting Data...4141294519</v>
         <stp/>
         <stp>BDP|7940113982976758589</stp>
         <tr r="E95" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4236477633</v>
+        <v>#N/A Requesting Data...4114652571</v>
         <stp/>
         <stp>BDP|9093620553903200797</stp>
         <tr r="C105" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4269467212</v>
+        <v>#N/A Requesting Data...4156493636</v>
         <stp/>
         <stp>BDP|2405932012622401695</stp>
         <tr r="G77" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4266164066</v>
+        <v>#N/A Requesting Data...4260118207</v>
         <stp/>
         <stp>BDP|9175353808212225665</stp>
         <tr r="C66" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4193381099</v>
+        <v>#N/A Requesting Data...4216807160</v>
         <stp/>
         <stp>BDP|1414608591110891051</stp>
         <tr r="F9" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4291367155</v>
+        <v>#N/A Requesting Data...4083828523</v>
         <stp/>
         <stp>BDP|3649732806419915339</stp>
         <tr r="G14" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4230660934</v>
+        <v>#N/A Requesting Data...4217343641</v>
         <stp/>
         <stp>BDP|7006257261095505888</stp>
         <tr r="F54" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4294689463</v>
+        <v>#N/A Requesting Data...4258199924</v>
         <stp/>
         <stp>BDP|9781989741438009272</stp>
         <tr r="C39" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4272519622</v>
+        <v>#N/A Requesting Data...4235430061</v>
         <stp/>
         <stp>BDP|7532189862547338936</stp>
         <tr r="F58" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4175556237</v>
+        <v>#N/A Requesting Data...4113498576</v>
         <stp/>
         <stp>BDP|4286027170164748985</stp>
         <tr r="G113" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4202149636</v>
+        <v>#N/A Requesting Data...4039053940</v>
         <stp/>
         <stp>BDP|4691882821088256816</stp>
         <tr r="F126" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4231738254</v>
+        <v>#N/A Requesting Data...4084460802</v>
         <stp/>
         <stp>BDP|4974055815239706225</stp>
         <tr r="G110" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4199211634</v>
+        <v>#N/A Requesting Data...4074951647</v>
         <stp/>
         <stp>BDP|5916130291376545539</stp>
         <tr r="F73" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4175314278</v>
+        <v>#N/A Requesting Data...4030072965</v>
         <stp/>
         <stp>BDP|9535646277681935723</stp>
         <tr r="E60" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4261845675</v>
+        <v>#N/A Requesting Data...4024262874</v>
         <stp/>
         <stp>BDP|3472420329653378814</stp>
         <tr r="G4" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4192616098</v>
+        <v>#N/A Requesting Data...4043912315</v>
         <stp/>
         <stp>BDP|9676580711333862054</stp>
         <tr r="E135" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4224850532</v>
+        <v>#N/A Requesting Data...4124399086</v>
         <stp/>
         <stp>BDP|8651287802994649096</stp>
         <tr r="E77" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4241285780</v>
+        <v>#N/A Requesting Data...4266541641</v>
         <stp/>
         <stp>BDP|5552297197720045083</stp>
         <tr r="E118" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4221760258</v>
+        <v>#N/A Requesting Data...4180638834</v>
         <stp/>
         <stp>BDP|6195991527552839107</stp>
         <tr r="C61" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4191142298</v>
+        <v>#N/A Requesting Data...4231365302</v>
         <stp/>
         <stp>BDP|2785537291931900199</stp>
         <tr r="G91" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4177243459</v>
+        <v>#N/A Requesting Data...4001734655</v>
         <stp/>
         <stp>BDP|9875435960971965593</stp>
         <tr r="C11" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4277279652</v>
+        <v>#N/A Requesting Data...4137648557</v>
         <stp/>
         <stp>BDP|7662972721973338089</stp>
         <tr r="F107" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4202007928</v>
+        <v>#N/A Requesting Data...4008262823</v>
         <stp/>
         <stp>BDP|4282903616430488389</stp>
         <tr r="G9" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4262590637</v>
+        <v>#N/A Requesting Data...4110115524</v>
         <stp/>
         <stp>BDP|6606398548307737925</stp>
         <tr r="C70" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4199704593</v>
+        <v>#N/A Requesting Data...4217351844</v>
         <stp/>
         <stp>BDP|2310021551041423963</stp>
         <tr r="F123" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4273172314</v>
+        <v>#N/A Requesting Data...4260593752</v>
         <stp/>
         <stp>BDP|1666950877162018261</stp>
         <tr r="E87" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4247851091</v>
+        <v>#N/A Requesting Data...4267345485</v>
         <stp/>
         <stp>BDP|6280569068792932854</stp>
         <tr r="C46" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4284550654</v>
+        <v>#N/A Requesting Data...4096766064</v>
         <stp/>
         <stp>BDP|9635152443296662577</stp>
         <tr r="C16" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4232777372</v>
+        <v>#N/A Requesting Data...4110478362</v>
         <stp/>
         <stp>BDP|5935740968278021330</stp>
         <tr r="C96" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4186116908</v>
+        <v>#N/A Requesting Data...4016344274</v>
         <stp/>
         <stp>BDP|8225387168083679130</stp>
         <tr r="E57" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4265981759</v>
+        <v>#N/A Requesting Data...4241517311</v>
         <stp/>
         <stp>BDP|8741792397660502982</stp>
         <tr r="G24" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4270347395</v>
+        <v>#N/A Requesting Data...4124877443</v>
         <stp/>
         <stp>BDP|1988621838892198978</stp>
         <tr r="F82" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4220116631</v>
+        <v>#N/A Requesting Data...4203430329</v>
         <stp/>
         <stp>BDP|5160947801244572083</stp>
         <tr r="C97" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4204653187</v>
+        <v>#N/A Requesting Data...4058357607</v>
         <stp/>
         <stp>BDP|8781684350665372626</stp>
         <tr r="G64" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4281679497</v>
+        <v>#N/A Requesting Data...4088047522</v>
         <stp/>
         <stp>BDP|8866465832365619258</stp>
         <tr r="F120" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4193967797</v>
+        <v>#N/A Requesting Data...4230166511</v>
         <stp/>
         <stp>BDP|1231973558974048121</stp>
         <tr r="E123" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4220863716</v>
+        <v>#N/A Requesting Data...4114695091</v>
         <stp/>
         <stp>BDP|9011959145835954962</stp>
         <tr r="E102" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4240706823</v>
+        <v>#N/A Requesting Data...4042925524</v>
         <stp/>
         <stp>BDP|7048111723254898858</stp>
         <tr r="E70" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4248409224</v>
+        <v>#N/A Requesting Data...4035131771</v>
         <stp/>
         <stp>BDP|7514426398370500271</stp>
         <tr r="F84" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4256049071</v>
+        <v>#N/A Requesting Data...4148728193</v>
         <stp/>
         <stp>BDP|2286847884578687294</stp>
         <tr r="C64" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4248617159</v>
+        <v>#N/A Requesting Data...4292259595</v>
         <stp/>
         <stp>BDP|8581359335587083771</stp>
         <tr r="G40" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4204969758</v>
+        <v>#N/A Requesting Data...4180550797</v>
         <stp/>
         <stp>BDP|9176352611073152053</stp>
         <tr r="G52" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4278130762</v>
+        <v>#N/A Requesting Data...4127792532</v>
         <stp/>
         <stp>BDP|3761613276703138977</stp>
         <tr r="C22" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4206978521</v>
+        <v>#N/A Requesting Data...4270794025</v>
         <stp/>
         <stp>BDP|2402283480247992710</stp>
         <tr r="G65" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4214323520</v>
+        <v>#N/A Requesting Data...4121465250</v>
         <stp/>
         <stp>BDP|2496054182730824314</stp>
         <tr r="F108" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4245069072</v>
+        <v>#N/A Requesting Data...4185235680</v>
         <stp/>
         <stp>BDP|1156198294412416234</stp>
         <tr r="G48" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4232801230</v>
+        <v>#N/A Requesting Data...4080638452</v>
         <stp/>
         <stp>BDP|1935863512592400318</stp>
         <tr r="G99" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4292750752</v>
+        <v>#N/A Requesting Data...4198201776</v>
         <stp/>
         <stp>BDP|1182070188629538920</stp>
         <tr r="F85" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4256480783</v>
+        <v>#N/A Requesting Data...4154639777</v>
         <stp/>
         <stp>BDP|9924697901094165296</stp>
         <tr r="E38" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4291896345</v>
+        <v>#N/A Requesting Data...4194915678</v>
         <stp/>
         <stp>BDP|6412137247758825261</stp>
         <tr r="G10" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4246980787</v>
+        <v>#N/A Requesting Data...4097878890</v>
         <stp/>
         <stp>BDP|6277108296426856136</stp>
         <tr r="G122" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4267605346</v>
+        <v>#N/A Requesting Data...4279539750</v>
         <stp/>
         <stp>BDP|2351176324921816947</stp>
         <tr r="E117" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4290149978</v>
+        <v>#N/A Requesting Data...4259418694</v>
         <stp/>
         <stp>BDP|6406207188846485346</stp>
         <tr r="C37" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4278656782</v>
+        <v>#N/A Requesting Data...4216606896</v>
         <stp/>
         <stp>BDP|8112280367483097628</stp>
         <tr r="F16" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4257707996</v>
+        <v>#N/A Requesting Data...4151893060</v>
         <stp/>
         <stp>BDP|6484624822372932905</stp>
         <tr r="C108" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4289885141</v>
+        <v>#N/A Requesting Data...4083861198</v>
         <stp/>
         <stp>BDP|8605875253514357834</stp>
         <tr r="C116" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4271306657</v>
+        <v>#N/A Requesting Data...4081497365</v>
         <stp/>
         <stp>BDP|2842991807747556512</stp>
         <tr r="E110" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4243420576</v>
+        <v>#N/A Requesting Data...4046362942</v>
         <stp/>
         <stp>BDP|1377759003508711718</stp>
         <tr r="E55" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4259764932</v>
+        <v>#N/A Requesting Data...4280227827</v>
         <stp/>
         <stp>BDP|1711361391887412536</stp>
         <tr r="G47" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4260442174</v>
+        <v>#N/A Requesting Data...4286640457</v>
         <stp/>
         <stp>BDP|4564815655442574234</stp>
         <tr r="F114" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4271845568</v>
+        <v>#N/A Requesting Data...4074257609</v>
         <stp/>
         <stp>BDP|6557751567646791843</stp>
         <tr r="C85" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4286574921</v>
+        <v>#N/A Requesting Data...4251900310</v>
         <stp/>
         <stp>BDP|5018226780961297742</stp>
         <tr r="E138" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4247455862</v>
+        <v>#N/A Requesting Data...4137298874</v>
         <stp/>
         <stp>BDP|7190582290036507495</stp>
         <tr r="E48" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4279917839</v>
+        <v>#N/A Requesting Data...4126875382</v>
         <stp/>
         <stp>BDP|7268732641219205478</stp>
         <tr r="F111" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4273405602</v>
+        <v>#N/A Requesting Data...4287333017</v>
         <stp/>
         <stp>BDP|5085458293997400582</stp>
         <tr r="C30" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4276346217</v>
+        <v>#N/A Requesting Data...4220865126</v>
         <stp/>
         <stp>BDP|2916061605678582044</stp>
         <tr r="E27" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4253847585</v>
+        <v>#N/A Requesting Data...4096166077</v>
         <stp/>
         <stp>BDP|5645196194854205325</stp>
         <tr r="E19" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4282732681</v>
+        <v>#N/A Requesting Data...4205431670</v>
         <stp/>
         <stp>BDP|8929421222763426766</stp>
         <tr r="F112" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4287593501</v>
+        <v>#N/A Requesting Data...4242242025</v>
         <stp/>
         <stp>BDP|2815946348173965667</stp>
         <tr r="C137" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4277973045</v>
+        <v>#N/A Requesting Data...4062140015</v>
         <stp/>
         <stp>BDP|6645611732949919042</stp>
         <tr r="G95" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4289756908</v>
+        <v>#N/A Requesting Data...4062275810</v>
         <stp/>
         <stp>BDP|8744658502964028082</stp>
         <tr r="F139" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4290660915</v>
+        <v>#N/A Requesting Data...4211850039</v>
         <stp/>
         <stp>BDP|4077907452745230782</stp>
         <tr r="C130" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4270322122</v>
+        <v>#N/A Requesting Data...4259778935</v>
         <stp/>
         <stp>BDP|8975856381415089739</stp>
         <tr r="E75" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4263511174</v>
+        <v>#N/A Requesting Data...4082431523</v>
         <stp/>
         <stp>BDP|5738611839292209825</stp>
         <tr r="G107" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4267013029</v>
+        <v>#N/A Requesting Data...4171328222</v>
         <stp/>
         <stp>BDP|4996818111432201578</stp>
         <tr r="G134" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4283164756</v>
+        <v>#N/A Requesting Data...4160182087</v>
         <stp/>
         <stp>BDP|5458032582021895609</stp>
         <tr r="E89" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4294580133</v>
+        <v>#N/A Requesting Data...4262102881</v>
         <stp/>
         <stp>BDP|2612461303954522846</stp>
         <tr r="F21" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4284853951</v>
+        <v>#N/A Requesting Data...4250298769</v>
         <stp/>
         <stp>BDP|5852840000806674187</stp>
         <tr r="F75" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4291444476</v>
+        <v>#N/A Requesting Data...4099057511</v>
         <stp/>
         <stp>BDP|7947641811679527399</stp>
         <tr r="G13" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4294046931</v>
+        <v>#N/A Requesting Data...4249974173</v>
         <stp/>
         <stp>BDP|8407769428857900025</stp>
         <tr r="C132" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4278556231</v>
+        <v>#N/A Requesting Data...4225677840</v>
         <stp/>
         <stp>BDP|1313714864639868399</stp>
         <tr r="F87" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4292613932</v>
+        <v>#N/A Requesting Data...4281886868</v>
         <stp/>
         <stp>BDP|2531298252748844733</stp>
         <tr r="F115" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4281922589</v>
+        <v>#N/A Requesting Data...4106765695</v>
         <stp/>
         <stp>BDP|8965389266391509672</stp>
         <tr r="C41" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4284209880</v>
+        <v>#N/A Requesting Data...4280341763</v>
         <stp/>
         <stp>BDP|9146373380128430189</stp>
         <tr r="F60" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4285415355</v>
+        <v>#N/A Requesting Data...4271703871</v>
         <stp/>
         <stp>BDP|8769626454200391097</stp>
         <tr r="G85" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4291108054</v>
+        <v>#N/A Requesting Data...4180022670</v>
         <stp/>
         <stp>BDP|7701346097304455298</stp>
         <tr r="C73" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4293083136</v>
+        <v>#N/A Requesting Data...4276702843</v>
         <stp/>
         <stp>BDP|1201589979318261083</stp>
         <tr r="G123" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4291775463</v>
+        <v>#N/A Requesting Data...4117657732</v>
         <stp/>
         <stp>BDP|9994425762708075853</stp>
         <tr r="G88" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4294106765</v>
+        <v>#N/A Requesting Data...4137249136</v>
         <stp/>
         <stp>BDP|8238868892513701135</stp>
         <tr r="G137" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4294664615</v>
+        <v>#N/A Requesting Data...4251829887</v>
         <stp/>
         <stp>BDP|3321556007464177923</stp>
         <tr r="E109" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1071692591</v>
+        <v>#N/A Requesting Data...4220005355</v>
         <stp/>
         <stp>BDP|8367368187378355023</stp>
         <tr r="F64" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3820836795</v>
+        <v>#N/A Requesting Data...4271937895</v>
         <stp/>
         <stp>BDP|9054142235387080711</stp>
         <tr r="F11" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1998729970</v>
+        <v>#N/A Requesting Data...4188191774</v>
         <stp/>
         <stp>BDP|4797724273716399932</stp>
         <tr r="C5" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3900063910</v>
+        <v>#N/A Requesting Data...4270037777</v>
         <stp/>
         <stp>BDP|3084971212582403246</stp>
         <tr r="F121" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2901830721</v>
+        <v>#N/A Requesting Data...4200064194</v>
         <stp/>
         <stp>BDP|6948762204713990690</stp>
         <tr r="G90" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...721574389</v>
+        <v>#N/A Requesting Data...4265350391</v>
         <stp/>
         <stp>BDP|1832764578595986067</stp>
         <tr r="G119" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2399543749</v>
+        <v>#N/A Requesting Data...4130995580</v>
         <stp/>
         <stp>BDP|4156639623951685595</stp>
         <tr r="F13" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3654038026</v>
+        <v>#N/A Requesting Data...4200622876</v>
         <stp/>
         <stp>BDP|5919761437851372455</stp>
         <tr r="C2" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3214164253</v>
+        <v>#N/A Requesting Data...4129452485</v>
         <stp/>
         <stp>BDP|1551339666687413790</stp>
         <tr r="F40" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4130049046</v>
+        <v>#N/A Requesting Data...4199727439</v>
         <stp/>
         <stp>BDP|6420437202397070174</stp>
         <tr r="C8" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2672098065</v>
+        <v>#N/A Requesting Data...4195785560</v>
         <stp/>
         <stp>BDP|1708381902825815365</stp>
         <tr r="C101" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...740457014</v>
+        <v>#N/A Requesting Data...4158106240</v>
         <stp/>
         <stp>BDP|4945796250777738578</stp>
         <tr r="G21" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1166328388</v>
+        <v>#N/A Requesting Data...4288558790</v>
         <stp/>
         <stp>BDP|6746841414412327938</stp>
         <tr r="G75" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4095843971</v>
+        <v>#N/A Requesting Data...4207373712</v>
         <stp/>
         <stp>BDP|1709445403856801620</stp>
         <tr r="E85" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...497844212</v>
+        <v>#N/A Requesting Data...4199580400</v>
         <stp/>
         <stp>BDP|9398823419477440265</stp>
         <tr r="G125" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...684846550</v>
+        <v>#N/A Requesting Data...4139336638</v>
         <stp/>
         <stp>BDP|3430878723724827801</stp>
         <tr r="G41" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3639432326</v>
+        <v>#N/A Requesting Data...4183568938</v>
         <stp/>
         <stp>BDP|9698422803149077198</stp>
         <tr r="C100" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3631701222</v>
+        <v>#N/A Requesting Data...4159270619</v>
         <stp/>
         <stp>BDP|2887002514665714363</stp>
         <tr r="G59" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3604828910</v>
+        <v>#N/A Requesting Data...4294428234</v>
         <stp/>
         <stp>BDP|2668814054578766269</stp>
         <tr r="E31" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2621738040</v>
+        <v>#N/A Requesting Data...4245265484</v>
         <stp/>
         <stp>BDP|8894702939828266110</stp>
         <tr r="C7" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2635019879</v>
+        <v>#N/A Requesting Data...4222059759</v>
         <stp/>
         <stp>BDP|3410885660260666884</stp>
         <tr r="E64" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2901602263</v>
+        <v>#N/A Requesting Data...4289704347</v>
         <stp/>
         <stp>BDP|3658713905400418152</stp>
         <tr r="E35" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...603569397</v>
+        <v>#N/A Requesting Data...4134301133</v>
         <stp/>
         <stp>BDP|7570300716478486864</stp>
         <tr r="E32" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1908330760</v>
+        <v>#N/A Requesting Data...4146402688</v>
         <stp/>
         <stp>BDP|7851492951527237434</stp>
         <tr r="E52" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...543333208</v>
+        <v>#N/A Requesting Data...4264081085</v>
         <stp/>
         <stp>BDP|7352242467910007671</stp>
         <tr r="F124" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...846418447</v>
+        <v>#N/A Requesting Data...4163030200</v>
         <stp/>
         <stp>BDP|5657563513753480721</stp>
         <tr r="E80" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...539023031</v>
+        <v>#N/A Requesting Data...4269577577</v>
         <stp/>
         <stp>BDP|5976587264538865878</stp>
         <tr r="E62" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3070017442</v>
+        <v>#N/A Requesting Data...4284661862</v>
         <stp/>
         <stp>BDP|7151318027339523982</stp>
         <tr r="F91" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1252287385</v>
+        <v>#N/A Requesting Data...4147587948</v>
         <stp/>
         <stp>BDP|1896477110772260049</stp>
         <tr r="C91" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2871705921</v>
+        <v>#N/A Requesting Data...4292686124</v>
         <stp/>
         <stp>BDP|4252725967471187287</stp>
         <tr r="F44" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...904831573</v>
+        <v>#N/A Requesting Data...4226801068</v>
         <stp/>
         <stp>BDP|6943451920864586278</stp>
         <tr r="C118" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1299275027</v>
+        <v>#N/A Requesting Data...4247392108</v>
         <stp/>
         <stp>BDP|5838113265174067025</stp>
         <tr r="F39" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...962171211</v>
+        <v>#N/A Requesting Data...4265498737</v>
         <stp/>
         <stp>BDP|3456718228377624745</stp>
         <tr r="E111" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3963617241</v>
+        <v>#N/A Requesting Data...4138899058</v>
         <stp/>
         <stp>BDP|5917425194519245724</stp>
         <tr r="E79" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...489879547</v>
+        <v>#N/A Requesting Data...4149307085</v>
         <stp/>
         <stp>BDP|6787533358407016713</stp>
         <tr r="F135" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1776775180</v>
+        <v>#N/A Requesting Data...4151054806</v>
         <stp/>
         <stp>BDP|5576451913756991076</stp>
         <tr r="E16" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3810601124</v>
+        <v>#N/A Requesting Data...4139920155</v>
         <stp/>
         <stp>BDP|5284390591628042184</stp>
         <tr r="C24" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2576341386</v>
+        <v>#N/A Requesting Data...4234530291</v>
         <stp/>
         <stp>BDP|5412037028917536689</stp>
         <tr r="G115" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2318562047</v>
+        <v>#N/A Requesting Data...4147557743</v>
         <stp/>
         <stp>BDP|8966942938724477029</stp>
         <tr r="C15" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3758920202</v>
+        <v>#N/A Requesting Data...4288191532</v>
         <stp/>
         <stp>BDP|2938144706552859709</stp>
         <tr r="G81" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4276014147</v>
+        <v>#N/A Requesting Data...4181691642</v>
         <stp/>
         <stp>BDP|3632949480676633244</stp>
         <tr r="F31" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1862665342</v>
+        <v>#N/A Requesting Data...4218930960</v>
         <stp/>
         <stp>BDP|3513418606797579639</stp>
         <tr r="F90" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...158900855</v>
+        <v>#N/A Requesting Data...4168054275</v>
         <stp/>
         <stp>BDP|1733520919261908213</stp>
         <tr r="G73" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4033642533</v>
+        <v>#N/A Requesting Data...4160873188</v>
         <stp/>
         <stp>BDP|8368969127023380651</stp>
         <tr r="F28" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1682075787</v>
+        <v>#N/A Requesting Data...4248876766</v>
         <stp/>
         <stp>BDP|7172716621593553717</stp>
         <tr r="F53" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3246897924</v>
+        <v>#N/A Requesting Data...4279578889</v>
         <stp/>
         <stp>BDP|2954250373819174944</stp>
         <tr r="F119" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4144803481</v>
+        <v>#N/A Requesting Data...4233412722</v>
         <stp/>
         <stp>BDP|4728287753511799518</stp>
         <tr r="F3" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1627844761</v>
+        <v>#N/A Requesting Data...4236883261</v>
         <stp/>
         <stp>BDP|6348617969513327227</stp>
         <tr r="E104" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...562430782</v>
+        <v>#N/A Requesting Data...4229925503</v>
         <stp/>
         <stp>BDP|7694099704858685831</stp>
         <tr r="C107" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2727593618</v>
+        <v>#N/A Requesting Data...4269863408</v>
         <stp/>
         <stp>BDP|4106834752526835861</stp>
         <tr r="F55" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1617906066</v>
+        <v>#N/A Requesting Data...4197362911</v>
         <stp/>
         <stp>BDP|7951337561756108354</stp>
         <tr r="G112" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1847649889</v>
+        <v>#N/A Requesting Data...4215052214</v>
         <stp/>
         <stp>BDP|5468867501418549294</stp>
         <tr r="E86" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...685395104</v>
+        <v>#N/A Requesting Data...4224958693</v>
         <stp/>
         <stp>BDP|4546740053823447251</stp>
         <tr r="C32" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...273786180</v>
+        <v>#N/A Requesting Data...4256458874</v>
         <stp/>
         <stp>BDP|7484527599745538990</stp>
         <tr r="F76" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2011943504</v>
+        <v>#N/A Requesting Data...4241066528</v>
         <stp/>
         <stp>BDP|5578475423865159117</stp>
         <tr r="E61" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3358808996</v>
+        <v>#N/A Requesting Data...4203483138</v>
         <stp/>
         <stp>BDP|6158107237024797760</stp>
         <tr r="E45" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3111052683</v>
+        <v>#N/A Requesting Data...4230418165</v>
         <stp/>
         <stp>BDP|4143076943390197735</stp>
         <tr r="F97" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2248640331</v>
+        <v>#N/A Requesting Data...4246977775</v>
         <stp/>
         <stp>BDP|1762196091349932721</stp>
         <tr r="E82" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3613556866</v>
+        <v>#N/A Requesting Data...4254617411</v>
         <stp/>
         <stp>BDP|4189169184528349241</stp>
         <tr r="F137" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2140485529</v>
+        <v>#N/A Requesting Data...4223766264</v>
         <stp/>
         <stp>BDP|9103140635044368872</stp>
         <tr r="F29" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3094006030</v>
+        <v>#N/A Requesting Data...4294516157</v>
         <stp/>
         <stp>BDP|5519603296584718917</stp>
         <tr r="G54" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3702600589</v>
+        <v>#N/A Requesting Data...4287812584</v>
         <stp/>
         <stp>BDP|1156250824766982737</stp>
         <tr r="G44" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3807423107</v>
+        <v>#N/A Requesting Data...4257533221</v>
         <stp/>
         <stp>BDP|6031605254431729496</stp>
         <tr r="G86" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3823866440</v>
+        <v>#N/A Requesting Data...4254809594</v>
         <stp/>
         <stp>BDP|2649489454114394728</stp>
         <tr r="C14" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3442284446</v>
+        <v>#N/A Requesting Data...4291669942</v>
         <stp/>
         <stp>BDP|8999377595616850481</stp>
         <tr r="E108" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1630830603</v>
+        <v>#N/A Requesting Data...4270176205</v>
         <stp/>
         <stp>BDP|8988928209665280487</stp>
         <tr r="F71" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1270291899</v>
+        <v>#N/A Requesting Data...4269425269</v>
         <stp/>
         <stp>BDP|8368023487691952119</stp>
         <tr r="F88" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3410914556</v>
+        <v>#N/A Requesting Data...4290447745</v>
         <stp/>
         <stp>BDP|5199287207907438042</stp>
         <tr r="E66" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...879482463</v>
+        <v>#N/A Requesting Data...4293820776</v>
         <stp/>
         <stp>BDP|7460099446995728631</stp>
         <tr r="F134" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3152408193</v>
+        <v>#N/A Requesting Data...4288126937</v>
         <stp/>
         <stp>BDP|6160638673325976246</stp>
         <tr r="C104" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2730230269</v>
+        <v>#N/A Requesting Data...4285147491</v>
         <stp/>
         <stp>BDP|5660731962530222490</stp>
         <tr r="E128" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3443603122</v>
+        <v>#N/A Requesting Data...4287122544</v>
         <stp/>
         <stp>BDP|3355023726294311595</stp>
         <tr r="G114" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3895655251</v>
+        <v>#N/A Requesting Data...4282423763</v>
         <stp/>
         <stp>BDP|5604474461391860653</stp>
         <tr r="E130" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2839063709</v>
+        <v>#N/A Requesting Data...4291923392</v>
         <stp/>
         <stp>BDP|3542140114402066179</stp>
         <tr r="E78" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...585342809</v>
+        <v>#N/A Requesting Data...4288035469</v>
         <stp/>
         <stp>BDP|2942496252996870592</stp>
         <tr r="G121" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1296625952</v>
+        <v>#N/A Requesting Data...4293961519</v>
         <stp/>
         <stp>BDP|1823820926283534897</stp>
         <tr r="G18" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4070576303</v>
+        <v>#N/A Requesting Data...4288888954</v>
         <stp/>
         <stp>BDP|3716189405712826043</stp>
         <tr r="G92" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2578697276</v>
+        <v>#N/A Requesting Data...4291577387</v>
         <stp/>
         <stp>BDP|9344147089140006098</stp>
         <tr r="E83" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1795473537</v>
+        <v>#N/A Requesting Data...4290002374</v>
         <stp/>
         <stp>BDP|6993061706081965773</stp>
         <tr r="F81" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2555000785</v>
+        <v>#N/A Requesting Data...4293340241</v>
         <stp/>
         <stp>BDP|6176792116871092198</stp>
         <tr r="C68" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3393347828</v>
+        <v>#N/A Requesting Data...4294086770</v>
         <stp/>
         <stp>BDP|7185432584822399912</stp>
         <tr r="F131" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4180535081</v>
+        <v>#N/A Requesting Data...4294939060</v>
         <stp/>
         <stp>BDP|8280856169194643320</stp>
         <tr r="G49" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2560508925</v>
+        <v>#N/A Requesting Data...1016579491</v>
         <stp/>
         <stp>BDP|9399109618929306123</stp>
         <tr r="F37" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1045896722</v>
+        <v>#N/A Requesting Data...3053799266</v>
         <stp/>
         <stp>BDP|6669663699409638145</stp>
         <tr r="C123" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1293258873</v>
+        <v>#N/A Requesting Data...1712569240</v>
         <stp/>
         <stp>BDP|6175693122901836298</stp>
         <tr r="C36" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3000955300</v>
+        <v>#N/A Requesting Data...312641488</v>
         <stp/>
         <stp>BDP|8135075327118072391</stp>
         <tr r="C17" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1401640340</v>
+        <v>#N/A Requesting Data...761725067</v>
         <stp/>
         <stp>BDP|5726291712345411206</stp>
         <tr r="G28" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2599812721</v>
+        <v>#N/A Requesting Data...3683100579</v>
         <stp/>
         <stp>BDP|8698973352783506690</stp>
         <tr r="F25" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...971739106</v>
+        <v>#N/A Requesting Data...2609666150</v>
         <stp/>
         <stp>BDP|5493604681742158862</stp>
         <tr r="G63" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2447213607</v>
+        <v>#N/A Requesting Data...3929608783</v>
         <stp/>
         <stp>BDP|3239104742287612040</stp>
         <tr r="E39" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1329516875</v>
+        <v>#N/A Requesting Data...656294143</v>
         <stp/>
         <stp>BDP|3381147726641663059</stp>
         <tr r="C122" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3924319202</v>
+        <v>#N/A Requesting Data...1872362720</v>
         <stp/>
         <stp>BDP|6625906764329795167</stp>
         <tr r="F56" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...693802879</v>
+        <v>#N/A Requesting Data...2790770356</v>
         <stp/>
         <stp>BDP|3325218238213801010</stp>
         <tr r="F57" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1467034879</v>
+        <v>#N/A Requesting Data...1714273785</v>
         <stp/>
         <stp>BDP|1313137390988032037</stp>
         <tr r="C83" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1895797623</v>
+        <v>#N/A Requesting Data...107662531</v>
         <stp/>
         <stp>BDP|3702733300853619616</stp>
         <tr r="G34" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2053828784</v>
+        <v>#N/A Requesting Data...2684866455</v>
         <stp/>
         <stp>BDP|8558611930018338475</stp>
         <tr r="F35" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1082072708</v>
+        <v>#N/A Requesting Data...1444309142</v>
         <stp/>
         <stp>BDP|5387098906493173798</stp>
         <tr r="G62" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1028063893</v>
+        <v>#N/A Requesting Data...3398722907</v>
         <stp/>
         <stp>BDP|1951038018907673608</stp>
         <tr r="C126" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1530718492</v>
+        <v>#N/A Requesting Data...4156673045</v>
         <stp/>
         <stp>BDP|9253802402770546012</stp>
         <tr r="F74" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...300115044</v>
+        <v>#N/A Requesting Data...681218879</v>
         <stp/>
         <stp>BDP|1884505914021260664</stp>
         <tr r="E96" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...805846788</v>
+        <v>#N/A Requesting Data...2893159190</v>
         <stp/>
         <stp>BDP|3540127028674193608</stp>
         <tr r="F94" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...561577568</v>
+        <v>#N/A Requesting Data...115285391</v>
         <stp/>
         <stp>BDP|5372375359741187031</stp>
         <tr r="F27" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3913583138</v>
+        <v>#N/A Requesting Data...1380274923</v>
         <stp/>
         <stp>BDP|5121625602631825066</stp>
         <tr r="E81" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...485847461</v>
+        <v>#N/A Requesting Data...1931469533</v>
         <stp/>
         <stp>BDP|5282708515920897138</stp>
         <tr r="F43" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2422177114</v>
+        <v>#N/A Requesting Data...3612486215</v>
         <stp/>
         <stp>BDP|1250299291741371958</stp>
         <tr r="G31" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2466524275</v>
+        <v>#N/A Requesting Data...3164370212</v>
         <stp/>
         <stp>BDP|4253176148933327033</stp>
         <tr r="C133" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2126099631</v>
+        <v>#N/A Requesting Data...126210314</v>
         <stp/>
         <stp>BDP|9704751602229087502</stp>
         <tr r="F49" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3408572325</v>
+        <v>#N/A Requesting Data...2806684590</v>
         <stp/>
         <stp>BDP|6775233901286469015</stp>
         <tr r="E125" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4136465889</v>
+        <v>#N/A Requesting Data...683667451</v>
         <stp/>
         <stp>BDP|7918289416910309647</stp>
         <tr r="C56" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3735476387</v>
+        <v>#N/A Requesting Data...3183409510</v>
         <stp/>
         <stp>BDP|3731272815900600241</stp>
         <tr r="C53" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2456424239</v>
+        <v>#N/A Requesting Data...4190425212</v>
         <stp/>
         <stp>BDP|1685459166489439868</stp>
         <tr r="F133" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2319607493</v>
+        <v>#N/A Requesting Data...1232707616</v>
         <stp/>
         <stp>BDP|2506644172580171154</stp>
         <tr r="C119" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3731020097</v>
+        <v>#N/A Requesting Data...448774662</v>
         <stp/>
         <stp>BDP|1995353227627490580</stp>
         <tr r="E119" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2681698086</v>
+        <v>#N/A Requesting Data...1526827554</v>
         <stp/>
         <stp>BDP|9173868178561206592</stp>
         <tr r="C77" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2190573044</v>
+        <v>#N/A Requesting Data...1894040366</v>
         <stp/>
         <stp>BDP|4008096672221657096</stp>
         <tr r="G43" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2702441856</v>
+        <v>#N/A Requesting Data...2799052284</v>
         <stp/>
         <stp>BDP|5434663182001395869</stp>
         <tr r="E107" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2389228051</v>
+        <v>#N/A Requesting Data...3821400396</v>
         <stp/>
         <stp>BDP|8686279502629263146</stp>
         <tr r="C129" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2469870097</v>
+        <v>#N/A Requesting Data...978848911</v>
         <stp/>
         <stp>BDP|4576300957588172984</stp>
         <tr r="E63" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...351790709</v>
+        <v>#N/A Requesting Data...2408099135</v>
         <stp/>
         <stp>BDP|7469671678835895086</stp>
         <tr r="E2" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4079582727</v>
+        <v>#N/A Requesting Data...2119159650</v>
         <stp/>
         <stp>BDP|5444751401066968714</stp>
         <tr r="E73" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1940062175</v>
+        <v>#N/A Requesting Data...194462724</v>
         <stp/>
         <stp>BDP|2824124077350027748</stp>
         <tr r="E136" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2035583668</v>
+        <v>#N/A Requesting Data...3563007873</v>
         <stp/>
         <stp>BDP|3708851985886704699</stp>
         <tr r="C19" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...784695384</v>
+        <v>#N/A Requesting Data...3541395595</v>
         <stp/>
         <stp>BDP|1006071828475585561</stp>
         <tr r="F116" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3116382646</v>
+        <v>#N/A Requesting Data...139508987</v>
         <stp/>
         <stp>BDP|1086712249007771639</stp>
         <tr r="G26" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1791983300</v>
+        <v>#N/A Requesting Data...3098159571</v>
         <stp/>
         <stp>BDP|6634730869724168016</stp>
         <tr r="E103" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3242101159</v>
+        <v>#N/A Requesting Data...2496445709</v>
         <stp/>
         <stp>BDP|3520366017777816505</stp>
         <tr r="E97" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1968516232</v>
+        <v>#N/A Requesting Data...739122462</v>
         <stp/>
         <stp>BDP|2995135217932647367</stp>
         <tr r="F105" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1553319952</v>
+        <v>#N/A Requesting Data...542554286</v>
         <stp/>
         <stp>BDP|3565057922625094707</stp>
         <tr r="G45" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...707843900</v>
+        <v>#N/A Requesting Data...3716962810</v>
         <stp/>
         <stp>BDP|1485569542807651461</stp>
         <tr r="C86" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2258840816</v>
+        <v>#N/A Requesting Data...4168046004</v>
         <stp/>
         <stp>BDP|1159006460850353421</stp>
         <tr r="E46" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1687551099</v>
+        <v>#N/A Requesting Data...4032219627</v>
         <stp/>
         <stp>BDP|5113311422502283510</stp>
         <tr r="C84" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2166236961</v>
+        <v>#N/A Requesting Data...1077436861</v>
         <stp/>
         <stp>BDP|4420649803735408460</stp>
         <tr r="F117" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3583274590</v>
+        <v>#N/A Requesting Data...1434038112</v>
         <stp/>
         <stp>BDP|9873235984695079585</stp>
         <tr r="C60" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1418251196</v>
+        <v>#N/A Requesting Data...766119899</v>
         <stp/>
         <stp>BDP|4726106605717010168</stp>
         <tr r="G46" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...962349098</v>
+        <v>#N/A Requesting Data...894546836</v>
         <stp/>
         <stp>BDP|97453184744598227</stp>
         <tr r="G135" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3068691434</v>
+        <v>#N/A Requesting Data...908651188</v>
         <stp/>
         <stp>BDP|71129432364790944</stp>
         <tr r="E105" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2379323885</v>
+        <v>#N/A Requesting Data...4103186300</v>
         <stp/>
         <stp>BDP|13870968378316918</stp>
         <tr r="F38" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3056260177</v>
+        <v>#N/A Requesting Data...346097211</v>
         <stp/>
         <stp>BDP|545017254499479967</stp>
         <tr r="E23" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3328124415</v>
+        <v>#N/A Requesting Data...1284058557</v>
         <stp/>
         <stp>BDP|562457211792430265</stp>
         <tr r="G116" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2745532812</v>
+        <v>#N/A Requesting Data...2782535074</v>
         <stp/>
         <stp>BDP|752318736222262646</stp>
         <tr r="F83" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1039452847</v>
+        <v>#N/A Requesting Data...2186791608</v>
         <stp/>
         <stp>BDP|926433161397617222</stp>
         <tr r="F10" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1578030767</v>
+        <v>#N/A Requesting Data...2880969603</v>
         <stp/>
         <stp>BDP|455507803480864317</stp>
         <tr r="C51" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...731725267</v>
+        <v>#N/A Requesting Data...2726596238</v>
         <stp/>
         <stp>BDP|738430784972633891</stp>
         <tr r="F41" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3841115006</v>
+        <v>#N/A Requesting Data...3650247459</v>
         <stp/>
         <stp>BDP|226270545351892196</stp>
         <tr r="F61" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2691003662</v>
+        <v>#N/A Requesting Data...2387106255</v>
         <stp/>
         <stp>BDP|478534605105814154</stp>
         <tr r="G12" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1958546446</v>
+        <v>#N/A Requesting Data...787125045</v>
         <stp/>
         <stp>BDP|292697057297288557</stp>
         <tr r="C106" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...397084305</v>
+        <v>#N/A Requesting Data...1254820502</v>
         <stp/>
         <stp>BDP|449489448517477649</stp>
         <tr r="E99" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2596088543</v>
+        <v>#N/A Requesting Data...3971948262</v>
         <stp/>
         <stp>BDP|477239144286521179</stp>
         <tr r="G138" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3818480537</v>
+        <v>#N/A Requesting Data...98894971</v>
         <stp/>
         <stp>BDP|136361134742057301</stp>
         <tr r="C57" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1081337134</v>
+        <v>#N/A Requesting Data...3947544311</v>
         <stp/>
         <stp>BDP|282958180978155995</stp>
         <tr r="C59" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2149068026</v>
+        <v>#N/A Requesting Data...375523780</v>
         <stp/>
         <stp>BDP|991366924295531418</stp>
         <tr r="F2" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...879621665</v>
+        <v>#N/A Requesting Data...747193868</v>
         <stp/>
         <stp>BDP|934073235795196633</stp>
         <tr r="F62" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3369521901</v>
+        <v>#N/A Requesting Data...612123527</v>
         <stp/>
         <stp>BDP|266608211912165570</stp>
         <tr r="E113" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2201742269</v>
+        <v>#N/A Requesting Data...1954824844</v>
         <stp/>
         <stp>BDP|910156400954699593</stp>
         <tr r="G8" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1205873420</v>
+        <v>#N/A Requesting Data...1581577410</v>
         <stp/>
         <stp>BDP|794293317440269040</stp>
         <tr r="E100" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...874882949</v>
+        <v>#N/A Requesting Data...1553344589</v>
         <stp/>
         <stp>BDP|206766873121157269</stp>
         <tr r="E41" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...561086920</v>
+        <v>#N/A Requesting Data...772570773</v>
         <stp/>
         <stp>BDP|315261912951356153</stp>
         <tr r="E21" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3336453589</v>
+        <v>#N/A Requesting Data...1815034721</v>
         <stp/>
         <stp>BDP|169080827246056602</stp>
         <tr r="G126" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1465953930</v>
+        <v>#N/A Requesting Data...3016355865</v>
         <stp/>
         <stp>BDP|454779781439338455</stp>
         <tr r="E36" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1500735387</v>
+        <v>#N/A Requesting Data...1004182890</v>
         <stp/>
         <stp>BDP|198524097739196711</stp>
         <tr r="F92" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...381673587</v>
+        <v>#N/A Requesting Data...1191875690</v>
         <stp/>
         <stp>BDP|618726407191106421</stp>
         <tr r="C92" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3208964420</v>
+        <v>#N/A Requesting Data...1264689479</v>
         <stp/>
         <stp>BDP|442808307356626303</stp>
         <tr r="F20" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...658459705</v>
+        <v>#N/A Requesting Data...2135705584</v>
         <stp/>
         <stp>BDP|304889655090792147</stp>
         <tr r="E58" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2645937915</v>
+        <v>#N/A Requesting Data...1776330005</v>
         <stp/>
         <stp>BDP|427627592191043219</stp>
         <tr r="C87" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2815603378</v>
+        <v>#N/A Requesting Data...495681633</v>
         <stp/>
         <stp>BDP|768711067038142524</stp>
         <tr r="G25" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...803219654</v>
+        <v>#N/A Requesting Data...2711586275</v>
         <stp/>
         <stp>BDP|447365482187669383</stp>
         <tr r="C95" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4112111639</v>
+        <v>#N/A Requesting Data...2565747856</v>
         <stp/>
         <stp>BDP|901925773788783965</stp>
         <tr r="G67" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4197691464</v>
+        <v>#N/A Requesting Data...3894958011</v>
         <stp/>
         <stp>BDP|511429594874391764</stp>
         <tr r="G117" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1105949847</v>
+        <v>#N/A Requesting Data...3318177731</v>
         <stp/>
         <stp>BDP|544620567958067604</stp>
         <tr r="C131" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2191416518</v>
+        <v>#N/A Requesting Data...1146846109</v>
         <stp/>
         <stp>BDP|945569483354328027</stp>
         <tr r="C21" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4241470712</v>
+        <v>#N/A Requesting Data...2597459438</v>
         <stp/>
         <stp>BDP|691281527639744142</stp>
         <tr r="E8" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1496509379</v>
+        <v>#N/A Requesting Data...3501980360</v>
         <stp/>
         <stp>BDP|968314719543295935</stp>
         <tr r="E68" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2123118018</v>
+        <v>#N/A Requesting Data...149330339</v>
         <stp/>
         <stp>BDP|760426044168153386</stp>
         <tr r="G7" s="1"/>
@@ -4810,7 +4813,7 @@
   <dimension ref="A1:E139"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4880,7 +4883,7 @@
         <v>289</v>
       </c>
       <c r="E4" t="s">
-        <v>290</v>
+        <v>353</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -5642,7 +5645,7 @@
         <v>335</v>
       </c>
       <c r="D49" t="s">
-        <v>332</v>
+        <v>313</v>
       </c>
       <c r="E49" t="s">
         <v>333</v>
@@ -5693,7 +5696,7 @@
         <v>297</v>
       </c>
       <c r="D52" t="s">
-        <v>284</v>
+        <v>298</v>
       </c>
       <c r="E52" t="s">
         <v>284</v>
@@ -7084,7 +7087,7 @@
         <v>267</v>
       </c>
       <c r="C134" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="D134" t="s">
         <v>296</v>
@@ -7187,8 +7190,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5352835-5CFD-46EC-8CDA-5672A55A22F5}">
   <dimension ref="A1:G139"/>
   <sheetViews>
-    <sheetView topLeftCell="A113" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:G139"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7299,7 +7302,7 @@
       </c>
       <c r="G4" t="str">
         <f>_xll.BDP(D4,"RTG_FITCH_LT_ISSUER_DEFAULT")</f>
-        <v>CCCu</v>
+        <v>CCC+u</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -8510,7 +8513,7 @@
       </c>
       <c r="F49" t="str">
         <f>_xll.BDP(D49,"RTG_SP_LT_FC_ISSUER_CREDIT")</f>
-        <v>SD</v>
+        <v>CCC+</v>
       </c>
       <c r="G49" t="str">
         <f>_xll.BDP(D49,"RTG_FITCH_LT_ISSUER_DEFAULT")</f>
@@ -8591,7 +8594,7 @@
       </c>
       <c r="F52" t="str">
         <f>_xll.BDP(D52,"RTG_SP_LT_FC_ISSUER_CREDIT")</f>
-        <v>BB</v>
+        <v>BB+</v>
       </c>
       <c r="G52" t="str">
         <f>_xll.BDP(D52,"RTG_FITCH_LT_ISSUER_DEFAULT")</f>
@@ -10801,7 +10804,7 @@
       </c>
       <c r="E134" t="str">
         <f>_xll.BDP(D134,"RTG_MDY_FC_CURR_ISSUER_RATING")</f>
-        <v>Aaa</v>
+        <v>Aa1</v>
       </c>
       <c r="F134" t="str">
         <f>_xll.BDP(D134,"RTG_SP_LT_FC_ISSUER_CREDIT")</f>

</xml_diff>

<commit_message>
solved for the LS_rating dot problems!
</commit_message>
<xml_diff>
--- a/index_bbg_rating_live.xlsx
+++ b/index_bbg_rating_live.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kaimin Khaw\Desktop\credit-rating-deploy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F68CB52C-E6FC-48D4-8661-C49279E1A100}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29F80B58-AC38-42B6-B532-050E3682DECC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2A12413E-A5EC-426E-A187-DE07F52921C3}"/>
+    <workbookView xWindow="22932" yWindow="-72" windowWidth="23256" windowHeight="12576" xr2:uid="{2A12413E-A5EC-426E-A187-DE07F52921C3}"/>
   </bookViews>
   <sheets>
     <sheet name="hard_code" sheetId="2" r:id="rId1"/>
@@ -1195,1531 +1195,1531 @@
   <volType type="realTimeData">
     <main first="bofaddin.rtdserver">
       <tp t="s">
-        <v>#N/A Requesting Data...4084940804</v>
+        <v>#N/A Requesting Data...3405054975</v>
         <stp/>
         <stp>BDP|13719527809048657439</stp>
         <tr r="E3" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3818166150</v>
+        <v>#N/A Requesting Data...3314670704</v>
         <stp/>
         <stp>BDP|12363409739849183621</stp>
         <tr r="G98" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3936637966</v>
+        <v>#N/A Requesting Data...3501796012</v>
         <stp/>
         <stp>BDP|17606584297068117917</stp>
         <tr r="G105" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3582039849</v>
+        <v>#N/A Requesting Data...3197300115</v>
         <stp/>
         <stp>BDP|12825277506793769973</stp>
         <tr r="F22" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4167090013</v>
+        <v>#N/A Requesting Data...3205553724</v>
         <stp/>
         <stp>BDP|13615906068526188051</stp>
         <tr r="G101" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4215472552</v>
+        <v>#N/A Requesting Data...3652431554</v>
         <stp/>
         <stp>BDP|10912677687245148127</stp>
         <tr r="G106" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4071996823</v>
+        <v>#N/A Requesting Data...4142656771</v>
         <stp/>
         <stp>BDP|16221541486007837625</stp>
         <tr r="G58" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4114476026</v>
+        <v>#N/A Requesting Data...3379196753</v>
         <stp/>
         <stp>BDP|14989839765876665645</stp>
         <tr r="C81" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3668815360</v>
+        <v>#N/A Requesting Data...3448874223</v>
         <stp/>
         <stp>BDP|16792452589360294083</stp>
         <tr r="E11" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3955049544</v>
+        <v>#N/A Requesting Data...3774125838</v>
         <stp/>
         <stp>BDP|16409240184993364568</stp>
         <tr r="E54" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4066999936</v>
+        <v>#N/A Requesting Data...3036922047</v>
         <stp/>
         <stp>BDP|12376141866138693768</stp>
         <tr r="C88" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3799792905</v>
+        <v>#N/A Requesting Data...4188443841</v>
         <stp/>
         <stp>BDP|13146963289471890960</stp>
         <tr r="C18" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3914697931</v>
+        <v>#N/A Requesting Data...4005998733</v>
         <stp/>
         <stp>BDP|10167725043130019931</stp>
         <tr r="C110" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3655857831</v>
+        <v>#N/A Requesting Data...3471027565</v>
         <stp/>
         <stp>BDP|10589422899161895655</stp>
         <tr r="G76" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4026033311</v>
+        <v>#N/A Requesting Data...3278939878</v>
         <stp/>
         <stp>BDP|15228795190517586693</stp>
         <tr r="E84" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3942019898</v>
+        <v>#N/A Requesting Data...3764835243</v>
         <stp/>
         <stp>BDP|10096201946458505444</stp>
         <tr r="G97" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3814219693</v>
+        <v>#N/A Requesting Data...3845523602</v>
         <stp/>
         <stp>BDP|18253401034836307331</stp>
         <tr r="F99" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4003975361</v>
+        <v>#N/A Requesting Data...3980246801</v>
         <stp/>
         <stp>BDP|10867273920449518201</stp>
         <tr r="G71" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4030248805</v>
+        <v>#N/A Requesting Data...3263001505</v>
         <stp/>
         <stp>BDP|14811872563886412749</stp>
         <tr r="E114" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4173553565</v>
+        <v>#N/A Requesting Data...3674258977</v>
         <stp/>
         <stp>BDP|15237334583701669483</stp>
         <tr r="C112" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4248521151</v>
+        <v>#N/A Requesting Data...3593803265</v>
         <stp/>
         <stp>BDP|14006145231309322495</stp>
         <tr r="C65" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3973396673</v>
+        <v>#N/A Requesting Data...2980606960</v>
         <stp/>
         <stp>BDP|14761213634019822741</stp>
         <tr r="G2" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3769923197</v>
+        <v>#N/A Requesting Data...3365837352</v>
         <stp/>
         <stp>BDP|15399231330039360601</stp>
         <tr r="E42" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4134176344</v>
+        <v>#N/A Requesting Data...3813033407</v>
         <stp/>
         <stp>BDP|11120752607359953480</stp>
         <tr r="G61" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3745060468</v>
+        <v>#N/A Requesting Data...3043236109</v>
         <stp/>
         <stp>BDP|15939978441203902037</stp>
         <tr r="C26" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3782108872</v>
+        <v>#N/A Requesting Data...3828681121</v>
         <stp/>
         <stp>BDP|18066043829836356791</stp>
         <tr r="G78" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4066827677</v>
+        <v>#N/A Requesting Data...3780940323</v>
         <stp/>
         <stp>BDP|14168806967588813989</stp>
         <tr r="F77" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4102979142</v>
+        <v>#N/A Requesting Data...2889907669</v>
         <stp/>
         <stp>BDP|18397803367339867766</stp>
         <tr r="F101" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3770151263</v>
+        <v>#N/A Requesting Data...3043235616</v>
         <stp/>
         <stp>BDP|15895803206017416271</stp>
         <tr r="C33" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4083708151</v>
+        <v>#N/A Requesting Data...2856046515</v>
         <stp/>
         <stp>BDP|14908732543227691836</stp>
         <tr r="E94" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3911993897</v>
+        <v>#N/A Requesting Data...3751684388</v>
         <stp/>
         <stp>BDP|12957817799052931996</stp>
         <tr r="E120" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4025837358</v>
+        <v>#N/A Requesting Data...3068845822</v>
         <stp/>
         <stp>BDP|16275205432289392600</stp>
         <tr r="E101" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3869758937</v>
+        <v>#N/A Requesting Data...4099401609</v>
         <stp/>
         <stp>BDP|10407655300028223605</stp>
         <tr r="F47" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3856786581</v>
+        <v>#N/A Requesting Data...3764274608</v>
         <stp/>
         <stp>BDP|14031612538318230186</stp>
         <tr r="C136" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3726006503</v>
+        <v>#N/A Requesting Data...3314431677</v>
         <stp/>
         <stp>BDP|13840587393604095357</stp>
         <tr r="G3" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3948414322</v>
+        <v>#N/A Requesting Data...4293449479</v>
         <stp/>
         <stp>BDP|18397555740376217727</stp>
         <tr r="F17" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3843665062</v>
+        <v>#N/A Requesting Data...3034795402</v>
         <stp/>
         <stp>BDP|15886108592084595196</stp>
         <tr r="F19" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4090535034</v>
+        <v>#N/A Requesting Data...2960778996</v>
         <stp/>
         <stp>BDP|12574943311804341655</stp>
         <tr r="C58" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4056868476</v>
+        <v>#N/A Requesting Data...3421895955</v>
         <stp/>
         <stp>BDP|15276164033266227932</stp>
         <tr r="C121" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3726393719</v>
+        <v>#N/A Requesting Data...2956911296</v>
         <stp/>
         <stp>BDP|11413915902765857449</stp>
         <tr r="C135" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3798936595</v>
+        <v>#N/A Requesting Data...3733032685</v>
         <stp/>
         <stp>BDP|10888161880627674738</stp>
         <tr r="G74" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3926614609</v>
+        <v>#N/A Requesting Data...4142653432</v>
         <stp/>
         <stp>BDP|18252264749434830399</stp>
         <tr r="E91" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3672628817</v>
+        <v>#N/A Requesting Data...3216121156</v>
         <stp/>
         <stp>BDP|16230814927561165496</stp>
         <tr r="C25" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4216089997</v>
+        <v>#N/A Requesting Data...3352937560</v>
         <stp/>
         <stp>BDP|11669407615485914850</stp>
         <tr r="E28" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3830389832</v>
+        <v>#N/A Requesting Data...3296570632</v>
         <stp/>
         <stp>BDP|15385895124225473341</stp>
         <tr r="F89" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3942830157</v>
+        <v>#N/A Requesting Data...3577091399</v>
         <stp/>
         <stp>BDP|16215575297831427265</stp>
         <tr r="G19" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4272428885</v>
+        <v>#N/A Requesting Data...3905250868</v>
         <stp/>
         <stp>BDP|15664489079057139842</stp>
         <tr r="C50" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3789272974</v>
+        <v>#N/A Requesting Data...4053035324</v>
         <stp/>
         <stp>BDP|13556466380534139208</stp>
         <tr r="C63" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4182875044</v>
+        <v>#N/A Requesting Data...3648257222</v>
         <stp/>
         <stp>BDP|12426034393664290636</stp>
         <tr r="G70" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3949420847</v>
+        <v>#N/A Requesting Data...3663799992</v>
         <stp/>
         <stp>BDP|11206974657257798316</stp>
         <tr r="G5" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4158614471</v>
+        <v>#N/A Requesting Data...3092948676</v>
         <stp/>
         <stp>BDP|15687672872765725835</stp>
         <tr r="G133" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3859021594</v>
+        <v>#N/A Requesting Data...3049640752</v>
         <stp/>
         <stp>BDP|10646340980557108540</stp>
         <tr r="G83" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4043172443</v>
+        <v>#N/A Requesting Data...3940463716</v>
         <stp/>
         <stp>BDP|13932387258969800286</stp>
         <tr r="G30" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3842083138</v>
+        <v>#N/A Requesting Data...3930117946</v>
         <stp/>
         <stp>BDP|14685689793557045247</stp>
         <tr r="G11" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3853686362</v>
+        <v>#N/A Requesting Data...3148685211</v>
         <stp/>
         <stp>BDP|11792528289940283264</stp>
         <tr r="G39" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3925565773</v>
+        <v>#N/A Requesting Data...3984617166</v>
         <stp/>
         <stp>BDP|14038814629908297802</stp>
         <tr r="E14" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3819747339</v>
+        <v>#N/A Requesting Data...4003824437</v>
         <stp/>
         <stp>BDP|17960836852555549100</stp>
         <tr r="F79" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4288117455</v>
+        <v>#N/A Requesting Data...3146428841</v>
         <stp/>
         <stp>BDP|12258786923690042954</stp>
         <tr r="G82" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4291596956</v>
+        <v>#N/A Requesting Data...4223217655</v>
         <stp/>
         <stp>BDP|11831892951331348329</stp>
         <tr r="C35" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4217312828</v>
+        <v>#N/A Requesting Data...3457592315</v>
         <stp/>
         <stp>BDP|12634554786653062247</stp>
         <tr r="F34" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4054871828</v>
+        <v>#N/A Requesting Data...3094597817</v>
         <stp/>
         <stp>BDP|10304787173197381988</stp>
         <tr r="G53" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3843648100</v>
+        <v>#N/A Requesting Data...3738538409</v>
         <stp/>
         <stp>BDP|15772343051115104818</stp>
         <tr r="C127" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3980979718</v>
+        <v>#N/A Requesting Data...3003990171</v>
         <stp/>
         <stp>BDP|13619322587163510542</stp>
         <tr r="C45" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4063486971</v>
+        <v>#N/A Requesting Data...3537993231</v>
         <stp/>
         <stp>BDP|13709828003397613269</stp>
         <tr r="C54" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4136110991</v>
+        <v>#N/A Requesting Data...2998451544</v>
         <stp/>
         <stp>BDP|11596891797659679653</stp>
         <tr r="C89" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3836849735</v>
+        <v>#N/A Requesting Data...3275457939</v>
         <stp/>
         <stp>BDP|18339290641951108002</stp>
         <tr r="E17" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4257494646</v>
+        <v>#N/A Requesting Data...3778070141</v>
         <stp/>
         <stp>BDP|10418265688390464525</stp>
         <tr r="E18" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4086890445</v>
+        <v>#N/A Requesting Data...4045344785</v>
         <stp/>
         <stp>BDP|14859691791600738447</stp>
         <tr r="F45" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3789630501</v>
+        <v>#N/A Requesting Data...3609068319</v>
         <stp/>
         <stp>BDP|18255708956124343152</stp>
         <tr r="E26" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4242777602</v>
+        <v>#N/A Requesting Data...3954270222</v>
         <stp/>
         <stp>BDP|16855823919014233436</stp>
         <tr r="F30" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4055919642</v>
+        <v>#N/A Requesting Data...3384296123</v>
         <stp/>
         <stp>BDP|12821872971201299383</stp>
         <tr r="G124" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3715815420</v>
+        <v>#N/A Requesting Data...3197709226</v>
         <stp/>
         <stp>BDP|11466185903217969815</stp>
         <tr r="F33" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3739842703</v>
+        <v>#N/A Requesting Data...3058982925</v>
         <stp/>
         <stp>BDP|13711300257260836914</stp>
         <tr r="C102" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3813514650</v>
+        <v>#N/A Requesting Data...3752848657</v>
         <stp/>
         <stp>BDP|11622318103537999967</stp>
         <tr r="F15" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4108278260</v>
+        <v>#N/A Requesting Data...3196646591</v>
         <stp/>
         <stp>BDP|10597445640754361898</stp>
         <tr r="F50" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4015507631</v>
+        <v>#N/A Requesting Data...4189921364</v>
         <stp/>
         <stp>BDP|13987588094432951117</stp>
         <tr r="E127" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4004672391</v>
+        <v>#N/A Requesting Data...3731722036</v>
         <stp/>
         <stp>BDP|11655961067423868102</stp>
         <tr r="G104" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3855903510</v>
+        <v>#N/A Requesting Data...3123387887</v>
         <stp/>
         <stp>BDP|12468839190466923900</stp>
         <tr r="C20" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3763639943</v>
+        <v>#N/A Requesting Data...3544425914</v>
         <stp/>
         <stp>BDP|18411047804853597705</stp>
         <tr r="C67" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3874574207</v>
+        <v>#N/A Requesting Data...3991446024</v>
         <stp/>
         <stp>BDP|18331339124097518219</stp>
         <tr r="F66" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3735618464</v>
+        <v>#N/A Requesting Data...3822987888</v>
         <stp/>
         <stp>BDP|14983531083496973331</stp>
         <tr r="G132" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4252362543</v>
+        <v>#N/A Requesting Data...3471654031</v>
         <stp/>
         <stp>BDP|14115869171127460078</stp>
         <tr r="G37" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3712586628</v>
+        <v>#N/A Requesting Data...4017743675</v>
         <stp/>
         <stp>BDP|16963038037211063893</stp>
         <tr r="C13" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3862194290</v>
+        <v>#N/A Requesting Data...3346663403</v>
         <stp/>
         <stp>BDP|13900268704084418991</stp>
         <tr r="E37" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3937501614</v>
+        <v>#N/A Requesting Data...3162882692</v>
         <stp/>
         <stp>BDP|16311230542528118454</stp>
         <tr r="E9" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4068844929</v>
+        <v>#N/A Requesting Data...3188145326</v>
         <stp/>
         <stp>BDP|12403550728001134908</stp>
         <tr r="G38" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3849263416</v>
+        <v>#N/A Requesting Data...3043373855</v>
         <stp/>
         <stp>BDP|10528694388950747396</stp>
         <tr r="F80" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4225330012</v>
+        <v>#N/A Requesting Data...3486133797</v>
         <stp/>
         <stp>BDP|17962073596443790028</stp>
         <tr r="F23" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4214888431</v>
+        <v>#N/A Requesting Data...3294822692</v>
         <stp/>
         <stp>BDP|11322749828038387103</stp>
         <tr r="E122" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4157874441</v>
+        <v>#N/A Requesting Data...4040052893</v>
         <stp/>
         <stp>BDP|14872467854648029062</stp>
         <tr r="C75" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4003540637</v>
+        <v>#N/A Requesting Data...3836478021</v>
         <stp/>
         <stp>BDP|14951668809329151689</stp>
         <tr r="E56" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3949838596</v>
+        <v>#N/A Requesting Data...3729152781</v>
         <stp/>
         <stp>BDP|14211231849266296941</stp>
         <tr r="G103" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4217759461</v>
+        <v>#N/A Requesting Data...3960030981</v>
         <stp/>
         <stp>BDP|15282935006718574931</stp>
         <tr r="E92" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4288776602</v>
+        <v>#N/A Requesting Data...3807568849</v>
         <stp/>
         <stp>BDP|16389940868391785591</stp>
         <tr r="C120" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3782460224</v>
+        <v>#N/A Requesting Data...3719750554</v>
         <stp/>
         <stp>BDP|10830300668358540045</stp>
         <tr r="C115" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4038101368</v>
+        <v>#N/A Requesting Data...3543710970</v>
         <stp/>
         <stp>BDP|15417892931237679498</stp>
         <tr r="F8" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3720466309</v>
+        <v>#N/A Requesting Data...3090241531</v>
         <stp/>
         <stp>BDP|13776760394691002167</stp>
         <tr r="C4" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4255608986</v>
+        <v>#N/A Requesting Data...3573924657</v>
         <stp/>
         <stp>BDP|12950924085148446689</stp>
         <tr r="E121" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4103173843</v>
+        <v>#N/A Requesting Data...3394037490</v>
         <stp/>
         <stp>BDP|11202744698684518690</stp>
         <tr r="G111" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4134471993</v>
+        <v>#N/A Requesting Data...4230039360</v>
         <stp/>
         <stp>BDP|11005719894013994183</stp>
         <tr r="C3" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4010740088</v>
+        <v>#N/A Requesting Data...3470290569</v>
         <stp/>
         <stp>BDP|17061881470574956177</stp>
         <tr r="C69" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4232809097</v>
+        <v>#N/A Requesting Data...3516310073</v>
         <stp/>
         <stp>BDP|10195299258766033392</stp>
         <tr r="E90" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4239449222</v>
+        <v>#N/A Requesting Data...3966900038</v>
         <stp/>
         <stp>BDP|17559180385128709479</stp>
         <tr r="E15" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4184478731</v>
+        <v>#N/A Requesting Data...4228773360</v>
         <stp/>
         <stp>BDP|10477087317801173223</stp>
         <tr r="F125" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3885165547</v>
+        <v>#N/A Requesting Data...3670795405</v>
         <stp/>
         <stp>BDP|10431478218456128129</stp>
         <tr r="G32" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3719541900</v>
+        <v>#N/A Requesting Data...3041054403</v>
         <stp/>
         <stp>BDP|12817533695869473568</stp>
         <tr r="C82" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4028779754</v>
+        <v>#N/A Requesting Data...4188317355</v>
         <stp/>
         <stp>BDP|16722436137983528090</stp>
         <tr r="F127" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3866216667</v>
+        <v>#N/A Requesting Data...3287923159</v>
         <stp/>
         <stp>BDP|14949322880769358496</stp>
         <tr r="G16" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3845850965</v>
+        <v>#N/A Requesting Data...4102285617</v>
         <stp/>
         <stp>BDP|12620594347341901004</stp>
         <tr r="C76" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3994768203</v>
+        <v>#N/A Requesting Data...3562564489</v>
         <stp/>
         <stp>BDP|12047021516217693612</stp>
         <tr r="E126" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3965853537</v>
+        <v>#N/A Requesting Data...3978546887</v>
         <stp/>
         <stp>BDP|13612225533853005354</stp>
         <tr r="F102" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3923948554</v>
+        <v>#N/A Requesting Data...3982601953</v>
         <stp/>
         <stp>BDP|11536436753390219250</stp>
         <tr r="F129" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3888980933</v>
+        <v>#N/A Requesting Data...3440154757</v>
         <stp/>
         <stp>BDP|12946334758336119017</stp>
         <tr r="E72" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3972359311</v>
+        <v>#N/A Requesting Data...3728576680</v>
         <stp/>
         <stp>BDP|17733998071078953332</stp>
         <tr r="C23" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4128145364</v>
+        <v>#N/A Requesting Data...3074756175</v>
         <stp/>
         <stp>BDP|16362559715466602618</stp>
         <tr r="F68" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3923441085</v>
+        <v>#N/A Requesting Data...4055891841</v>
         <stp/>
         <stp>BDP|16070475881909673177</stp>
         <tr r="E112" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3821166789</v>
+        <v>#N/A Requesting Data...3590473319</v>
         <stp/>
         <stp>BDP|17590878194950224438</stp>
         <tr r="G87" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3736919126</v>
+        <v>#N/A Requesting Data...3461616743</v>
         <stp/>
         <stp>BDP|12427007793358727164</stp>
         <tr r="F100" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4192301686</v>
+        <v>#N/A Requesting Data...4157302775</v>
         <stp/>
         <stp>BDP|15601293270144483737</stp>
         <tr r="G15" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4142318778</v>
+        <v>#N/A Requesting Data...3393353083</v>
         <stp/>
         <stp>BDP|13723200346810339697</stp>
         <tr r="C38" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3780791477</v>
+        <v>#N/A Requesting Data...4220224910</v>
         <stp/>
         <stp>BDP|18086118189074176643</stp>
         <tr r="E88" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3850562052</v>
+        <v>#N/A Requesting Data...3245376130</v>
         <stp/>
         <stp>BDP|15679917748483251829</stp>
         <tr r="E6" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3811928410</v>
+        <v>#N/A Requesting Data...3713449924</v>
         <stp/>
         <stp>BDP|13421293548936861023</stp>
         <tr r="G66" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4055253438</v>
+        <v>#N/A Requesting Data...4240906325</v>
         <stp/>
         <stp>BDP|10594946509929542325</stp>
         <tr r="F5" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3916528819</v>
+        <v>#N/A Requesting Data...4144490778</v>
         <stp/>
         <stp>BDP|10668212108445960480</stp>
         <tr r="G57" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3981055296</v>
+        <v>#N/A Requesting Data...4185463958</v>
         <stp/>
         <stp>BDP|10103273213286136651</stp>
         <tr r="C6" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4029407828</v>
+        <v>#N/A Requesting Data...3748642028</v>
         <stp/>
         <stp>BDP|11259721862376480554</stp>
         <tr r="G69" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4084600666</v>
+        <v>#N/A Requesting Data...3192428560</v>
         <stp/>
         <stp>BDP|14885566279524266176</stp>
         <tr r="E30" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3782025563</v>
+        <v>#N/A Requesting Data...3520510423</v>
         <stp/>
         <stp>BDP|14519079130534129014</stp>
         <tr r="C49" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4157772126</v>
+        <v>#N/A Requesting Data...4158136921</v>
         <stp/>
         <stp>BDP|14873136635550817546</stp>
         <tr r="G130" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3906845388</v>
+        <v>#N/A Requesting Data...3129005777</v>
         <stp/>
         <stp>BDP|16641457892301341972</stp>
         <tr r="F130" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3820605786</v>
+        <v>#N/A Requesting Data...3666883803</v>
         <stp/>
         <stp>BDP|13231746637163726724</stp>
         <tr r="E7" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3769824919</v>
+        <v>#N/A Requesting Data...4161169397</v>
         <stp/>
         <stp>BDP|12945735048800380256</stp>
         <tr r="G118" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4135619376</v>
+        <v>#N/A Requesting Data...3554319588</v>
         <stp/>
         <stp>BDP|11265248170961260631</stp>
         <tr r="E47" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4015549366</v>
+        <v>#N/A Requesting Data...3969816548</v>
         <stp/>
         <stp>BDP|16351851074029385080</stp>
         <tr r="G35" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4289574953</v>
+        <v>#N/A Requesting Data...3677578220</v>
         <stp/>
         <stp>BDP|11944358991052271970</stp>
         <tr r="C103" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4274985090</v>
+        <v>#N/A Requesting Data...3915193628</v>
         <stp/>
         <stp>BDP|18410981990650283866</stp>
         <tr r="C99" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3925195095</v>
+        <v>#N/A Requesting Data...3494180109</v>
         <stp/>
         <stp>BDP|14383773052580838655</stp>
         <tr r="F104" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3970206489</v>
+        <v>#N/A Requesting Data...3545267496</v>
         <stp/>
         <stp>BDP|10871340643964419300</stp>
         <tr r="F95" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3962101529</v>
+        <v>#N/A Requesting Data...3973084306</v>
         <stp/>
         <stp>BDP|14690280185656044816</stp>
         <tr r="C94" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4009385647</v>
+        <v>#N/A Requesting Data...4236089494</v>
         <stp/>
         <stp>BDP|18305693996456795112</stp>
         <tr r="G80" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3903956740</v>
+        <v>#N/A Requesting Data...4251039407</v>
         <stp/>
         <stp>BDP|16273225567973824127</stp>
         <tr r="C79" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3910445700</v>
+        <v>#N/A Requesting Data...4170202761</v>
         <stp/>
         <stp>BDP|13313129291618997350</stp>
         <tr r="C43" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4002531030</v>
+        <v>#N/A Requesting Data...3182394496</v>
         <stp/>
         <stp>BDP|15444947284180871401</stp>
         <tr r="G27" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4183457531</v>
+        <v>#N/A Requesting Data...3169639484</v>
         <stp/>
         <stp>BDP|12935317504846234704</stp>
         <tr r="F98" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4293866495</v>
+        <v>#N/A Requesting Data...4127291409</v>
         <stp/>
         <stp>BDP|13057895365605005829</stp>
         <tr r="C138" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4233928023</v>
+        <v>#N/A Requesting Data...3170347288</v>
         <stp/>
         <stp>BDP|16160321537943284588</stp>
         <tr r="E76" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4063682295</v>
+        <v>#N/A Requesting Data...3892064516</v>
         <stp/>
         <stp>BDP|10621599828921836610</stp>
         <tr r="C12" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3982100701</v>
+        <v>#N/A Requesting Data...3149402736</v>
         <stp/>
         <stp>BDP|14881076967673386157</stp>
         <tr r="F122" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3958830716</v>
+        <v>#N/A Requesting Data...3493752479</v>
         <stp/>
         <stp>BDP|17321553610055816607</stp>
         <tr r="F96" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3831490489</v>
+        <v>#N/A Requesting Data...3485359228</v>
         <stp/>
         <stp>BDP|12793555755147383546</stp>
         <tr r="F42" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4008837764</v>
+        <v>#N/A Requesting Data...3490501896</v>
         <stp/>
         <stp>BDP|10194327202093986081</stp>
         <tr r="F132" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3882152658</v>
+        <v>#N/A Requesting Data...4285045475</v>
         <stp/>
         <stp>BDP|12798194599768683232</stp>
         <tr r="C42" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3789432313</v>
+        <v>#N/A Requesting Data...3993505275</v>
         <stp/>
         <stp>BDP|15675203172551734114</stp>
         <tr r="F12" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4181608202</v>
+        <v>#N/A Requesting Data...3147085628</v>
         <stp/>
         <stp>BDP|17779010845097021465</stp>
         <tr r="G23" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3827215005</v>
+        <v>#N/A Requesting Data...4168180470</v>
         <stp/>
         <stp>BDP|14698661432127374654</stp>
         <tr r="E53" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3937527172</v>
+        <v>#N/A Requesting Data...3416637872</v>
         <stp/>
         <stp>BDP|16055018629402477686</stp>
         <tr r="F18" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4273072254</v>
+        <v>#N/A Requesting Data...4104856594</v>
         <stp/>
         <stp>BDP|14191015466523343124</stp>
         <tr r="G42" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4179056873</v>
+        <v>#N/A Requesting Data...3331851571</v>
         <stp/>
         <stp>BDP|16690545673604064064</stp>
         <tr r="G6" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3950885477</v>
+        <v>#N/A Requesting Data...3514575084</v>
         <stp/>
         <stp>BDP|11057556593645206836</stp>
         <tr r="E116" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4064659021</v>
+        <v>#N/A Requesting Data...3226905597</v>
         <stp/>
         <stp>BDP|14753168038796700174</stp>
         <tr r="E131" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4049160098</v>
+        <v>#N/A Requesting Data...3493860623</v>
         <stp/>
         <stp>BDP|18400936140157917378</stp>
         <tr r="G108" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4255801130</v>
+        <v>#N/A Requesting Data...3708128234</v>
         <stp/>
         <stp>BDP|11308062409311166143</stp>
         <tr r="F138" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4119105963</v>
+        <v>#N/A Requesting Data...3708192006</v>
         <stp/>
         <stp>BDP|14929251921187622207</stp>
         <tr r="G120" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3868926601</v>
+        <v>#N/A Requesting Data...3402636482</v>
         <stp/>
         <stp>BDP|13312546151322475095</stp>
         <tr r="C117" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3797662668</v>
+        <v>#N/A Requesting Data...3393251429</v>
         <stp/>
         <stp>BDP|10370784365528062849</stp>
         <tr r="G51" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4195869048</v>
+        <v>#N/A Requesting Data...3804205935</v>
         <stp/>
         <stp>BDP|17808503947101138629</stp>
         <tr r="F128" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4262530422</v>
+        <v>#N/A Requesting Data...3241612746</v>
         <stp/>
         <stp>BDP|17640270888515662931</stp>
         <tr r="E20" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4174920295</v>
+        <v>#N/A Requesting Data...3626121513</v>
         <stp/>
         <stp>BDP|17853766030844520642</stp>
         <tr r="F65" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4175396313</v>
+        <v>#N/A Requesting Data...3506683705</v>
         <stp/>
         <stp>BDP|17345319339237647129</stp>
         <tr r="C10" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3913439302</v>
+        <v>#N/A Requesting Data...3507324553</v>
         <stp/>
         <stp>BDP|18428163184190295050</stp>
         <tr r="C48" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3996076963</v>
+        <v>#N/A Requesting Data...3677019370</v>
         <stp/>
         <stp>BDP|11469771160883398201</stp>
         <tr r="G20" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4110630158</v>
+        <v>#N/A Requesting Data...3336822258</v>
         <stp/>
         <stp>BDP|12945229628891094206</stp>
         <tr r="F36" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4236264309</v>
+        <v>#N/A Requesting Data...3429951515</v>
         <stp/>
         <stp>BDP|13088969316699575369</stp>
         <tr r="G17" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4146450232</v>
+        <v>#N/A Requesting Data...3645482285</v>
         <stp/>
         <stp>BDP|14386928546318260068</stp>
         <tr r="C78" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4277446044</v>
+        <v>#N/A Requesting Data...3674544966</v>
         <stp/>
         <stp>BDP|16250000632946565269</stp>
         <tr r="F32" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4268161809</v>
+        <v>#N/A Requesting Data...3925934282</v>
         <stp/>
         <stp>BDP|10062445544650347114</stp>
         <tr r="E69" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4243878473</v>
+        <v>#N/A Requesting Data...3784590489</v>
         <stp/>
         <stp>BDP|18056984346180923430</stp>
         <tr r="F67" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3961603607</v>
+        <v>#N/A Requesting Data...3304813178</v>
         <stp/>
         <stp>BDP|13607419850307697457</stp>
         <tr r="G55" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3840721055</v>
+        <v>#N/A Requesting Data...4237562332</v>
         <stp/>
         <stp>BDP|17151526894293450943</stp>
         <tr r="E34" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4109307142</v>
+        <v>#N/A Requesting Data...3574760850</v>
         <stp/>
         <stp>BDP|14769233272840536059</stp>
         <tr r="F48" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4245254799</v>
+        <v>#N/A Requesting Data...3666563512</v>
         <stp/>
         <stp>BDP|16347078018142331376</stp>
         <tr r="E59" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3984816695</v>
+        <v>#N/A Requesting Data...3493669526</v>
         <stp/>
         <stp>BDP|12157937398585487157</stp>
         <tr r="F69" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3964908911</v>
+        <v>#N/A Requesting Data...3524659136</v>
         <stp/>
         <stp>BDP|10450024654077121490</stp>
         <tr r="G29" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3843968508</v>
+        <v>#N/A Requesting Data...3820310805</v>
         <stp/>
         <stp>BDP|12405274734177384298</stp>
         <tr r="G109" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4287409680</v>
+        <v>#N/A Requesting Data...3406819238</v>
         <stp/>
         <stp>BDP|11693290023110245727</stp>
         <tr r="F93" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3972799483</v>
+        <v>#N/A Requesting Data...3705242328</v>
         <stp/>
         <stp>BDP|16857915317939051104</stp>
         <tr r="E4" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4127353415</v>
+        <v>#N/A Requesting Data...3580965524</v>
         <stp/>
         <stp>BDP|13092630751014311204</stp>
         <tr r="C29" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3882015561</v>
+        <v>#N/A Requesting Data...4264326768</v>
         <stp/>
         <stp>BDP|16560165422091315234</stp>
         <tr r="E74" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3880459477</v>
+        <v>#N/A Requesting Data...3991482365</v>
         <stp/>
         <stp>BDP|15578620992514708823</stp>
         <tr r="C74" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4106623690</v>
+        <v>#N/A Requesting Data...3518566259</v>
         <stp/>
         <stp>BDP|16311826266949112751</stp>
         <tr r="E137" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3892413226</v>
+        <v>#N/A Requesting Data...3608732213</v>
         <stp/>
         <stp>BDP|12423551309476829732</stp>
         <tr r="E29" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3903370690</v>
+        <v>#N/A Requesting Data...3747633098</v>
         <stp/>
         <stp>BDP|15334425393507822980</stp>
         <tr r="C71" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4172102319</v>
+        <v>#N/A Requesting Data...4093488717</v>
         <stp/>
         <stp>BDP|14187404668490888034</stp>
         <tr r="E115" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4207626703</v>
+        <v>#N/A Requesting Data...3231082495</v>
         <stp/>
         <stp>BDP|14038301256494491076</stp>
         <tr r="E12" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3988065021</v>
+        <v>#N/A Requesting Data...4276478843</v>
         <stp/>
         <stp>BDP|12212063840830333025</stp>
         <tr r="E132" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4011930538</v>
+        <v>#N/A Requesting Data...3708230351</v>
         <stp/>
         <stp>BDP|12411228970299104833</stp>
         <tr r="E40" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4246691729</v>
+        <v>#N/A Requesting Data...3616863844</v>
         <stp/>
         <stp>BDP|11324255971734653659</stp>
         <tr r="G93" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3945092227</v>
+        <v>#N/A Requesting Data...3614542424</v>
         <stp/>
         <stp>BDP|15080702944965265524</stp>
         <tr r="E5" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4110323298</v>
+        <v>#N/A Requesting Data...4247109615</v>
         <stp/>
         <stp>BDP|12709330545317601409</stp>
         <tr r="F78" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3980255103</v>
+        <v>#N/A Requesting Data...4197431495</v>
         <stp/>
         <stp>BDP|17558583635766924170</stp>
         <tr r="C139" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4224113963</v>
+        <v>#N/A Requesting Data...3372619209</v>
         <stp/>
         <stp>BDP|14043797868641345244</stp>
         <tr r="G127" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3942705804</v>
+        <v>#N/A Requesting Data...3771179257</v>
         <stp/>
         <stp>BDP|11097146762171726091</stp>
         <tr r="C125" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4235245989</v>
+        <v>#N/A Requesting Data...4179765312</v>
         <stp/>
         <stp>BDP|10083242995488903402</stp>
         <tr r="E22" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4100293387</v>
+        <v>#N/A Requesting Data...3987115575</v>
         <stp/>
         <stp>BDP|14104003677163905777</stp>
         <tr r="G89" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4143639241</v>
+        <v>#N/A Requesting Data...3553438549</v>
         <stp/>
         <stp>BDP|10493155251505330684</stp>
         <tr r="F113" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4075777882</v>
+        <v>#N/A Requesting Data...3380193512</v>
         <stp/>
         <stp>BDP|17307159600861837050</stp>
         <tr r="C28" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4086712737</v>
+        <v>#N/A Requesting Data...4135783417</v>
         <stp/>
         <stp>BDP|11974207352247436657</stp>
         <tr r="G84" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3922265052</v>
+        <v>#N/A Requesting Data...3611046417</v>
         <stp/>
         <stp>BDP|12417029733397010193</stp>
         <tr r="G129" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4272931456</v>
+        <v>#N/A Requesting Data...3394139868</v>
         <stp/>
         <stp>BDP|13696428749777505366</stp>
         <tr r="C128" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4288303824</v>
+        <v>#N/A Requesting Data...3827132427</v>
         <stp/>
         <stp>BDP|10265435339313984301</stp>
         <tr r="F136" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4079119593</v>
+        <v>#N/A Requesting Data...3551379511</v>
         <stp/>
         <stp>BDP|16742662035804692035</stp>
         <tr r="E24" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4093720398</v>
+        <v>#N/A Requesting Data...3699426474</v>
         <stp/>
         <stp>BDP|13311072247345018521</stp>
         <tr r="E129" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4192760549</v>
+        <v>#N/A Requesting Data...4215803204</v>
         <stp/>
         <stp>BDP|14635385909938704819</stp>
         <tr r="E106" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4179204759</v>
+        <v>#N/A Requesting Data...3191443594</v>
         <stp/>
         <stp>BDP|17965266240553639582</stp>
         <tr r="E10" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4097899956</v>
+        <v>#N/A Requesting Data...3903445112</v>
         <stp/>
         <stp>BDP|14559650107303581628</stp>
         <tr r="C72" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4047406248</v>
+        <v>#N/A Requesting Data...3766326374</v>
         <stp/>
         <stp>BDP|12078771150016496119</stp>
         <tr r="G102" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4290665076</v>
+        <v>#N/A Requesting Data...3739390957</v>
         <stp/>
         <stp>BDP|13437131854538783812</stp>
         <tr r="G22" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4283773006</v>
+        <v>#N/A Requesting Data...3234208018</v>
         <stp/>
         <stp>BDP|11816803688615161347</stp>
         <tr r="E51" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3900232939</v>
+        <v>#N/A Requesting Data...4064540484</v>
         <stp/>
         <stp>BDP|11136233214231371414</stp>
         <tr r="G139" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4135146810</v>
+        <v>#N/A Requesting Data...3323402211</v>
         <stp/>
         <stp>BDP|16387121100332435221</stp>
         <tr r="G96" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4088537188</v>
+        <v>#N/A Requesting Data...3879244917</v>
         <stp/>
         <stp>BDP|10044993787394494110</stp>
         <tr r="C113" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4043925487</v>
+        <v>#N/A Requesting Data...4044819010</v>
         <stp/>
         <stp>BDP|16851432539276999316</stp>
         <tr r="E44" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4102075933</v>
+        <v>#N/A Requesting Data...3592266465</v>
         <stp/>
         <stp>BDP|17514330731974993734</stp>
         <tr r="E65" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3903739618</v>
+        <v>#N/A Requesting Data...3752607429</v>
         <stp/>
         <stp>BDP|13397290692205579908</stp>
         <tr r="G128" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3912652524</v>
+        <v>#N/A Requesting Data...3947562296</v>
         <stp/>
         <stp>BDP|11770519860203890508</stp>
         <tr r="F106" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4136430582</v>
+        <v>#N/A Requesting Data...3415652065</v>
         <stp/>
         <stp>BDP|11828615722360397168</stp>
         <tr r="E71" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4147888412</v>
+        <v>#N/A Requesting Data...3216335608</v>
         <stp/>
         <stp>BDP|12429929188915695292</stp>
         <tr r="F109" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3898002279</v>
+        <v>#N/A Requesting Data...3586566627</v>
         <stp/>
         <stp>BDP|14807781952773549162</stp>
         <tr r="G33" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3910882585</v>
+        <v>#N/A Requesting Data...3486301321</v>
         <stp/>
         <stp>BDP|14141528956866623622</stp>
         <tr r="C134" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4218229505</v>
+        <v>#N/A Requesting Data...4128809829</v>
         <stp/>
         <stp>BDP|11925450918217650729</stp>
         <tr r="F86" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3997814971</v>
+        <v>#N/A Requesting Data...3872386634</v>
         <stp/>
         <stp>BDP|10075353521710450506</stp>
         <tr r="C109" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4156746288</v>
+        <v>#N/A Requesting Data...3764776078</v>
         <stp/>
         <stp>BDP|14507687284196916837</stp>
         <tr r="F6" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4062077742</v>
+        <v>#N/A Requesting Data...4054949150</v>
         <stp/>
         <stp>BDP|17592946715913980887</stp>
         <tr r="F7" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3936975363</v>
+        <v>#N/A Requesting Data...3349845810</v>
         <stp/>
         <stp>BDP|12670343566891576248</stp>
         <tr r="G36" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4268450078</v>
+        <v>#N/A Requesting Data...3988100849</v>
         <stp/>
         <stp>BDP|16059776447550017157</stp>
         <tr r="F63" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3897561636</v>
+        <v>#N/A Requesting Data...4104083271</v>
         <stp/>
         <stp>BDP|13709786759646324310</stp>
         <tr r="F46" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4016344473</v>
+        <v>#N/A Requesting Data...3296658722</v>
         <stp/>
         <stp>BDP|17680007951225535344</stp>
         <tr r="C93" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4147190011</v>
+        <v>#N/A Requesting Data...4247731898</v>
         <stp/>
         <stp>BDP|14249466628496635139</stp>
         <tr r="F26" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4220379217</v>
+        <v>#N/A Requesting Data...3345739188</v>
         <stp/>
         <stp>BDP|12616286245214000526</stp>
         <tr r="C114" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4117358004</v>
+        <v>#N/A Requesting Data...3334302027</v>
         <stp/>
         <stp>BDP|13229487552560837780</stp>
         <tr r="E139" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4114908813</v>
+        <v>#N/A Requesting Data...3506713025</v>
         <stp/>
         <stp>BDP|18412208651713792994</stp>
         <tr r="F118" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3914998288</v>
+        <v>#N/A Requesting Data...3537723037</v>
         <stp/>
         <stp>BDP|16919456577607807790</stp>
         <tr r="G56" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4240735050</v>
+        <v>#N/A Requesting Data...3623457801</v>
         <stp/>
         <stp>BDP|14958917677776306912</stp>
         <tr r="E124" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4106643057</v>
+        <v>#N/A Requesting Data...3768828636</v>
         <stp/>
         <stp>BDP|16906362551851442479</stp>
         <tr r="F14" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4041295239</v>
+        <v>#N/A Requesting Data...4293238683</v>
         <stp/>
         <stp>BDP|13303498173634341154</stp>
         <tr r="G72" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4126853206</v>
+        <v>#N/A Requesting Data...3980274367</v>
         <stp/>
         <stp>BDP|11394026073756494578</stp>
         <tr r="F4" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4044536328</v>
+        <v>#N/A Requesting Data...3890783513</v>
         <stp/>
         <stp>BDP|12821707660430898618</stp>
         <tr r="C40" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4093385864</v>
+        <v>#N/A Requesting Data...3834731504</v>
         <stp/>
         <stp>BDP|12207042919767891145</stp>
         <tr r="G131" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4148270083</v>
+        <v>#N/A Requesting Data...3567978505</v>
         <stp/>
         <stp>BDP|17617562141366516571</stp>
         <tr r="F24" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4186174723</v>
+        <v>#N/A Requesting Data...3748462168</v>
         <stp/>
         <stp>BDP|13776066979946925741</stp>
         <tr r="C90" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3953853568</v>
+        <v>#N/A Requesting Data...3928647144</v>
         <stp/>
         <stp>BDP|15429465971742273156</stp>
         <tr r="E67" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4168485936</v>
+        <v>#N/A Requesting Data...3980236047</v>
         <stp/>
         <stp>BDP|13319017160191784122</stp>
         <tr r="E43" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4244600025</v>
+        <v>#N/A Requesting Data...3477495585</v>
         <stp/>
         <stp>BDP|17197570677470339052</stp>
         <tr r="E33" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4260703250</v>
+        <v>#N/A Requesting Data...3552707100</v>
         <stp/>
         <stp>BDP|18198100188843948773</stp>
         <tr r="G60" s="1"/>
@@ -2727,1783 +2727,1783 @@
     </main>
     <main first="bofaddin.rtdserver">
       <tp t="s">
-        <v>#N/A Requesting Data...3923079893</v>
+        <v>#N/A Requesting Data...3605158723</v>
         <stp/>
         <stp>BDP|3930904544763426134</stp>
         <tr r="C55" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4095691644</v>
+        <v>#N/A Requesting Data...3598951803</v>
         <stp/>
         <stp>BDP|7103625188072362707</stp>
         <tr r="E98" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4246259143</v>
+        <v>#N/A Requesting Data...3666790958</v>
         <stp/>
         <stp>BDP|9365312653090978315</stp>
         <tr r="G136" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3977594600</v>
+        <v>#N/A Requesting Data...4108060357</v>
         <stp/>
         <stp>BDP|6412151529379694002</stp>
         <tr r="F110" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4051958392</v>
+        <v>#N/A Requesting Data...3675488035</v>
         <stp/>
         <stp>BDP|6245426297947871034</stp>
         <tr r="C80" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4253564460</v>
+        <v>#N/A Requesting Data...3302106807</v>
         <stp/>
         <stp>BDP|2350385774053258906</stp>
         <tr r="F72" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4004663020</v>
+        <v>#N/A Requesting Data...3578875276</v>
         <stp/>
         <stp>BDP|8530657130876609747</stp>
         <tr r="C44" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4265411192</v>
+        <v>#N/A Requesting Data...3989406698</v>
         <stp/>
         <stp>BDP|7198979431090342164</stp>
         <tr r="E50" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4198570260</v>
+        <v>#N/A Requesting Data...3645498119</v>
         <stp/>
         <stp>BDP|9075300299347332881</stp>
         <tr r="G79" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3971912727</v>
+        <v>#N/A Requesting Data...3872330048</v>
         <stp/>
         <stp>BDP|5029740995104753357</stp>
         <tr r="C111" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4141519438</v>
+        <v>#N/A Requesting Data...4000352122</v>
         <stp/>
         <stp>BDP|8128743572863334748</stp>
         <tr r="C47" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4042984356</v>
+        <v>#N/A Requesting Data...4250293771</v>
         <stp/>
         <stp>BDP|6339719327836450907</stp>
         <tr r="C98" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4237773302</v>
+        <v>#N/A Requesting Data...3572284145</v>
         <stp/>
         <stp>BDP|4200580269163222863</stp>
         <tr r="E25" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4029251741</v>
+        <v>#N/A Requesting Data...3676796815</v>
         <stp/>
         <stp>BDP|5989352249668473659</stp>
         <tr r="G50" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4278589162</v>
+        <v>#N/A Requesting Data...3277268131</v>
         <stp/>
         <stp>BDP|2484433252649720677</stp>
         <tr r="G68" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3964639861</v>
+        <v>#N/A Requesting Data...3686952118</v>
         <stp/>
         <stp>BDP|6249870436562567333</stp>
         <tr r="E49" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4052716193</v>
+        <v>#N/A Requesting Data...3582332437</v>
         <stp/>
         <stp>BDP|9572192910556051262</stp>
         <tr r="E134" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4157966939</v>
+        <v>#N/A Requesting Data...3813685083</v>
         <stp/>
         <stp>BDP|7540551159163224910</stp>
         <tr r="F51" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4291924839</v>
+        <v>#N/A Requesting Data...3387461578</v>
         <stp/>
         <stp>BDP|8451204331587951367</stp>
         <tr r="F52" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4163563999</v>
+        <v>#N/A Requesting Data...3740730954</v>
         <stp/>
         <stp>BDP|3109256470563958869</stp>
         <tr r="C52" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4262880956</v>
+        <v>#N/A Requesting Data...3885467143</v>
         <stp/>
         <stp>BDP|3590543194827878545</stp>
         <tr r="F59" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4206181717</v>
+        <v>#N/A Requesting Data...3404117526</v>
         <stp/>
         <stp>BDP|3009997314886390075</stp>
         <tr r="G100" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4287833446</v>
+        <v>#N/A Requesting Data...3723439433</v>
         <stp/>
         <stp>BDP|4777106988391072114</stp>
         <tr r="F103" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3977810480</v>
+        <v>#N/A Requesting Data...3567169388</v>
         <stp/>
         <stp>BDP|4303401897634933024</stp>
         <tr r="E93" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3985851484</v>
+        <v>#N/A Requesting Data...3419411689</v>
         <stp/>
         <stp>BDP|9055938583773500695</stp>
         <tr r="C34" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4288560979</v>
+        <v>#N/A Requesting Data...3490543002</v>
         <stp/>
         <stp>BDP|1573317174439842142</stp>
         <tr r="E133" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4219555876</v>
+        <v>#N/A Requesting Data...3790917777</v>
         <stp/>
         <stp>BDP|7180318607099335068</stp>
         <tr r="C9" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4171464529</v>
+        <v>#N/A Requesting Data...3724512472</v>
         <stp/>
         <stp>BDP|8371873502449565411</stp>
         <tr r="C62" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3997055861</v>
+        <v>#N/A Requesting Data...4192255739</v>
         <stp/>
         <stp>BDP|9300723062997279226</stp>
         <tr r="C124" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3973618511</v>
+        <v>#N/A Requesting Data...3799730524</v>
         <stp/>
         <stp>BDP|5492561896244379063</stp>
         <tr r="F70" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4258716274</v>
+        <v>#N/A Requesting Data...4184940464</v>
         <stp/>
         <stp>BDP|8460669760190400504</stp>
         <tr r="C27" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3999859084</v>
+        <v>#N/A Requesting Data...3779737274</v>
         <stp/>
         <stp>BDP|7634975275120208406</stp>
         <tr r="C31" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4066268547</v>
+        <v>#N/A Requesting Data...4012613392</v>
         <stp/>
         <stp>BDP|4040591290066838371</stp>
         <tr r="E13" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4293769777</v>
+        <v>#N/A Requesting Data...3459404835</v>
         <stp/>
         <stp>BDP|9247766641156585153</stp>
         <tr r="G94" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4141294519</v>
+        <v>#N/A Requesting Data...3303844930</v>
         <stp/>
         <stp>BDP|7940113982976758589</stp>
         <tr r="E95" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4114652571</v>
+        <v>#N/A Requesting Data...3822393536</v>
         <stp/>
         <stp>BDP|9093620553903200797</stp>
         <tr r="C105" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4156493636</v>
+        <v>#N/A Requesting Data...4280131187</v>
         <stp/>
         <stp>BDP|2405932012622401695</stp>
         <tr r="G77" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4260118207</v>
+        <v>#N/A Requesting Data...3903073989</v>
         <stp/>
         <stp>BDP|9175353808212225665</stp>
         <tr r="C66" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4216807160</v>
+        <v>#N/A Requesting Data...3731320224</v>
         <stp/>
         <stp>BDP|1414608591110891051</stp>
         <tr r="F9" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4083828523</v>
+        <v>#N/A Requesting Data...3967764164</v>
         <stp/>
         <stp>BDP|3649732806419915339</stp>
         <tr r="G14" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4217343641</v>
+        <v>#N/A Requesting Data...3747649529</v>
         <stp/>
         <stp>BDP|7006257261095505888</stp>
         <tr r="F54" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4258199924</v>
+        <v>#N/A Requesting Data...3867979784</v>
         <stp/>
         <stp>BDP|9781989741438009272</stp>
         <tr r="C39" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4235430061</v>
+        <v>#N/A Requesting Data...3650636379</v>
         <stp/>
         <stp>BDP|7532189862547338936</stp>
         <tr r="F58" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4113498576</v>
+        <v>#N/A Requesting Data...3451604990</v>
         <stp/>
         <stp>BDP|4286027170164748985</stp>
         <tr r="G113" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4039053940</v>
+        <v>#N/A Requesting Data...3616157284</v>
         <stp/>
         <stp>BDP|4691882821088256816</stp>
         <tr r="F126" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4084460802</v>
+        <v>#N/A Requesting Data...3642303685</v>
         <stp/>
         <stp>BDP|4974055815239706225</stp>
         <tr r="G110" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4074951647</v>
+        <v>#N/A Requesting Data...3445153548</v>
         <stp/>
         <stp>BDP|5916130291376545539</stp>
         <tr r="F73" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4030072965</v>
+        <v>#N/A Requesting Data...3804274213</v>
         <stp/>
         <stp>BDP|9535646277681935723</stp>
         <tr r="E60" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4024262874</v>
+        <v>#N/A Requesting Data...3489913978</v>
         <stp/>
         <stp>BDP|3472420329653378814</stp>
         <tr r="G4" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4043912315</v>
+        <v>#N/A Requesting Data...4066242343</v>
         <stp/>
         <stp>BDP|9676580711333862054</stp>
         <tr r="E135" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4124399086</v>
+        <v>#N/A Requesting Data...3752653767</v>
         <stp/>
         <stp>BDP|8651287802994649096</stp>
         <tr r="E77" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4266541641</v>
+        <v>#N/A Requesting Data...3932494045</v>
         <stp/>
         <stp>BDP|5552297197720045083</stp>
         <tr r="E118" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4180638834</v>
+        <v>#N/A Requesting Data...3850152651</v>
         <stp/>
         <stp>BDP|6195991527552839107</stp>
         <tr r="C61" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4231365302</v>
+        <v>#N/A Requesting Data...3700554648</v>
         <stp/>
         <stp>BDP|2785537291931900199</stp>
         <tr r="G91" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4001734655</v>
+        <v>#N/A Requesting Data...4026594359</v>
         <stp/>
         <stp>BDP|9875435960971965593</stp>
         <tr r="C11" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4137648557</v>
+        <v>#N/A Requesting Data...4198338860</v>
         <stp/>
         <stp>BDP|7662972721973338089</stp>
         <tr r="F107" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4008262823</v>
+        <v>#N/A Requesting Data...3775500932</v>
         <stp/>
         <stp>BDP|4282903616430488389</stp>
         <tr r="G9" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4110115524</v>
+        <v>#N/A Requesting Data...3852715428</v>
         <stp/>
         <stp>BDP|6606398548307737925</stp>
         <tr r="C70" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4217351844</v>
+        <v>#N/A Requesting Data...4242681681</v>
         <stp/>
         <stp>BDP|2310021551041423963</stp>
         <tr r="F123" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4260593752</v>
+        <v>#N/A Requesting Data...4064451495</v>
         <stp/>
         <stp>BDP|1666950877162018261</stp>
         <tr r="E87" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4267345485</v>
+        <v>#N/A Requesting Data...3791705429</v>
         <stp/>
         <stp>BDP|6280569068792932854</stp>
         <tr r="C46" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4096766064</v>
+        <v>#N/A Requesting Data...3461000951</v>
         <stp/>
         <stp>BDP|9635152443296662577</stp>
         <tr r="C16" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4110478362</v>
+        <v>#N/A Requesting Data...4183624707</v>
         <stp/>
         <stp>BDP|5935740968278021330</stp>
         <tr r="C96" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4016344274</v>
+        <v>#N/A Requesting Data...3744979701</v>
         <stp/>
         <stp>BDP|8225387168083679130</stp>
         <tr r="E57" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4241517311</v>
+        <v>#N/A Requesting Data...3456612160</v>
         <stp/>
         <stp>BDP|8741792397660502982</stp>
         <tr r="G24" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4124877443</v>
+        <v>#N/A Requesting Data...4201724292</v>
         <stp/>
         <stp>BDP|1988621838892198978</stp>
         <tr r="F82" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4203430329</v>
+        <v>#N/A Requesting Data...3455556907</v>
         <stp/>
         <stp>BDP|5160947801244572083</stp>
         <tr r="C97" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4058357607</v>
+        <v>#N/A Requesting Data...3848150506</v>
         <stp/>
         <stp>BDP|8781684350665372626</stp>
         <tr r="G64" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4088047522</v>
+        <v>#N/A Requesting Data...3405068012</v>
         <stp/>
         <stp>BDP|8866465832365619258</stp>
         <tr r="F120" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4230166511</v>
+        <v>#N/A Requesting Data...3744152045</v>
         <stp/>
         <stp>BDP|1231973558974048121</stp>
         <tr r="E123" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4114695091</v>
+        <v>#N/A Requesting Data...3598793658</v>
         <stp/>
         <stp>BDP|9011959145835954962</stp>
         <tr r="E102" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4042925524</v>
+        <v>#N/A Requesting Data...3854323898</v>
         <stp/>
         <stp>BDP|7048111723254898858</stp>
         <tr r="E70" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4035131771</v>
+        <v>#N/A Requesting Data...3981058696</v>
         <stp/>
         <stp>BDP|7514426398370500271</stp>
         <tr r="F84" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4148728193</v>
+        <v>#N/A Requesting Data...4079122545</v>
         <stp/>
         <stp>BDP|2286847884578687294</stp>
         <tr r="C64" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4292259595</v>
+        <v>#N/A Requesting Data...4290837888</v>
         <stp/>
         <stp>BDP|8581359335587083771</stp>
         <tr r="G40" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4180550797</v>
+        <v>#N/A Requesting Data...4146781669</v>
         <stp/>
         <stp>BDP|9176352611073152053</stp>
         <tr r="G52" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4127792532</v>
+        <v>#N/A Requesting Data...3746544847</v>
         <stp/>
         <stp>BDP|3761613276703138977</stp>
         <tr r="C22" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4270794025</v>
+        <v>#N/A Requesting Data...4086175820</v>
         <stp/>
         <stp>BDP|2402283480247992710</stp>
         <tr r="G65" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4121465250</v>
+        <v>#N/A Requesting Data...3841843109</v>
         <stp/>
         <stp>BDP|2496054182730824314</stp>
         <tr r="F108" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4185235680</v>
+        <v>#N/A Requesting Data...3953538442</v>
         <stp/>
         <stp>BDP|1156198294412416234</stp>
         <tr r="G48" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4080638452</v>
+        <v>#N/A Requesting Data...3559094281</v>
         <stp/>
         <stp>BDP|1935863512592400318</stp>
         <tr r="G99" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4198201776</v>
+        <v>#N/A Requesting Data...4230400493</v>
         <stp/>
         <stp>BDP|1182070188629538920</stp>
         <tr r="F85" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4154639777</v>
+        <v>#N/A Requesting Data...3734896783</v>
         <stp/>
         <stp>BDP|9924697901094165296</stp>
         <tr r="E38" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4194915678</v>
+        <v>#N/A Requesting Data...4038839296</v>
         <stp/>
         <stp>BDP|6412137247758825261</stp>
         <tr r="G10" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4097878890</v>
+        <v>#N/A Requesting Data...3765728204</v>
         <stp/>
         <stp>BDP|6277108296426856136</stp>
         <tr r="G122" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4279539750</v>
+        <v>#N/A Requesting Data...3430133886</v>
         <stp/>
         <stp>BDP|2351176324921816947</stp>
         <tr r="E117" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4259418694</v>
+        <v>#N/A Requesting Data...3680340320</v>
         <stp/>
         <stp>BDP|6406207188846485346</stp>
         <tr r="C37" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4216606896</v>
+        <v>#N/A Requesting Data...4251247080</v>
         <stp/>
         <stp>BDP|8112280367483097628</stp>
         <tr r="F16" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4151893060</v>
+        <v>#N/A Requesting Data...3450161699</v>
         <stp/>
         <stp>BDP|6484624822372932905</stp>
         <tr r="C108" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4083861198</v>
+        <v>#N/A Requesting Data...3882926769</v>
         <stp/>
         <stp>BDP|8605875253514357834</stp>
         <tr r="C116" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4081497365</v>
+        <v>#N/A Requesting Data...3698988732</v>
         <stp/>
         <stp>BDP|2842991807747556512</stp>
         <tr r="E110" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4046362942</v>
+        <v>#N/A Requesting Data...3506934034</v>
         <stp/>
         <stp>BDP|1377759003508711718</stp>
         <tr r="E55" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4280227827</v>
+        <v>#N/A Requesting Data...4223001658</v>
         <stp/>
         <stp>BDP|1711361391887412536</stp>
         <tr r="G47" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4286640457</v>
+        <v>#N/A Requesting Data...3950374813</v>
         <stp/>
         <stp>BDP|4564815655442574234</stp>
         <tr r="F114" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4074257609</v>
+        <v>#N/A Requesting Data...4080457113</v>
         <stp/>
         <stp>BDP|6557751567646791843</stp>
         <tr r="C85" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4251900310</v>
+        <v>#N/A Requesting Data...4117900545</v>
         <stp/>
         <stp>BDP|5018226780961297742</stp>
         <tr r="E138" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4137298874</v>
+        <v>#N/A Requesting Data...4248819866</v>
         <stp/>
         <stp>BDP|7190582290036507495</stp>
         <tr r="E48" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4126875382</v>
+        <v>#N/A Requesting Data...3700906882</v>
         <stp/>
         <stp>BDP|7268732641219205478</stp>
         <tr r="F111" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4287333017</v>
+        <v>#N/A Requesting Data...4261942656</v>
         <stp/>
         <stp>BDP|5085458293997400582</stp>
         <tr r="C30" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4220865126</v>
+        <v>#N/A Requesting Data...3798715328</v>
         <stp/>
         <stp>BDP|2916061605678582044</stp>
         <tr r="E27" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4096166077</v>
+        <v>#N/A Requesting Data...3610026488</v>
         <stp/>
         <stp>BDP|5645196194854205325</stp>
         <tr r="E19" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4205431670</v>
+        <v>#N/A Requesting Data...3985680352</v>
         <stp/>
         <stp>BDP|8929421222763426766</stp>
         <tr r="F112" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4242242025</v>
+        <v>#N/A Requesting Data...3550730914</v>
         <stp/>
         <stp>BDP|2815946348173965667</stp>
         <tr r="C137" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4062140015</v>
+        <v>#N/A Requesting Data...4111627705</v>
         <stp/>
         <stp>BDP|6645611732949919042</stp>
         <tr r="G95" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4062275810</v>
+        <v>#N/A Requesting Data...3651952776</v>
         <stp/>
         <stp>BDP|8744658502964028082</stp>
         <tr r="F139" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4211850039</v>
+        <v>#N/A Requesting Data...3990872356</v>
         <stp/>
         <stp>BDP|4077907452745230782</stp>
         <tr r="C130" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4259778935</v>
+        <v>#N/A Requesting Data...4162852069</v>
         <stp/>
         <stp>BDP|8975856381415089739</stp>
         <tr r="E75" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4082431523</v>
+        <v>#N/A Requesting Data...3917277833</v>
         <stp/>
         <stp>BDP|5738611839292209825</stp>
         <tr r="G107" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4171328222</v>
+        <v>#N/A Requesting Data...4161210846</v>
         <stp/>
         <stp>BDP|4996818111432201578</stp>
         <tr r="G134" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4160182087</v>
+        <v>#N/A Requesting Data...4077655794</v>
         <stp/>
         <stp>BDP|5458032582021895609</stp>
         <tr r="E89" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4262102881</v>
+        <v>#N/A Requesting Data...3651453690</v>
         <stp/>
         <stp>BDP|2612461303954522846</stp>
         <tr r="F21" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4250298769</v>
+        <v>#N/A Requesting Data...3674352493</v>
         <stp/>
         <stp>BDP|5852840000806674187</stp>
         <tr r="F75" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4099057511</v>
+        <v>#N/A Requesting Data...3942035610</v>
         <stp/>
         <stp>BDP|7947641811679527399</stp>
         <tr r="G13" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4249974173</v>
+        <v>#N/A Requesting Data...4157410816</v>
         <stp/>
         <stp>BDP|8407769428857900025</stp>
         <tr r="C132" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4225677840</v>
+        <v>#N/A Requesting Data...3799893450</v>
         <stp/>
         <stp>BDP|1313714864639868399</stp>
         <tr r="F87" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4281886868</v>
+        <v>#N/A Requesting Data...3851233314</v>
         <stp/>
         <stp>BDP|2531298252748844733</stp>
         <tr r="F115" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4106765695</v>
+        <v>#N/A Requesting Data...4011453050</v>
         <stp/>
         <stp>BDP|8965389266391509672</stp>
         <tr r="C41" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4280341763</v>
+        <v>#N/A Requesting Data...3866377842</v>
         <stp/>
         <stp>BDP|9146373380128430189</stp>
         <tr r="F60" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4271703871</v>
+        <v>#N/A Requesting Data...4283937865</v>
         <stp/>
         <stp>BDP|8769626454200391097</stp>
         <tr r="G85" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4180022670</v>
+        <v>#N/A Requesting Data...4037319283</v>
         <stp/>
         <stp>BDP|7701346097304455298</stp>
         <tr r="C73" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4276702843</v>
+        <v>#N/A Requesting Data...3468760062</v>
         <stp/>
         <stp>BDP|1201589979318261083</stp>
         <tr r="G123" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4117657732</v>
+        <v>#N/A Requesting Data...3456535614</v>
         <stp/>
         <stp>BDP|9994425762708075853</stp>
         <tr r="G88" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4137249136</v>
+        <v>#N/A Requesting Data...3748409604</v>
         <stp/>
         <stp>BDP|8238868892513701135</stp>
         <tr r="G137" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4251829887</v>
+        <v>#N/A Requesting Data...4232044929</v>
         <stp/>
         <stp>BDP|3321556007464177923</stp>
         <tr r="E109" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4220005355</v>
+        <v>#N/A Requesting Data...3802873400</v>
         <stp/>
         <stp>BDP|8367368187378355023</stp>
         <tr r="F64" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4271937895</v>
+        <v>#N/A Requesting Data...3637178829</v>
         <stp/>
         <stp>BDP|9054142235387080711</stp>
         <tr r="F11" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4188191774</v>
+        <v>#N/A Requesting Data...3855887989</v>
         <stp/>
         <stp>BDP|4797724273716399932</stp>
         <tr r="C5" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4270037777</v>
+        <v>#N/A Requesting Data...4254492525</v>
         <stp/>
         <stp>BDP|3084971212582403246</stp>
         <tr r="F121" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4200064194</v>
+        <v>#N/A Requesting Data...3514263818</v>
         <stp/>
         <stp>BDP|6948762204713990690</stp>
         <tr r="G90" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4265350391</v>
+        <v>#N/A Requesting Data...3838895348</v>
         <stp/>
         <stp>BDP|1832764578595986067</stp>
         <tr r="G119" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4130995580</v>
+        <v>#N/A Requesting Data...3831320803</v>
         <stp/>
         <stp>BDP|4156639623951685595</stp>
         <tr r="F13" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4200622876</v>
+        <v>#N/A Requesting Data...4036108927</v>
         <stp/>
         <stp>BDP|5919761437851372455</stp>
         <tr r="C2" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4129452485</v>
+        <v>#N/A Requesting Data...3448523614</v>
         <stp/>
         <stp>BDP|1551339666687413790</stp>
         <tr r="F40" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4199727439</v>
+        <v>#N/A Requesting Data...3662943929</v>
         <stp/>
         <stp>BDP|6420437202397070174</stp>
         <tr r="C8" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4195785560</v>
+        <v>#N/A Requesting Data...3508817368</v>
         <stp/>
         <stp>BDP|1708381902825815365</stp>
         <tr r="C101" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4158106240</v>
+        <v>#N/A Requesting Data...3874342072</v>
         <stp/>
         <stp>BDP|4945796250777738578</stp>
         <tr r="G21" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4288558790</v>
+        <v>#N/A Requesting Data...3455596664</v>
         <stp/>
         <stp>BDP|6746841414412327938</stp>
         <tr r="G75" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4207373712</v>
+        <v>#N/A Requesting Data...3627047384</v>
         <stp/>
         <stp>BDP|1709445403856801620</stp>
         <tr r="E85" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4199580400</v>
+        <v>#N/A Requesting Data...3920996205</v>
         <stp/>
         <stp>BDP|9398823419477440265</stp>
         <tr r="G125" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4139336638</v>
+        <v>#N/A Requesting Data...4195405791</v>
         <stp/>
         <stp>BDP|3430878723724827801</stp>
         <tr r="G41" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4183568938</v>
+        <v>#N/A Requesting Data...3793476279</v>
         <stp/>
         <stp>BDP|9698422803149077198</stp>
         <tr r="C100" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4159270619</v>
+        <v>#N/A Requesting Data...3550444705</v>
         <stp/>
         <stp>BDP|2887002514665714363</stp>
         <tr r="G59" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4294428234</v>
+        <v>#N/A Requesting Data...4249466449</v>
         <stp/>
         <stp>BDP|2668814054578766269</stp>
         <tr r="E31" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4245265484</v>
+        <v>#N/A Requesting Data...3544186199</v>
         <stp/>
         <stp>BDP|8894702939828266110</stp>
         <tr r="C7" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4222059759</v>
+        <v>#N/A Requesting Data...3551843192</v>
         <stp/>
         <stp>BDP|3410885660260666884</stp>
         <tr r="E64" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4289704347</v>
+        <v>#N/A Requesting Data...3902589894</v>
         <stp/>
         <stp>BDP|3658713905400418152</stp>
         <tr r="E35" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4134301133</v>
+        <v>#N/A Requesting Data...3487407109</v>
         <stp/>
         <stp>BDP|7570300716478486864</stp>
         <tr r="E32" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4146402688</v>
+        <v>#N/A Requesting Data...4147614086</v>
         <stp/>
         <stp>BDP|7851492951527237434</stp>
         <tr r="E52" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4264081085</v>
+        <v>#N/A Requesting Data...3828182474</v>
         <stp/>
         <stp>BDP|7352242467910007671</stp>
         <tr r="F124" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4163030200</v>
+        <v>#N/A Requesting Data...3654829496</v>
         <stp/>
         <stp>BDP|5657563513753480721</stp>
         <tr r="E80" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4269577577</v>
+        <v>#N/A Requesting Data...4132090169</v>
         <stp/>
         <stp>BDP|5976587264538865878</stp>
         <tr r="E62" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4284661862</v>
+        <v>#N/A Requesting Data...4153260948</v>
         <stp/>
         <stp>BDP|7151318027339523982</stp>
         <tr r="F91" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4147587948</v>
+        <v>#N/A Requesting Data...3939181628</v>
         <stp/>
         <stp>BDP|1896477110772260049</stp>
         <tr r="C91" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4292686124</v>
+        <v>#N/A Requesting Data...4069173580</v>
         <stp/>
         <stp>BDP|4252725967471187287</stp>
         <tr r="F44" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4226801068</v>
+        <v>#N/A Requesting Data...4194022908</v>
         <stp/>
         <stp>BDP|6943451920864586278</stp>
         <tr r="C118" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4247392108</v>
+        <v>#N/A Requesting Data...3727121078</v>
         <stp/>
         <stp>BDP|5838113265174067025</stp>
         <tr r="F39" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4265498737</v>
+        <v>#N/A Requesting Data...3903186600</v>
         <stp/>
         <stp>BDP|3456718228377624745</stp>
         <tr r="E111" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4138899058</v>
+        <v>#N/A Requesting Data...3912669632</v>
         <stp/>
         <stp>BDP|5917425194519245724</stp>
         <tr r="E79" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4149307085</v>
+        <v>#N/A Requesting Data...3915288167</v>
         <stp/>
         <stp>BDP|6787533358407016713</stp>
         <tr r="F135" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4151054806</v>
+        <v>#N/A Requesting Data...3468550840</v>
         <stp/>
         <stp>BDP|5576451913756991076</stp>
         <tr r="E16" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4139920155</v>
+        <v>#N/A Requesting Data...4235969747</v>
         <stp/>
         <stp>BDP|5284390591628042184</stp>
         <tr r="C24" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4234530291</v>
+        <v>#N/A Requesting Data...4155809922</v>
         <stp/>
         <stp>BDP|5412037028917536689</stp>
         <tr r="G115" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4147557743</v>
+        <v>#N/A Requesting Data...3988512981</v>
         <stp/>
         <stp>BDP|8966942938724477029</stp>
         <tr r="C15" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4288191532</v>
+        <v>#N/A Requesting Data...4226164559</v>
         <stp/>
         <stp>BDP|2938144706552859709</stp>
         <tr r="G81" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4181691642</v>
+        <v>#N/A Requesting Data...3970413342</v>
         <stp/>
         <stp>BDP|3632949480676633244</stp>
         <tr r="F31" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4218930960</v>
+        <v>#N/A Requesting Data...4166891912</v>
         <stp/>
         <stp>BDP|3513418606797579639</stp>
         <tr r="F90" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4168054275</v>
+        <v>#N/A Requesting Data...3754808536</v>
         <stp/>
         <stp>BDP|1733520919261908213</stp>
         <tr r="G73" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4160873188</v>
+        <v>#N/A Requesting Data...3514018445</v>
         <stp/>
         <stp>BDP|8368969127023380651</stp>
         <tr r="F28" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4248876766</v>
+        <v>#N/A Requesting Data...3689354906</v>
         <stp/>
         <stp>BDP|7172716621593553717</stp>
         <tr r="F53" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4279578889</v>
+        <v>#N/A Requesting Data...4196915565</v>
         <stp/>
         <stp>BDP|2954250373819174944</stp>
         <tr r="F119" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4233412722</v>
+        <v>#N/A Requesting Data...3957297202</v>
         <stp/>
         <stp>BDP|4728287753511799518</stp>
         <tr r="F3" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4236883261</v>
+        <v>#N/A Requesting Data...4040550599</v>
         <stp/>
         <stp>BDP|6348617969513327227</stp>
         <tr r="E104" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4229925503</v>
+        <v>#N/A Requesting Data...4064321166</v>
         <stp/>
         <stp>BDP|7694099704858685831</stp>
         <tr r="C107" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4269863408</v>
+        <v>#N/A Requesting Data...3584329829</v>
         <stp/>
         <stp>BDP|4106834752526835861</stp>
         <tr r="F55" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4197362911</v>
+        <v>#N/A Requesting Data...3530352606</v>
         <stp/>
         <stp>BDP|7951337561756108354</stp>
         <tr r="G112" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4215052214</v>
+        <v>#N/A Requesting Data...3699307442</v>
         <stp/>
         <stp>BDP|5468867501418549294</stp>
         <tr r="E86" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4224958693</v>
+        <v>#N/A Requesting Data...4278226972</v>
         <stp/>
         <stp>BDP|4546740053823447251</stp>
         <tr r="C32" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4256458874</v>
+        <v>#N/A Requesting Data...4278656418</v>
         <stp/>
         <stp>BDP|7484527599745538990</stp>
         <tr r="F76" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4241066528</v>
+        <v>#N/A Requesting Data...4211730362</v>
         <stp/>
         <stp>BDP|5578475423865159117</stp>
         <tr r="E61" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4203483138</v>
+        <v>#N/A Requesting Data...4161199871</v>
         <stp/>
         <stp>BDP|6158107237024797760</stp>
         <tr r="E45" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4230418165</v>
+        <v>#N/A Requesting Data...3742712942</v>
         <stp/>
         <stp>BDP|4143076943390197735</stp>
         <tr r="F97" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4246977775</v>
+        <v>#N/A Requesting Data...4052034498</v>
         <stp/>
         <stp>BDP|1762196091349932721</stp>
         <tr r="E82" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4254617411</v>
+        <v>#N/A Requesting Data...3706389947</v>
         <stp/>
         <stp>BDP|4189169184528349241</stp>
         <tr r="F137" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4223766264</v>
+        <v>#N/A Requesting Data...3720749937</v>
         <stp/>
         <stp>BDP|9103140635044368872</stp>
         <tr r="F29" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4294516157</v>
+        <v>#N/A Requesting Data...3643517639</v>
         <stp/>
         <stp>BDP|5519603296584718917</stp>
         <tr r="G54" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4287812584</v>
+        <v>#N/A Requesting Data...3837983187</v>
         <stp/>
         <stp>BDP|1156250824766982737</stp>
         <tr r="G44" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4257533221</v>
+        <v>#N/A Requesting Data...3680692592</v>
         <stp/>
         <stp>BDP|6031605254431729496</stp>
         <tr r="G86" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4254809594</v>
+        <v>#N/A Requesting Data...4135640445</v>
         <stp/>
         <stp>BDP|2649489454114394728</stp>
         <tr r="C14" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4291669942</v>
+        <v>#N/A Requesting Data...3689892564</v>
         <stp/>
         <stp>BDP|8999377595616850481</stp>
         <tr r="E108" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4270176205</v>
+        <v>#N/A Requesting Data...4192178338</v>
         <stp/>
         <stp>BDP|8988928209665280487</stp>
         <tr r="F71" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4269425269</v>
+        <v>#N/A Requesting Data...4206081279</v>
         <stp/>
         <stp>BDP|8368023487691952119</stp>
         <tr r="F88" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4290447745</v>
+        <v>#N/A Requesting Data...3582218822</v>
         <stp/>
         <stp>BDP|5199287207907438042</stp>
         <tr r="E66" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4293820776</v>
+        <v>#N/A Requesting Data...3933079240</v>
         <stp/>
         <stp>BDP|7460099446995728631</stp>
         <tr r="F134" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4288126937</v>
+        <v>#N/A Requesting Data...3548352630</v>
         <stp/>
         <stp>BDP|6160638673325976246</stp>
         <tr r="C104" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4285147491</v>
+        <v>#N/A Requesting Data...4069842569</v>
         <stp/>
         <stp>BDP|5660731962530222490</stp>
         <tr r="E128" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4287122544</v>
+        <v>#N/A Requesting Data...4092530921</v>
         <stp/>
         <stp>BDP|3355023726294311595</stp>
         <tr r="G114" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4282423763</v>
+        <v>#N/A Requesting Data...4137442694</v>
         <stp/>
         <stp>BDP|5604474461391860653</stp>
         <tr r="E130" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4291923392</v>
+        <v>#N/A Requesting Data...4132625147</v>
         <stp/>
         <stp>BDP|3542140114402066179</stp>
         <tr r="E78" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4288035469</v>
+        <v>#N/A Requesting Data...3947117955</v>
         <stp/>
         <stp>BDP|2942496252996870592</stp>
         <tr r="G121" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4293961519</v>
+        <v>#N/A Requesting Data...4226656865</v>
         <stp/>
         <stp>BDP|1823820926283534897</stp>
         <tr r="G18" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4288888954</v>
+        <v>#N/A Requesting Data...3961581669</v>
         <stp/>
         <stp>BDP|3716189405712826043</stp>
         <tr r="G92" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4291577387</v>
+        <v>#N/A Requesting Data...4088214970</v>
         <stp/>
         <stp>BDP|9344147089140006098</stp>
         <tr r="E83" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4290002374</v>
+        <v>#N/A Requesting Data...3753902096</v>
         <stp/>
         <stp>BDP|6993061706081965773</stp>
         <tr r="F81" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4293340241</v>
+        <v>#N/A Requesting Data...3702310602</v>
         <stp/>
         <stp>BDP|6176792116871092198</stp>
         <tr r="C68" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4294086770</v>
+        <v>#N/A Requesting Data...4231398513</v>
         <stp/>
         <stp>BDP|7185432584822399912</stp>
         <tr r="F131" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4294939060</v>
+        <v>#N/A Requesting Data...4094780228</v>
         <stp/>
         <stp>BDP|8280856169194643320</stp>
         <tr r="G49" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1016579491</v>
+        <v>#N/A Requesting Data...3616906373</v>
         <stp/>
         <stp>BDP|9399109618929306123</stp>
         <tr r="F37" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3053799266</v>
+        <v>#N/A Requesting Data...3834635112</v>
         <stp/>
         <stp>BDP|6669663699409638145</stp>
         <tr r="C123" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1712569240</v>
+        <v>#N/A Requesting Data...3557771281</v>
         <stp/>
         <stp>BDP|6175693122901836298</stp>
         <tr r="C36" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...312641488</v>
+        <v>#N/A Requesting Data...4274130658</v>
         <stp/>
         <stp>BDP|8135075327118072391</stp>
         <tr r="C17" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...761725067</v>
+        <v>#N/A Requesting Data...4124272603</v>
         <stp/>
         <stp>BDP|5726291712345411206</stp>
         <tr r="G28" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3683100579</v>
+        <v>#N/A Requesting Data...3635504775</v>
         <stp/>
         <stp>BDP|8698973352783506690</stp>
         <tr r="F25" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2609666150</v>
+        <v>#N/A Requesting Data...3566996585</v>
         <stp/>
         <stp>BDP|5493604681742158862</stp>
         <tr r="G63" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3929608783</v>
+        <v>#N/A Requesting Data...4146437562</v>
         <stp/>
         <stp>BDP|3239104742287612040</stp>
         <tr r="E39" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...656294143</v>
+        <v>#N/A Requesting Data...3826736748</v>
         <stp/>
         <stp>BDP|3381147726641663059</stp>
         <tr r="C122" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1872362720</v>
+        <v>#N/A Requesting Data...3921670384</v>
         <stp/>
         <stp>BDP|6625906764329795167</stp>
         <tr r="F56" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2790770356</v>
+        <v>#N/A Requesting Data...4079678298</v>
         <stp/>
         <stp>BDP|3325218238213801010</stp>
         <tr r="F57" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1714273785</v>
+        <v>#N/A Requesting Data...3872678760</v>
         <stp/>
         <stp>BDP|1313137390988032037</stp>
         <tr r="C83" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...107662531</v>
+        <v>#N/A Requesting Data...4112447941</v>
         <stp/>
         <stp>BDP|3702733300853619616</stp>
         <tr r="G34" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2684866455</v>
+        <v>#N/A Requesting Data...4032549951</v>
         <stp/>
         <stp>BDP|8558611930018338475</stp>
         <tr r="F35" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1444309142</v>
+        <v>#N/A Requesting Data...4011847556</v>
         <stp/>
         <stp>BDP|5387098906493173798</stp>
         <tr r="G62" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3398722907</v>
+        <v>#N/A Requesting Data...3829683557</v>
         <stp/>
         <stp>BDP|1951038018907673608</stp>
         <tr r="C126" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4156673045</v>
+        <v>#N/A Requesting Data...3557893438</v>
         <stp/>
         <stp>BDP|9253802402770546012</stp>
         <tr r="F74" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...681218879</v>
+        <v>#N/A Requesting Data...3771071714</v>
         <stp/>
         <stp>BDP|1884505914021260664</stp>
         <tr r="E96" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2893159190</v>
+        <v>#N/A Requesting Data...4238912568</v>
         <stp/>
         <stp>BDP|3540127028674193608</stp>
         <tr r="F94" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...115285391</v>
+        <v>#N/A Requesting Data...4200135703</v>
         <stp/>
         <stp>BDP|5372375359741187031</stp>
         <tr r="F27" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1380274923</v>
+        <v>#N/A Requesting Data...3945888569</v>
         <stp/>
         <stp>BDP|5121625602631825066</stp>
         <tr r="E81" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1931469533</v>
+        <v>#N/A Requesting Data...4092806661</v>
         <stp/>
         <stp>BDP|5282708515920897138</stp>
         <tr r="F43" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3612486215</v>
+        <v>#N/A Requesting Data...3597804093</v>
         <stp/>
         <stp>BDP|1250299291741371958</stp>
         <tr r="G31" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3164370212</v>
+        <v>#N/A Requesting Data...4220770477</v>
         <stp/>
         <stp>BDP|4253176148933327033</stp>
         <tr r="C133" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...126210314</v>
+        <v>#N/A Requesting Data...3981071218</v>
         <stp/>
         <stp>BDP|9704751602229087502</stp>
         <tr r="F49" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2806684590</v>
+        <v>#N/A Requesting Data...3857777524</v>
         <stp/>
         <stp>BDP|6775233901286469015</stp>
         <tr r="E125" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...683667451</v>
+        <v>#N/A Requesting Data...3913476355</v>
         <stp/>
         <stp>BDP|7918289416910309647</stp>
         <tr r="C56" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3183409510</v>
+        <v>#N/A Requesting Data...3623753372</v>
         <stp/>
         <stp>BDP|3731272815900600241</stp>
         <tr r="C53" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4190425212</v>
+        <v>#N/A Requesting Data...3688067192</v>
         <stp/>
         <stp>BDP|1685459166489439868</stp>
         <tr r="F133" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1232707616</v>
+        <v>#N/A Requesting Data...4230126216</v>
         <stp/>
         <stp>BDP|2506644172580171154</stp>
         <tr r="C119" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...448774662</v>
+        <v>#N/A Requesting Data...3893196657</v>
         <stp/>
         <stp>BDP|1995353227627490580</stp>
         <tr r="E119" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1526827554</v>
+        <v>#N/A Requesting Data...4252423028</v>
         <stp/>
         <stp>BDP|9173868178561206592</stp>
         <tr r="C77" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1894040366</v>
+        <v>#N/A Requesting Data...3779007505</v>
         <stp/>
         <stp>BDP|4008096672221657096</stp>
         <tr r="G43" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2799052284</v>
+        <v>#N/A Requesting Data...3978250977</v>
         <stp/>
         <stp>BDP|5434663182001395869</stp>
         <tr r="E107" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3821400396</v>
+        <v>#N/A Requesting Data...3839738004</v>
         <stp/>
         <stp>BDP|8686279502629263146</stp>
         <tr r="C129" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...978848911</v>
+        <v>#N/A Requesting Data...3806058285</v>
         <stp/>
         <stp>BDP|4576300957588172984</stp>
         <tr r="E63" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2408099135</v>
+        <v>#N/A Requesting Data...3786046441</v>
         <stp/>
         <stp>BDP|7469671678835895086</stp>
         <tr r="E2" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2119159650</v>
+        <v>#N/A Requesting Data...4155905767</v>
         <stp/>
         <stp>BDP|5444751401066968714</stp>
         <tr r="E73" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...194462724</v>
+        <v>#N/A Requesting Data...3815755264</v>
         <stp/>
         <stp>BDP|2824124077350027748</stp>
         <tr r="E136" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3563007873</v>
+        <v>#N/A Requesting Data...3679437409</v>
         <stp/>
         <stp>BDP|3708851985886704699</stp>
         <tr r="C19" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3541395595</v>
+        <v>#N/A Requesting Data...4239166003</v>
         <stp/>
         <stp>BDP|1006071828475585561</stp>
         <tr r="F116" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...139508987</v>
+        <v>#N/A Requesting Data...4216315843</v>
         <stp/>
         <stp>BDP|1086712249007771639</stp>
         <tr r="G26" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3098159571</v>
+        <v>#N/A Requesting Data...3994386433</v>
         <stp/>
         <stp>BDP|6634730869724168016</stp>
         <tr r="E103" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2496445709</v>
+        <v>#N/A Requesting Data...3689202610</v>
         <stp/>
         <stp>BDP|3520366017777816505</stp>
         <tr r="E97" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...739122462</v>
+        <v>#N/A Requesting Data...3988353792</v>
         <stp/>
         <stp>BDP|2995135217932647367</stp>
         <tr r="F105" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...542554286</v>
+        <v>#N/A Requesting Data...4106647630</v>
         <stp/>
         <stp>BDP|3565057922625094707</stp>
         <tr r="G45" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3716962810</v>
+        <v>#N/A Requesting Data...3694925288</v>
         <stp/>
         <stp>BDP|1485569542807651461</stp>
         <tr r="C86" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4168046004</v>
+        <v>#N/A Requesting Data...4073762370</v>
         <stp/>
         <stp>BDP|1159006460850353421</stp>
         <tr r="E46" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4032219627</v>
+        <v>#N/A Requesting Data...3645744595</v>
         <stp/>
         <stp>BDP|5113311422502283510</stp>
         <tr r="C84" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1077436861</v>
+        <v>#N/A Requesting Data...4178484689</v>
         <stp/>
         <stp>BDP|4420649803735408460</stp>
         <tr r="F117" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1434038112</v>
+        <v>#N/A Requesting Data...3986473672</v>
         <stp/>
         <stp>BDP|9873235984695079585</stp>
         <tr r="C60" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...766119899</v>
+        <v>#N/A Requesting Data...3622886214</v>
         <stp/>
         <stp>BDP|4726106605717010168</stp>
         <tr r="G46" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...894546836</v>
+        <v>#N/A Requesting Data...4016393022</v>
         <stp/>
         <stp>BDP|97453184744598227</stp>
         <tr r="G135" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...908651188</v>
+        <v>#N/A Requesting Data...4226139642</v>
         <stp/>
         <stp>BDP|71129432364790944</stp>
         <tr r="E105" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4103186300</v>
+        <v>#N/A Requesting Data...4217683274</v>
         <stp/>
         <stp>BDP|13870968378316918</stp>
         <tr r="F38" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...346097211</v>
+        <v>#N/A Requesting Data...3665953841</v>
         <stp/>
         <stp>BDP|545017254499479967</stp>
         <tr r="E23" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1284058557</v>
+        <v>#N/A Requesting Data...3911408063</v>
         <stp/>
         <stp>BDP|562457211792430265</stp>
         <tr r="G116" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2782535074</v>
+        <v>#N/A Requesting Data...3921177674</v>
         <stp/>
         <stp>BDP|752318736222262646</stp>
         <tr r="F83" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2186791608</v>
+        <v>#N/A Requesting Data...3950199830</v>
         <stp/>
         <stp>BDP|926433161397617222</stp>
         <tr r="F10" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2880969603</v>
+        <v>#N/A Requesting Data...3610124077</v>
         <stp/>
         <stp>BDP|455507803480864317</stp>
         <tr r="C51" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2726596238</v>
+        <v>#N/A Requesting Data...3721872527</v>
         <stp/>
         <stp>BDP|738430784972633891</stp>
         <tr r="F41" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3650247459</v>
+        <v>#N/A Requesting Data...4244300710</v>
         <stp/>
         <stp>BDP|226270545351892196</stp>
         <tr r="F61" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2387106255</v>
+        <v>#N/A Requesting Data...3948019938</v>
         <stp/>
         <stp>BDP|478534605105814154</stp>
         <tr r="G12" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...787125045</v>
+        <v>#N/A Requesting Data...4030700920</v>
         <stp/>
         <stp>BDP|292697057297288557</stp>
         <tr r="C106" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1254820502</v>
+        <v>#N/A Requesting Data...3860786571</v>
         <stp/>
         <stp>BDP|449489448517477649</stp>
         <tr r="E99" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3971948262</v>
+        <v>#N/A Requesting Data...3692731597</v>
         <stp/>
         <stp>BDP|477239144286521179</stp>
         <tr r="G138" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...98894971</v>
+        <v>#N/A Requesting Data...3624824885</v>
         <stp/>
         <stp>BDP|136361134742057301</stp>
         <tr r="C57" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3947544311</v>
+        <v>#N/A Requesting Data...3922322345</v>
         <stp/>
         <stp>BDP|282958180978155995</stp>
         <tr r="C59" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...375523780</v>
+        <v>#N/A Requesting Data...3946151833</v>
         <stp/>
         <stp>BDP|991366924295531418</stp>
         <tr r="F2" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...747193868</v>
+        <v>#N/A Requesting Data...3739518615</v>
         <stp/>
         <stp>BDP|934073235795196633</stp>
         <tr r="F62" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...612123527</v>
+        <v>#N/A Requesting Data...3636666283</v>
         <stp/>
         <stp>BDP|266608211912165570</stp>
         <tr r="E113" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1954824844</v>
+        <v>#N/A Requesting Data...4083388935</v>
         <stp/>
         <stp>BDP|910156400954699593</stp>
         <tr r="G8" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1581577410</v>
+        <v>#N/A Requesting Data...3736717580</v>
         <stp/>
         <stp>BDP|794293317440269040</stp>
         <tr r="E100" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1553344589</v>
+        <v>#N/A Requesting Data...3862218914</v>
         <stp/>
         <stp>BDP|206766873121157269</stp>
         <tr r="E41" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...772570773</v>
+        <v>#N/A Requesting Data...4247430059</v>
         <stp/>
         <stp>BDP|315261912951356153</stp>
         <tr r="E21" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1815034721</v>
+        <v>#N/A Requesting Data...4162761922</v>
         <stp/>
         <stp>BDP|169080827246056602</stp>
         <tr r="G126" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3016355865</v>
+        <v>#N/A Requesting Data...3957709800</v>
         <stp/>
         <stp>BDP|454779781439338455</stp>
         <tr r="E36" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1004182890</v>
+        <v>#N/A Requesting Data...4125155612</v>
         <stp/>
         <stp>BDP|198524097739196711</stp>
         <tr r="F92" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1191875690</v>
+        <v>#N/A Requesting Data...3995863723</v>
         <stp/>
         <stp>BDP|618726407191106421</stp>
         <tr r="C92" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1264689479</v>
+        <v>#N/A Requesting Data...4246817325</v>
         <stp/>
         <stp>BDP|442808307356626303</stp>
         <tr r="F20" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2135705584</v>
+        <v>#N/A Requesting Data...4215120110</v>
         <stp/>
         <stp>BDP|304889655090792147</stp>
         <tr r="E58" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1776330005</v>
+        <v>#N/A Requesting Data...4222045105</v>
         <stp/>
         <stp>BDP|427627592191043219</stp>
         <tr r="C87" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...495681633</v>
+        <v>#N/A Requesting Data...4245370262</v>
         <stp/>
         <stp>BDP|768711067038142524</stp>
         <tr r="G25" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2711586275</v>
+        <v>#N/A Requesting Data...3784000869</v>
         <stp/>
         <stp>BDP|447365482187669383</stp>
         <tr r="C95" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2565747856</v>
+        <v>#N/A Requesting Data...4269008050</v>
         <stp/>
         <stp>BDP|901925773788783965</stp>
         <tr r="G67" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3894958011</v>
+        <v>#N/A Requesting Data...4152849250</v>
         <stp/>
         <stp>BDP|511429594874391764</stp>
         <tr r="G117" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3318177731</v>
+        <v>#N/A Requesting Data...4226912598</v>
         <stp/>
         <stp>BDP|544620567958067604</stp>
         <tr r="C131" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1146846109</v>
+        <v>#N/A Requesting Data...4214931684</v>
         <stp/>
         <stp>BDP|945569483354328027</stp>
         <tr r="C21" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2597459438</v>
+        <v>#N/A Requesting Data...4248823905</v>
         <stp/>
         <stp>BDP|691281527639744142</stp>
         <tr r="E8" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3501980360</v>
+        <v>#N/A Requesting Data...4291961818</v>
         <stp/>
         <stp>BDP|968314719543295935</stp>
         <tr r="E68" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...149330339</v>
+        <v>#N/A Requesting Data...4035836776</v>
         <stp/>
         <stp>BDP|760426044168153386</stp>
         <tr r="G7" s="1"/>
@@ -4813,7 +4813,7 @@
   <dimension ref="A1:E139"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4877,7 +4877,7 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>288</v>
+        <v>310</v>
       </c>
       <c r="D4" t="s">
         <v>289</v>
@@ -4934,7 +4934,7 @@
         <v>295</v>
       </c>
       <c r="E7" t="s">
-        <v>296</v>
+        <v>308</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -4945,7 +4945,7 @@
         <v>92</v>
       </c>
       <c r="C8" t="s">
-        <v>297</v>
+        <v>336</v>
       </c>
       <c r="D8" t="s">
         <v>298</v>
@@ -5036,7 +5036,7 @@
         <v>308</v>
       </c>
       <c r="E13" t="s">
-        <v>309</v>
+        <v>331</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -5084,7 +5084,7 @@
         <v>312</v>
       </c>
       <c r="D16" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="E16" t="s">
         <v>314</v>
@@ -5152,10 +5152,10 @@
         <v>317</v>
       </c>
       <c r="D20" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="E20" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -5285,10 +5285,10 @@
         <v>12</v>
       </c>
       <c r="C28" t="s">
-        <v>327</v>
+        <v>336</v>
       </c>
       <c r="D28" t="s">
-        <v>298</v>
+        <v>284</v>
       </c>
       <c r="E28" t="s">
         <v>298</v>
@@ -5546,7 +5546,7 @@
         <v>296</v>
       </c>
       <c r="E43" t="s">
-        <v>295</v>
+        <v>338</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
@@ -5648,7 +5648,7 @@
         <v>313</v>
       </c>
       <c r="E49" t="s">
-        <v>333</v>
+        <v>287</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
@@ -6407,7 +6407,7 @@
         <v>80</v>
       </c>
       <c r="C94" t="s">
-        <v>310</v>
+        <v>286</v>
       </c>
       <c r="D94" t="s">
         <v>287</v>
@@ -6441,7 +6441,7 @@
         <v>47</v>
       </c>
       <c r="C96" t="s">
-        <v>297</v>
+        <v>336</v>
       </c>
       <c r="D96" t="s">
         <v>299</v>
@@ -6461,7 +6461,7 @@
         <v>335</v>
       </c>
       <c r="D97" t="s">
-        <v>313</v>
+        <v>287</v>
       </c>
       <c r="E97" t="s">
         <v>287</v>
@@ -6699,7 +6699,7 @@
         <v>286</v>
       </c>
       <c r="D111" t="s">
-        <v>303</v>
+        <v>287</v>
       </c>
       <c r="E111" t="s">
         <v>285</v>
@@ -6784,7 +6784,7 @@
         <v>315</v>
       </c>
       <c r="D116" t="s">
-        <v>329</v>
+        <v>338</v>
       </c>
       <c r="E116" t="s">
         <v>322</v>
@@ -7002,7 +7002,7 @@
         <v>0</v>
       </c>
       <c r="C129" t="s">
-        <v>311</v>
+        <v>283</v>
       </c>
       <c r="D129" t="s">
         <v>342</v>
@@ -7056,7 +7056,7 @@
         <v>343</v>
       </c>
       <c r="D132" t="s">
-        <v>285</v>
+        <v>338</v>
       </c>
       <c r="E132" t="s">
         <v>329</v>
@@ -7127,7 +7127,7 @@
         <v>291</v>
       </c>
       <c r="E136" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.3">
@@ -7191,7 +7191,7 @@
   <dimension ref="A1:G139"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7294,7 +7294,7 @@
       </c>
       <c r="E4" t="str">
         <f>_xll.BDP(D4,"RTG_MDY_FC_CURR_ISSUER_RATING")</f>
-        <v>Caa3</v>
+        <v>Caa1</v>
       </c>
       <c r="F4" t="str">
         <f>_xll.BDP(D4,"RTG_SP_LT_FC_ISSUER_CREDIT")</f>
@@ -7383,7 +7383,7 @@
       </c>
       <c r="G7" t="str">
         <f>_xll.BDP(D7,"RTG_FITCH_LT_ISSUER_DEFAULT")</f>
-        <v>AA+u</v>
+        <v>AAu</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -7402,7 +7402,7 @@
       </c>
       <c r="E8" t="str">
         <f>_xll.BDP(D8,"RTG_MDY_FC_CURR_ISSUER_RATING")</f>
-        <v>Ba1</v>
+        <v>Baa3</v>
       </c>
       <c r="F8" t="str">
         <f>_xll.BDP(D8,"RTG_SP_LT_FC_ISSUER_CREDIT")</f>
@@ -7545,7 +7545,7 @@
       </c>
       <c r="G13" t="str">
         <f>_xll.BDP(D13,"RTG_FITCH_LT_ISSUER_DEFAULT")</f>
-        <v>AA-u</v>
+        <v>A+u</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -7622,7 +7622,7 @@
       </c>
       <c r="F16" t="str">
         <f>_xll.BDP(D16,"RTG_SP_LT_FC_ISSUER_CREDIT")</f>
-        <v>CCC+</v>
+        <v>CCC-</v>
       </c>
       <c r="G16" t="str">
         <f>_xll.BDP(D16,"RTG_FITCH_LT_ISSUER_DEFAULT")</f>
@@ -7730,11 +7730,11 @@
       </c>
       <c r="F20" t="str">
         <f>_xll.BDP(D20,"RTG_SP_LT_FC_ISSUER_CREDIT")</f>
-        <v>BBB</v>
+        <v>BBB+</v>
       </c>
       <c r="G20" t="str">
         <f>_xll.BDP(D20,"RTG_FITCH_LT_ISSUER_DEFAULT")</f>
-        <v>BBB</v>
+        <v>BBB+</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
@@ -7942,11 +7942,11 @@
       </c>
       <c r="E28" t="str">
         <f>_xll.BDP(D28,"RTG_MDY_FC_CURR_ISSUER_RATING")</f>
-        <v>Baa2</v>
+        <v>Baa3</v>
       </c>
       <c r="F28" t="str">
         <f>_xll.BDP(D28,"RTG_SP_LT_FC_ISSUER_CREDIT")</f>
-        <v>BB+</v>
+        <v>BB</v>
       </c>
       <c r="G28" t="str">
         <f>_xll.BDP(D28,"RTG_FITCH_LT_ISSUER_DEFAULT")</f>
@@ -8355,7 +8355,7 @@
       </c>
       <c r="G43" t="str">
         <f>_xll.BDP(D43,"RTG_FITCH_LT_ISSUER_DEFAULT")</f>
-        <v>AA+</v>
+        <v>AA</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
@@ -8517,7 +8517,7 @@
       </c>
       <c r="G49" t="str">
         <f>_xll.BDP(D49,"RTG_FITCH_LT_ISSUER_DEFAULT")</f>
-        <v>RD</v>
+        <v>B-</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
@@ -9724,7 +9724,7 @@
       </c>
       <c r="E94" t="str">
         <f>_xll.BDP(D94,"RTG_MDY_FC_CURR_ISSUER_RATING")</f>
-        <v>Caa1</v>
+        <v>B3</v>
       </c>
       <c r="F94" t="str">
         <f>_xll.BDP(D94,"RTG_SP_LT_FC_ISSUER_CREDIT")</f>
@@ -9778,7 +9778,7 @@
       </c>
       <c r="E96" t="str">
         <f>_xll.BDP(D96,"RTG_MDY_FC_CURR_ISSUER_RATING")</f>
-        <v>Ba1</v>
+        <v>Baa3</v>
       </c>
       <c r="F96" t="str">
         <f>_xll.BDP(D96,"RTG_SP_LT_FC_ISSUER_CREDIT")</f>
@@ -9809,7 +9809,7 @@
       </c>
       <c r="F97" t="str">
         <f>_xll.BDP(D97,"RTG_SP_LT_FC_ISSUER_CREDIT")</f>
-        <v>CCC+</v>
+        <v>B-</v>
       </c>
       <c r="G97" t="str">
         <f>_xll.BDP(D97,"RTG_FITCH_LT_ISSUER_DEFAULT")</f>
@@ -10187,7 +10187,7 @@
       </c>
       <c r="F111" t="str">
         <f>_xll.BDP(D111,"RTG_SP_LT_FC_ISSUER_CREDIT")</f>
-        <v>B</v>
+        <v>B-</v>
       </c>
       <c r="G111" t="str">
         <f>_xll.BDP(D111,"RTG_FITCH_LT_ISSUER_DEFAULT")</f>
@@ -10322,7 +10322,7 @@
       </c>
       <c r="F116" t="str">
         <f>_xll.BDP(D116,"RTG_SP_LT_FC_ISSUER_CREDIT")</f>
-        <v>AA-</v>
+        <v>AA</v>
       </c>
       <c r="G116" t="str">
         <f>_xll.BDP(D116,"RTG_FITCH_LT_ISSUER_DEFAULT")</f>
@@ -10669,7 +10669,7 @@
       </c>
       <c r="E129" t="str">
         <f>_xll.BDP(D129,"RTG_MDY_FC_CURR_ISSUER_RATING")</f>
-        <v>B1</v>
+        <v>Ba3</v>
       </c>
       <c r="F129" t="str">
         <f>_xll.BDP(D129,"RTG_SP_LT_FC_ISSUER_CREDIT")</f>
@@ -10754,7 +10754,7 @@
       </c>
       <c r="F132" t="str">
         <f>_xll.BDP(D132,"RTG_SP_LT_FC_ISSUER_CREDIT")</f>
-        <v>#N/A N/A</v>
+        <v>AA</v>
       </c>
       <c r="G132" t="str">
         <f>_xll.BDP(D132,"RTG_FITCH_LT_ISSUER_DEFAULT")</f>
@@ -10866,7 +10866,7 @@
       </c>
       <c r="G136" t="str">
         <f>_xll.BDP(D136,"RTG_FITCH_LT_ISSUER_DEFAULT")</f>
-        <v>BB-</v>
+        <v>BB</v>
       </c>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
updated the rating_clean file
</commit_message>
<xml_diff>
--- a/index_bbg_rating_live.xlsx
+++ b/index_bbg_rating_live.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kaimin Khaw\Desktop\credit-rating-deploy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6794F2E-F4CA-48B4-ADA7-DA75A068A61D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6112D99D-7C68-4F4A-9C57-3436FC5FEA1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-72" windowWidth="23256" windowHeight="12576" xr2:uid="{2A12413E-A5EC-426E-A187-DE07F52921C3}"/>
   </bookViews>
@@ -1195,1531 +1195,1531 @@
   <volType type="realTimeData">
     <main first="bofaddin.rtdserver">
       <tp t="s">
-        <v>#N/A Requesting Data...2107463244</v>
+        <v>#N/A Requesting Data...4186815821</v>
         <stp/>
         <stp>BDP|13719527809048657439</stp>
         <tr r="E3" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3549081715</v>
+        <v>#N/A Requesting Data...4268988418</v>
         <stp/>
         <stp>BDP|12363409739849183621</stp>
         <tr r="G98" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1704552989</v>
+        <v>#N/A Requesting Data...4243947365</v>
         <stp/>
         <stp>BDP|17606584297068117917</stp>
         <tr r="G105" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3926101436</v>
+        <v>#N/A Requesting Data...4280164983</v>
         <stp/>
         <stp>BDP|12825277506793769973</stp>
         <tr r="F22" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3707228658</v>
+        <v>#N/A Requesting Data...4223809792</v>
         <stp/>
         <stp>BDP|13615906068526188051</stp>
         <tr r="G101" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3436055014</v>
+        <v>#N/A Requesting Data...4143782239</v>
         <stp/>
         <stp>BDP|10912677687245148127</stp>
         <tr r="G106" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3187040659</v>
+        <v>#N/A Requesting Data...4167548540</v>
         <stp/>
         <stp>BDP|16221541486007837625</stp>
         <tr r="G58" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3059577451</v>
+        <v>#N/A Requesting Data...4100556200</v>
         <stp/>
         <stp>BDP|14989839765876665645</stp>
         <tr r="C81" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4193194016</v>
+        <v>#N/A Requesting Data...4093762392</v>
         <stp/>
         <stp>BDP|16792452589360294083</stp>
         <tr r="E11" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4086610365</v>
+        <v>#N/A Requesting Data...4126695427</v>
         <stp/>
         <stp>BDP|16409240184993364568</stp>
         <tr r="E54" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1695515610</v>
+        <v>#N/A Requesting Data...4132674545</v>
         <stp/>
         <stp>BDP|12376141866138693768</stp>
         <tr r="C88" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3045618734</v>
+        <v>#N/A Requesting Data...4128663810</v>
         <stp/>
         <stp>BDP|13146963289471890960</stp>
         <tr r="C18" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1876722609</v>
+        <v>#N/A Requesting Data...4105738590</v>
         <stp/>
         <stp>BDP|10167725043130019931</stp>
         <tr r="C110" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3282360204</v>
+        <v>#N/A Requesting Data...4092225112</v>
         <stp/>
         <stp>BDP|10589422899161895655</stp>
         <tr r="G76" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2394067348</v>
+        <v>#N/A Requesting Data...4117941697</v>
         <stp/>
         <stp>BDP|15228795190517586693</stp>
         <tr r="E84" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3263077674</v>
+        <v>#N/A Requesting Data...4090360014</v>
         <stp/>
         <stp>BDP|10096201946458505444</stp>
         <tr r="G97" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2251216082</v>
+        <v>#N/A Requesting Data...4199378942</v>
         <stp/>
         <stp>BDP|18253401034836307331</stp>
         <tr r="F99" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3052032331</v>
+        <v>#N/A Requesting Data...4282901328</v>
         <stp/>
         <stp>BDP|10867273920449518201</stp>
         <tr r="G71" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3260563306</v>
+        <v>#N/A Requesting Data...4267255060</v>
         <stp/>
         <stp>BDP|14811872563886412749</stp>
         <tr r="E114" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2412780261</v>
+        <v>#N/A Requesting Data...4240164967</v>
         <stp/>
         <stp>BDP|15237334583701669483</stp>
         <tr r="C112" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3046975569</v>
+        <v>#N/A Requesting Data...4177605810</v>
         <stp/>
         <stp>BDP|14006145231309322495</stp>
         <tr r="C65" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4107059514</v>
+        <v>#N/A Requesting Data...4283086687</v>
         <stp/>
         <stp>BDP|14761213634019822741</stp>
         <tr r="G2" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2548282268</v>
+        <v>#N/A Requesting Data...4095778308</v>
         <stp/>
         <stp>BDP|15399231330039360601</stp>
         <tr r="E42" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1912505342</v>
+        <v>#N/A Requesting Data...4175929565</v>
         <stp/>
         <stp>BDP|11120752607359953480</stp>
         <tr r="G61" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2701862109</v>
+        <v>#N/A Requesting Data...4266321939</v>
         <stp/>
         <stp>BDP|15939978441203902037</stp>
         <tr r="C26" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3840975086</v>
+        <v>#N/A Requesting Data...4174988873</v>
         <stp/>
         <stp>BDP|18066043829836356791</stp>
         <tr r="G78" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3138968911</v>
+        <v>#N/A Requesting Data...4231647315</v>
         <stp/>
         <stp>BDP|14168806967588813989</stp>
         <tr r="F77" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2187550272</v>
+        <v>#N/A Requesting Data...4120457048</v>
         <stp/>
         <stp>BDP|18397803367339867766</stp>
         <tr r="F101" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4045434595</v>
+        <v>#N/A Requesting Data...4263385857</v>
         <stp/>
         <stp>BDP|15895803206017416271</stp>
         <tr r="C33" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3730147769</v>
+        <v>#N/A Requesting Data...4231611571</v>
         <stp/>
         <stp>BDP|14908732543227691836</stp>
         <tr r="E94" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2876597772</v>
+        <v>#N/A Requesting Data...4275600954</v>
         <stp/>
         <stp>BDP|12957817799052931996</stp>
         <tr r="E120" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3887662702</v>
+        <v>#N/A Requesting Data...4167629372</v>
         <stp/>
         <stp>BDP|16275205432289392600</stp>
         <tr r="E101" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3381780242</v>
+        <v>#N/A Requesting Data...4133971901</v>
         <stp/>
         <stp>BDP|10407655300028223605</stp>
         <tr r="F47" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2468512648</v>
+        <v>#N/A Requesting Data...4264615264</v>
         <stp/>
         <stp>BDP|14031612538318230186</stp>
         <tr r="C136" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2570220032</v>
+        <v>#N/A Requesting Data...4114727405</v>
         <stp/>
         <stp>BDP|13840587393604095357</stp>
         <tr r="G3" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2654660084</v>
+        <v>#N/A Requesting Data...4161497926</v>
         <stp/>
         <stp>BDP|18397555740376217727</stp>
         <tr r="F17" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3096532008</v>
+        <v>#N/A Requesting Data...4283959980</v>
         <stp/>
         <stp>BDP|15886108592084595196</stp>
         <tr r="F19" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3456857460</v>
+        <v>#N/A Requesting Data...4263259790</v>
         <stp/>
         <stp>BDP|12574943311804341655</stp>
         <tr r="C58" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1841348062</v>
+        <v>#N/A Requesting Data...4191943296</v>
         <stp/>
         <stp>BDP|15276164033266227932</stp>
         <tr r="C121" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4161760260</v>
+        <v>#N/A Requesting Data...4139469606</v>
         <stp/>
         <stp>BDP|11413915902765857449</stp>
         <tr r="C135" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2584469126</v>
+        <v>#N/A Requesting Data...4160725974</v>
         <stp/>
         <stp>BDP|10888161880627674738</stp>
         <tr r="G74" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4035885829</v>
+        <v>#N/A Requesting Data...4200242404</v>
         <stp/>
         <stp>BDP|18252264749434830399</stp>
         <tr r="E91" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3620620683</v>
+        <v>#N/A Requesting Data...4229756841</v>
         <stp/>
         <stp>BDP|16230814927561165496</stp>
         <tr r="C25" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2402806884</v>
+        <v>#N/A Requesting Data...4235304024</v>
         <stp/>
         <stp>BDP|11669407615485914850</stp>
         <tr r="E28" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4061778350</v>
+        <v>#N/A Requesting Data...4290322939</v>
         <stp/>
         <stp>BDP|15385895124225473341</stp>
         <tr r="F89" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1794020027</v>
+        <v>#N/A Requesting Data...4280144738</v>
         <stp/>
         <stp>BDP|16215575297831427265</stp>
         <tr r="G19" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3838624921</v>
+        <v>#N/A Requesting Data...4217080195</v>
         <stp/>
         <stp>BDP|15664489079057139842</stp>
         <tr r="C50" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3787387429</v>
+        <v>#N/A Requesting Data...4171184031</v>
         <stp/>
         <stp>BDP|13556466380534139208</stp>
         <tr r="C63" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2574524255</v>
+        <v>#N/A Requesting Data...4160225761</v>
         <stp/>
         <stp>BDP|12426034393664290636</stp>
         <tr r="G70" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3431626488</v>
+        <v>#N/A Requesting Data...4211602934</v>
         <stp/>
         <stp>BDP|11206974657257798316</stp>
         <tr r="G5" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3934789569</v>
+        <v>#N/A Requesting Data...4206662322</v>
         <stp/>
         <stp>BDP|15687672872765725835</stp>
         <tr r="G133" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2478667729</v>
+        <v>#N/A Requesting Data...4213848887</v>
         <stp/>
         <stp>BDP|10646340980557108540</stp>
         <tr r="G83" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3781750892</v>
+        <v>#N/A Requesting Data...4146715748</v>
         <stp/>
         <stp>BDP|13932387258969800286</stp>
         <tr r="G30" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3093892690</v>
+        <v>#N/A Requesting Data...4154625596</v>
         <stp/>
         <stp>BDP|14685689793557045247</stp>
         <tr r="G11" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3429629731</v>
+        <v>#N/A Requesting Data...4140676162</v>
         <stp/>
         <stp>BDP|11792528289940283264</stp>
         <tr r="G39" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2790994861</v>
+        <v>#N/A Requesting Data...4157274015</v>
         <stp/>
         <stp>BDP|14038814629908297802</stp>
         <tr r="E14" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2457664588</v>
+        <v>#N/A Requesting Data...4253541846</v>
         <stp/>
         <stp>BDP|17960836852555549100</stp>
         <tr r="F79" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1699122393</v>
+        <v>#N/A Requesting Data...4260562914</v>
         <stp/>
         <stp>BDP|12258786923690042954</stp>
         <tr r="G82" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4049715144</v>
+        <v>#N/A Requesting Data...4279158532</v>
         <stp/>
         <stp>BDP|11831892951331348329</stp>
         <tr r="C35" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2571696498</v>
+        <v>#N/A Requesting Data...4210921419</v>
         <stp/>
         <stp>BDP|12634554786653062247</stp>
         <tr r="F34" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3352935521</v>
+        <v>#N/A Requesting Data...4260216388</v>
         <stp/>
         <stp>BDP|10304787173197381988</stp>
         <tr r="G53" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2213989752</v>
+        <v>#N/A Requesting Data...4253822457</v>
         <stp/>
         <stp>BDP|15772343051115104818</stp>
         <tr r="C127" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3130398973</v>
+        <v>#N/A Requesting Data...4290058603</v>
         <stp/>
         <stp>BDP|13619322587163510542</stp>
         <tr r="C45" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3378121996</v>
+        <v>#N/A Requesting Data...4249191393</v>
         <stp/>
         <stp>BDP|13709828003397613269</stp>
         <tr r="C54" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2927787871</v>
+        <v>#N/A Requesting Data...4268015896</v>
         <stp/>
         <stp>BDP|11596891797659679653</stp>
         <tr r="C89" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3520519748</v>
+        <v>#N/A Requesting Data...4189067619</v>
         <stp/>
         <stp>BDP|18339290641951108002</stp>
         <tr r="E17" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3709571680</v>
+        <v>#N/A Requesting Data...4221251230</v>
         <stp/>
         <stp>BDP|10418265688390464525</stp>
         <tr r="E18" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2985531109</v>
+        <v>#N/A Requesting Data...4228735028</v>
         <stp/>
         <stp>BDP|14859691791600738447</stp>
         <tr r="F45" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3016619667</v>
+        <v>#N/A Requesting Data...4260294121</v>
         <stp/>
         <stp>BDP|18255708956124343152</stp>
         <tr r="E26" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3960681229</v>
+        <v>#N/A Requesting Data...4233767123</v>
         <stp/>
         <stp>BDP|16855823919014233436</stp>
         <tr r="F30" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2978926217</v>
+        <v>#N/A Requesting Data...4287245332</v>
         <stp/>
         <stp>BDP|12821872971201299383</stp>
         <tr r="G124" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2684625690</v>
+        <v>#N/A Requesting Data...4258628376</v>
         <stp/>
         <stp>BDP|11466185903217969815</stp>
         <tr r="F33" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1805620886</v>
+        <v>#N/A Requesting Data...4262414000</v>
         <stp/>
         <stp>BDP|13711300257260836914</stp>
         <tr r="C102" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3028908612</v>
+        <v>#N/A Requesting Data...4188759529</v>
         <stp/>
         <stp>BDP|11622318103537999967</stp>
         <tr r="F15" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2295825060</v>
+        <v>#N/A Requesting Data...4230790021</v>
         <stp/>
         <stp>BDP|10597445640754361898</stp>
         <tr r="F50" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2099698893</v>
+        <v>#N/A Requesting Data...4283736893</v>
         <stp/>
         <stp>BDP|13987588094432951117</stp>
         <tr r="E127" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2741222102</v>
+        <v>#N/A Requesting Data...4214531387</v>
         <stp/>
         <stp>BDP|11655961067423868102</stp>
         <tr r="G104" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2353650311</v>
+        <v>#N/A Requesting Data...4252607344</v>
         <stp/>
         <stp>BDP|12468839190466923900</stp>
         <tr r="C20" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4121655636</v>
+        <v>#N/A Requesting Data...4174535891</v>
         <stp/>
         <stp>BDP|18411047804853597705</stp>
         <tr r="C67" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4258426274</v>
+        <v>#N/A Requesting Data...4206152461</v>
         <stp/>
         <stp>BDP|18331339124097518219</stp>
         <tr r="F66" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1916879142</v>
+        <v>#N/A Requesting Data...4227572686</v>
         <stp/>
         <stp>BDP|14983531083496973331</stp>
         <tr r="G132" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4257133322</v>
+        <v>#N/A Requesting Data...4289348765</v>
         <stp/>
         <stp>BDP|14115869171127460078</stp>
         <tr r="G37" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2622592430</v>
+        <v>#N/A Requesting Data...4281825053</v>
         <stp/>
         <stp>BDP|16963038037211063893</stp>
         <tr r="C13" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1820409092</v>
+        <v>#N/A Requesting Data...4227642507</v>
         <stp/>
         <stp>BDP|13900268704084418991</stp>
         <tr r="E37" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2396287285</v>
+        <v>#N/A Requesting Data...4284452742</v>
         <stp/>
         <stp>BDP|16311230542528118454</stp>
         <tr r="E9" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2518392880</v>
+        <v>#N/A Requesting Data...4194213491</v>
         <stp/>
         <stp>BDP|12403550728001134908</stp>
         <tr r="G38" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3049262980</v>
+        <v>#N/A Requesting Data...4245132665</v>
         <stp/>
         <stp>BDP|10528694388950747396</stp>
         <tr r="F80" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3320449687</v>
+        <v>#N/A Requesting Data...4288068475</v>
         <stp/>
         <stp>BDP|17962073596443790028</stp>
         <tr r="F23" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3127371177</v>
+        <v>#N/A Requesting Data...4291982975</v>
         <stp/>
         <stp>BDP|11322749828038387103</stp>
         <tr r="E122" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3114061877</v>
+        <v>#N/A Requesting Data...4198057644</v>
         <stp/>
         <stp>BDP|14872467854648029062</stp>
         <tr r="C75" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3522252363</v>
+        <v>#N/A Requesting Data...4283636375</v>
         <stp/>
         <stp>BDP|14951668809329151689</stp>
         <tr r="E56" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1899619137</v>
+        <v>#N/A Requesting Data...4191611531</v>
         <stp/>
         <stp>BDP|14211231849266296941</stp>
         <tr r="G103" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3963809788</v>
+        <v>#N/A Requesting Data...4218018825</v>
         <stp/>
         <stp>BDP|15282935006718574931</stp>
         <tr r="E92" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2141397876</v>
+        <v>#N/A Requesting Data...4230688101</v>
         <stp/>
         <stp>BDP|16389940868391785591</stp>
         <tr r="C120" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4191484968</v>
+        <v>#N/A Requesting Data...4287875180</v>
         <stp/>
         <stp>BDP|10830300668358540045</stp>
         <tr r="C115" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2002658634</v>
+        <v>#N/A Requesting Data...4257065146</v>
         <stp/>
         <stp>BDP|15417892931237679498</stp>
         <tr r="F8" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2567976584</v>
+        <v>#N/A Requesting Data...4291986719</v>
         <stp/>
         <stp>BDP|13776760394691002167</stp>
         <tr r="C4" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3122564252</v>
+        <v>#N/A Requesting Data...4280608638</v>
         <stp/>
         <stp>BDP|12950924085148446689</stp>
         <tr r="E121" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2270099532</v>
+        <v>#N/A Requesting Data...4232891131</v>
         <stp/>
         <stp>BDP|11202744698684518690</stp>
         <tr r="G111" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2397193877</v>
+        <v>#N/A Requesting Data...4239569910</v>
         <stp/>
         <stp>BDP|11005719894013994183</stp>
         <tr r="C3" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3064721293</v>
+        <v>#N/A Requesting Data...4267731409</v>
         <stp/>
         <stp>BDP|17061881470574956177</stp>
         <tr r="C69" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3870846949</v>
+        <v>#N/A Requesting Data...4210377259</v>
         <stp/>
         <stp>BDP|10195299258766033392</stp>
         <tr r="E90" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2836129947</v>
+        <v>#N/A Requesting Data...4282622666</v>
         <stp/>
         <stp>BDP|17559180385128709479</stp>
         <tr r="E15" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3536669092</v>
+        <v>#N/A Requesting Data...4285612727</v>
         <stp/>
         <stp>BDP|10477087317801173223</stp>
         <tr r="F125" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2963056312</v>
+        <v>#N/A Requesting Data...4252562883</v>
         <stp/>
         <stp>BDP|10431478218456128129</stp>
         <tr r="G32" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4007139048</v>
+        <v>#N/A Requesting Data...4293321154</v>
         <stp/>
         <stp>BDP|12817533695869473568</stp>
         <tr r="C82" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2841810931</v>
+        <v>#N/A Requesting Data...4273931968</v>
         <stp/>
         <stp>BDP|16722436137983528090</stp>
         <tr r="F127" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3758936344</v>
+        <v>#N/A Requesting Data...4277241441</v>
         <stp/>
         <stp>BDP|14949322880769358496</stp>
         <tr r="G16" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2827107266</v>
+        <v>#N/A Requesting Data...4266837037</v>
         <stp/>
         <stp>BDP|12620594347341901004</stp>
         <tr r="C76" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2827516565</v>
+        <v>#N/A Requesting Data...4254106608</v>
         <stp/>
         <stp>BDP|12047021516217693612</stp>
         <tr r="E126" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3342298779</v>
+        <v>#N/A Requesting Data...4285330251</v>
         <stp/>
         <stp>BDP|13612225533853005354</stp>
         <tr r="F102" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3525207976</v>
+        <v>#N/A Requesting Data...4242653861</v>
         <stp/>
         <stp>BDP|11536436753390219250</stp>
         <tr r="F129" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2359827064</v>
+        <v>#N/A Requesting Data...4241415117</v>
         <stp/>
         <stp>BDP|12946334758336119017</stp>
         <tr r="E72" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3691872333</v>
+        <v>#N/A Requesting Data...4265179776</v>
         <stp/>
         <stp>BDP|17733998071078953332</stp>
         <tr r="C23" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3256770034</v>
+        <v>#N/A Requesting Data...4229267964</v>
         <stp/>
         <stp>BDP|16362559715466602618</stp>
         <tr r="F68" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3714397600</v>
+        <v>#N/A Requesting Data...4292546374</v>
         <stp/>
         <stp>BDP|16070475881909673177</stp>
         <tr r="E112" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2442809867</v>
+        <v>#N/A Requesting Data...4230682612</v>
         <stp/>
         <stp>BDP|17590878194950224438</stp>
         <tr r="G87" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2214134540</v>
+        <v>#N/A Requesting Data...4244028153</v>
         <stp/>
         <stp>BDP|12427007793358727164</stp>
         <tr r="F100" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2330641663</v>
+        <v>#N/A Requesting Data...4252699241</v>
         <stp/>
         <stp>BDP|15601293270144483737</stp>
         <tr r="G15" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2470336764</v>
+        <v>#N/A Requesting Data...4242771770</v>
         <stp/>
         <stp>BDP|13723200346810339697</stp>
         <tr r="C38" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3689427384</v>
+        <v>#N/A Requesting Data...4251226301</v>
         <stp/>
         <stp>BDP|18086118189074176643</stp>
         <tr r="E88" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3429730382</v>
+        <v>#N/A Requesting Data...4279514833</v>
         <stp/>
         <stp>BDP|15679917748483251829</stp>
         <tr r="E6" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3237232448</v>
+        <v>#N/A Requesting Data...4249389263</v>
         <stp/>
         <stp>BDP|13421293548936861023</stp>
         <tr r="G66" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1766023786</v>
+        <v>#N/A Requesting Data...4281081689</v>
         <stp/>
         <stp>BDP|10594946509929542325</stp>
         <tr r="F5" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2792093783</v>
+        <v>#N/A Requesting Data...4239411313</v>
         <stp/>
         <stp>BDP|10668212108445960480</stp>
         <tr r="G57" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2102428027</v>
+        <v>#N/A Requesting Data...4289135259</v>
         <stp/>
         <stp>BDP|10103273213286136651</stp>
         <tr r="C6" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2512298070</v>
+        <v>#N/A Requesting Data...4278066437</v>
         <stp/>
         <stp>BDP|11259721862376480554</stp>
         <tr r="G69" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3288732964</v>
+        <v>#N/A Requesting Data...4287779863</v>
         <stp/>
         <stp>BDP|14885566279524266176</stp>
         <tr r="E30" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2636475556</v>
+        <v>#N/A Requesting Data...4274225231</v>
         <stp/>
         <stp>BDP|14519079130534129014</stp>
         <tr r="C49" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3274994652</v>
+        <v>#N/A Requesting Data...4266515570</v>
         <stp/>
         <stp>BDP|14873136635550817546</stp>
         <tr r="G130" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2727591020</v>
+        <v>#N/A Requesting Data...4276880164</v>
         <stp/>
         <stp>BDP|16641457892301341972</stp>
         <tr r="F130" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4157147014</v>
+        <v>#N/A Requesting Data...4261252057</v>
         <stp/>
         <stp>BDP|13231746637163726724</stp>
         <tr r="E7" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2123908363</v>
+        <v>#N/A Requesting Data...4291173173</v>
         <stp/>
         <stp>BDP|12945735048800380256</stp>
         <tr r="G118" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3067610560</v>
+        <v>#N/A Requesting Data...4281317453</v>
         <stp/>
         <stp>BDP|11265248170961260631</stp>
         <tr r="E47" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1846204089</v>
+        <v>#N/A Requesting Data...4282453967</v>
         <stp/>
         <stp>BDP|16351851074029385080</stp>
         <tr r="G35" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2020461398</v>
+        <v>#N/A Requesting Data...4287849703</v>
         <stp/>
         <stp>BDP|11944358991052271970</stp>
         <tr r="C103" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2952595607</v>
+        <v>#N/A Requesting Data...4282311813</v>
         <stp/>
         <stp>BDP|18410981990650283866</stp>
         <tr r="C99" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3728575440</v>
+        <v>#N/A Requesting Data...4291527582</v>
         <stp/>
         <stp>BDP|14383773052580838655</stp>
         <tr r="F104" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1991024163</v>
+        <v>#N/A Requesting Data...4289061743</v>
         <stp/>
         <stp>BDP|10871340643964419300</stp>
         <tr r="F95" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2791826194</v>
+        <v>#N/A Requesting Data...4265093936</v>
         <stp/>
         <stp>BDP|14690280185656044816</stp>
         <tr r="C94" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2136531433</v>
+        <v>#N/A Requesting Data...4259904339</v>
         <stp/>
         <stp>BDP|18305693996456795112</stp>
         <tr r="G80" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2087103560</v>
+        <v>#N/A Requesting Data...4285144643</v>
         <stp/>
         <stp>BDP|16273225567973824127</stp>
         <tr r="C79" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2154044579</v>
+        <v>#N/A Requesting Data...4270554692</v>
         <stp/>
         <stp>BDP|13313129291618997350</stp>
         <tr r="C43" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3628036387</v>
+        <v>#N/A Requesting Data...4260968213</v>
         <stp/>
         <stp>BDP|15444947284180871401</stp>
         <tr r="G27" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2607754331</v>
+        <v>#N/A Requesting Data...4272985842</v>
         <stp/>
         <stp>BDP|12935317504846234704</stp>
         <tr r="F98" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2002014035</v>
+        <v>#N/A Requesting Data...4270640679</v>
         <stp/>
         <stp>BDP|13057895365605005829</stp>
         <tr r="C138" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3597451478</v>
+        <v>#N/A Requesting Data...4266849129</v>
         <stp/>
         <stp>BDP|16160321537943284588</stp>
         <tr r="E76" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4218611401</v>
+        <v>#N/A Requesting Data...4291647812</v>
         <stp/>
         <stp>BDP|10621599828921836610</stp>
         <tr r="C12" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2137724854</v>
+        <v>#N/A Requesting Data...4291839285</v>
         <stp/>
         <stp>BDP|14881076967673386157</stp>
         <tr r="F122" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3522408201</v>
+        <v>#N/A Requesting Data...4294686261</v>
         <stp/>
         <stp>BDP|17321553610055816607</stp>
         <tr r="F96" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2010033713</v>
+        <v>#N/A Requesting Data...4290488806</v>
         <stp/>
         <stp>BDP|12793555755147383546</stp>
         <tr r="F42" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3126693748</v>
+        <v>#N/A Requesting Data...4282530121</v>
         <stp/>
         <stp>BDP|10194327202093986081</stp>
         <tr r="F132" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2039488357</v>
+        <v>#N/A Requesting Data...4282773353</v>
         <stp/>
         <stp>BDP|12798194599768683232</stp>
         <tr r="C42" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3051948007</v>
+        <v>#N/A Requesting Data...4283285023</v>
         <stp/>
         <stp>BDP|15675203172551734114</stp>
         <tr r="F12" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2981865443</v>
+        <v>#N/A Requesting Data...4273946918</v>
         <stp/>
         <stp>BDP|17779010845097021465</stp>
         <tr r="G23" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3066988398</v>
+        <v>#N/A Requesting Data...4276266439</v>
         <stp/>
         <stp>BDP|14698661432127374654</stp>
         <tr r="E53" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4046279979</v>
+        <v>#N/A Requesting Data...4285022780</v>
         <stp/>
         <stp>BDP|16055018629402477686</stp>
         <tr r="F18" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4088580490</v>
+        <v>#N/A Requesting Data...4284137679</v>
         <stp/>
         <stp>BDP|14191015466523343124</stp>
         <tr r="G42" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3056460847</v>
+        <v>#N/A Requesting Data...4293276582</v>
         <stp/>
         <stp>BDP|16690545673604064064</stp>
         <tr r="G6" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3553622724</v>
+        <v>#N/A Requesting Data...4293162983</v>
         <stp/>
         <stp>BDP|11057556593645206836</stp>
         <tr r="E116" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3017558203</v>
+        <v>#N/A Requesting Data...4285834221</v>
         <stp/>
         <stp>BDP|14753168038796700174</stp>
         <tr r="E131" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3188231060</v>
+        <v>#N/A Requesting Data...4294804932</v>
         <stp/>
         <stp>BDP|18400936140157917378</stp>
         <tr r="G108" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1901708028</v>
+        <v>#N/A Requesting Data...4289282233</v>
         <stp/>
         <stp>BDP|11308062409311166143</stp>
         <tr r="F138" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3845916802</v>
+        <v>#N/A Requesting Data...4284982241</v>
         <stp/>
         <stp>BDP|14929251921187622207</stp>
         <tr r="G120" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3271638382</v>
+        <v>#N/A Requesting Data...4289789905</v>
         <stp/>
         <stp>BDP|13312546151322475095</stp>
         <tr r="C117" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2474041548</v>
+        <v>#N/A Requesting Data...4292337871</v>
         <stp/>
         <stp>BDP|10370784365528062849</stp>
         <tr r="G51" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3765195563</v>
+        <v>#N/A Requesting Data...4289148660</v>
         <stp/>
         <stp>BDP|17808503947101138629</stp>
         <tr r="F128" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2607258046</v>
+        <v>#N/A Requesting Data...4292380157</v>
         <stp/>
         <stp>BDP|17640270888515662931</stp>
         <tr r="E20" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2926985400</v>
+        <v>#N/A Requesting Data...4292174698</v>
         <stp/>
         <stp>BDP|17853766030844520642</stp>
         <tr r="F65" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4022191346</v>
+        <v>#N/A Requesting Data...4293134536</v>
         <stp/>
         <stp>BDP|17345319339237647129</stp>
         <tr r="C10" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4028760138</v>
+        <v>#N/A Requesting Data...4294597731</v>
         <stp/>
         <stp>BDP|18428163184190295050</stp>
         <tr r="C48" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3824878520</v>
+        <v>#N/A Requesting Data...2353952441</v>
         <stp/>
         <stp>BDP|11469771160883398201</stp>
         <tr r="G20" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2066172754</v>
+        <v>#N/A Requesting Data...3950173086</v>
         <stp/>
         <stp>BDP|12945229628891094206</stp>
         <tr r="F36" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2508615031</v>
+        <v>#N/A Requesting Data...1677834400</v>
         <stp/>
         <stp>BDP|13088969316699575369</stp>
         <tr r="G17" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4030649407</v>
+        <v>#N/A Requesting Data...4071833981</v>
         <stp/>
         <stp>BDP|14386928546318260068</stp>
         <tr r="C78" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2915223369</v>
+        <v>#N/A Requesting Data...3545132757</v>
         <stp/>
         <stp>BDP|16250000632946565269</stp>
         <tr r="F32" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4032184592</v>
+        <v>#N/A Requesting Data...680543529</v>
         <stp/>
         <stp>BDP|10062445544650347114</stp>
         <tr r="E69" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1992127646</v>
+        <v>#N/A Requesting Data...3677706456</v>
         <stp/>
         <stp>BDP|18056984346180923430</stp>
         <tr r="F67" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3799346613</v>
+        <v>#N/A Requesting Data...4294157107</v>
         <stp/>
         <stp>BDP|13607419850307697457</stp>
         <tr r="G55" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3039985972</v>
+        <v>#N/A Requesting Data...42965078</v>
         <stp/>
         <stp>BDP|17151526894293450943</stp>
         <tr r="E34" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2330003170</v>
+        <v>#N/A Requesting Data...2783010836</v>
         <stp/>
         <stp>BDP|14769233272840536059</stp>
         <tr r="F48" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2331065356</v>
+        <v>#N/A Requesting Data...3559780967</v>
         <stp/>
         <stp>BDP|16347078018142331376</stp>
         <tr r="E59" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2648822168</v>
+        <v>#N/A Requesting Data...168259912</v>
         <stp/>
         <stp>BDP|12157937398585487157</stp>
         <tr r="F69" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2572545798</v>
+        <v>#N/A Requesting Data...2805025393</v>
         <stp/>
         <stp>BDP|10450024654077121490</stp>
         <tr r="G29" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4227542227</v>
+        <v>#N/A Requesting Data...3618336482</v>
         <stp/>
         <stp>BDP|12405274734177384298</stp>
         <tr r="G109" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2318489569</v>
+        <v>#N/A Requesting Data...529593156</v>
         <stp/>
         <stp>BDP|11693290023110245727</stp>
         <tr r="F93" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2090158987</v>
+        <v>#N/A Requesting Data...1243419621</v>
         <stp/>
         <stp>BDP|16857915317939051104</stp>
         <tr r="E4" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3212152103</v>
+        <v>#N/A Requesting Data...285362000</v>
         <stp/>
         <stp>BDP|13092630751014311204</stp>
         <tr r="C29" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2359436855</v>
+        <v>#N/A Requesting Data...1677747148</v>
         <stp/>
         <stp>BDP|16560165422091315234</stp>
         <tr r="E74" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3652457446</v>
+        <v>#N/A Requesting Data...2897134251</v>
         <stp/>
         <stp>BDP|15578620992514708823</stp>
         <tr r="C74" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2567574091</v>
+        <v>#N/A Requesting Data...2726778989</v>
         <stp/>
         <stp>BDP|16311826266949112751</stp>
         <tr r="E137" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3328419111</v>
+        <v>#N/A Requesting Data...2414825236</v>
         <stp/>
         <stp>BDP|12423551309476829732</stp>
         <tr r="E29" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1910169275</v>
+        <v>#N/A Requesting Data...3595046903</v>
         <stp/>
         <stp>BDP|15334425393507822980</stp>
         <tr r="C71" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3859151741</v>
+        <v>#N/A Requesting Data...3211529712</v>
         <stp/>
         <stp>BDP|14187404668490888034</stp>
         <tr r="E115" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3125032431</v>
+        <v>#N/A Requesting Data...2302453812</v>
         <stp/>
         <stp>BDP|14038301256494491076</stp>
         <tr r="E12" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2831171146</v>
+        <v>#N/A Requesting Data...1941624254</v>
         <stp/>
         <stp>BDP|12212063840830333025</stp>
         <tr r="E132" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2370327747</v>
+        <v>#N/A Requesting Data...3437104623</v>
         <stp/>
         <stp>BDP|12411228970299104833</stp>
         <tr r="E40" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2291590046</v>
+        <v>#N/A Requesting Data...484421689</v>
         <stp/>
         <stp>BDP|11324255971734653659</stp>
         <tr r="G93" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1883142615</v>
+        <v>#N/A Requesting Data...2583473614</v>
         <stp/>
         <stp>BDP|15080702944965265524</stp>
         <tr r="E5" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3168780129</v>
+        <v>#N/A Requesting Data...301280822</v>
         <stp/>
         <stp>BDP|12709330545317601409</stp>
         <tr r="F78" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4026471511</v>
+        <v>#N/A Requesting Data...2251474870</v>
         <stp/>
         <stp>BDP|17558583635766924170</stp>
         <tr r="C139" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4032279872</v>
+        <v>#N/A Requesting Data...3623923230</v>
         <stp/>
         <stp>BDP|14043797868641345244</stp>
         <tr r="G127" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3118295428</v>
+        <v>#N/A Requesting Data...2336453956</v>
         <stp/>
         <stp>BDP|11097146762171726091</stp>
         <tr r="C125" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2388992677</v>
+        <v>#N/A Requesting Data...652282090</v>
         <stp/>
         <stp>BDP|10083242995488903402</stp>
         <tr r="E22" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2922383670</v>
+        <v>#N/A Requesting Data...4220511926</v>
         <stp/>
         <stp>BDP|14104003677163905777</stp>
         <tr r="G89" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2490012625</v>
+        <v>#N/A Requesting Data...2692626695</v>
         <stp/>
         <stp>BDP|10493155251505330684</stp>
         <tr r="F113" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3990441893</v>
+        <v>#N/A Requesting Data...3269357357</v>
         <stp/>
         <stp>BDP|17307159600861837050</stp>
         <tr r="C28" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4077984355</v>
+        <v>#N/A Requesting Data...495919606</v>
         <stp/>
         <stp>BDP|11974207352247436657</stp>
         <tr r="G84" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3516369965</v>
+        <v>#N/A Requesting Data...451313750</v>
         <stp/>
         <stp>BDP|12417029733397010193</stp>
         <tr r="G129" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3126477480</v>
+        <v>#N/A Requesting Data...1310986358</v>
         <stp/>
         <stp>BDP|13696428749777505366</stp>
         <tr r="C128" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3375509817</v>
+        <v>#N/A Requesting Data...1521389203</v>
         <stp/>
         <stp>BDP|10265435339313984301</stp>
         <tr r="F136" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2179651596</v>
+        <v>#N/A Requesting Data...2841938616</v>
         <stp/>
         <stp>BDP|16742662035804692035</stp>
         <tr r="E24" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3352527793</v>
+        <v>#N/A Requesting Data...1212405923</v>
         <stp/>
         <stp>BDP|13311072247345018521</stp>
         <tr r="E129" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4086450799</v>
+        <v>#N/A Requesting Data...982649746</v>
         <stp/>
         <stp>BDP|14635385909938704819</stp>
         <tr r="E106" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2445902867</v>
+        <v>#N/A Requesting Data...2142712063</v>
         <stp/>
         <stp>BDP|17965266240553639582</stp>
         <tr r="E10" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2311068372</v>
+        <v>#N/A Requesting Data...3300062522</v>
         <stp/>
         <stp>BDP|14559650107303581628</stp>
         <tr r="C72" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2774933425</v>
+        <v>#N/A Requesting Data...3365535594</v>
         <stp/>
         <stp>BDP|12078771150016496119</stp>
         <tr r="G102" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4236260447</v>
+        <v>#N/A Requesting Data...3607947763</v>
         <stp/>
         <stp>BDP|13437131854538783812</stp>
         <tr r="G22" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3652737200</v>
+        <v>#N/A Requesting Data...2592367265</v>
         <stp/>
         <stp>BDP|11816803688615161347</stp>
         <tr r="E51" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3260295154</v>
+        <v>#N/A Requesting Data...171447647</v>
         <stp/>
         <stp>BDP|11136233214231371414</stp>
         <tr r="G139" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2076498160</v>
+        <v>#N/A Requesting Data...4175413419</v>
         <stp/>
         <stp>BDP|16387121100332435221</stp>
         <tr r="G96" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3213934796</v>
+        <v>#N/A Requesting Data...4079682147</v>
         <stp/>
         <stp>BDP|10044993787394494110</stp>
         <tr r="C113" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2738653140</v>
+        <v>#N/A Requesting Data...3887850995</v>
         <stp/>
         <stp>BDP|16851432539276999316</stp>
         <tr r="E44" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2222974798</v>
+        <v>#N/A Requesting Data...2091981827</v>
         <stp/>
         <stp>BDP|17514330731974993734</stp>
         <tr r="E65" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3920061705</v>
+        <v>#N/A Requesting Data...846771515</v>
         <stp/>
         <stp>BDP|13397290692205579908</stp>
         <tr r="G128" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3018822492</v>
+        <v>#N/A Requesting Data...135259311</v>
         <stp/>
         <stp>BDP|11770519860203890508</stp>
         <tr r="F106" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3029989202</v>
+        <v>#N/A Requesting Data...2064089653</v>
         <stp/>
         <stp>BDP|11828615722360397168</stp>
         <tr r="E71" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2586887597</v>
+        <v>#N/A Requesting Data...3619154602</v>
         <stp/>
         <stp>BDP|12429929188915695292</stp>
         <tr r="F109" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2434345315</v>
+        <v>#N/A Requesting Data...4202681170</v>
         <stp/>
         <stp>BDP|14807781952773549162</stp>
         <tr r="G33" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3164104569</v>
+        <v>#N/A Requesting Data...2477742805</v>
         <stp/>
         <stp>BDP|14141528956866623622</stp>
         <tr r="C134" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4170154153</v>
+        <v>#N/A Requesting Data...629596663</v>
         <stp/>
         <stp>BDP|11925450918217650729</stp>
         <tr r="F86" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4190209182</v>
+        <v>#N/A Requesting Data...1087818421</v>
         <stp/>
         <stp>BDP|10075353521710450506</stp>
         <tr r="C109" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2729565454</v>
+        <v>#N/A Requesting Data...3113267647</v>
         <stp/>
         <stp>BDP|14507687284196916837</stp>
         <tr r="F6" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2266924642</v>
+        <v>#N/A Requesting Data...2542296570</v>
         <stp/>
         <stp>BDP|17592946715913980887</stp>
         <tr r="F7" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2579174730</v>
+        <v>#N/A Requesting Data...1636355663</v>
         <stp/>
         <stp>BDP|12670343566891576248</stp>
         <tr r="G36" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2438522980</v>
+        <v>#N/A Requesting Data...3647490644</v>
         <stp/>
         <stp>BDP|16059776447550017157</stp>
         <tr r="F63" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3446459888</v>
+        <v>#N/A Requesting Data...3686594476</v>
         <stp/>
         <stp>BDP|13709786759646324310</stp>
         <tr r="F46" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3839558467</v>
+        <v>#N/A Requesting Data...1471960267</v>
         <stp/>
         <stp>BDP|17680007951225535344</stp>
         <tr r="C93" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3924149240</v>
+        <v>#N/A Requesting Data...3569834447</v>
         <stp/>
         <stp>BDP|14249466628496635139</stp>
         <tr r="F26" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2663866701</v>
+        <v>#N/A Requesting Data...3215832181</v>
         <stp/>
         <stp>BDP|12616286245214000526</stp>
         <tr r="C114" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3030689360</v>
+        <v>#N/A Requesting Data...3746883806</v>
         <stp/>
         <stp>BDP|13229487552560837780</stp>
         <tr r="E139" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4128910748</v>
+        <v>#N/A Requesting Data...977436660</v>
         <stp/>
         <stp>BDP|18412208651713792994</stp>
         <tr r="F118" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2470102806</v>
+        <v>#N/A Requesting Data...1450446113</v>
         <stp/>
         <stp>BDP|16919456577607807790</stp>
         <tr r="G56" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3301071999</v>
+        <v>#N/A Requesting Data...3510691599</v>
         <stp/>
         <stp>BDP|14958917677776306912</stp>
         <tr r="E124" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3882393875</v>
+        <v>#N/A Requesting Data...1203042260</v>
         <stp/>
         <stp>BDP|16906362551851442479</stp>
         <tr r="F14" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3724630282</v>
+        <v>#N/A Requesting Data...925040863</v>
         <stp/>
         <stp>BDP|13303498173634341154</stp>
         <tr r="G72" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3895282739</v>
+        <v>#N/A Requesting Data...746052207</v>
         <stp/>
         <stp>BDP|11394026073756494578</stp>
         <tr r="F4" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3173342436</v>
+        <v>#N/A Requesting Data...3272882135</v>
         <stp/>
         <stp>BDP|12821707660430898618</stp>
         <tr r="C40" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2919589553</v>
+        <v>#N/A Requesting Data...4023475247</v>
         <stp/>
         <stp>BDP|12207042919767891145</stp>
         <tr r="G131" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2050600085</v>
+        <v>#N/A Requesting Data...3580095228</v>
         <stp/>
         <stp>BDP|17617562141366516571</stp>
         <tr r="F24" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3466017294</v>
+        <v>#N/A Requesting Data...3834960161</v>
         <stp/>
         <stp>BDP|13776066979946925741</stp>
         <tr r="C90" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4118660159</v>
+        <v>#N/A Requesting Data...144086488</v>
         <stp/>
         <stp>BDP|15429465971742273156</stp>
         <tr r="E67" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3023920867</v>
+        <v>#N/A Requesting Data...1756754924</v>
         <stp/>
         <stp>BDP|13319017160191784122</stp>
         <tr r="E43" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3743096158</v>
+        <v>#N/A Requesting Data...2512273129</v>
         <stp/>
         <stp>BDP|17197570677470339052</stp>
         <tr r="E33" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3031876908</v>
+        <v>#N/A Requesting Data...350741535</v>
         <stp/>
         <stp>BDP|18198100188843948773</stp>
         <tr r="G60" s="1"/>
@@ -2727,1783 +2727,1783 @@
     </main>
     <main first="bofaddin.rtdserver">
       <tp t="s">
-        <v>#N/A Requesting Data...3869373421</v>
+        <v>#N/A Requesting Data...907991018</v>
         <stp/>
         <stp>BDP|3930904544763426134</stp>
         <tr r="C55" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2143862368</v>
+        <v>#N/A Requesting Data...202089569</v>
         <stp/>
         <stp>BDP|7103625188072362707</stp>
         <tr r="E98" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3047763129</v>
+        <v>#N/A Requesting Data...3253845189</v>
         <stp/>
         <stp>BDP|9365312653090978315</stp>
         <tr r="G136" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2219011589</v>
+        <v>#N/A Requesting Data...3761034595</v>
         <stp/>
         <stp>BDP|6412151529379694002</stp>
         <tr r="F110" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3492126999</v>
+        <v>#N/A Requesting Data...3591391663</v>
         <stp/>
         <stp>BDP|6245426297947871034</stp>
         <tr r="C80" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2286486250</v>
+        <v>#N/A Requesting Data...2104554100</v>
         <stp/>
         <stp>BDP|2350385774053258906</stp>
         <tr r="F72" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2202633563</v>
+        <v>#N/A Requesting Data...2271845947</v>
         <stp/>
         <stp>BDP|8530657130876609747</stp>
         <tr r="C44" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2638802090</v>
+        <v>#N/A Requesting Data...3298541794</v>
         <stp/>
         <stp>BDP|7198979431090342164</stp>
         <tr r="E50" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3205912142</v>
+        <v>#N/A Requesting Data...337107109</v>
         <stp/>
         <stp>BDP|9075300299347332881</stp>
         <tr r="G79" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2086224537</v>
+        <v>#N/A Requesting Data...255156545</v>
         <stp/>
         <stp>BDP|5029740995104753357</stp>
         <tr r="C111" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3133607326</v>
+        <v>#N/A Requesting Data...3222601932</v>
         <stp/>
         <stp>BDP|8128743572863334748</stp>
         <tr r="C47" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3368586597</v>
+        <v>#N/A Requesting Data...2575056393</v>
         <stp/>
         <stp>BDP|6339719327836450907</stp>
         <tr r="C98" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3072841009</v>
+        <v>#N/A Requesting Data...457955473</v>
         <stp/>
         <stp>BDP|4200580269163222863</stp>
         <tr r="E25" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2142085137</v>
+        <v>#N/A Requesting Data...3690638518</v>
         <stp/>
         <stp>BDP|5989352249668473659</stp>
         <tr r="G50" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4230442633</v>
+        <v>#N/A Requesting Data...3248072706</v>
         <stp/>
         <stp>BDP|2484433252649720677</stp>
         <tr r="G68" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2810433887</v>
+        <v>#N/A Requesting Data...643027206</v>
         <stp/>
         <stp>BDP|6249870436562567333</stp>
         <tr r="E49" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2053690751</v>
+        <v>#N/A Requesting Data...3999009772</v>
         <stp/>
         <stp>BDP|9572192910556051262</stp>
         <tr r="E134" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2420532872</v>
+        <v>#N/A Requesting Data...2592893844</v>
         <stp/>
         <stp>BDP|7540551159163224910</stp>
         <tr r="F51" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3613294768</v>
+        <v>#N/A Requesting Data...3421647282</v>
         <stp/>
         <stp>BDP|8451204331587951367</stp>
         <tr r="F52" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3485310052</v>
+        <v>#N/A Requesting Data...1004072364</v>
         <stp/>
         <stp>BDP|3109256470563958869</stp>
         <tr r="C52" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4139427721</v>
+        <v>#N/A Requesting Data...3870651525</v>
         <stp/>
         <stp>BDP|3590543194827878545</stp>
         <tr r="F59" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3583502792</v>
+        <v>#N/A Requesting Data...1487125515</v>
         <stp/>
         <stp>BDP|3009997314886390075</stp>
         <tr r="G100" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3504997310</v>
+        <v>#N/A Requesting Data...493989363</v>
         <stp/>
         <stp>BDP|4777106988391072114</stp>
         <tr r="F103" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2908732125</v>
+        <v>#N/A Requesting Data...3406688626</v>
         <stp/>
         <stp>BDP|4303401897634933024</stp>
         <tr r="E93" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2006511920</v>
+        <v>#N/A Requesting Data...2062715648</v>
         <stp/>
         <stp>BDP|9055938583773500695</stp>
         <tr r="C34" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2949123990</v>
+        <v>#N/A Requesting Data...3135568650</v>
         <stp/>
         <stp>BDP|1573317174439842142</stp>
         <tr r="E133" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4069954158</v>
+        <v>#N/A Requesting Data...3403273206</v>
         <stp/>
         <stp>BDP|7180318607099335068</stp>
         <tr r="C9" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3207539661</v>
+        <v>#N/A Requesting Data...1251075997</v>
         <stp/>
         <stp>BDP|8371873502449565411</stp>
         <tr r="C62" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2662576980</v>
+        <v>#N/A Requesting Data...3010086441</v>
         <stp/>
         <stp>BDP|9300723062997279226</stp>
         <tr r="C124" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2338660409</v>
+        <v>#N/A Requesting Data...3820974280</v>
         <stp/>
         <stp>BDP|5492561896244379063</stp>
         <tr r="F70" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3174750513</v>
+        <v>#N/A Requesting Data...3478067057</v>
         <stp/>
         <stp>BDP|8460669760190400504</stp>
         <tr r="C27" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4259083997</v>
+        <v>#N/A Requesting Data...2860419453</v>
         <stp/>
         <stp>BDP|7634975275120208406</stp>
         <tr r="C31" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2504075111</v>
+        <v>#N/A Requesting Data...218662518</v>
         <stp/>
         <stp>BDP|4040591290066838371</stp>
         <tr r="E13" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2916609190</v>
+        <v>#N/A Requesting Data...2793204680</v>
         <stp/>
         <stp>BDP|9247766641156585153</stp>
         <tr r="G94" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2222695875</v>
+        <v>#N/A Requesting Data...529765156</v>
         <stp/>
         <stp>BDP|7940113982976758589</stp>
         <tr r="E95" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2078566008</v>
+        <v>#N/A Requesting Data...1522519790</v>
         <stp/>
         <stp>BDP|9093620553903200797</stp>
         <tr r="C105" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3218946090</v>
+        <v>#N/A Requesting Data...1560585607</v>
         <stp/>
         <stp>BDP|2405932012622401695</stp>
         <tr r="G77" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3648052563</v>
+        <v>#N/A Requesting Data...559493945</v>
         <stp/>
         <stp>BDP|9175353808212225665</stp>
         <tr r="C66" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3621056837</v>
+        <v>#N/A Requesting Data...2008024708</v>
         <stp/>
         <stp>BDP|1414608591110891051</stp>
         <tr r="F9" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3511415641</v>
+        <v>#N/A Requesting Data...1635546453</v>
         <stp/>
         <stp>BDP|3649732806419915339</stp>
         <tr r="G14" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2737417256</v>
+        <v>#N/A Requesting Data...3479603562</v>
         <stp/>
         <stp>BDP|7006257261095505888</stp>
         <tr r="F54" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2028911843</v>
+        <v>#N/A Requesting Data...1457416997</v>
         <stp/>
         <stp>BDP|9781989741438009272</stp>
         <tr r="C39" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2683914465</v>
+        <v>#N/A Requesting Data...2086262641</v>
         <stp/>
         <stp>BDP|7532189862547338936</stp>
         <tr r="F58" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3411815168</v>
+        <v>#N/A Requesting Data...2437390511</v>
         <stp/>
         <stp>BDP|4286027170164748985</stp>
         <tr r="G113" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4294141492</v>
+        <v>#N/A Requesting Data...2783686925</v>
         <stp/>
         <stp>BDP|4691882821088256816</stp>
         <tr r="F126" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3896566353</v>
+        <v>#N/A Requesting Data...829393331</v>
         <stp/>
         <stp>BDP|4974055815239706225</stp>
         <tr r="G110" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4272410218</v>
+        <v>#N/A Requesting Data...365314646</v>
         <stp/>
         <stp>BDP|5916130291376545539</stp>
         <tr r="F73" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2473640713</v>
+        <v>#N/A Requesting Data...2399086423</v>
         <stp/>
         <stp>BDP|9535646277681935723</stp>
         <tr r="E60" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2766627727</v>
+        <v>#N/A Requesting Data...631417868</v>
         <stp/>
         <stp>BDP|3472420329653378814</stp>
         <tr r="G4" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3608989258</v>
+        <v>#N/A Requesting Data...3391266729</v>
         <stp/>
         <stp>BDP|9676580711333862054</stp>
         <tr r="E135" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3255624492</v>
+        <v>#N/A Requesting Data...1371331657</v>
         <stp/>
         <stp>BDP|8651287802994649096</stp>
         <tr r="E77" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2663407931</v>
+        <v>#N/A Requesting Data...1902393205</v>
         <stp/>
         <stp>BDP|5552297197720045083</stp>
         <tr r="E118" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2363168165</v>
+        <v>#N/A Requesting Data...687759518</v>
         <stp/>
         <stp>BDP|6195991527552839107</stp>
         <tr r="C61" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2938497462</v>
+        <v>#N/A Requesting Data...4247889737</v>
         <stp/>
         <stp>BDP|2785537291931900199</stp>
         <tr r="G91" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2778827096</v>
+        <v>#N/A Requesting Data...3350601235</v>
         <stp/>
         <stp>BDP|9875435960971965593</stp>
         <tr r="C11" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2810441358</v>
+        <v>#N/A Requesting Data...3827501411</v>
         <stp/>
         <stp>BDP|7662972721973338089</stp>
         <tr r="F107" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4162531382</v>
+        <v>#N/A Requesting Data...2878355253</v>
         <stp/>
         <stp>BDP|4282903616430488389</stp>
         <tr r="G9" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3196736194</v>
+        <v>#N/A Requesting Data...1151730805</v>
         <stp/>
         <stp>BDP|6606398548307737925</stp>
         <tr r="C70" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2107138330</v>
+        <v>#N/A Requesting Data...1009058452</v>
         <stp/>
         <stp>BDP|2310021551041423963</stp>
         <tr r="F123" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2146976177</v>
+        <v>#N/A Requesting Data...2088411473</v>
         <stp/>
         <stp>BDP|1666950877162018261</stp>
         <tr r="E87" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2995675651</v>
+        <v>#N/A Requesting Data...1555524418</v>
         <stp/>
         <stp>BDP|6280569068792932854</stp>
         <tr r="C46" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3948819079</v>
+        <v>#N/A Requesting Data...4273983450</v>
         <stp/>
         <stp>BDP|9635152443296662577</stp>
         <tr r="C16" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3656997189</v>
+        <v>#N/A Requesting Data...2846466107</v>
         <stp/>
         <stp>BDP|5935740968278021330</stp>
         <tr r="C96" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2193426113</v>
+        <v>#N/A Requesting Data...3468548188</v>
         <stp/>
         <stp>BDP|8225387168083679130</stp>
         <tr r="E57" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3085482530</v>
+        <v>#N/A Requesting Data...4027656051</v>
         <stp/>
         <stp>BDP|8741792397660502982</stp>
         <tr r="G24" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2947003561</v>
+        <v>#N/A Requesting Data...3762361686</v>
         <stp/>
         <stp>BDP|1988621838892198978</stp>
         <tr r="F82" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3315282929</v>
+        <v>#N/A Requesting Data...1575918792</v>
         <stp/>
         <stp>BDP|5160947801244572083</stp>
         <tr r="C97" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3686072653</v>
+        <v>#N/A Requesting Data...422026595</v>
         <stp/>
         <stp>BDP|8781684350665372626</stp>
         <tr r="G64" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3153496665</v>
+        <v>#N/A Requesting Data...4209746769</v>
         <stp/>
         <stp>BDP|8866465832365619258</stp>
         <tr r="F120" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3744022608</v>
+        <v>#N/A Requesting Data...924949363</v>
         <stp/>
         <stp>BDP|1231973558974048121</stp>
         <tr r="E123" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2500783707</v>
+        <v>#N/A Requesting Data...551549430</v>
         <stp/>
         <stp>BDP|9011959145835954962</stp>
         <tr r="E102" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3678147654</v>
+        <v>#N/A Requesting Data...3313217507</v>
         <stp/>
         <stp>BDP|7048111723254898858</stp>
         <tr r="E70" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3786841807</v>
+        <v>#N/A Requesting Data...1339152273</v>
         <stp/>
         <stp>BDP|7514426398370500271</stp>
         <tr r="F84" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3044131876</v>
+        <v>#N/A Requesting Data...3470205080</v>
         <stp/>
         <stp>BDP|2286847884578687294</stp>
         <tr r="C64" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4047958435</v>
+        <v>#N/A Requesting Data...446272464</v>
         <stp/>
         <stp>BDP|8581359335587083771</stp>
         <tr r="G40" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3208438686</v>
+        <v>#N/A Requesting Data...1046977711</v>
         <stp/>
         <stp>BDP|9176352611073152053</stp>
         <tr r="G52" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2087428032</v>
+        <v>#N/A Requesting Data...228657069</v>
         <stp/>
         <stp>BDP|3761613276703138977</stp>
         <tr r="C22" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3190105644</v>
+        <v>#N/A Requesting Data...1949598300</v>
         <stp/>
         <stp>BDP|2402283480247992710</stp>
         <tr r="G65" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2471410607</v>
+        <v>#N/A Requesting Data...3721668630</v>
         <stp/>
         <stp>BDP|2496054182730824314</stp>
         <tr r="F108" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2978067607</v>
+        <v>#N/A Requesting Data...2063322369</v>
         <stp/>
         <stp>BDP|1156198294412416234</stp>
         <tr r="G48" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3484901760</v>
+        <v>#N/A Requesting Data...874371576</v>
         <stp/>
         <stp>BDP|1935863512592400318</stp>
         <tr r="G99" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3229643830</v>
+        <v>#N/A Requesting Data...2310234799</v>
         <stp/>
         <stp>BDP|1182070188629538920</stp>
         <tr r="F85" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4213563743</v>
+        <v>#N/A Requesting Data...3155506878</v>
         <stp/>
         <stp>BDP|9924697901094165296</stp>
         <tr r="E38" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3876296179</v>
+        <v>#N/A Requesting Data...1307939066</v>
         <stp/>
         <stp>BDP|6412137247758825261</stp>
         <tr r="G10" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4185355806</v>
+        <v>#N/A Requesting Data...2254392763</v>
         <stp/>
         <stp>BDP|6277108296426856136</stp>
         <tr r="G122" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4070801035</v>
+        <v>#N/A Requesting Data...632526504</v>
         <stp/>
         <stp>BDP|2351176324921816947</stp>
         <tr r="E117" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2241162764</v>
+        <v>#N/A Requesting Data...2990697652</v>
         <stp/>
         <stp>BDP|6406207188846485346</stp>
         <tr r="C37" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2907058977</v>
+        <v>#N/A Requesting Data...1681898767</v>
         <stp/>
         <stp>BDP|8112280367483097628</stp>
         <tr r="F16" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2930807949</v>
+        <v>#N/A Requesting Data...2363099286</v>
         <stp/>
         <stp>BDP|6484624822372932905</stp>
         <tr r="C108" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3588698903</v>
+        <v>#N/A Requesting Data...562815820</v>
         <stp/>
         <stp>BDP|8605875253514357834</stp>
         <tr r="C116" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3287808336</v>
+        <v>#N/A Requesting Data...2918291105</v>
         <stp/>
         <stp>BDP|2842991807747556512</stp>
         <tr r="E110" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2147336850</v>
+        <v>#N/A Requesting Data...3213067806</v>
         <stp/>
         <stp>BDP|1377759003508711718</stp>
         <tr r="E55" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2302790564</v>
+        <v>#N/A Requesting Data...530598548</v>
         <stp/>
         <stp>BDP|1711361391887412536</stp>
         <tr r="G47" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2965271460</v>
+        <v>#N/A Requesting Data...4101764410</v>
         <stp/>
         <stp>BDP|4564815655442574234</stp>
         <tr r="F114" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4087035376</v>
+        <v>#N/A Requesting Data...1903531560</v>
         <stp/>
         <stp>BDP|6557751567646791843</stp>
         <tr r="C85" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4201183387</v>
+        <v>#N/A Requesting Data...2960764772</v>
         <stp/>
         <stp>BDP|5018226780961297742</stp>
         <tr r="E138" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2162586453</v>
+        <v>#N/A Requesting Data...1337513204</v>
         <stp/>
         <stp>BDP|7190582290036507495</stp>
         <tr r="E48" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3246597746</v>
+        <v>#N/A Requesting Data...3176882471</v>
         <stp/>
         <stp>BDP|7268732641219205478</stp>
         <tr r="F111" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3096094862</v>
+        <v>#N/A Requesting Data...3251387681</v>
         <stp/>
         <stp>BDP|5085458293997400582</stp>
         <tr r="C30" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2759077986</v>
+        <v>#N/A Requesting Data...1985911820</v>
         <stp/>
         <stp>BDP|2916061605678582044</stp>
         <tr r="E27" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2918194827</v>
+        <v>#N/A Requesting Data...2971376033</v>
         <stp/>
         <stp>BDP|5645196194854205325</stp>
         <tr r="E19" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2662158536</v>
+        <v>#N/A Requesting Data...1055061258</v>
         <stp/>
         <stp>BDP|8929421222763426766</stp>
         <tr r="F112" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4203624490</v>
+        <v>#N/A Requesting Data...646972861</v>
         <stp/>
         <stp>BDP|2815946348173965667</stp>
         <tr r="C137" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3487869211</v>
+        <v>#N/A Requesting Data...651963080</v>
         <stp/>
         <stp>BDP|6645611732949919042</stp>
         <tr r="G95" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3190740903</v>
+        <v>#N/A Requesting Data...2893679147</v>
         <stp/>
         <stp>BDP|8744658502964028082</stp>
         <tr r="F139" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2158822481</v>
+        <v>#N/A Requesting Data...1756179285</v>
         <stp/>
         <stp>BDP|4077907452745230782</stp>
         <tr r="C130" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2079709540</v>
+        <v>#N/A Requesting Data...894137046</v>
         <stp/>
         <stp>BDP|8975856381415089739</stp>
         <tr r="E75" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3707021606</v>
+        <v>#N/A Requesting Data...1586016779</v>
         <stp/>
         <stp>BDP|5738611839292209825</stp>
         <tr r="G107" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3829515204</v>
+        <v>#N/A Requesting Data...1955672097</v>
         <stp/>
         <stp>BDP|4996818111432201578</stp>
         <tr r="G134" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3212560818</v>
+        <v>#N/A Requesting Data...1105616827</v>
         <stp/>
         <stp>BDP|5458032582021895609</stp>
         <tr r="E89" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2517749811</v>
+        <v>#N/A Requesting Data...1155625366</v>
         <stp/>
         <stp>BDP|2612461303954522846</stp>
         <tr r="F21" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3713883017</v>
+        <v>#N/A Requesting Data...1557715666</v>
         <stp/>
         <stp>BDP|5852840000806674187</stp>
         <tr r="F75" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2250456966</v>
+        <v>#N/A Requesting Data...1297814730</v>
         <stp/>
         <stp>BDP|7947641811679527399</stp>
         <tr r="G13" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3654169986</v>
+        <v>#N/A Requesting Data...2329308895</v>
         <stp/>
         <stp>BDP|8407769428857900025</stp>
         <tr r="C132" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4129973616</v>
+        <v>#N/A Requesting Data...2787125864</v>
         <stp/>
         <stp>BDP|1313714864639868399</stp>
         <tr r="F87" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3058417624</v>
+        <v>#N/A Requesting Data...1651523053</v>
         <stp/>
         <stp>BDP|2531298252748844733</stp>
         <tr r="F115" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3476867575</v>
+        <v>#N/A Requesting Data...1525375936</v>
         <stp/>
         <stp>BDP|8965389266391509672</stp>
         <tr r="C41" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2805803094</v>
+        <v>#N/A Requesting Data...3975517550</v>
         <stp/>
         <stp>BDP|9146373380128430189</stp>
         <tr r="F60" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3374432423</v>
+        <v>#N/A Requesting Data...3397861761</v>
         <stp/>
         <stp>BDP|8769626454200391097</stp>
         <tr r="G85" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4057318249</v>
+        <v>#N/A Requesting Data...1295470583</v>
         <stp/>
         <stp>BDP|7701346097304455298</stp>
         <tr r="C73" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2744733074</v>
+        <v>#N/A Requesting Data...3045832439</v>
         <stp/>
         <stp>BDP|1201589979318261083</stp>
         <tr r="G123" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3504894709</v>
+        <v>#N/A Requesting Data...304187581</v>
         <stp/>
         <stp>BDP|9994425762708075853</stp>
         <tr r="G88" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3359572780</v>
+        <v>#N/A Requesting Data...4099283221</v>
         <stp/>
         <stp>BDP|8238868892513701135</stp>
         <tr r="G137" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2851487181</v>
+        <v>#N/A Requesting Data...3265568655</v>
         <stp/>
         <stp>BDP|3321556007464177923</stp>
         <tr r="E109" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3963321798</v>
+        <v>#N/A Requesting Data...978031333</v>
         <stp/>
         <stp>BDP|8367368187378355023</stp>
         <tr r="F64" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2941110063</v>
+        <v>#N/A Requesting Data...857698492</v>
         <stp/>
         <stp>BDP|9054142235387080711</stp>
         <tr r="F11" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3341842078</v>
+        <v>#N/A Requesting Data...1195898908</v>
         <stp/>
         <stp>BDP|4797724273716399932</stp>
         <tr r="C5" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3536129242</v>
+        <v>#N/A Requesting Data...3576764429</v>
         <stp/>
         <stp>BDP|3084971212582403246</stp>
         <tr r="F121" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2789133234</v>
+        <v>#N/A Requesting Data...448684065</v>
         <stp/>
         <stp>BDP|6948762204713990690</stp>
         <tr r="G90" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3934976456</v>
+        <v>#N/A Requesting Data...4227222810</v>
         <stp/>
         <stp>BDP|1832764578595986067</stp>
         <tr r="G119" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2209686272</v>
+        <v>#N/A Requesting Data...2843754662</v>
         <stp/>
         <stp>BDP|4156639623951685595</stp>
         <tr r="F13" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3744316688</v>
+        <v>#N/A Requesting Data...3770857286</v>
         <stp/>
         <stp>BDP|5919761437851372455</stp>
         <tr r="C2" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3304046624</v>
+        <v>#N/A Requesting Data...560072832</v>
         <stp/>
         <stp>BDP|1551339666687413790</stp>
         <tr r="F40" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3949730619</v>
+        <v>#N/A Requesting Data...2884632242</v>
         <stp/>
         <stp>BDP|6420437202397070174</stp>
         <tr r="C8" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2876774030</v>
+        <v>#N/A Requesting Data...823870296</v>
         <stp/>
         <stp>BDP|1708381902825815365</stp>
         <tr r="C101" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3551024837</v>
+        <v>#N/A Requesting Data...3179298912</v>
         <stp/>
         <stp>BDP|4945796250777738578</stp>
         <tr r="G21" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3309569033</v>
+        <v>#N/A Requesting Data...891948136</v>
         <stp/>
         <stp>BDP|6746841414412327938</stp>
         <tr r="G75" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3120682854</v>
+        <v>#N/A Requesting Data...4292324813</v>
         <stp/>
         <stp>BDP|1709445403856801620</stp>
         <tr r="E85" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4199388458</v>
+        <v>#N/A Requesting Data...2533982283</v>
         <stp/>
         <stp>BDP|9398823419477440265</stp>
         <tr r="G125" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3521883141</v>
+        <v>#N/A Requesting Data...917955551</v>
         <stp/>
         <stp>BDP|3430878723724827801</stp>
         <tr r="G41" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2330853018</v>
+        <v>#N/A Requesting Data...829852121</v>
         <stp/>
         <stp>BDP|9698422803149077198</stp>
         <tr r="C100" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4272165654</v>
+        <v>#N/A Requesting Data...4280435359</v>
         <stp/>
         <stp>BDP|2887002514665714363</stp>
         <tr r="G59" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2608498852</v>
+        <v>#N/A Requesting Data...3260228688</v>
         <stp/>
         <stp>BDP|2668814054578766269</stp>
         <tr r="E31" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4108301233</v>
+        <v>#N/A Requesting Data...1422833224</v>
         <stp/>
         <stp>BDP|8894702939828266110</stp>
         <tr r="C7" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2986645645</v>
+        <v>#N/A Requesting Data...3834695885</v>
         <stp/>
         <stp>BDP|3410885660260666884</stp>
         <tr r="E64" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3059010464</v>
+        <v>#N/A Requesting Data...2143400879</v>
         <stp/>
         <stp>BDP|3658713905400418152</stp>
         <tr r="E35" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2644780298</v>
+        <v>#N/A Requesting Data...1144432037</v>
         <stp/>
         <stp>BDP|7570300716478486864</stp>
         <tr r="E32" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2312597369</v>
+        <v>#N/A Requesting Data...1909446016</v>
         <stp/>
         <stp>BDP|7851492951527237434</stp>
         <tr r="E52" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2899207809</v>
+        <v>#N/A Requesting Data...2162898645</v>
         <stp/>
         <stp>BDP|7352242467910007671</stp>
         <tr r="F124" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4286254706</v>
+        <v>#N/A Requesting Data...3563013023</v>
         <stp/>
         <stp>BDP|5657563513753480721</stp>
         <tr r="E80" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4035006027</v>
+        <v>#N/A Requesting Data...811899395</v>
         <stp/>
         <stp>BDP|5976587264538865878</stp>
         <tr r="E62" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3176447079</v>
+        <v>#N/A Requesting Data...1926508208</v>
         <stp/>
         <stp>BDP|7151318027339523982</stp>
         <tr r="F91" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4058665934</v>
+        <v>#N/A Requesting Data...761635329</v>
         <stp/>
         <stp>BDP|1896477110772260049</stp>
         <tr r="C91" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4042288415</v>
+        <v>#N/A Requesting Data...4139087936</v>
         <stp/>
         <stp>BDP|4252725967471187287</stp>
         <tr r="F44" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4236038527</v>
+        <v>#N/A Requesting Data...1244235669</v>
         <stp/>
         <stp>BDP|6943451920864586278</stp>
         <tr r="C118" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2524288194</v>
+        <v>#N/A Requesting Data...2969571127</v>
         <stp/>
         <stp>BDP|5838113265174067025</stp>
         <tr r="F39" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2913194332</v>
+        <v>#N/A Requesting Data...2161245101</v>
         <stp/>
         <stp>BDP|3456718228377624745</stp>
         <tr r="E111" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3838771378</v>
+        <v>#N/A Requesting Data...784619859</v>
         <stp/>
         <stp>BDP|5917425194519245724</stp>
         <tr r="E79" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4032305058</v>
+        <v>#N/A Requesting Data...2614367450</v>
         <stp/>
         <stp>BDP|6787533358407016713</stp>
         <tr r="F135" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4026659571</v>
+        <v>#N/A Requesting Data...796871633</v>
         <stp/>
         <stp>BDP|5576451913756991076</stp>
         <tr r="E16" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4012810339</v>
+        <v>#N/A Requesting Data...799403250</v>
         <stp/>
         <stp>BDP|5284390591628042184</stp>
         <tr r="C24" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2857240293</v>
+        <v>#N/A Requesting Data...1503550885</v>
         <stp/>
         <stp>BDP|5412037028917536689</stp>
         <tr r="G115" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3841376672</v>
+        <v>#N/A Requesting Data...2415567951</v>
         <stp/>
         <stp>BDP|8966942938724477029</stp>
         <tr r="C15" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4228137713</v>
+        <v>#N/A Requesting Data...2546528156</v>
         <stp/>
         <stp>BDP|2938144706552859709</stp>
         <tr r="G81" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4050405213</v>
+        <v>#N/A Requesting Data...718737511</v>
         <stp/>
         <stp>BDP|3632949480676633244</stp>
         <tr r="F31" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2957224968</v>
+        <v>#N/A Requesting Data...800010350</v>
         <stp/>
         <stp>BDP|3513418606797579639</stp>
         <tr r="F90" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2914524537</v>
+        <v>#N/A Requesting Data...425163818</v>
         <stp/>
         <stp>BDP|1733520919261908213</stp>
         <tr r="G73" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3500198761</v>
+        <v>#N/A Requesting Data...3820756748</v>
         <stp/>
         <stp>BDP|8368969127023380651</stp>
         <tr r="F28" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3586096155</v>
+        <v>#N/A Requesting Data...3794478646</v>
         <stp/>
         <stp>BDP|7172716621593553717</stp>
         <tr r="F53" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3770214933</v>
+        <v>#N/A Requesting Data...1389565829</v>
         <stp/>
         <stp>BDP|2954250373819174944</stp>
         <tr r="F119" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4003591213</v>
+        <v>#N/A Requesting Data...2198442512</v>
         <stp/>
         <stp>BDP|4728287753511799518</stp>
         <tr r="F3" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2905761142</v>
+        <v>#N/A Requesting Data...1907260176</v>
         <stp/>
         <stp>BDP|6348617969513327227</stp>
         <tr r="E104" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2664866704</v>
+        <v>#N/A Requesting Data...2487498112</v>
         <stp/>
         <stp>BDP|7694099704858685831</stp>
         <tr r="C107" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2404893993</v>
+        <v>#N/A Requesting Data...3385522058</v>
         <stp/>
         <stp>BDP|4106834752526835861</stp>
         <tr r="F55" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3302070381</v>
+        <v>#N/A Requesting Data...2646557355</v>
         <stp/>
         <stp>BDP|7951337561756108354</stp>
         <tr r="G112" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3069135532</v>
+        <v>#N/A Requesting Data...3668974226</v>
         <stp/>
         <stp>BDP|5468867501418549294</stp>
         <tr r="E86" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3166055786</v>
+        <v>#N/A Requesting Data...3549939681</v>
         <stp/>
         <stp>BDP|4546740053823447251</stp>
         <tr r="C32" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2922197351</v>
+        <v>#N/A Requesting Data...1428668156</v>
         <stp/>
         <stp>BDP|7484527599745538990</stp>
         <tr r="F76" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3529598635</v>
+        <v>#N/A Requesting Data...3871022924</v>
         <stp/>
         <stp>BDP|5578475423865159117</stp>
         <tr r="E61" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3148089534</v>
+        <v>#N/A Requesting Data...4011956218</v>
         <stp/>
         <stp>BDP|6158107237024797760</stp>
         <tr r="E45" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2276060999</v>
+        <v>#N/A Requesting Data...919619847</v>
         <stp/>
         <stp>BDP|4143076943390197735</stp>
         <tr r="F97" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2437381932</v>
+        <v>#N/A Requesting Data...3388148647</v>
         <stp/>
         <stp>BDP|1762196091349932721</stp>
         <tr r="E82" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2646514057</v>
+        <v>#N/A Requesting Data...680102332</v>
         <stp/>
         <stp>BDP|4189169184528349241</stp>
         <tr r="F137" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2254478638</v>
+        <v>#N/A Requesting Data...3425644231</v>
         <stp/>
         <stp>BDP|9103140635044368872</stp>
         <tr r="F29" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2904842019</v>
+        <v>#N/A Requesting Data...3955775105</v>
         <stp/>
         <stp>BDP|5519603296584718917</stp>
         <tr r="G54" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3833529754</v>
+        <v>#N/A Requesting Data...1930049489</v>
         <stp/>
         <stp>BDP|1156250824766982737</stp>
         <tr r="G44" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2652977590</v>
+        <v>#N/A Requesting Data...2496440739</v>
         <stp/>
         <stp>BDP|6031605254431729496</stp>
         <tr r="G86" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3645584974</v>
+        <v>#N/A Requesting Data...4061456857</v>
         <stp/>
         <stp>BDP|2649489454114394728</stp>
         <tr r="C14" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2694828383</v>
+        <v>#N/A Requesting Data...1809442788</v>
         <stp/>
         <stp>BDP|8999377595616850481</stp>
         <tr r="E108" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2326733779</v>
+        <v>#N/A Requesting Data...3776669481</v>
         <stp/>
         <stp>BDP|8988928209665280487</stp>
         <tr r="F71" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3653920232</v>
+        <v>#N/A Requesting Data...1861923152</v>
         <stp/>
         <stp>BDP|8368023487691952119</stp>
         <tr r="F88" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2640527916</v>
+        <v>#N/A Requesting Data...1451817228</v>
         <stp/>
         <stp>BDP|5199287207907438042</stp>
         <tr r="E66" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2766874484</v>
+        <v>#N/A Requesting Data...2823538643</v>
         <stp/>
         <stp>BDP|7460099446995728631</stp>
         <tr r="F134" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2697733954</v>
+        <v>#N/A Requesting Data...3814137739</v>
         <stp/>
         <stp>BDP|6160638673325976246</stp>
         <tr r="C104" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4274660092</v>
+        <v>#N/A Requesting Data...1087292410</v>
         <stp/>
         <stp>BDP|5660731962530222490</stp>
         <tr r="E128" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2904223918</v>
+        <v>#N/A Requesting Data...871235480</v>
         <stp/>
         <stp>BDP|3355023726294311595</stp>
         <tr r="G114" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3292303272</v>
+        <v>#N/A Requesting Data...960451760</v>
         <stp/>
         <stp>BDP|5604474461391860653</stp>
         <tr r="E130" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2922057059</v>
+        <v>#N/A Requesting Data...2731362747</v>
         <stp/>
         <stp>BDP|3542140114402066179</stp>
         <tr r="E78" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2299840185</v>
+        <v>#N/A Requesting Data...4151085390</v>
         <stp/>
         <stp>BDP|2942496252996870592</stp>
         <tr r="G121" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3562555131</v>
+        <v>#N/A Requesting Data...1223198763</v>
         <stp/>
         <stp>BDP|1823820926283534897</stp>
         <tr r="G18" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2951210153</v>
+        <v>#N/A Requesting Data...3821990051</v>
         <stp/>
         <stp>BDP|3716189405712826043</stp>
         <tr r="G92" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2818806369</v>
+        <v>#N/A Requesting Data...2510073345</v>
         <stp/>
         <stp>BDP|9344147089140006098</stp>
         <tr r="E83" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2624549374</v>
+        <v>#N/A Requesting Data...3598545022</v>
         <stp/>
         <stp>BDP|6993061706081965773</stp>
         <tr r="F81" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4257644005</v>
+        <v>#N/A Requesting Data...4252931641</v>
         <stp/>
         <stp>BDP|6176792116871092198</stp>
         <tr r="C68" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2674869255</v>
+        <v>#N/A Requesting Data...1148472517</v>
         <stp/>
         <stp>BDP|7185432584822399912</stp>
         <tr r="F131" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3292275189</v>
+        <v>#N/A Requesting Data...2572271485</v>
         <stp/>
         <stp>BDP|8280856169194643320</stp>
         <tr r="G49" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2495770492</v>
+        <v>#N/A Requesting Data...2961906640</v>
         <stp/>
         <stp>BDP|9399109618929306123</stp>
         <tr r="F37" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2481050666</v>
+        <v>#N/A Requesting Data...2356882252</v>
         <stp/>
         <stp>BDP|6669663699409638145</stp>
         <tr r="C123" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2286369069</v>
+        <v>#N/A Requesting Data...1575860190</v>
         <stp/>
         <stp>BDP|6175693122901836298</stp>
         <tr r="C36" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3725341236</v>
+        <v>#N/A Requesting Data...4189300819</v>
         <stp/>
         <stp>BDP|8135075327118072391</stp>
         <tr r="C17" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2723215567</v>
+        <v>#N/A Requesting Data...3714863956</v>
         <stp/>
         <stp>BDP|5726291712345411206</stp>
         <tr r="G28" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2878065664</v>
+        <v>#N/A Requesting Data...2770426492</v>
         <stp/>
         <stp>BDP|8698973352783506690</stp>
         <tr r="F25" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4168641775</v>
+        <v>#N/A Requesting Data...2876673990</v>
         <stp/>
         <stp>BDP|5493604681742158862</stp>
         <tr r="G63" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3544966261</v>
+        <v>#N/A Requesting Data...2259887157</v>
         <stp/>
         <stp>BDP|3239104742287612040</stp>
         <tr r="E39" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2367241352</v>
+        <v>#N/A Requesting Data...3314667218</v>
         <stp/>
         <stp>BDP|3381147726641663059</stp>
         <tr r="C122" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3836589193</v>
+        <v>#N/A Requesting Data...2840445266</v>
         <stp/>
         <stp>BDP|6625906764329795167</stp>
         <tr r="F56" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2715766779</v>
+        <v>#N/A Requesting Data...1349990125</v>
         <stp/>
         <stp>BDP|3325218238213801010</stp>
         <tr r="F57" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2766461850</v>
+        <v>#N/A Requesting Data...3413711025</v>
         <stp/>
         <stp>BDP|1313137390988032037</stp>
         <tr r="C83" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2813949976</v>
+        <v>#N/A Requesting Data...1605896945</v>
         <stp/>
         <stp>BDP|3702733300853619616</stp>
         <tr r="G34" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4125618631</v>
+        <v>#N/A Requesting Data...2678436222</v>
         <stp/>
         <stp>BDP|8558611930018338475</stp>
         <tr r="F35" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3796199091</v>
+        <v>#N/A Requesting Data...2553296275</v>
         <stp/>
         <stp>BDP|5387098906493173798</stp>
         <tr r="G62" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3717108312</v>
+        <v>#N/A Requesting Data...3960441666</v>
         <stp/>
         <stp>BDP|1951038018907673608</stp>
         <tr r="C126" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3310279815</v>
+        <v>#N/A Requesting Data...3192987853</v>
         <stp/>
         <stp>BDP|9253802402770546012</stp>
         <tr r="F74" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4276589791</v>
+        <v>#N/A Requesting Data...3823331915</v>
         <stp/>
         <stp>BDP|1884505914021260664</stp>
         <tr r="E96" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3138423907</v>
+        <v>#N/A Requesting Data...1982571561</v>
         <stp/>
         <stp>BDP|3540127028674193608</stp>
         <tr r="F94" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2396167833</v>
+        <v>#N/A Requesting Data...2766909291</v>
         <stp/>
         <stp>BDP|5372375359741187031</stp>
         <tr r="F27" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2440069100</v>
+        <v>#N/A Requesting Data...785193560</v>
         <stp/>
         <stp>BDP|5121625602631825066</stp>
         <tr r="E81" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3860153553</v>
+        <v>#N/A Requesting Data...1514278790</v>
         <stp/>
         <stp>BDP|5282708515920897138</stp>
         <tr r="F43" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2363556198</v>
+        <v>#N/A Requesting Data...3886273874</v>
         <stp/>
         <stp>BDP|1250299291741371958</stp>
         <tr r="G31" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3073303234</v>
+        <v>#N/A Requesting Data...944573103</v>
         <stp/>
         <stp>BDP|4253176148933327033</stp>
         <tr r="C133" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2861779211</v>
+        <v>#N/A Requesting Data...670495749</v>
         <stp/>
         <stp>BDP|9704751602229087502</stp>
         <tr r="F49" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3279559179</v>
+        <v>#N/A Requesting Data...2435250785</v>
         <stp/>
         <stp>BDP|6775233901286469015</stp>
         <tr r="E125" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2857795407</v>
+        <v>#N/A Requesting Data...3548717052</v>
         <stp/>
         <stp>BDP|7918289416910309647</stp>
         <tr r="C56" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3040956290</v>
+        <v>#N/A Requesting Data...1113372904</v>
         <stp/>
         <stp>BDP|3731272815900600241</stp>
         <tr r="C53" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3646300417</v>
+        <v>#N/A Requesting Data...3788467310</v>
         <stp/>
         <stp>BDP|1685459166489439868</stp>
         <tr r="F133" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3536348972</v>
+        <v>#N/A Requesting Data...2269685671</v>
         <stp/>
         <stp>BDP|2506644172580171154</stp>
         <tr r="C119" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4095808341</v>
+        <v>#N/A Requesting Data...3398074879</v>
         <stp/>
         <stp>BDP|1995353227627490580</stp>
         <tr r="E119" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4164166061</v>
+        <v>#N/A Requesting Data...3212677901</v>
         <stp/>
         <stp>BDP|9173868178561206592</stp>
         <tr r="C77" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3714606979</v>
+        <v>#N/A Requesting Data...2593133824</v>
         <stp/>
         <stp>BDP|4008096672221657096</stp>
         <tr r="G43" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3368285915</v>
+        <v>#N/A Requesting Data...3763011591</v>
         <stp/>
         <stp>BDP|5434663182001395869</stp>
         <tr r="E107" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3868940695</v>
+        <v>#N/A Requesting Data...3512733941</v>
         <stp/>
         <stp>BDP|8686279502629263146</stp>
         <tr r="C129" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3441559026</v>
+        <v>#N/A Requesting Data...2398563818</v>
         <stp/>
         <stp>BDP|4576300957588172984</stp>
         <tr r="E63" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3981867502</v>
+        <v>#N/A Requesting Data...2459782536</v>
         <stp/>
         <stp>BDP|7469671678835895086</stp>
         <tr r="E2" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3351809772</v>
+        <v>#N/A Requesting Data...4290458713</v>
         <stp/>
         <stp>BDP|5444751401066968714</stp>
         <tr r="E73" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3649919630</v>
+        <v>#N/A Requesting Data...982445367</v>
         <stp/>
         <stp>BDP|2824124077350027748</stp>
         <tr r="E136" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2999589210</v>
+        <v>#N/A Requesting Data...1125118417</v>
         <stp/>
         <stp>BDP|3708851985886704699</stp>
         <tr r="C19" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3873171708</v>
+        <v>#N/A Requesting Data...865977820</v>
         <stp/>
         <stp>BDP|1006071828475585561</stp>
         <tr r="F116" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3768072159</v>
+        <v>#N/A Requesting Data...1945418884</v>
         <stp/>
         <stp>BDP|1086712249007771639</stp>
         <tr r="G26" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3698294201</v>
+        <v>#N/A Requesting Data...2740895212</v>
         <stp/>
         <stp>BDP|6634730869724168016</stp>
         <tr r="E103" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2464008701</v>
+        <v>#N/A Requesting Data...1085165631</v>
         <stp/>
         <stp>BDP|3520366017777816505</stp>
         <tr r="E97" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3965245036</v>
+        <v>#N/A Requesting Data...2388425723</v>
         <stp/>
         <stp>BDP|2995135217932647367</stp>
         <tr r="F105" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3083529143</v>
+        <v>#N/A Requesting Data...1959531363</v>
         <stp/>
         <stp>BDP|3565057922625094707</stp>
         <tr r="G45" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2721361101</v>
+        <v>#N/A Requesting Data...1757461754</v>
         <stp/>
         <stp>BDP|1485569542807651461</stp>
         <tr r="C86" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2928247920</v>
+        <v>#N/A Requesting Data...3640993036</v>
         <stp/>
         <stp>BDP|1159006460850353421</stp>
         <tr r="E46" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2923080211</v>
+        <v>#N/A Requesting Data...3503147809</v>
         <stp/>
         <stp>BDP|5113311422502283510</stp>
         <tr r="C84" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2280088494</v>
+        <v>#N/A Requesting Data...952714652</v>
         <stp/>
         <stp>BDP|4420649803735408460</stp>
         <tr r="F117" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2622587879</v>
+        <v>#N/A Requesting Data...958432140</v>
         <stp/>
         <stp>BDP|9873235984695079585</stp>
         <tr r="C60" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3898496294</v>
+        <v>#N/A Requesting Data...4252618910</v>
         <stp/>
         <stp>BDP|4726106605717010168</stp>
         <tr r="G46" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3968115623</v>
+        <v>#N/A Requesting Data...1163234842</v>
         <stp/>
         <stp>BDP|97453184744598227</stp>
         <tr r="G135" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3594451385</v>
+        <v>#N/A Requesting Data...2535868210</v>
         <stp/>
         <stp>BDP|71129432364790944</stp>
         <tr r="E105" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4273335848</v>
+        <v>#N/A Requesting Data...3338254174</v>
         <stp/>
         <stp>BDP|13870968378316918</stp>
         <tr r="F38" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3038872270</v>
+        <v>#N/A Requesting Data...1637819643</v>
         <stp/>
         <stp>BDP|545017254499479967</stp>
         <tr r="E23" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2590921368</v>
+        <v>#N/A Requesting Data...3466794058</v>
         <stp/>
         <stp>BDP|562457211792430265</stp>
         <tr r="G116" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3930986533</v>
+        <v>#N/A Requesting Data...1875528951</v>
         <stp/>
         <stp>BDP|752318736222262646</stp>
         <tr r="F83" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3785494276</v>
+        <v>#N/A Requesting Data...934185561</v>
         <stp/>
         <stp>BDP|926433161397617222</stp>
         <tr r="F10" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3802938082</v>
+        <v>#N/A Requesting Data...2710663568</v>
         <stp/>
         <stp>BDP|455507803480864317</stp>
         <tr r="C51" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2910077767</v>
+        <v>#N/A Requesting Data...3179151313</v>
         <stp/>
         <stp>BDP|738430784972633891</stp>
         <tr r="F41" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2675424048</v>
+        <v>#N/A Requesting Data...1456039183</v>
         <stp/>
         <stp>BDP|226270545351892196</stp>
         <tr r="F61" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2523882898</v>
+        <v>#N/A Requesting Data...2198600032</v>
         <stp/>
         <stp>BDP|478534605105814154</stp>
         <tr r="G12" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3612204506</v>
+        <v>#N/A Requesting Data...3550085258</v>
         <stp/>
         <stp>BDP|292697057297288557</stp>
         <tr r="C106" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3704313745</v>
+        <v>#N/A Requesting Data...4025197882</v>
         <stp/>
         <stp>BDP|449489448517477649</stp>
         <tr r="E99" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4276324063</v>
+        <v>#N/A Requesting Data...1076425593</v>
         <stp/>
         <stp>BDP|477239144286521179</stp>
         <tr r="G138" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2509738314</v>
+        <v>#N/A Requesting Data...1300280954</v>
         <stp/>
         <stp>BDP|136361134742057301</stp>
         <tr r="C57" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3209803443</v>
+        <v>#N/A Requesting Data...1810329733</v>
         <stp/>
         <stp>BDP|282958180978155995</stp>
         <tr r="C59" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3887785919</v>
+        <v>#N/A Requesting Data...2667627713</v>
         <stp/>
         <stp>BDP|991366924295531418</stp>
         <tr r="F2" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4267630643</v>
+        <v>#N/A Requesting Data...1664672706</v>
         <stp/>
         <stp>BDP|934073235795196633</stp>
         <tr r="F62" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3451967278</v>
+        <v>#N/A Requesting Data...2151375438</v>
         <stp/>
         <stp>BDP|266608211912165570</stp>
         <tr r="E113" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2460228668</v>
+        <v>#N/A Requesting Data...1573868978</v>
         <stp/>
         <stp>BDP|910156400954699593</stp>
         <tr r="G8" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3573886771</v>
+        <v>#N/A Requesting Data...2614419859</v>
         <stp/>
         <stp>BDP|794293317440269040</stp>
         <tr r="E100" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3887557093</v>
+        <v>#N/A Requesting Data...1820812164</v>
         <stp/>
         <stp>BDP|206766873121157269</stp>
         <tr r="E41" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3605588468</v>
+        <v>#N/A Requesting Data...1261357359</v>
         <stp/>
         <stp>BDP|315261912951356153</stp>
         <tr r="E21" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3404968689</v>
+        <v>#N/A Requesting Data...1680858022</v>
         <stp/>
         <stp>BDP|169080827246056602</stp>
         <tr r="G126" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2549947066</v>
+        <v>#N/A Requesting Data...902314763</v>
         <stp/>
         <stp>BDP|454779781439338455</stp>
         <tr r="E36" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2576946696</v>
+        <v>#N/A Requesting Data...2708409197</v>
         <stp/>
         <stp>BDP|198524097739196711</stp>
         <tr r="F92" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3146905401</v>
+        <v>#N/A Requesting Data...1846429795</v>
         <stp/>
         <stp>BDP|618726407191106421</stp>
         <tr r="C92" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2863232273</v>
+        <v>#N/A Requesting Data...3740701098</v>
         <stp/>
         <stp>BDP|442808307356626303</stp>
         <tr r="F20" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3354275099</v>
+        <v>#N/A Requesting Data...597270679</v>
         <stp/>
         <stp>BDP|304889655090792147</stp>
         <tr r="E58" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3364684796</v>
+        <v>#N/A Requesting Data...1341058508</v>
         <stp/>
         <stp>BDP|427627592191043219</stp>
         <tr r="C87" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3592331781</v>
+        <v>#N/A Requesting Data...3842402475</v>
         <stp/>
         <stp>BDP|768711067038142524</stp>
         <tr r="G25" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3880711681</v>
+        <v>#N/A Requesting Data...4092147632</v>
         <stp/>
         <stp>BDP|447365482187669383</stp>
         <tr r="C95" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3951322710</v>
+        <v>#N/A Requesting Data...598766212</v>
         <stp/>
         <stp>BDP|901925773788783965</stp>
         <tr r="G67" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4293061246</v>
+        <v>#N/A Requesting Data...4125527448</v>
         <stp/>
         <stp>BDP|511429594874391764</stp>
         <tr r="G117" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3461432090</v>
+        <v>#N/A Requesting Data...1506612255</v>
         <stp/>
         <stp>BDP|544620567958067604</stp>
         <tr r="C131" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4085555371</v>
+        <v>#N/A Requesting Data...1408626457</v>
         <stp/>
         <stp>BDP|945569483354328027</stp>
         <tr r="C21" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2979716402</v>
+        <v>#N/A Requesting Data...2225556539</v>
         <stp/>
         <stp>BDP|691281527639744142</stp>
         <tr r="E8" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2842878399</v>
+        <v>#N/A Requesting Data...2561577769</v>
         <stp/>
         <stp>BDP|968314719543295935</stp>
         <tr r="E68" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3240094750</v>
+        <v>#N/A Requesting Data...3575330960</v>
         <stp/>
         <stp>BDP|760426044168153386</stp>
         <tr r="G7" s="1"/>
@@ -4813,7 +4813,7 @@
   <dimension ref="A1:E139"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7190,7 +7190,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5352835-5CFD-46EC-8CDA-5672A55A22F5}">
   <dimension ref="A1:G139"/>
   <sheetViews>
-    <sheetView topLeftCell="A111" workbookViewId="0">
+    <sheetView topLeftCell="A45" workbookViewId="0">
       <selection activeCell="E2" sqref="E2:G139"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updated rating file to incl. algeria
</commit_message>
<xml_diff>
--- a/index_bbg_rating_live.xlsx
+++ b/index_bbg_rating_live.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kaimin Khaw\Desktop\credit-rating-deploy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B7A7B46-A890-42A2-B099-6A8BC7C10825}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BBB445D-0338-48E1-835D-2ACB32098003}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-72" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{2A12413E-A5EC-426E-A187-DE07F52921C3}"/>
+    <workbookView xWindow="22932" yWindow="-72" windowWidth="23256" windowHeight="12456" xr2:uid="{2A12413E-A5EC-426E-A187-DE07F52921C3}"/>
   </bookViews>
   <sheets>
     <sheet name="hard_code" sheetId="2" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="353">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="846" uniqueCount="356">
   <si>
     <t>Turkey</t>
   </si>
@@ -1107,6 +1107,15 @@
   </si>
   <si>
     <t>CCC+u</t>
+  </si>
+  <si>
+    <t>Algeria</t>
+  </si>
+  <si>
+    <t>3700Z US Equity</t>
+  </si>
+  <si>
+    <t>B- *-</t>
   </si>
 </sst>
 </file>
@@ -1192,1531 +1201,1537 @@
   <volType type="realTimeData">
     <main first="bofaddin.rtdserver">
       <tp t="s">
-        <v>#N/A Requesting Data...1393973396</v>
+        <v>#N/A Requesting Data...3469221504</v>
         <stp/>
         <stp>BDP|13719527809048657439</stp>
         <tr r="E3" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1387541483</v>
+        <v>#N/A Requesting Data...4026000411</v>
         <stp/>
         <stp>BDP|12363409739849183621</stp>
         <tr r="G98" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2596115898</v>
+        <v>#N/A Requesting Data...2097201990</v>
         <stp/>
         <stp>BDP|17606584297068117917</stp>
         <tr r="G105" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1088612670</v>
+        <v>#N/A Requesting Data...2483144695</v>
         <stp/>
         <stp>BDP|12825277506793769973</stp>
         <tr r="F22" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2669613270</v>
+        <v>#N/A Requesting Data...757932436</v>
         <stp/>
         <stp>BDP|13615906068526188051</stp>
         <tr r="G101" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3287439784</v>
+        <v>#N/A Requesting Data...2190318939</v>
         <stp/>
         <stp>BDP|10912677687245148127</stp>
         <tr r="G106" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3134572433</v>
+        <v>#N/A Requesting Data...1280301803</v>
         <stp/>
         <stp>BDP|16221541486007837625</stp>
         <tr r="G58" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2419385622</v>
+        <v>#N/A Requesting Data...2281158124</v>
         <stp/>
         <stp>BDP|14989839765876665645</stp>
         <tr r="C81" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2895914362</v>
+        <v>#N/A Requesting Data...3291580075</v>
         <stp/>
         <stp>BDP|16792452589360294083</stp>
         <tr r="E11" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2925720591</v>
+        <v>#N/A Requesting Data...3282485542</v>
         <stp/>
         <stp>BDP|16409240184993364568</stp>
         <tr r="E54" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2378611094</v>
+        <v>#N/A Requesting Data...2991655323</v>
         <stp/>
         <stp>BDP|12376141866138693768</stp>
         <tr r="C88" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2909010441</v>
+        <v>#N/A Requesting Data...2534845178</v>
         <stp/>
         <stp>BDP|13146963289471890960</stp>
         <tr r="C18" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3582752084</v>
+        <v>#N/A Requesting Data...3321695672</v>
         <stp/>
         <stp>BDP|10167725043130019931</stp>
         <tr r="C110" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2358549511</v>
+        <v>#N/A Requesting Data...1389474271</v>
         <stp/>
         <stp>BDP|10589422899161895655</stp>
         <tr r="G76" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3684289492</v>
+        <v>#N/A Requesting Data...802018258</v>
         <stp/>
         <stp>BDP|15228795190517586693</stp>
         <tr r="E84" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2457307666</v>
+        <v>#N/A Requesting Data...1569896394</v>
         <stp/>
         <stp>BDP|10096201946458505444</stp>
         <tr r="G97" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1285024810</v>
+        <v>#N/A Requesting Data...1857433059</v>
         <stp/>
         <stp>BDP|18253401034836307331</stp>
         <tr r="F99" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2958086290</v>
+        <v>#N/A Requesting Data...3676881851</v>
         <stp/>
         <stp>BDP|10867273920449518201</stp>
         <tr r="G71" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1140967481</v>
+        <v>#N/A Requesting Data...2557369291</v>
         <stp/>
         <stp>BDP|14811872563886412749</stp>
         <tr r="E114" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2923447981</v>
+        <v>#N/A Requesting Data...762284618</v>
         <stp/>
         <stp>BDP|15237334583701669483</stp>
         <tr r="C112" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...947855092</v>
+        <v>#N/A Requesting Data...3509488155</v>
         <stp/>
         <stp>BDP|14006145231309322495</stp>
         <tr r="C65" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2959502213</v>
+        <v>#N/A Requesting Data...1584714792</v>
         <stp/>
         <stp>BDP|14761213634019822741</stp>
         <tr r="G2" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1667184540</v>
+        <v>#N/A Requesting Data...2474911944</v>
         <stp/>
         <stp>BDP|15399231330039360601</stp>
         <tr r="E42" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2644824801</v>
+        <v>#N/A Requesting Data...2929906347</v>
         <stp/>
         <stp>BDP|11120752607359953480</stp>
         <tr r="G61" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1238522551</v>
+        <v>#N/A Requesting Data...3548035795</v>
         <stp/>
         <stp>BDP|15939978441203902037</stp>
         <tr r="C26" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2962634374</v>
+        <v>#N/A Requesting Data...2772966588</v>
         <stp/>
         <stp>BDP|18066043829836356791</stp>
         <tr r="G78" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1274672067</v>
+        <v>#N/A Requesting Data...1167331241</v>
         <stp/>
         <stp>BDP|14168806967588813989</stp>
         <tr r="F77" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1805699082</v>
+        <v>#N/A Requesting Data...2262806649</v>
         <stp/>
         <stp>BDP|18397803367339867766</stp>
         <tr r="F101" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2649186466</v>
+        <v>#N/A Requesting Data...3394163086</v>
         <stp/>
         <stp>BDP|15895803206017416271</stp>
         <tr r="C33" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3375204117</v>
+        <v>#N/A Requesting Data...2787318579</v>
         <stp/>
         <stp>BDP|14908732543227691836</stp>
         <tr r="E94" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1690454332</v>
+        <v>#N/A Requesting Data...3208314582</v>
         <stp/>
         <stp>BDP|12957817799052931996</stp>
         <tr r="E120" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4048775071</v>
+        <v>#N/A Requesting Data...1878838918</v>
         <stp/>
         <stp>BDP|16275205432289392600</stp>
         <tr r="E101" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2076039650</v>
+        <v>#N/A Requesting Data...1170960444</v>
         <stp/>
         <stp>BDP|10407655300028223605</stp>
         <tr r="F47" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2157881744</v>
+        <v>#N/A Requesting Data...3712458942</v>
         <stp/>
         <stp>BDP|14031612538318230186</stp>
         <tr r="C136" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2673658635</v>
+        <v>#N/A Requesting Data...1207156183</v>
         <stp/>
         <stp>BDP|13840587393604095357</stp>
         <tr r="G3" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3897829225</v>
+        <v>#N/A Requesting Data...2827354773</v>
         <stp/>
         <stp>BDP|18397555740376217727</stp>
         <tr r="F17" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3658856289</v>
+        <v>#N/A Requesting Data...3785788442</v>
         <stp/>
         <stp>BDP|15886108592084595196</stp>
         <tr r="F19" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...792239508</v>
+        <v>#N/A Requesting Data...3313793692</v>
         <stp/>
         <stp>BDP|12574943311804341655</stp>
         <tr r="C58" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...636458521</v>
+        <v>#N/A Requesting Data...3435445995</v>
         <stp/>
         <stp>BDP|15276164033266227932</stp>
         <tr r="C121" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2516764119</v>
+        <v>#N/A Requesting Data...2799197514</v>
         <stp/>
         <stp>BDP|11413915902765857449</stp>
         <tr r="C135" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3161981991</v>
+        <v>#N/A Requesting Data...3127246163</v>
         <stp/>
         <stp>BDP|10888161880627674738</stp>
         <tr r="G74" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1672848675</v>
+        <v>#N/A Requesting Data...1701006661</v>
         <stp/>
         <stp>BDP|18252264749434830399</stp>
         <tr r="E91" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1210099786</v>
+        <v>#N/A Requesting Data...2776621519</v>
         <stp/>
         <stp>BDP|16230814927561165496</stp>
         <tr r="C25" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1621140205</v>
+        <v>#N/A Requesting Data...1837621096</v>
         <stp/>
         <stp>BDP|11669407615485914850</stp>
         <tr r="E28" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1458276021</v>
+        <v>#N/A Requesting Data...3184069362</v>
         <stp/>
         <stp>BDP|15385895124225473341</stp>
         <tr r="F89" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1058093410</v>
+        <v>#N/A Requesting Data...1073077122</v>
         <stp/>
         <stp>BDP|16215575297831427265</stp>
         <tr r="G19" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4269500627</v>
+        <v>#N/A Requesting Data...1457582627</v>
         <stp/>
         <stp>BDP|15664489079057139842</stp>
         <tr r="C50" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3535792662</v>
+        <v>#N/A Requesting Data...3358140717</v>
         <stp/>
         <stp>BDP|13556466380534139208</stp>
         <tr r="C63" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3087436622</v>
+        <v>#N/A Requesting Data...3878905229</v>
         <stp/>
         <stp>BDP|12426034393664290636</stp>
         <tr r="G70" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2059183852</v>
+        <v>#N/A Requesting Data...503387570</v>
         <stp/>
         <stp>BDP|11206974657257798316</stp>
         <tr r="G5" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1956912799</v>
+        <v>#N/A Requesting Data...1371457682</v>
         <stp/>
         <stp>BDP|15687672872765725835</stp>
         <tr r="G133" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4147652237</v>
+        <v>#N/A Requesting Data...4156172873</v>
         <stp/>
         <stp>BDP|10646340980557108540</stp>
         <tr r="G83" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4073203591</v>
+        <v>#N/A Requesting Data...3731788715</v>
         <stp/>
         <stp>BDP|13932387258969800286</stp>
         <tr r="G30" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2164178460</v>
+        <v>#N/A Requesting Data...3815902941</v>
         <stp/>
         <stp>BDP|14685689793557045247</stp>
         <tr r="G11" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1109622400</v>
+        <v>#N/A Requesting Data...1303460890</v>
         <stp/>
         <stp>BDP|11792528289940283264</stp>
         <tr r="G39" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2349074300</v>
+        <v>#N/A Requesting Data...2017370435</v>
         <stp/>
         <stp>BDP|14038814629908297802</stp>
         <tr r="E14" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3522709182</v>
+        <v>#N/A Requesting Data...3361837077</v>
         <stp/>
         <stp>BDP|17960836852555549100</stp>
         <tr r="F79" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...788110350</v>
+        <v>#N/A Requesting Data...3121777466</v>
         <stp/>
         <stp>BDP|12258786923690042954</stp>
         <tr r="G82" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1156040933</v>
+        <v>#N/A Requesting Data...3259998277</v>
         <stp/>
         <stp>BDP|11831892951331348329</stp>
         <tr r="C35" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3341506853</v>
+        <v>#N/A Requesting Data...3162529413</v>
         <stp/>
         <stp>BDP|12634554786653062247</stp>
         <tr r="F34" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2817532102</v>
+        <v>#N/A Requesting Data...1012669930</v>
         <stp/>
         <stp>BDP|10304787173197381988</stp>
         <tr r="G53" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...967429172</v>
+        <v>#N/A Requesting Data...1749506975</v>
         <stp/>
         <stp>BDP|15772343051115104818</stp>
         <tr r="C127" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1526828901</v>
+        <v>#N/A Requesting Data...1660206629</v>
         <stp/>
         <stp>BDP|13619322587163510542</stp>
         <tr r="C45" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3026830164</v>
+        <v>#N/A Requesting Data...1747990127</v>
         <stp/>
         <stp>BDP|13709828003397613269</stp>
         <tr r="C54" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3152035800</v>
+        <v>#N/A Requesting Data...3607852767</v>
         <stp/>
         <stp>BDP|11596891797659679653</stp>
         <tr r="C89" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1566936622</v>
+        <v>#N/A Requesting Data...1483074579</v>
         <stp/>
         <stp>BDP|18339290641951108002</stp>
         <tr r="E17" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1341436030</v>
+        <v>#N/A Requesting Data...3846379806</v>
         <stp/>
         <stp>BDP|10418265688390464525</stp>
         <tr r="E18" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2323999569</v>
+        <v>#N/A Requesting Data...1118672302</v>
         <stp/>
         <stp>BDP|14859691791600738447</stp>
         <tr r="F45" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1835528082</v>
+        <v>#N/A Requesting Data...3191517874</v>
         <stp/>
         <stp>BDP|18255708956124343152</stp>
         <tr r="E26" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3866307331</v>
+        <v>#N/A Requesting Data...2962769239</v>
         <stp/>
         <stp>BDP|16855823919014233436</stp>
         <tr r="F30" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2738643903</v>
+        <v>#N/A Requesting Data...1436410056</v>
         <stp/>
         <stp>BDP|12821872971201299383</stp>
         <tr r="G124" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2470508403</v>
+        <v>#N/A Requesting Data...3454449464</v>
         <stp/>
         <stp>BDP|11466185903217969815</stp>
         <tr r="F33" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1851890810</v>
+        <v>#N/A Requesting Data...4153861783</v>
         <stp/>
         <stp>BDP|13711300257260836914</stp>
         <tr r="C102" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1206683649</v>
+        <v>#N/A Requesting Data...4236355901</v>
         <stp/>
         <stp>BDP|11622318103537999967</stp>
         <tr r="F15" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4209252840</v>
+        <v>#N/A Requesting Data...1459584173</v>
         <stp/>
         <stp>BDP|10597445640754361898</stp>
         <tr r="F50" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1527644178</v>
+        <v>#N/A Requesting Data...1059002892</v>
         <stp/>
         <stp>BDP|13987588094432951117</stp>
         <tr r="E127" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...716314919</v>
+        <v>#N/A Requesting Data...1642178506</v>
         <stp/>
         <stp>BDP|11655961067423868102</stp>
         <tr r="G104" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2040804701</v>
+        <v>#N/A Requesting Data...3039541095</v>
         <stp/>
         <stp>BDP|12468839190466923900</stp>
         <tr r="C20" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1246836466</v>
+        <v>#N/A Requesting Data...1670756863</v>
         <stp/>
         <stp>BDP|18411047804853597705</stp>
         <tr r="C67" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1504528992</v>
+        <v>#N/A Requesting Data...2543208507</v>
         <stp/>
         <stp>BDP|18331339124097518219</stp>
         <tr r="F66" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...686066202</v>
+        <v>#N/A Requesting Data...931586932</v>
         <stp/>
         <stp>BDP|14983531083496973331</stp>
         <tr r="G132" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2820738758</v>
+        <v>#N/A Requesting Data...2464608095</v>
         <stp/>
         <stp>BDP|14115869171127460078</stp>
         <tr r="G37" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4247231165</v>
+        <v>#N/A Requesting Data...2691967196</v>
         <stp/>
         <stp>BDP|16963038037211063893</stp>
         <tr r="C13" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2168007445</v>
+        <v>#N/A Requesting Data...733555754</v>
         <stp/>
         <stp>BDP|13900268704084418991</stp>
         <tr r="E37" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1933807551</v>
+        <v>#N/A Requesting Data...2564141710</v>
         <stp/>
         <stp>BDP|16311230542528118454</stp>
         <tr r="E9" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3598291299</v>
+        <v>#N/A Requesting Data...818461321</v>
         <stp/>
         <stp>BDP|12403550728001134908</stp>
         <tr r="G38" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1548539341</v>
+        <v>#N/A Requesting Data...3577817020</v>
         <stp/>
         <stp>BDP|10528694388950747396</stp>
         <tr r="F80" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2244008820</v>
+        <v>#N/A Requesting Data...3462870917</v>
         <stp/>
         <stp>BDP|17962073596443790028</stp>
         <tr r="F23" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...854343235</v>
+        <v>#N/A Requesting Data...3433140974</v>
         <stp/>
         <stp>BDP|11322749828038387103</stp>
         <tr r="E122" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2867771827</v>
+        <v>#N/A Requesting Data...1893436700</v>
         <stp/>
         <stp>BDP|14872467854648029062</stp>
         <tr r="C75" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1057827372</v>
+        <v>#N/A Requesting Data...2179592472</v>
         <stp/>
         <stp>BDP|14951668809329151689</stp>
         <tr r="E56" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4237801746</v>
+        <v>#N/A Requesting Data...1214829725</v>
         <stp/>
         <stp>BDP|14211231849266296941</stp>
         <tr r="G103" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1200910698</v>
+        <v>#N/A Requesting Data...786205641</v>
         <stp/>
         <stp>BDP|15282935006718574931</stp>
         <tr r="E92" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1853437086</v>
+        <v>#N/A Requesting Data...2042873640</v>
         <stp/>
         <stp>BDP|16389940868391785591</stp>
         <tr r="C120" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4289560641</v>
+        <v>#N/A Requesting Data...4224485094</v>
         <stp/>
         <stp>BDP|10830300668358540045</stp>
         <tr r="C115" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2098034165</v>
+        <v>#N/A Requesting Data...1050533426</v>
         <stp/>
         <stp>BDP|15417892931237679498</stp>
         <tr r="F8" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1231034010</v>
+        <v>#N/A Requesting Data...2674341264</v>
         <stp/>
         <stp>BDP|13776760394691002167</stp>
         <tr r="C4" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...938251547</v>
+        <v>#N/A Requesting Data...2382557114</v>
         <stp/>
         <stp>BDP|12950924085148446689</stp>
         <tr r="E121" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2412840944</v>
+        <v>#N/A Requesting Data...1236128874</v>
         <stp/>
         <stp>BDP|11202744698684518690</stp>
         <tr r="G111" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2352617009</v>
+        <v>#N/A Requesting Data...2976688885</v>
         <stp/>
         <stp>BDP|11005719894013994183</stp>
         <tr r="C3" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2404474414</v>
+        <v>#N/A Requesting Data...2501659359</v>
         <stp/>
         <stp>BDP|17061881470574956177</stp>
         <tr r="C69" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3059746317</v>
+        <v>#N/A Requesting Data...4006309743</v>
         <stp/>
         <stp>BDP|10195299258766033392</stp>
         <tr r="E90" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3933607268</v>
+        <v>#N/A Requesting Data...2753041888</v>
         <stp/>
         <stp>BDP|17559180385128709479</stp>
         <tr r="E15" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2509958720</v>
+        <v>#N/A Requesting Data...1243850635</v>
         <stp/>
         <stp>BDP|10477087317801173223</stp>
         <tr r="F125" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1696299183</v>
+        <v>#N/A Requesting Data...4094783320</v>
         <stp/>
         <stp>BDP|10431478218456128129</stp>
         <tr r="G32" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3076740935</v>
+        <v>#N/A Requesting Data...3409683099</v>
         <stp/>
         <stp>BDP|12817533695869473568</stp>
         <tr r="C82" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3472580146</v>
+        <v>#N/A Requesting Data...2229016864</v>
         <stp/>
         <stp>BDP|16722436137983528090</stp>
         <tr r="F127" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1686534252</v>
+        <v>#N/A Requesting Data...3260889302</v>
         <stp/>
         <stp>BDP|14949322880769358496</stp>
         <tr r="G16" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2047200883</v>
+        <v>#N/A Requesting Data...1404786241</v>
         <stp/>
         <stp>BDP|12620594347341901004</stp>
         <tr r="C76" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3909344887</v>
+        <v>#N/A Requesting Data...1450782809</v>
         <stp/>
         <stp>BDP|12047021516217693612</stp>
         <tr r="E126" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3262787072</v>
+        <v>#N/A Requesting Data...1585734847</v>
         <stp/>
         <stp>BDP|13612225533853005354</stp>
         <tr r="F102" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1739359656</v>
+        <v>#N/A Requesting Data...3220350261</v>
         <stp/>
         <stp>BDP|11536436753390219250</stp>
         <tr r="F129" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2647234073</v>
+        <v>#N/A Requesting Data...3868495510</v>
         <stp/>
         <stp>BDP|12946334758336119017</stp>
         <tr r="E72" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3983773641</v>
+        <v>#N/A Requesting Data...929939509</v>
         <stp/>
         <stp>BDP|17733998071078953332</stp>
         <tr r="C23" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2635514128</v>
+        <v>#N/A Requesting Data...2759974875</v>
         <stp/>
         <stp>BDP|16362559715466602618</stp>
         <tr r="F68" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2840409522</v>
+        <v>#N/A Requesting Data...1260071379</v>
         <stp/>
         <stp>BDP|16070475881909673177</stp>
         <tr r="E112" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2757595476</v>
+        <v>#N/A Requesting Data...4149285303</v>
         <stp/>
         <stp>BDP|17590878194950224438</stp>
         <tr r="G87" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1976356095</v>
+        <v>#N/A Requesting Data...2513603988</v>
         <stp/>
         <stp>BDP|12427007793358727164</stp>
         <tr r="F100" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...821546481</v>
+        <v>#N/A Requesting Data...4101415419</v>
         <stp/>
         <stp>BDP|15601293270144483737</stp>
         <tr r="G15" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1875652475</v>
+        <v>#N/A Requesting Data...2177398823</v>
         <stp/>
         <stp>BDP|13723200346810339697</stp>
         <tr r="C38" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3032914515</v>
+        <v>#N/A Requesting Data...2253547025</v>
         <stp/>
         <stp>BDP|18086118189074176643</stp>
         <tr r="E88" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...859570471</v>
+        <v>#N/A Requesting Data...886130094</v>
         <stp/>
         <stp>BDP|15679917748483251829</stp>
         <tr r="E6" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1940584453</v>
+        <v>#N/A Requesting Data...2510287358</v>
         <stp/>
         <stp>BDP|13421293548936861023</stp>
         <tr r="G66" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1853877163</v>
+        <v>#N/A Requesting Data...4116093787</v>
         <stp/>
         <stp>BDP|10594946509929542325</stp>
         <tr r="F5" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1825788351</v>
+        <v>#N/A Requesting Data...1606588796</v>
         <stp/>
         <stp>BDP|10668212108445960480</stp>
         <tr r="G57" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3145032320</v>
+        <v>#N/A Requesting Data...1488733058</v>
         <stp/>
         <stp>BDP|10103273213286136651</stp>
         <tr r="C6" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4042758882</v>
+        <v>#N/A Requesting Data...2015787689</v>
         <stp/>
         <stp>BDP|11259721862376480554</stp>
         <tr r="G69" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3876743375</v>
+        <v>#N/A Requesting Data...3867433897</v>
         <stp/>
         <stp>BDP|14885566279524266176</stp>
         <tr r="E30" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3823111994</v>
+        <v>#N/A Requesting Data...789410965</v>
         <stp/>
         <stp>BDP|14519079130534129014</stp>
         <tr r="C49" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1777557586</v>
+        <v>#N/A Requesting Data...2424556266</v>
         <stp/>
         <stp>BDP|14873136635550817546</stp>
         <tr r="G130" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1061315127</v>
+        <v>#N/A Requesting Data...2290211675</v>
         <stp/>
         <stp>BDP|16641457892301341972</stp>
         <tr r="F130" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4051428208</v>
+        <v>#N/A Requesting Data...2734710752</v>
         <stp/>
         <stp>BDP|13231746637163726724</stp>
         <tr r="E7" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...953711454</v>
+        <v>#N/A Requesting Data...1649949747</v>
         <stp/>
         <stp>BDP|12945735048800380256</stp>
         <tr r="G118" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...996357533</v>
+        <v>#N/A Requesting Data...2926127580</v>
         <stp/>
         <stp>BDP|11265248170961260631</stp>
         <tr r="E47" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3566857987</v>
+        <v>#N/A Requesting Data...820339038</v>
         <stp/>
         <stp>BDP|16351851074029385080</stp>
         <tr r="G35" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2682977260</v>
+        <v>#N/A Requesting Data...1838918113</v>
         <stp/>
         <stp>BDP|11944358991052271970</stp>
         <tr r="C103" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1227369618</v>
+        <v>#N/A Requesting Data...1612516393</v>
         <stp/>
         <stp>BDP|18410981990650283866</stp>
         <tr r="C99" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3265768833</v>
+        <v>#N/A Requesting Data...2218487944</v>
         <stp/>
         <stp>BDP|14383773052580838655</stp>
         <tr r="F104" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2388546553</v>
+        <v>#N/A Requesting Data...3369478515</v>
         <stp/>
         <stp>BDP|10871340643964419300</stp>
         <tr r="F95" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2857137344</v>
+        <v>#N/A Requesting Data...1840230434</v>
         <stp/>
         <stp>BDP|14690280185656044816</stp>
         <tr r="C94" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1135952546</v>
+        <v>#N/A Requesting Data...2178095358</v>
         <stp/>
         <stp>BDP|18305693996456795112</stp>
         <tr r="G80" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1341718502</v>
+        <v>#N/A Requesting Data...2642890408</v>
         <stp/>
         <stp>BDP|16273225567973824127</stp>
         <tr r="C79" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2282669700</v>
+        <v>#N/A Requesting Data...4201411901</v>
         <stp/>
         <stp>BDP|13313129291618997350</stp>
         <tr r="C43" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2266068535</v>
+        <v>#N/A Requesting Data...3185351005</v>
         <stp/>
         <stp>BDP|15444947284180871401</stp>
         <tr r="G27" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4178501717</v>
+        <v>#N/A Requesting Data...1792449690</v>
         <stp/>
         <stp>BDP|12935317504846234704</stp>
         <tr r="F98" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4108397422</v>
+        <v>#N/A Requesting Data...4262631996</v>
         <stp/>
         <stp>BDP|13057895365605005829</stp>
         <tr r="C138" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2431486926</v>
+        <v>#N/A Requesting Data...1400510134</v>
         <stp/>
         <stp>BDP|16160321537943284588</stp>
         <tr r="E76" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2023498454</v>
+        <v>#N/A Requesting Data...3407504857</v>
         <stp/>
         <stp>BDP|10621599828921836610</stp>
         <tr r="C12" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1341040589</v>
+        <v>#N/A Requesting Data...1609971585</v>
         <stp/>
         <stp>BDP|14881076967673386157</stp>
         <tr r="F122" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2818306851</v>
+        <v>#N/A Requesting Data...4244789896</v>
         <stp/>
         <stp>BDP|17321553610055816607</stp>
         <tr r="F96" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1420684773</v>
+        <v>#N/A Requesting Data...1215170446</v>
         <stp/>
         <stp>BDP|12793555755147383546</stp>
         <tr r="F42" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1993805517</v>
+        <v>#N/A Requesting Data...1072925730</v>
         <stp/>
         <stp>BDP|10194327202093986081</stp>
         <tr r="F132" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3414725116</v>
+        <v>#N/A Requesting Data...2497613595</v>
         <stp/>
         <stp>BDP|12798194599768683232</stp>
         <tr r="C42" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1817651679</v>
+        <v>#N/A Requesting Data...1129732024</v>
         <stp/>
         <stp>BDP|15675203172551734114</stp>
         <tr r="F12" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1718480633</v>
+        <v>#N/A Requesting Data...1693336900</v>
         <stp/>
         <stp>BDP|17779010845097021465</stp>
         <tr r="G23" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3126147801</v>
+        <v>#N/A Requesting Data...815107798</v>
         <stp/>
         <stp>BDP|14698661432127374654</stp>
         <tr r="E53" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1727638698</v>
+        <v>#N/A Requesting Data...3873374339</v>
         <stp/>
         <stp>BDP|16055018629402477686</stp>
         <tr r="F18" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4108556463</v>
+        <v>#N/A Requesting Data...2097125028</v>
         <stp/>
         <stp>BDP|14191015466523343124</stp>
         <tr r="G42" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1774957625</v>
+        <v>#N/A Requesting Data...1285784491</v>
         <stp/>
         <stp>BDP|16690545673604064064</stp>
         <tr r="G6" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3676520191</v>
+        <v>#N/A Requesting Data...2530356064</v>
         <stp/>
         <stp>BDP|11057556593645206836</stp>
         <tr r="E116" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1029287567</v>
+        <v>#N/A Requesting Data...1931289579</v>
         <stp/>
         <stp>BDP|14753168038796700174</stp>
         <tr r="E131" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3737068614</v>
+        <v>#N/A Requesting Data...1123981030</v>
         <stp/>
         <stp>BDP|18400936140157917378</stp>
         <tr r="G108" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1369435671</v>
+        <v>#N/A Requesting Data...4107569244</v>
         <stp/>
         <stp>BDP|11308062409311166143</stp>
         <tr r="F138" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2650950611</v>
+        <v>#N/A Requesting Data...2165782506</v>
         <stp/>
         <stp>BDP|14929251921187622207</stp>
         <tr r="G120" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2464060287</v>
+        <v>#N/A Requesting Data...2233660972</v>
         <stp/>
         <stp>BDP|13312546151322475095</stp>
         <tr r="C117" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3550489157</v>
+        <v>#N/A Requesting Data...2677887888</v>
         <stp/>
         <stp>BDP|10370784365528062849</stp>
         <tr r="G51" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4211816687</v>
+        <v>#N/A Requesting Data...865460929</v>
         <stp/>
         <stp>BDP|17808503947101138629</stp>
         <tr r="F128" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3762018233</v>
+        <v>#N/A Requesting Data...1828435451</v>
         <stp/>
         <stp>BDP|17640270888515662931</stp>
         <tr r="E20" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2718580980</v>
+        <v>#N/A Requesting Data...1734735328</v>
         <stp/>
         <stp>BDP|17853766030844520642</stp>
         <tr r="F65" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3823581658</v>
+        <v>#N/A Requesting Data...784949662</v>
         <stp/>
         <stp>BDP|17345319339237647129</stp>
         <tr r="C10" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2809896158</v>
+        <v>#N/A Requesting Data...2667662498</v>
         <stp/>
         <stp>BDP|18428163184190295050</stp>
         <tr r="C48" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4086326415</v>
+        <v>#N/A Requesting Data...2337065076</v>
         <stp/>
         <stp>BDP|11469771160883398201</stp>
         <tr r="G20" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1821162104</v>
+        <v>#N/A Requesting Data...3183573758</v>
         <stp/>
         <stp>BDP|12945229628891094206</stp>
         <tr r="F36" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2331247098</v>
+        <v>#N/A Requesting Data...3772741407</v>
         <stp/>
         <stp>BDP|13088969316699575369</stp>
         <tr r="G17" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1328823440</v>
+        <v>#N/A Requesting Data...3523072682</v>
         <stp/>
         <stp>BDP|14386928546318260068</stp>
         <tr r="C78" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1756514352</v>
+        <v>#N/A Requesting Data...3647320543</v>
         <stp/>
         <stp>BDP|16250000632946565269</stp>
         <tr r="F32" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2417511522</v>
+        <v>#N/A Requesting Data...1999441671</v>
         <stp/>
         <stp>BDP|10062445544650347114</stp>
         <tr r="E69" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4138239511</v>
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDP|16445974490524697317</stp>
+        <tr r="F140" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A Requesting Data...1408220706</v>
         <stp/>
         <stp>BDP|18056984346180923430</stp>
         <tr r="F67" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1590556116</v>
+        <v>#N/A Requesting Data...2274418682</v>
         <stp/>
         <stp>BDP|13607419850307697457</stp>
         <tr r="G55" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1757645956</v>
+        <v>#N/A Requesting Data...3915070250</v>
         <stp/>
         <stp>BDP|17151526894293450943</stp>
         <tr r="E34" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2511428625</v>
+        <v>#N/A Requesting Data...3221859879</v>
         <stp/>
         <stp>BDP|14769233272840536059</stp>
         <tr r="F48" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2068625720</v>
+        <v>#N/A Requesting Data...1772038875</v>
         <stp/>
         <stp>BDP|16347078018142331376</stp>
         <tr r="E59" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2436605977</v>
+        <v>#N/A Requesting Data...2775869243</v>
         <stp/>
         <stp>BDP|12157937398585487157</stp>
         <tr r="F69" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1112496292</v>
+        <v>#N/A Requesting Data...3450845366</v>
         <stp/>
         <stp>BDP|10450024654077121490</stp>
         <tr r="G29" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1853850542</v>
+        <v>#N/A Requesting Data...1968387828</v>
         <stp/>
         <stp>BDP|12405274734177384298</stp>
         <tr r="G109" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1455101656</v>
+        <v>#N/A Requesting Data...2545328806</v>
         <stp/>
         <stp>BDP|11693290023110245727</stp>
         <tr r="F93" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4171418070</v>
+        <v>#N/A Requesting Data...2404597129</v>
         <stp/>
         <stp>BDP|16857915317939051104</stp>
         <tr r="E4" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1479287655</v>
+        <v>#N/A Requesting Data...3842909688</v>
         <stp/>
         <stp>BDP|13092630751014311204</stp>
         <tr r="C29" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2882824492</v>
+        <v>#N/A Requesting Data...3000192752</v>
         <stp/>
         <stp>BDP|16560165422091315234</stp>
         <tr r="E74" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...869680939</v>
+        <v>#N/A Requesting Data...4196404766</v>
         <stp/>
         <stp>BDP|15578620992514708823</stp>
         <tr r="C74" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1650762713</v>
+        <v>#N/A Requesting Data...2667998084</v>
         <stp/>
         <stp>BDP|16311826266949112751</stp>
         <tr r="E137" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2460191925</v>
+        <v>#N/A Requesting Data...2992969174</v>
         <stp/>
         <stp>BDP|12423551309476829732</stp>
         <tr r="E29" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3956733924</v>
+        <v>#N/A Requesting Data...3199490161</v>
         <stp/>
         <stp>BDP|15334425393507822980</stp>
         <tr r="C71" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3797436960</v>
+        <v>#N/A Requesting Data...4009317134</v>
         <stp/>
         <stp>BDP|14187404668490888034</stp>
         <tr r="E115" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3256904526</v>
+        <v>#N/A Requesting Data...983205183</v>
         <stp/>
         <stp>BDP|14038301256494491076</stp>
         <tr r="E12" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2578751198</v>
+        <v>#N/A Requesting Data...2945250430</v>
         <stp/>
         <stp>BDP|12212063840830333025</stp>
         <tr r="E132" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2842773462</v>
+        <v>#N/A Requesting Data...4147170793</v>
         <stp/>
         <stp>BDP|12411228970299104833</stp>
         <tr r="E40" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3683561867</v>
+        <v>#N/A Requesting Data...1937545442</v>
         <stp/>
         <stp>BDP|11324255971734653659</stp>
         <tr r="G93" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2966458821</v>
+        <v>#N/A Requesting Data...923444276</v>
         <stp/>
         <stp>BDP|15080702944965265524</stp>
         <tr r="E5" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4217914683</v>
+        <v>#N/A Requesting Data...1863246818</v>
         <stp/>
         <stp>BDP|12709330545317601409</stp>
         <tr r="F78" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2567303335</v>
+        <v>#N/A Requesting Data...2003989593</v>
         <stp/>
         <stp>BDP|17558583635766924170</stp>
         <tr r="C139" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3324673038</v>
+        <v>#N/A Requesting Data...3368278043</v>
         <stp/>
         <stp>BDP|14043797868641345244</stp>
         <tr r="G127" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1662671366</v>
+        <v>#N/A Requesting Data...2821920190</v>
         <stp/>
         <stp>BDP|11097146762171726091</stp>
         <tr r="C125" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3839984278</v>
+        <v>#N/A Requesting Data...2346385945</v>
         <stp/>
         <stp>BDP|10083242995488903402</stp>
         <tr r="E22" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...885051645</v>
+        <v>#N/A Requesting Data...1973534664</v>
         <stp/>
         <stp>BDP|14104003677163905777</stp>
         <tr r="G89" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2282252628</v>
+        <v>#N/A Requesting Data...1417872037</v>
         <stp/>
         <stp>BDP|10493155251505330684</stp>
         <tr r="F113" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1896647921</v>
+        <v>#N/A Requesting Data...2109775885</v>
         <stp/>
         <stp>BDP|17307159600861837050</stp>
         <tr r="C28" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2827816739</v>
+        <v>#N/A Requesting Data...3337612575</v>
         <stp/>
         <stp>BDP|11974207352247436657</stp>
         <tr r="G84" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2906318413</v>
+        <v>#N/A Requesting Data...4044932811</v>
         <stp/>
         <stp>BDP|12417029733397010193</stp>
         <tr r="G129" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1133784036</v>
+        <v>#N/A Requesting Data...1616245422</v>
         <stp/>
         <stp>BDP|13696428749777505366</stp>
         <tr r="C128" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4020320739</v>
+        <v>#N/A Requesting Data...1732287721</v>
         <stp/>
         <stp>BDP|10265435339313984301</stp>
         <tr r="F136" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3750350656</v>
+        <v>#N/A Requesting Data...1590202008</v>
         <stp/>
         <stp>BDP|16742662035804692035</stp>
         <tr r="E24" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4013490733</v>
+        <v>#N/A Requesting Data...4003227884</v>
         <stp/>
         <stp>BDP|13311072247345018521</stp>
         <tr r="E129" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4159799853</v>
+        <v>#N/A Requesting Data...2172624229</v>
         <stp/>
         <stp>BDP|14635385909938704819</stp>
         <tr r="E106" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3214156506</v>
+        <v>#N/A Requesting Data...2469301612</v>
         <stp/>
         <stp>BDP|17965266240553639582</stp>
         <tr r="E10" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3109250006</v>
+        <v>#N/A Requesting Data...2445012252</v>
         <stp/>
         <stp>BDP|14559650107303581628</stp>
         <tr r="C72" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2192883120</v>
+        <v>#N/A Requesting Data...1174662566</v>
         <stp/>
         <stp>BDP|12078771150016496119</stp>
         <tr r="G102" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3171515223</v>
+        <v>#N/A Requesting Data...4069299378</v>
         <stp/>
         <stp>BDP|13437131854538783812</stp>
         <tr r="G22" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2650016210</v>
+        <v>#N/A Requesting Data...2382110685</v>
         <stp/>
         <stp>BDP|11816803688615161347</stp>
         <tr r="E51" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1906334483</v>
+        <v>#N/A Requesting Data...3950912559</v>
         <stp/>
         <stp>BDP|11136233214231371414</stp>
         <tr r="G139" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2762678911</v>
+        <v>#N/A Requesting Data...1745042404</v>
         <stp/>
         <stp>BDP|16387121100332435221</stp>
         <tr r="G96" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3468213277</v>
+        <v>#N/A Requesting Data...2705630820</v>
         <stp/>
         <stp>BDP|10044993787394494110</stp>
         <tr r="C113" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1368658396</v>
+        <v>#N/A Requesting Data...982662432</v>
         <stp/>
         <stp>BDP|16851432539276999316</stp>
         <tr r="E44" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4123983569</v>
+        <v>#N/A Requesting Data...3867532259</v>
         <stp/>
         <stp>BDP|17514330731974993734</stp>
         <tr r="E65" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1407689106</v>
+        <v>#N/A Requesting Data...1019695791</v>
         <stp/>
         <stp>BDP|13397290692205579908</stp>
         <tr r="G128" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2627169884</v>
+        <v>#N/A Requesting Data...2636015311</v>
         <stp/>
         <stp>BDP|11770519860203890508</stp>
         <tr r="F106" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2905631740</v>
+        <v>#N/A Requesting Data...1474495217</v>
         <stp/>
         <stp>BDP|11828615722360397168</stp>
         <tr r="E71" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1701952407</v>
+        <v>#N/A Requesting Data...2458220676</v>
         <stp/>
         <stp>BDP|12429929188915695292</stp>
         <tr r="F109" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3230430249</v>
+        <v>#N/A Requesting Data...4112057914</v>
         <stp/>
         <stp>BDP|14807781952773549162</stp>
         <tr r="G33" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3149073298</v>
+        <v>#N/A Requesting Data...3814046755</v>
         <stp/>
         <stp>BDP|14141528956866623622</stp>
         <tr r="C134" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1275367130</v>
+        <v>#N/A Requesting Data...1848116892</v>
         <stp/>
         <stp>BDP|11925450918217650729</stp>
         <tr r="F86" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...931820176</v>
+        <v>#N/A Requesting Data...1837900561</v>
         <stp/>
         <stp>BDP|10075353521710450506</stp>
         <tr r="C109" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1241620388</v>
+        <v>#N/A Requesting Data...1624881164</v>
         <stp/>
         <stp>BDP|14507687284196916837</stp>
         <tr r="F6" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2812950900</v>
+        <v>#N/A Requesting Data...3736635479</v>
         <stp/>
         <stp>BDP|17592946715913980887</stp>
         <tr r="F7" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2106666204</v>
+        <v>#N/A Requesting Data...2501564230</v>
         <stp/>
         <stp>BDP|12670343566891576248</stp>
         <tr r="G36" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3376317212</v>
+        <v>#N/A Requesting Data...734745559</v>
         <stp/>
         <stp>BDP|16059776447550017157</stp>
         <tr r="F63" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3298896255</v>
+        <v>#N/A Requesting Data...721339064</v>
         <stp/>
         <stp>BDP|13709786759646324310</stp>
         <tr r="F46" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1334809581</v>
+        <v>#N/A Requesting Data...1412980980</v>
         <stp/>
         <stp>BDP|17680007951225535344</stp>
         <tr r="C93" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3773611812</v>
+        <v>#N/A Requesting Data...838872620</v>
         <stp/>
         <stp>BDP|14249466628496635139</stp>
         <tr r="F26" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1331849298</v>
+        <v>#N/A Requesting Data...3110690599</v>
         <stp/>
         <stp>BDP|12616286245214000526</stp>
         <tr r="C114" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2901088649</v>
+        <v>#N/A Requesting Data...4067734432</v>
         <stp/>
         <stp>BDP|13229487552560837780</stp>
         <tr r="E139" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3736209459</v>
+        <v>#N/A Requesting Data...2370996999</v>
         <stp/>
         <stp>BDP|18412208651713792994</stp>
         <tr r="F118" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2232180673</v>
+        <v>#N/A Requesting Data...1829856501</v>
         <stp/>
         <stp>BDP|16919456577607807790</stp>
         <tr r="G56" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2707104266</v>
+        <v>#N/A Requesting Data...2602766238</v>
         <stp/>
         <stp>BDP|14958917677776306912</stp>
         <tr r="E124" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2733196753</v>
+        <v>#N/A Requesting Data...1007329525</v>
         <stp/>
         <stp>BDP|16906362551851442479</stp>
         <tr r="F14" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2408559196</v>
+        <v>#N/A Requesting Data...846132354</v>
         <stp/>
         <stp>BDP|13303498173634341154</stp>
         <tr r="G72" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3774244489</v>
+        <v>#N/A Requesting Data...2793440464</v>
         <stp/>
         <stp>BDP|11394026073756494578</stp>
         <tr r="F4" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2906645740</v>
+        <v>#N/A Requesting Data...3552590034</v>
         <stp/>
         <stp>BDP|12821707660430898618</stp>
         <tr r="C40" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2799398513</v>
+        <v>#N/A Requesting Data...3517907464</v>
         <stp/>
         <stp>BDP|12207042919767891145</stp>
         <tr r="G131" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2408606032</v>
+        <v>#N/A Requesting Data...1079518061</v>
         <stp/>
         <stp>BDP|17617562141366516571</stp>
         <tr r="F24" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1818603855</v>
+        <v>#N/A Requesting Data...3260258468</v>
         <stp/>
         <stp>BDP|13776066979946925741</stp>
         <tr r="C90" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1776370272</v>
+        <v>#N/A Requesting Data...4069297517</v>
         <stp/>
         <stp>BDP|15429465971742273156</stp>
         <tr r="E67" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3756155204</v>
+        <v>#N/A Requesting Data...3659029421</v>
         <stp/>
         <stp>BDP|13319017160191784122</stp>
         <tr r="E43" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3426447117</v>
+        <v>#N/A Requesting Data...1763276761</v>
         <stp/>
         <stp>BDP|17197570677470339052</stp>
         <tr r="E33" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1175510939</v>
+        <v>#N/A Requesting Data...3828931645</v>
         <stp/>
         <stp>BDP|18198100188843948773</stp>
         <tr r="G60" s="1"/>
@@ -2724,1783 +2739,1801 @@
     </main>
     <main first="bofaddin.rtdserver">
       <tp t="s">
-        <v>#N/A Requesting Data...2727331025</v>
+        <v>#N/A Requesting Data...3850857810</v>
         <stp/>
         <stp>BDP|3930904544763426134</stp>
         <tr r="C55" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3394084230</v>
+        <v>#N/A Requesting Data...3840038934</v>
         <stp/>
         <stp>BDP|7103625188072362707</stp>
         <tr r="E98" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3469397576</v>
+        <v>#N/A Requesting Data...1388759354</v>
         <stp/>
         <stp>BDP|9365312653090978315</stp>
         <tr r="G136" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1022650433</v>
+        <v>#N/A Requesting Data...1656475012</v>
         <stp/>
         <stp>BDP|6412151529379694002</stp>
         <tr r="F110" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3111120603</v>
+        <v>#N/A Requesting Data...1422556765</v>
         <stp/>
         <stp>BDP|6245426297947871034</stp>
         <tr r="C80" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1976312957</v>
+        <v>#N/A Requesting Data...3859937569</v>
         <stp/>
         <stp>BDP|2350385774053258906</stp>
         <tr r="F72" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...926085602</v>
+        <v>#N/A Requesting Data...3573570986</v>
         <stp/>
         <stp>BDP|8530657130876609747</stp>
         <tr r="C44" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3701373662</v>
+        <v>#N/A Requesting Data...1339043229</v>
         <stp/>
         <stp>BDP|7198979431090342164</stp>
         <tr r="E50" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2783683212</v>
+        <v>#N/A Requesting Data...1722508955</v>
         <stp/>
         <stp>BDP|9075300299347332881</stp>
         <tr r="G79" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2385792689</v>
+        <v>#N/A Requesting Data...2548627137</v>
         <stp/>
         <stp>BDP|5029740995104753357</stp>
         <tr r="C111" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3103128082</v>
+        <v>#N/A Requesting Data...1827813879</v>
         <stp/>
         <stp>BDP|8128743572863334748</stp>
         <tr r="C47" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3546821944</v>
+        <v>#N/A Requesting Data...2223087047</v>
         <stp/>
         <stp>BDP|6339719327836450907</stp>
         <tr r="C98" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4134033041</v>
+        <v>#N/A Requesting Data...2469111295</v>
         <stp/>
         <stp>BDP|4200580269163222863</stp>
         <tr r="E25" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1686326112</v>
+        <v>#N/A Requesting Data...4096192954</v>
         <stp/>
         <stp>BDP|5989352249668473659</stp>
         <tr r="G50" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1204579656</v>
+        <v>#N/A Requesting Data...1806556720</v>
         <stp/>
         <stp>BDP|2484433252649720677</stp>
         <tr r="G68" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3404497258</v>
+        <v>#N/A Requesting Data...1241414605</v>
         <stp/>
         <stp>BDP|6249870436562567333</stp>
         <tr r="E49" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3526834748</v>
+        <v>#N/A Requesting Data...1190487284</v>
         <stp/>
         <stp>BDP|9572192910556051262</stp>
         <tr r="E134" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3132778526</v>
+        <v>#N/A Requesting Data...3700882917</v>
         <stp/>
         <stp>BDP|7540551159163224910</stp>
         <tr r="F51" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2623547097</v>
+        <v>#N/A Requesting Data...3658410159</v>
         <stp/>
         <stp>BDP|8451204331587951367</stp>
         <tr r="F52" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1165311337</v>
+        <v>#N/A Requesting Data...2801672410</v>
         <stp/>
         <stp>BDP|3109256470563958869</stp>
         <tr r="C52" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3923840797</v>
+        <v>#N/A Requesting Data...2444939005</v>
         <stp/>
         <stp>BDP|3590543194827878545</stp>
         <tr r="F59" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1861664057</v>
+        <v>#N/A Requesting Data...1188735601</v>
         <stp/>
         <stp>BDP|3009997314886390075</stp>
         <tr r="G100" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1965406839</v>
+        <v>#N/A Requesting Data...3745215257</v>
         <stp/>
         <stp>BDP|4777106988391072114</stp>
         <tr r="F103" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3594293047</v>
+        <v>#N/A Requesting Data...3973868701</v>
         <stp/>
         <stp>BDP|4303401897634933024</stp>
         <tr r="E93" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1154860675</v>
+        <v>#N/A Requesting Data...1979890649</v>
         <stp/>
         <stp>BDP|9055938583773500695</stp>
         <tr r="C34" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1756978330</v>
+        <v>#N/A Requesting Data...3757163502</v>
         <stp/>
         <stp>BDP|1573317174439842142</stp>
         <tr r="E133" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3594803311</v>
+        <v>#N/A Requesting Data...2879471438</v>
         <stp/>
         <stp>BDP|7180318607099335068</stp>
         <tr r="C9" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1149212914</v>
+        <v>#N/A Requesting Data...4084744174</v>
         <stp/>
         <stp>BDP|8371873502449565411</stp>
         <tr r="C62" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3893052315</v>
+        <v>#N/A Requesting Data...2802451141</v>
         <stp/>
         <stp>BDP|9300723062997279226</stp>
         <tr r="C124" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1711342157</v>
+        <v>#N/A Requesting Data...1764868100</v>
         <stp/>
         <stp>BDP|5492561896244379063</stp>
         <tr r="F70" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2394127484</v>
+        <v>#N/A Requesting Data...3061775916</v>
         <stp/>
         <stp>BDP|8460669760190400504</stp>
         <tr r="C27" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4107052734</v>
+        <v>#N/A Requesting Data...2431591848</v>
         <stp/>
         <stp>BDP|7634975275120208406</stp>
         <tr r="C31" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4061347286</v>
+        <v>#N/A Requesting Data...1668716456</v>
         <stp/>
         <stp>BDP|4040591290066838371</stp>
         <tr r="E13" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1022489221</v>
+        <v>#N/A Requesting Data...1930496584</v>
         <stp/>
         <stp>BDP|9247766641156585153</stp>
         <tr r="G94" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3844988689</v>
+        <v>#N/A Requesting Data...1701672238</v>
         <stp/>
         <stp>BDP|7940113982976758589</stp>
         <tr r="E95" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2053460093</v>
+        <v>#N/A Requesting Data...1715920813</v>
         <stp/>
         <stp>BDP|9093620553903200797</stp>
         <tr r="C105" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2507794685</v>
+        <v>#N/A Requesting Data...2857710250</v>
         <stp/>
         <stp>BDP|2405932012622401695</stp>
         <tr r="G77" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4212958427</v>
+        <v>#N/A Requesting Data...2945886548</v>
         <stp/>
         <stp>BDP|9175353808212225665</stp>
         <tr r="C66" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2781103171</v>
+        <v>#N/A Requesting Data...2495424685</v>
         <stp/>
         <stp>BDP|1414608591110891051</stp>
         <tr r="F9" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1118439520</v>
+        <v>#N/A Requesting Data...809212008</v>
         <stp/>
         <stp>BDP|3649732806419915339</stp>
         <tr r="G14" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3875157717</v>
+        <v>#N/A Requesting Data...3458855116</v>
         <stp/>
         <stp>BDP|7006257261095505888</stp>
         <tr r="F54" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1827289789</v>
+        <v>#N/A Requesting Data...3229185616</v>
         <stp/>
         <stp>BDP|9781989741438009272</stp>
         <tr r="C39" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1553076140</v>
+        <v>#N/A Requesting Data...3563253576</v>
         <stp/>
         <stp>BDP|7532189862547338936</stp>
         <tr r="F58" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2646583815</v>
+        <v>#N/A Requesting Data...3618929613</v>
         <stp/>
         <stp>BDP|4286027170164748985</stp>
         <tr r="G113" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1999927459</v>
+        <v>#N/A Requesting Data...1847841285</v>
         <stp/>
         <stp>BDP|4691882821088256816</stp>
         <tr r="F126" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3962320771</v>
+        <v>#N/A Requesting Data...3886490395</v>
         <stp/>
         <stp>BDP|4974055815239706225</stp>
         <tr r="G110" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2257383469</v>
+        <v>#N/A Requesting Data...2173408838</v>
         <stp/>
         <stp>BDP|5916130291376545539</stp>
         <tr r="F73" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1723801070</v>
+        <v>#N/A Requesting Data...3363748330</v>
         <stp/>
         <stp>BDP|9535646277681935723</stp>
         <tr r="E60" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1053486970</v>
+        <v>#N/A Requesting Data...1784209331</v>
         <stp/>
         <stp>BDP|3472420329653378814</stp>
         <tr r="G4" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4250003407</v>
+        <v>#N/A Requesting Data...1958007647</v>
         <stp/>
         <stp>BDP|9676580711333862054</stp>
         <tr r="E135" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1144925420</v>
+        <v>#N/A Requesting Data...1534071596</v>
         <stp/>
         <stp>BDP|8651287802994649096</stp>
         <tr r="E77" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2245709272</v>
+        <v>#N/A Requesting Data...1456143147</v>
         <stp/>
         <stp>BDP|5552297197720045083</stp>
         <tr r="E118" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3515874432</v>
+        <v>#N/A Requesting Data...3996748132</v>
         <stp/>
         <stp>BDP|6195991527552839107</stp>
         <tr r="C61" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1391259373</v>
+        <v>#N/A Requesting Data...1020712784</v>
         <stp/>
         <stp>BDP|2785537291931900199</stp>
         <tr r="G91" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1176780584</v>
+        <v>#N/A Requesting Data...1867597406</v>
         <stp/>
         <stp>BDP|9875435960971965593</stp>
         <tr r="C11" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1431745509</v>
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDP|5969741853480600831</stp>
+        <tr r="E140" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A Requesting Data...2688645981</v>
         <stp/>
         <stp>BDP|7662972721973338089</stp>
         <tr r="F107" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3166759234</v>
+        <v>#N/A Requesting Data...2641994697</v>
         <stp/>
         <stp>BDP|4282903616430488389</stp>
         <tr r="G9" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1023033824</v>
+        <v>#N/A Requesting Data...1456911352</v>
         <stp/>
         <stp>BDP|6606398548307737925</stp>
         <tr r="C70" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2797223997</v>
+        <v>#N/A Requesting Data...3771140410</v>
         <stp/>
         <stp>BDP|2310021551041423963</stp>
         <tr r="F123" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1317809506</v>
+        <v>#N/A Requesting Data...3522025354</v>
         <stp/>
         <stp>BDP|1666950877162018261</stp>
         <tr r="E87" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2532162132</v>
+        <v>#N/A Requesting Data...3061400763</v>
         <stp/>
         <stp>BDP|6280569068792932854</stp>
         <tr r="C46" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3014623750</v>
+        <v>#N/A Requesting Data...1749681525</v>
         <stp/>
         <stp>BDP|9635152443296662577</stp>
         <tr r="C16" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3611279966</v>
+        <v>#N/A Requesting Data...3166443068</v>
         <stp/>
         <stp>BDP|5935740968278021330</stp>
         <tr r="C96" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3001066428</v>
+        <v>#N/A Requesting Data...3805962936</v>
         <stp/>
         <stp>BDP|8225387168083679130</stp>
         <tr r="E57" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2573523342</v>
+        <v>#N/A Requesting Data...2444643324</v>
         <stp/>
         <stp>BDP|8741792397660502982</stp>
         <tr r="G24" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1872000869</v>
+        <v>#N/A Requesting Data...1827678087</v>
         <stp/>
         <stp>BDP|1988621838892198978</stp>
         <tr r="F82" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1710253681</v>
+        <v>#N/A Requesting Data...4005314878</v>
         <stp/>
         <stp>BDP|5160947801244572083</stp>
         <tr r="C97" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3588919471</v>
+        <v>#N/A Requesting Data...3015630725</v>
         <stp/>
         <stp>BDP|8781684350665372626</stp>
         <tr r="G64" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3705754329</v>
+        <v>#N/A Requesting Data...2364846878</v>
         <stp/>
         <stp>BDP|8866465832365619258</stp>
         <tr r="F120" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2527269560</v>
+        <v>#N/A Requesting Data...3282035768</v>
         <stp/>
         <stp>BDP|1231973558974048121</stp>
         <tr r="E123" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4158310343</v>
+        <v>#N/A Requesting Data...1282592653</v>
         <stp/>
         <stp>BDP|9011959145835954962</stp>
         <tr r="E102" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1305271102</v>
+        <v>#N/A Requesting Data...3055012476</v>
         <stp/>
         <stp>BDP|7048111723254898858</stp>
         <tr r="E70" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1870375580</v>
+        <v>#N/A Requesting Data...2706477691</v>
         <stp/>
         <stp>BDP|7514426398370500271</stp>
         <tr r="F84" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3082589301</v>
+        <v>#N/A Requesting Data...2912707837</v>
         <stp/>
         <stp>BDP|2286847884578687294</stp>
         <tr r="C64" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3628541858</v>
+        <v>#N/A Requesting Data...3383613311</v>
         <stp/>
         <stp>BDP|8581359335587083771</stp>
         <tr r="G40" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1678783429</v>
+        <v>#N/A Requesting Data...3057584243</v>
         <stp/>
         <stp>BDP|9176352611073152053</stp>
         <tr r="G52" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3267488575</v>
+        <v>#N/A Requesting Data...1607815042</v>
         <stp/>
         <stp>BDP|3761613276703138977</stp>
         <tr r="C22" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3424891929</v>
+        <v>#N/A Requesting Data...2684974837</v>
         <stp/>
         <stp>BDP|2402283480247992710</stp>
         <tr r="G65" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2181488559</v>
+        <v>#N/A Requesting Data...1711933552</v>
         <stp/>
         <stp>BDP|2496054182730824314</stp>
         <tr r="F108" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2672340844</v>
+        <v>#N/A Requesting Data...3760375771</v>
         <stp/>
         <stp>BDP|1156198294412416234</stp>
         <tr r="G48" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3154316309</v>
+        <v>#N/A Requesting Data...3090064044</v>
         <stp/>
         <stp>BDP|1935863512592400318</stp>
         <tr r="G99" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4207117172</v>
+        <v>#N/A Requesting Data...1520524639</v>
         <stp/>
         <stp>BDP|1182070188629538920</stp>
         <tr r="F85" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1652031140</v>
+        <v>#N/A Requesting Data...2925929779</v>
         <stp/>
         <stp>BDP|9924697901094165296</stp>
         <tr r="E38" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3122451235</v>
+        <v>#N/A Requesting Data...2975857228</v>
         <stp/>
         <stp>BDP|6412137247758825261</stp>
         <tr r="G10" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2610301546</v>
+        <v>#N/A Requesting Data...4155990218</v>
         <stp/>
         <stp>BDP|6277108296426856136</stp>
         <tr r="G122" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3146360697</v>
+        <v>#N/A Requesting Data...885960325</v>
         <stp/>
         <stp>BDP|2351176324921816947</stp>
         <tr r="E117" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3021808606</v>
+        <v>#N/A Requesting Data...1271039753</v>
         <stp/>
         <stp>BDP|6406207188846485346</stp>
         <tr r="C37" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2404879933</v>
+        <v>#N/A Requesting Data...4005841240</v>
         <stp/>
         <stp>BDP|8112280367483097628</stp>
         <tr r="F16" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3849162750</v>
+        <v>#N/A Requesting Data...2048804741</v>
         <stp/>
         <stp>BDP|6484624822372932905</stp>
         <tr r="C108" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1480836978</v>
+        <v>#N/A Requesting Data...943375044</v>
         <stp/>
         <stp>BDP|8605875253514357834</stp>
         <tr r="C116" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2846135076</v>
+        <v>#N/A Requesting Data...2693908349</v>
         <stp/>
         <stp>BDP|2842991807747556512</stp>
         <tr r="E110" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3997622004</v>
+        <v>#N/A Requesting Data...1510681133</v>
         <stp/>
         <stp>BDP|1377759003508711718</stp>
         <tr r="E55" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3602119377</v>
+        <v>#N/A Requesting Data...2374925903</v>
         <stp/>
         <stp>BDP|1711361391887412536</stp>
         <tr r="G47" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1106757324</v>
+        <v>#N/A Requesting Data...2948989596</v>
         <stp/>
         <stp>BDP|4564815655442574234</stp>
         <tr r="F114" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2924476806</v>
+        <v>#N/A Requesting Data...1752702899</v>
         <stp/>
         <stp>BDP|6557751567646791843</stp>
         <tr r="C85" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2756606523</v>
+        <v>#N/A Requesting Data...2637631557</v>
         <stp/>
         <stp>BDP|5018226780961297742</stp>
         <tr r="E138" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4178849923</v>
+        <v>#N/A Requesting Data...3509800840</v>
         <stp/>
         <stp>BDP|7190582290036507495</stp>
         <tr r="E48" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1732374999</v>
+        <v>#N/A Requesting Data...1075507266</v>
         <stp/>
         <stp>BDP|7268732641219205478</stp>
         <tr r="F111" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1863628724</v>
+        <v>#N/A Requesting Data...3696721765</v>
         <stp/>
         <stp>BDP|5085458293997400582</stp>
         <tr r="C30" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2148530865</v>
+        <v>#N/A Requesting Data...2894195234</v>
         <stp/>
         <stp>BDP|2916061605678582044</stp>
         <tr r="E27" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4100172937</v>
+        <v>#N/A Requesting Data...873557922</v>
         <stp/>
         <stp>BDP|5645196194854205325</stp>
         <tr r="E19" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2487667593</v>
+        <v>#N/A Requesting Data...1245764625</v>
         <stp/>
         <stp>BDP|8929421222763426766</stp>
         <tr r="F112" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3075798682</v>
+        <v>#N/A Requesting Data...2068505916</v>
         <stp/>
         <stp>BDP|2815946348173965667</stp>
         <tr r="C137" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4177915846</v>
+        <v>#N/A Requesting Data...3908828213</v>
         <stp/>
         <stp>BDP|6645611732949919042</stp>
         <tr r="G95" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2031421965</v>
+        <v>#N/A Requesting Data...1755901299</v>
         <stp/>
         <stp>BDP|8744658502964028082</stp>
         <tr r="F139" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1206120917</v>
+        <v>#N/A Requesting Data...1984985695</v>
         <stp/>
         <stp>BDP|4077907452745230782</stp>
         <tr r="C130" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1533734711</v>
+        <v>#N/A Requesting Data...1766206147</v>
         <stp/>
         <stp>BDP|8975856381415089739</stp>
         <tr r="E75" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3822890546</v>
+        <v>#N/A Requesting Data...1764133455</v>
         <stp/>
         <stp>BDP|5738611839292209825</stp>
         <tr r="G107" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1057063411</v>
+        <v>#N/A Requesting Data...2367795726</v>
         <stp/>
         <stp>BDP|4996818111432201578</stp>
         <tr r="G134" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1840669000</v>
+        <v>#N/A Requesting Data...1814994336</v>
         <stp/>
         <stp>BDP|5458032582021895609</stp>
         <tr r="E89" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1228053102</v>
+        <v>#N/A Requesting Data...4263993066</v>
         <stp/>
         <stp>BDP|2612461303954522846</stp>
         <tr r="F21" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1508415142</v>
+        <v>#N/A Requesting Data...3004267743</v>
         <stp/>
         <stp>BDP|5852840000806674187</stp>
         <tr r="F75" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4260141196</v>
+        <v>#N/A Requesting Data...3815707830</v>
         <stp/>
         <stp>BDP|7947641811679527399</stp>
         <tr r="G13" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3590410220</v>
+        <v>#N/A Requesting Data...2344847530</v>
         <stp/>
         <stp>BDP|8407769428857900025</stp>
         <tr r="C132" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1164840577</v>
+        <v>#N/A Requesting Data...3319638468</v>
         <stp/>
         <stp>BDP|1313714864639868399</stp>
         <tr r="F87" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2744629790</v>
+        <v>#N/A Requesting Data...2131904760</v>
         <stp/>
         <stp>BDP|2531298252748844733</stp>
         <tr r="F115" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4182257036</v>
+        <v>#N/A Requesting Data...3104546847</v>
         <stp/>
         <stp>BDP|8965389266391509672</stp>
         <tr r="C41" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1433806424</v>
+        <v>#N/A Requesting Data...2081606004</v>
         <stp/>
         <stp>BDP|9146373380128430189</stp>
         <tr r="F60" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3097899368</v>
+        <v>#N/A Requesting Data...2681722967</v>
         <stp/>
         <stp>BDP|8769626454200391097</stp>
         <tr r="G85" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3980675632</v>
+        <v>#N/A Requesting Data...3810025657</v>
         <stp/>
         <stp>BDP|7701346097304455298</stp>
         <tr r="C73" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2902250834</v>
+        <v>#N/A Requesting Data...1817145433</v>
         <stp/>
         <stp>BDP|1201589979318261083</stp>
         <tr r="G123" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1334208987</v>
+        <v>#N/A Requesting Data...3347766849</v>
         <stp/>
         <stp>BDP|9994425762708075853</stp>
         <tr r="G88" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3943546061</v>
+        <v>#N/A Requesting Data...4061502689</v>
         <stp/>
         <stp>BDP|8238868892513701135</stp>
         <tr r="G137" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2767408278</v>
+        <v>#N/A Requesting Data...2282656091</v>
         <stp/>
         <stp>BDP|3321556007464177923</stp>
         <tr r="E109" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1657793333</v>
+        <v>#N/A Requesting Data...4158125882</v>
         <stp/>
         <stp>BDP|8367368187378355023</stp>
         <tr r="F64" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3516445936</v>
+        <v>#N/A Requesting Data...3915728486</v>
         <stp/>
         <stp>BDP|9054142235387080711</stp>
         <tr r="F11" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3552445822</v>
+        <v>#N/A Requesting Data...1624640732</v>
         <stp/>
         <stp>BDP|4797724273716399932</stp>
         <tr r="C5" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2440245122</v>
+        <v>#N/A Requesting Data...4057517051</v>
         <stp/>
         <stp>BDP|3084971212582403246</stp>
         <tr r="F121" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2102966773</v>
+        <v>#N/A Requesting Data...1312127835</v>
         <stp/>
         <stp>BDP|6948762204713990690</stp>
         <tr r="G90" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2626905824</v>
+        <v>#N/A Requesting Data...3029217342</v>
         <stp/>
         <stp>BDP|1832764578595986067</stp>
         <tr r="G119" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2347142622</v>
+        <v>#N/A Requesting Data...4038191518</v>
         <stp/>
         <stp>BDP|4156639623951685595</stp>
         <tr r="F13" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1340310894</v>
+        <v>#N/A Requesting Data...4102794281</v>
         <stp/>
         <stp>BDP|5919761437851372455</stp>
         <tr r="C2" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1954444459</v>
+        <v>#N/A Requesting Data...1358497038</v>
         <stp/>
         <stp>BDP|1551339666687413790</stp>
         <tr r="F40" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3441090535</v>
+        <v>#N/A Requesting Data...2670256419</v>
         <stp/>
         <stp>BDP|6420437202397070174</stp>
         <tr r="C8" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3465503458</v>
+        <v>#N/A Requesting Data...1270340641</v>
         <stp/>
         <stp>BDP|1708381902825815365</stp>
         <tr r="C101" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3479364666</v>
+        <v>#N/A Requesting Data...3598803370</v>
         <stp/>
         <stp>BDP|4945796250777738578</stp>
         <tr r="G21" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1229188527</v>
+        <v>#N/A Requesting Data...3677289348</v>
         <stp/>
         <stp>BDP|6746841414412327938</stp>
         <tr r="G75" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2277334616</v>
+        <v>#N/A Requesting Data...3616959773</v>
         <stp/>
         <stp>BDP|1709445403856801620</stp>
         <tr r="E85" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3075479161</v>
+        <v>#N/A Requesting Data...3174812154</v>
         <stp/>
         <stp>BDP|9398823419477440265</stp>
         <tr r="G125" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4014427710</v>
+        <v>#N/A Requesting Data...1320066910</v>
         <stp/>
         <stp>BDP|3430878723724827801</stp>
         <tr r="G41" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3933771267</v>
+        <v>#N/A Requesting Data...2910428025</v>
         <stp/>
         <stp>BDP|9698422803149077198</stp>
         <tr r="C100" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4162538041</v>
+        <v>#N/A Requesting Data...1483107005</v>
         <stp/>
         <stp>BDP|2887002514665714363</stp>
         <tr r="G59" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4216082074</v>
+        <v>#N/A Requesting Data...1086310647</v>
         <stp/>
         <stp>BDP|2668814054578766269</stp>
         <tr r="E31" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3355096869</v>
+        <v>#N/A Requesting Data...1301896798</v>
         <stp/>
         <stp>BDP|8894702939828266110</stp>
         <tr r="C7" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3172213387</v>
+        <v>#N/A Requesting Data...1459666417</v>
         <stp/>
         <stp>BDP|3410885660260666884</stp>
         <tr r="E64" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2076228531</v>
+        <v>#N/A Requesting Data...1425345845</v>
         <stp/>
         <stp>BDP|3658713905400418152</stp>
         <tr r="E35" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1735758125</v>
+        <v>#N/A Requesting Data...3998841534</v>
         <stp/>
         <stp>BDP|7570300716478486864</stp>
         <tr r="E32" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2894807428</v>
+        <v>#N/A Requesting Data...2494179008</v>
         <stp/>
         <stp>BDP|7851492951527237434</stp>
         <tr r="E52" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1215115936</v>
+        <v>#N/A Requesting Data...3165015246</v>
         <stp/>
         <stp>BDP|7352242467910007671</stp>
         <tr r="F124" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1635082211</v>
+        <v>#N/A Requesting Data...2295407790</v>
         <stp/>
         <stp>BDP|5657563513753480721</stp>
         <tr r="E80" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1887572155</v>
+        <v>#N/A Requesting Data...3425980426</v>
         <stp/>
         <stp>BDP|5976587264538865878</stp>
         <tr r="E62" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2771406075</v>
+        <v>#N/A Requesting Data...3040842551</v>
         <stp/>
         <stp>BDP|7151318027339523982</stp>
         <tr r="F91" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1299753417</v>
+        <v>#N/A Requesting Data...2067863983</v>
         <stp/>
         <stp>BDP|1896477110772260049</stp>
         <tr r="C91" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3662492062</v>
+        <v>#N/A Requesting Data...3395888376</v>
         <stp/>
         <stp>BDP|4252725967471187287</stp>
         <tr r="F44" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3458385674</v>
+        <v>#N/A Requesting Data...4191973330</v>
         <stp/>
         <stp>BDP|6943451920864586278</stp>
         <tr r="C118" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2731442523</v>
+        <v>#N/A Requesting Data...3188764126</v>
         <stp/>
         <stp>BDP|5838113265174067025</stp>
         <tr r="F39" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2951691625</v>
+        <v>#N/A Requesting Data...1144095221</v>
         <stp/>
         <stp>BDP|3456718228377624745</stp>
         <tr r="E111" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3735917319</v>
+        <v>#N/A Requesting Data...2651678235</v>
         <stp/>
         <stp>BDP|5917425194519245724</stp>
         <tr r="E79" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3879921229</v>
+        <v>#N/A Requesting Data...3081932147</v>
         <stp/>
         <stp>BDP|6787533358407016713</stp>
         <tr r="F135" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3221302262</v>
+        <v>#N/A Requesting Data...1282679593</v>
         <stp/>
         <stp>BDP|5576451913756991076</stp>
         <tr r="E16" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3355508793</v>
+        <v>#N/A Requesting Data...2263949882</v>
         <stp/>
         <stp>BDP|5284390591628042184</stp>
         <tr r="C24" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2535033016</v>
+        <v>#N/A Requesting Data...2450691228</v>
         <stp/>
         <stp>BDP|5412037028917536689</stp>
         <tr r="G115" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2923859301</v>
+        <v>#N/A Requesting Data...3231309567</v>
         <stp/>
         <stp>BDP|8966942938724477029</stp>
         <tr r="C15" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2570792258</v>
+        <v>#N/A Requesting Data...2781431614</v>
         <stp/>
         <stp>BDP|2938144706552859709</stp>
         <tr r="G81" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2158750819</v>
+        <v>#N/A Requesting Data...1097446561</v>
         <stp/>
         <stp>BDP|3632949480676633244</stp>
         <tr r="F31" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2366472739</v>
+        <v>#N/A Requesting Data...1494195449</v>
         <stp/>
         <stp>BDP|3513418606797579639</stp>
         <tr r="F90" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1252653849</v>
+        <v>#N/A Requesting Data...1207117214</v>
         <stp/>
         <stp>BDP|1733520919261908213</stp>
         <tr r="G73" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1991946178</v>
+        <v>#N/A Requesting Data...3843936070</v>
         <stp/>
         <stp>BDP|8368969127023380651</stp>
         <tr r="F28" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1994329449</v>
+        <v>#N/A Requesting Data...3138415599</v>
         <stp/>
         <stp>BDP|7172716621593553717</stp>
         <tr r="F53" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1799713148</v>
+        <v>#N/A Requesting Data...2530182526</v>
         <stp/>
         <stp>BDP|2954250373819174944</stp>
         <tr r="F119" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2701451378</v>
+        <v>#N/A Requesting Data...1211631174</v>
         <stp/>
         <stp>BDP|4728287753511799518</stp>
         <tr r="F3" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2616390358</v>
+        <v>#N/A Requesting Data...3805354439</v>
         <stp/>
         <stp>BDP|6348617969513327227</stp>
         <tr r="E104" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2349831583</v>
+        <v>#N/A Requesting Data...2272394103</v>
         <stp/>
         <stp>BDP|7694099704858685831</stp>
         <tr r="C107" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2168569663</v>
+        <v>#N/A Requesting Data...3889924940</v>
         <stp/>
         <stp>BDP|4106834752526835861</stp>
         <tr r="F55" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2140354661</v>
+        <v>#N/A Requesting Data...3117517842</v>
         <stp/>
         <stp>BDP|7951337561756108354</stp>
         <tr r="G112" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2104216016</v>
+        <v>#N/A Requesting Data...1455830185</v>
         <stp/>
         <stp>BDP|5468867501418549294</stp>
         <tr r="E86" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2119800775</v>
+        <v>#N/A Requesting Data...3341686779</v>
         <stp/>
         <stp>BDP|4546740053823447251</stp>
         <tr r="C32" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4004815144</v>
+        <v>#N/A Requesting Data...3505825017</v>
         <stp/>
         <stp>BDP|7484527599745538990</stp>
         <tr r="F76" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3862809776</v>
+        <v>#N/A Requesting Data...2301857210</v>
         <stp/>
         <stp>BDP|5578475423865159117</stp>
         <tr r="E61" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2001238928</v>
+        <v>#N/A Requesting Data...4097924273</v>
         <stp/>
         <stp>BDP|6158107237024797760</stp>
         <tr r="E45" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1637209549</v>
+        <v>#N/A Requesting Data...2638158749</v>
         <stp/>
         <stp>BDP|4143076943390197735</stp>
         <tr r="F97" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3838783310</v>
+        <v>#N/A Requesting Data...1242675291</v>
         <stp/>
         <stp>BDP|1762196091349932721</stp>
         <tr r="E82" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3117289232</v>
+        <v>#N/A Requesting Data...3482660034</v>
         <stp/>
         <stp>BDP|4189169184528349241</stp>
         <tr r="F137" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1575386176</v>
+        <v>#N/A Requesting Data...1240918565</v>
         <stp/>
         <stp>BDP|9103140635044368872</stp>
         <tr r="F29" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3097946235</v>
+        <v>#N/A Requesting Data...2979363983</v>
         <stp/>
         <stp>BDP|5519603296584718917</stp>
         <tr r="G54" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4024402692</v>
+        <v>#N/A Requesting Data...3607224321</v>
         <stp/>
         <stp>BDP|1156250824766982737</stp>
         <tr r="G44" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1946063998</v>
+        <v>#N/A Requesting Data...3643064057</v>
         <stp/>
         <stp>BDP|6031605254431729496</stp>
         <tr r="G86" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4182790043</v>
+        <v>#N/A Requesting Data...2227040547</v>
         <stp/>
         <stp>BDP|2649489454114394728</stp>
         <tr r="C14" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3463239265</v>
+        <v>#N/A Requesting Data...2554160395</v>
         <stp/>
         <stp>BDP|8999377595616850481</stp>
         <tr r="E108" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1988601098</v>
+        <v>#N/A Requesting Data...3636534756</v>
         <stp/>
         <stp>BDP|8988928209665280487</stp>
         <tr r="F71" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2196146068</v>
+        <v>#N/A Requesting Data...2079920517</v>
         <stp/>
         <stp>BDP|8368023487691952119</stp>
         <tr r="F88" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3216386302</v>
+        <v>#N/A Requesting Data...4060178811</v>
         <stp/>
         <stp>BDP|5199287207907438042</stp>
         <tr r="E66" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2883282124</v>
+        <v>#N/A Requesting Data...3313275961</v>
         <stp/>
         <stp>BDP|7460099446995728631</stp>
         <tr r="F134" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4198625966</v>
+        <v>#N/A Requesting Data...2312576859</v>
         <stp/>
         <stp>BDP|6160638673325976246</stp>
         <tr r="C104" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3089767102</v>
+        <v>#N/A Requesting Data...1853080294</v>
         <stp/>
         <stp>BDP|5660731962530222490</stp>
         <tr r="E128" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2928019945</v>
+        <v>#N/A Requesting Data...2841630111</v>
         <stp/>
         <stp>BDP|3355023726294311595</stp>
         <tr r="G114" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4065198363</v>
+        <v>#N/A Requesting Data...2920637192</v>
         <stp/>
         <stp>BDP|5604474461391860653</stp>
         <tr r="E130" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3497403082</v>
+        <v>#N/A Requesting Data...2857206261</v>
         <stp/>
         <stp>BDP|3542140114402066179</stp>
         <tr r="E78" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1267651342</v>
+        <v>#N/A Requesting Data...4081039713</v>
         <stp/>
         <stp>BDP|2942496252996870592</stp>
         <tr r="G121" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2547610678</v>
+        <v>#N/A Requesting Data...2533566179</v>
         <stp/>
         <stp>BDP|1823820926283534897</stp>
         <tr r="G18" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2417641207</v>
+        <v>#N/A Requesting Data...3996444994</v>
         <stp/>
         <stp>BDP|3716189405712826043</stp>
         <tr r="G92" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1466778176</v>
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDP|3228146609442097080</stp>
+        <tr r="C140" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A Requesting Data...3457981722</v>
         <stp/>
         <stp>BDP|9344147089140006098</stp>
         <tr r="E83" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2303917904</v>
+        <v>#N/A Requesting Data...4167042075</v>
         <stp/>
         <stp>BDP|6993061706081965773</stp>
         <tr r="F81" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3637701902</v>
+        <v>#N/A Requesting Data...2949027126</v>
         <stp/>
         <stp>BDP|6176792116871092198</stp>
         <tr r="C68" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2314867240</v>
+        <v>#N/A Requesting Data...3521126179</v>
         <stp/>
         <stp>BDP|7185432584822399912</stp>
         <tr r="F131" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3035948909</v>
+        <v>#N/A Requesting Data...3455908174</v>
         <stp/>
         <stp>BDP|8280856169194643320</stp>
         <tr r="G49" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2959079165</v>
+        <v>#N/A Requesting Data...2923300990</v>
         <stp/>
         <stp>BDP|9399109618929306123</stp>
         <tr r="F37" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4122086889</v>
+        <v>#N/A Requesting Data...3077051607</v>
         <stp/>
         <stp>BDP|6669663699409638145</stp>
         <tr r="C123" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1358779554</v>
+        <v>#N/A Requesting Data...2158535965</v>
         <stp/>
         <stp>BDP|6175693122901836298</stp>
         <tr r="C36" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2453935214</v>
+        <v>#N/A Requesting Data...1198607382</v>
         <stp/>
         <stp>BDP|8135075327118072391</stp>
         <tr r="C17" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3051695071</v>
+        <v>#N/A Requesting Data...2179139113</v>
         <stp/>
         <stp>BDP|5726291712345411206</stp>
         <tr r="G28" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1812782546</v>
+        <v>#N/A Requesting Data...4239908784</v>
         <stp/>
         <stp>BDP|8698973352783506690</stp>
         <tr r="F25" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4089768435</v>
+        <v>#N/A Requesting Data...2318547612</v>
         <stp/>
         <stp>BDP|5493604681742158862</stp>
         <tr r="G63" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3255617641</v>
+        <v>#N/A Requesting Data...1246532595</v>
         <stp/>
         <stp>BDP|3239104742287612040</stp>
         <tr r="E39" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2331974078</v>
+        <v>#N/A Requesting Data...4072869786</v>
         <stp/>
         <stp>BDP|3381147726641663059</stp>
         <tr r="C122" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3775107553</v>
+        <v>#N/A Requesting Data...3802330131</v>
         <stp/>
         <stp>BDP|6625906764329795167</stp>
         <tr r="F56" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3976825629</v>
+        <v>#N/A Requesting Data...3418195065</v>
         <stp/>
         <stp>BDP|3325218238213801010</stp>
         <tr r="F57" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3666614196</v>
+        <v>#N/A Requesting Data...2758475650</v>
         <stp/>
         <stp>BDP|1313137390988032037</stp>
         <tr r="C83" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4089098358</v>
+        <v>#N/A Requesting Data...1875467233</v>
         <stp/>
         <stp>BDP|3702733300853619616</stp>
         <tr r="G34" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3353833600</v>
+        <v>#N/A Requesting Data...1105296424</v>
         <stp/>
         <stp>BDP|8558611930018338475</stp>
         <tr r="F35" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1540250816</v>
+        <v>#N/A Requesting Data...4255201935</v>
         <stp/>
         <stp>BDP|5387098906493173798</stp>
         <tr r="G62" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2809671660</v>
+        <v>#N/A Requesting Data...3789769220</v>
         <stp/>
         <stp>BDP|1951038018907673608</stp>
         <tr r="C126" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1584502165</v>
+        <v>#N/A Requesting Data...2009334446</v>
         <stp/>
         <stp>BDP|9253802402770546012</stp>
         <tr r="F74" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1559483381</v>
+        <v>#N/A Requesting Data...3695275716</v>
         <stp/>
         <stp>BDP|1884505914021260664</stp>
         <tr r="E96" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2181878407</v>
+        <v>#N/A Requesting Data...2679831280</v>
         <stp/>
         <stp>BDP|3540127028674193608</stp>
         <tr r="F94" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1439146934</v>
+        <v>#N/A Requesting Data...2628704940</v>
         <stp/>
         <stp>BDP|5372375359741187031</stp>
         <tr r="F27" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3733774018</v>
+        <v>#N/A Requesting Data...1194205678</v>
         <stp/>
         <stp>BDP|5121625602631825066</stp>
         <tr r="E81" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1779878902</v>
+        <v>#N/A Requesting Data...1903778350</v>
         <stp/>
         <stp>BDP|5282708515920897138</stp>
         <tr r="F43" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4253634506</v>
+        <v>#N/A Requesting Data...1853388977</v>
         <stp/>
         <stp>BDP|1250299291741371958</stp>
         <tr r="G31" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2664372200</v>
+        <v>#N/A Requesting Data...2883616175</v>
         <stp/>
         <stp>BDP|4253176148933327033</stp>
         <tr r="C133" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2538457450</v>
+        <v>#N/A Requesting Data...1728374499</v>
         <stp/>
         <stp>BDP|9704751602229087502</stp>
         <tr r="F49" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3059613740</v>
+        <v>#N/A Requesting Data...3761824224</v>
         <stp/>
         <stp>BDP|6775233901286469015</stp>
         <tr r="E125" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3925342105</v>
+        <v>#N/A Requesting Data...2339955902</v>
         <stp/>
         <stp>BDP|7918289416910309647</stp>
         <tr r="C56" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1622341238</v>
+        <v>#N/A Requesting Data...3501091081</v>
         <stp/>
         <stp>BDP|3731272815900600241</stp>
         <tr r="C53" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3868104692</v>
+        <v>#N/A Requesting Data...3421836247</v>
         <stp/>
         <stp>BDP|1685459166489439868</stp>
         <tr r="F133" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1573328955</v>
+        <v>#N/A Requesting Data...3203319780</v>
         <stp/>
         <stp>BDP|2506644172580171154</stp>
         <tr r="C119" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2573619609</v>
+        <v>#N/A Requesting Data...1392842394</v>
         <stp/>
         <stp>BDP|1995353227627490580</stp>
         <tr r="E119" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2762439276</v>
+        <v>#N/A Requesting Data...3300623214</v>
         <stp/>
         <stp>BDP|9173868178561206592</stp>
         <tr r="C77" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3595389252</v>
+        <v>#N/A Requesting Data...1149555560</v>
         <stp/>
         <stp>BDP|4008096672221657096</stp>
         <tr r="G43" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2686239611</v>
+        <v>#N/A Requesting Data...1498338613</v>
         <stp/>
         <stp>BDP|5434663182001395869</stp>
         <tr r="E107" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1811344438</v>
+        <v>#N/A Requesting Data...4257408197</v>
         <stp/>
         <stp>BDP|8686279502629263146</stp>
         <tr r="C129" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4089089057</v>
+        <v>#N/A Requesting Data...2322562648</v>
         <stp/>
         <stp>BDP|4576300957588172984</stp>
         <tr r="E63" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4091265158</v>
+        <v>#N/A Requesting Data...1113118131</v>
         <stp/>
         <stp>BDP|7469671678835895086</stp>
         <tr r="E2" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3347393839</v>
+        <v>#N/A Requesting Data...2104394279</v>
         <stp/>
         <stp>BDP|5444751401066968714</stp>
         <tr r="E73" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3998234338</v>
+        <v>#N/A Requesting Data...4286367257</v>
         <stp/>
         <stp>BDP|2824124077350027748</stp>
         <tr r="E136" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3350912821</v>
+        <v>#N/A Requesting Data...2494334552</v>
         <stp/>
         <stp>BDP|3708851985886704699</stp>
         <tr r="C19" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2128474931</v>
+        <v>#N/A Requesting Data...1635770335</v>
         <stp/>
         <stp>BDP|1006071828475585561</stp>
         <tr r="F116" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2251406108</v>
+        <v>#N/A Requesting Data...3531987168</v>
         <stp/>
         <stp>BDP|1086712249007771639</stp>
         <tr r="G26" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1341345012</v>
+        <v>#N/A Requesting Data...4074378601</v>
         <stp/>
         <stp>BDP|6634730869724168016</stp>
         <tr r="E103" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3335019231</v>
+        <v>#N/A Requesting Data...2457924617</v>
         <stp/>
         <stp>BDP|3520366017777816505</stp>
         <tr r="E97" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2858242821</v>
+        <v>#N/A Requesting Data...1070287254</v>
         <stp/>
         <stp>BDP|2995135217932647367</stp>
         <tr r="F105" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4009096432</v>
+        <v>#N/A Requesting Data...3458541308</v>
         <stp/>
         <stp>BDP|3565057922625094707</stp>
         <tr r="G45" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1499626222</v>
+        <v>#N/A Requesting Data...1637723018</v>
         <stp/>
         <stp>BDP|1485569542807651461</stp>
         <tr r="C86" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1641679392</v>
+        <v>#N/A Requesting Data...2581743270</v>
         <stp/>
         <stp>BDP|1159006460850353421</stp>
         <tr r="E46" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2381067368</v>
+        <v>#N/A Requesting Data...1468506262</v>
         <stp/>
         <stp>BDP|5113311422502283510</stp>
         <tr r="C84" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3737774190</v>
+        <v>#N/A Requesting Data...2887735648</v>
         <stp/>
         <stp>BDP|4420649803735408460</stp>
         <tr r="F117" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3738988072</v>
+        <v>#N/A Requesting Data...1132838510</v>
         <stp/>
         <stp>BDP|9873235984695079585</stp>
         <tr r="C60" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2134975838</v>
+        <v>#N/A Requesting Data...2291847032</v>
         <stp/>
         <stp>BDP|4726106605717010168</stp>
         <tr r="G46" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2212294188</v>
+        <v>#N/A Requesting Data...3644448675</v>
         <stp/>
         <stp>BDP|97453184744598227</stp>
         <tr r="G135" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1828175249</v>
+        <v>#N/A Requesting Data...3995124466</v>
         <stp/>
         <stp>BDP|71129432364790944</stp>
         <tr r="E105" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3033783327</v>
+        <v>#N/A Requesting Data...2277765017</v>
         <stp/>
         <stp>BDP|13870968378316918</stp>
         <tr r="F38" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2741793585</v>
+        <v>#N/A Requesting Data...1550402552</v>
         <stp/>
         <stp>BDP|545017254499479967</stp>
         <tr r="E23" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3716650867</v>
+        <v>#N/A Requesting Data...1126631800</v>
         <stp/>
         <stp>BDP|562457211792430265</stp>
         <tr r="G116" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3411242957</v>
+        <v>#N/A Requesting Data...2958597565</v>
         <stp/>
         <stp>BDP|752318736222262646</stp>
         <tr r="F83" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3528149954</v>
+        <v>#N/A Requesting Data...1210056363</v>
         <stp/>
         <stp>BDP|926433161397617222</stp>
         <tr r="F10" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2776715399</v>
+        <v>#N/A Requesting Data...1077243446</v>
         <stp/>
         <stp>BDP|455507803480864317</stp>
         <tr r="C51" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2475219447</v>
+        <v>#N/A Requesting Data...1253044260</v>
         <stp/>
         <stp>BDP|738430784972633891</stp>
         <tr r="F41" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4226533763</v>
+        <v>#N/A Requesting Data...1222853957</v>
         <stp/>
         <stp>BDP|226270545351892196</stp>
         <tr r="F61" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2432726566</v>
+        <v>#N/A Requesting Data...2647917022</v>
         <stp/>
         <stp>BDP|478534605105814154</stp>
         <tr r="G12" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3323054151</v>
+        <v>#N/A Requesting Data...3633834868</v>
         <stp/>
         <stp>BDP|292697057297288557</stp>
         <tr r="C106" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1893602444</v>
+        <v>#N/A Requesting Data...1105510249</v>
         <stp/>
         <stp>BDP|449489448517477649</stp>
         <tr r="E99" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3827928223</v>
+        <v>#N/A Requesting Data...4135670200</v>
         <stp/>
         <stp>BDP|477239144286521179</stp>
         <tr r="G138" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4066961521</v>
+        <v>#N/A Requesting Data...2022772395</v>
         <stp/>
         <stp>BDP|136361134742057301</stp>
         <tr r="C57" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1650874791</v>
+        <v>#N/A Requesting Data...2556838060</v>
         <stp/>
         <stp>BDP|282958180978155995</stp>
         <tr r="C59" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2760594673</v>
+        <v>#N/A Requesting Data...2329102317</v>
         <stp/>
         <stp>BDP|991366924295531418</stp>
         <tr r="F2" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2989963216</v>
+        <v>#N/A Requesting Data...2027401332</v>
         <stp/>
         <stp>BDP|934073235795196633</stp>
         <tr r="F62" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2613645715</v>
+        <v>#N/A Requesting Data...3530671686</v>
         <stp/>
         <stp>BDP|266608211912165570</stp>
         <tr r="E113" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1514658076</v>
+        <v>#N/A Requesting Data...3113665726</v>
         <stp/>
         <stp>BDP|910156400954699593</stp>
         <tr r="G8" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4218781255</v>
+        <v>#N/A Requesting Data...3974993112</v>
         <stp/>
         <stp>BDP|794293317440269040</stp>
         <tr r="E100" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4170043361</v>
+        <v>#N/A Requesting Data...4077776812</v>
         <stp/>
         <stp>BDP|206766873121157269</stp>
         <tr r="E41" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1277386705</v>
+        <v>#N/A Requesting Data...4081095894</v>
         <stp/>
         <stp>BDP|315261912951356153</stp>
         <tr r="E21" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2792120261</v>
+        <v>#N/A Requesting Data...4029829725</v>
         <stp/>
         <stp>BDP|169080827246056602</stp>
         <tr r="G126" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1312504474</v>
+        <v>#N/A Requesting Data...3787822754</v>
         <stp/>
         <stp>BDP|454779781439338455</stp>
         <tr r="E36" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2733342501</v>
+        <v>#N/A Requesting Data...4207164293</v>
         <stp/>
         <stp>BDP|198524097739196711</stp>
         <tr r="F92" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1863689732</v>
+        <v>#N/A Requesting Data...1339984719</v>
         <stp/>
         <stp>BDP|618726407191106421</stp>
         <tr r="C92" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2353097160</v>
+        <v>#N/A Requesting Data...1964109500</v>
         <stp/>
         <stp>BDP|442808307356626303</stp>
         <tr r="F20" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3020667434</v>
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDP|624014897144495064</stp>
+        <tr r="G140" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A Requesting Data...2417705575</v>
         <stp/>
         <stp>BDP|304889655090792147</stp>
         <tr r="E58" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4256471264</v>
+        <v>#N/A Requesting Data...2198712958</v>
         <stp/>
         <stp>BDP|427627592191043219</stp>
         <tr r="C87" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2010843953</v>
+        <v>#N/A Requesting Data...2078385749</v>
         <stp/>
         <stp>BDP|768711067038142524</stp>
         <tr r="G25" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1970087866</v>
+        <v>#N/A Requesting Data...3144113388</v>
         <stp/>
         <stp>BDP|447365482187669383</stp>
         <tr r="C95" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4174105932</v>
+        <v>#N/A Requesting Data...3489956823</v>
         <stp/>
         <stp>BDP|901925773788783965</stp>
         <tr r="G67" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2038077141</v>
+        <v>#N/A Requesting Data...3317480784</v>
         <stp/>
         <stp>BDP|511429594874391764</stp>
         <tr r="G117" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1840664924</v>
+        <v>#N/A Requesting Data...4071104396</v>
         <stp/>
         <stp>BDP|544620567958067604</stp>
         <tr r="C131" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3613747412</v>
+        <v>#N/A Requesting Data...2770898833</v>
         <stp/>
         <stp>BDP|945569483354328027</stp>
         <tr r="C21" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2487445068</v>
+        <v>#N/A Requesting Data...4015290613</v>
         <stp/>
         <stp>BDP|691281527639744142</stp>
         <tr r="E8" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1314054133</v>
+        <v>#N/A Requesting Data...3627187458</v>
         <stp/>
         <stp>BDP|968314719543295935</stp>
         <tr r="E68" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2220147352</v>
+        <v>#N/A Requesting Data...3908949143</v>
         <stp/>
         <stp>BDP|760426044168153386</stp>
         <tr r="G7" s="1"/>
@@ -4807,10 +4840,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FDB3339-948E-458F-BDF3-DE9E0EAF9A7A}">
-  <dimension ref="A1:E139"/>
+  <dimension ref="A1:E140"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="A113" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:E140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5112,7 +5145,7 @@
         <v>162</v>
       </c>
       <c r="C18" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="D18" t="s">
         <v>318</v>
@@ -5302,7 +5335,7 @@
         <v>328</v>
       </c>
       <c r="D29" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="E29" t="s">
         <v>284</v>
@@ -5455,7 +5488,7 @@
         <v>310</v>
       </c>
       <c r="D38" t="s">
-        <v>287</v>
+        <v>303</v>
       </c>
       <c r="E38" t="s">
         <v>303</v>
@@ -5557,7 +5590,7 @@
         <v>334</v>
       </c>
       <c r="D44" t="s">
-        <v>309</v>
+        <v>331</v>
       </c>
       <c r="E44" t="s">
         <v>331</v>
@@ -5639,7 +5672,7 @@
         <v>71</v>
       </c>
       <c r="C49" t="s">
-        <v>335</v>
+        <v>310</v>
       </c>
       <c r="D49" t="s">
         <v>313</v>
@@ -5696,7 +5729,7 @@
         <v>298</v>
       </c>
       <c r="E52" t="s">
-        <v>284</v>
+        <v>298</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
@@ -6019,7 +6052,7 @@
         <v>285</v>
       </c>
       <c r="E71" t="s">
-        <v>306</v>
+        <v>313</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.3">
@@ -6135,7 +6168,7 @@
         <v>285</v>
       </c>
       <c r="D78" t="s">
-        <v>287</v>
+        <v>355</v>
       </c>
       <c r="E78" t="s">
         <v>285</v>
@@ -6237,7 +6270,7 @@
         <v>286</v>
       </c>
       <c r="D84" t="s">
-        <v>285</v>
+        <v>291</v>
       </c>
       <c r="E84" t="s">
         <v>301</v>
@@ -6251,7 +6284,7 @@
         <v>110</v>
       </c>
       <c r="C85" t="s">
-        <v>302</v>
+        <v>311</v>
       </c>
       <c r="D85" t="s">
         <v>301</v>
@@ -6693,7 +6726,7 @@
         <v>82</v>
       </c>
       <c r="C111" t="s">
-        <v>286</v>
+        <v>310</v>
       </c>
       <c r="D111" t="s">
         <v>287</v>
@@ -6784,7 +6817,7 @@
         <v>338</v>
       </c>
       <c r="E116" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.3">
@@ -7176,6 +7209,23 @@
       </c>
       <c r="E139" t="s">
         <v>333</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A140">
+        <v>612</v>
+      </c>
+      <c r="B140" t="s">
+        <v>353</v>
+      </c>
+      <c r="C140" t="s">
+        <v>285</v>
+      </c>
+      <c r="D140" t="s">
+        <v>285</v>
+      </c>
+      <c r="E140" t="s">
+        <v>285</v>
       </c>
     </row>
   </sheetData>
@@ -7185,10 +7235,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5352835-5CFD-46EC-8CDA-5672A55A22F5}">
-  <dimension ref="A1:G139"/>
+  <dimension ref="A1:G140"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="J117" sqref="J117"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G140" sqref="E2:G140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7669,7 +7719,7 @@
       </c>
       <c r="E18" t="str">
         <f>_xll.BDP(D18,"RTG_MDY_FC_CURR_ISSUER_RATING")</f>
-        <v>A3</v>
+        <v>Baa1</v>
       </c>
       <c r="F18" t="str">
         <f>_xll.BDP(D18,"RTG_SP_LT_FC_ISSUER_CREDIT")</f>
@@ -7970,7 +8020,7 @@
       </c>
       <c r="F29" t="str">
         <f>_xll.BDP(D29,"RTG_SP_LT_FC_ISSUER_CREDIT")</f>
-        <v>BB-</v>
+        <v>BB</v>
       </c>
       <c r="G29" t="str">
         <f>_xll.BDP(D29,"RTG_FITCH_LT_ISSUER_DEFAULT")</f>
@@ -8213,7 +8263,7 @@
       </c>
       <c r="F38" t="str">
         <f>_xll.BDP(D38,"RTG_SP_LT_FC_ISSUER_CREDIT")</f>
-        <v>B-</v>
+        <v>B</v>
       </c>
       <c r="G38" t="str">
         <f>_xll.BDP(D38,"RTG_FITCH_LT_ISSUER_DEFAULT")</f>
@@ -8375,7 +8425,7 @@
       </c>
       <c r="F44" t="str">
         <f>_xll.BDP(D44,"RTG_SP_LT_FC_ISSUER_CREDIT")</f>
-        <v>AA-u</v>
+        <v>A+u</v>
       </c>
       <c r="G44" t="str">
         <f>_xll.BDP(D44,"RTG_FITCH_LT_ISSUER_DEFAULT")</f>
@@ -8506,7 +8556,7 @@
       </c>
       <c r="E49" t="str">
         <f>_xll.BDP(D49,"RTG_MDY_FC_CURR_ISSUER_RATING")</f>
-        <v>Caa2</v>
+        <v>Caa1</v>
       </c>
       <c r="F49" t="str">
         <f>_xll.BDP(D49,"RTG_SP_LT_FC_ISSUER_CREDIT")</f>
@@ -8595,7 +8645,7 @@
       </c>
       <c r="G52" t="str">
         <f>_xll.BDP(D52,"RTG_FITCH_LT_ISSUER_DEFAULT")</f>
-        <v>BB</v>
+        <v>BB+</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
@@ -9108,7 +9158,7 @@
       </c>
       <c r="G71" t="str">
         <f>_xll.BDP(D71,"RTG_FITCH_LT_ISSUER_DEFAULT")</f>
-        <v>WD</v>
+        <v>CCC+</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.3">
@@ -9293,7 +9343,7 @@
       </c>
       <c r="F78" t="str">
         <f>_xll.BDP(D78,"RTG_SP_LT_FC_ISSUER_CREDIT")</f>
-        <v>B-</v>
+        <v>B- *-</v>
       </c>
       <c r="G78" t="str">
         <f>_xll.BDP(D78,"RTG_FITCH_LT_ISSUER_DEFAULT")</f>
@@ -9455,7 +9505,7 @@
       </c>
       <c r="F84" t="str">
         <f>_xll.BDP(D84,"RTG_SP_LT_FC_ISSUER_CREDIT")</f>
-        <v>#N/A N/A</v>
+        <v>BB-</v>
       </c>
       <c r="G84" t="str">
         <f>_xll.BDP(D84,"RTG_FITCH_LT_ISSUER_DEFAULT")</f>
@@ -9478,7 +9528,7 @@
       </c>
       <c r="E85" t="str">
         <f>_xll.BDP(D85,"RTG_MDY_FC_CURR_ISSUER_RATING")</f>
-        <v>B2</v>
+        <v>B1</v>
       </c>
       <c r="F85" t="str">
         <f>_xll.BDP(D85,"RTG_SP_LT_FC_ISSUER_CREDIT")</f>
@@ -10180,7 +10230,7 @@
       </c>
       <c r="E111" t="str">
         <f>_xll.BDP(D111,"RTG_MDY_FC_CURR_ISSUER_RATING")</f>
-        <v>B3</v>
+        <v>Caa1</v>
       </c>
       <c r="F111" t="str">
         <f>_xll.BDP(D111,"RTG_SP_LT_FC_ISSUER_CREDIT")</f>
@@ -10323,7 +10373,7 @@
       </c>
       <c r="G116" t="str">
         <f>_xll.BDP(D116,"RTG_FITCH_LT_ISSUER_DEFAULT")</f>
-        <v>A</v>
+        <v>A+</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.3">
@@ -10945,6 +10995,33 @@
       <c r="G139" t="str">
         <f>_xll.BDP(D139,"RTG_FITCH_LT_ISSUER_DEFAULT")</f>
         <v>RD</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A140">
+        <v>612</v>
+      </c>
+      <c r="B140" t="s">
+        <v>353</v>
+      </c>
+      <c r="C140" t="str">
+        <f>_xll.BDP(D140,"issuer")</f>
+        <v>People's Democratic Republic o</v>
+      </c>
+      <c r="D140" t="s">
+        <v>354</v>
+      </c>
+      <c r="E140" t="str">
+        <f>_xll.BDP(D140,"RTG_MDY_FC_CURR_ISSUER_RATING")</f>
+        <v>#N/A N/A</v>
+      </c>
+      <c r="F140" t="str">
+        <f>_xll.BDP(D140,"RTG_SP_LT_FC_ISSUER_CREDIT")</f>
+        <v>#N/A N/A</v>
+      </c>
+      <c r="G140" t="str">
+        <f>_xll.BDP(D140,"RTG_FITCH_LT_ISSUER_DEFAULT")</f>
+        <v>#N/A N/A</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cleaned up clean rating file where live ratings update
</commit_message>
<xml_diff>
--- a/index_bbg_rating_live.xlsx
+++ b/index_bbg_rating_live.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kaimin Khaw\Desktop\credit-rating-deploy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BBB445D-0338-48E1-835D-2ACB32098003}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6799922-4C01-46EF-BD85-1138BE784013}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-72" windowWidth="23256" windowHeight="12456" xr2:uid="{2A12413E-A5EC-426E-A187-DE07F52921C3}"/>
   </bookViews>
@@ -1201,1537 +1201,1537 @@
   <volType type="realTimeData">
     <main first="bofaddin.rtdserver">
       <tp t="s">
-        <v>#N/A Requesting Data...3469221504</v>
+        <v>#N/A Requesting Data...3169024748</v>
         <stp/>
         <stp>BDP|13719527809048657439</stp>
         <tr r="E3" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4026000411</v>
+        <v>#N/A Requesting Data...3454770539</v>
         <stp/>
         <stp>BDP|12363409739849183621</stp>
         <tr r="G98" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2097201990</v>
+        <v>#N/A Requesting Data...4157186516</v>
         <stp/>
         <stp>BDP|17606584297068117917</stp>
         <tr r="G105" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2483144695</v>
+        <v>#N/A Requesting Data...3046608927</v>
         <stp/>
         <stp>BDP|12825277506793769973</stp>
         <tr r="F22" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...757932436</v>
+        <v>#N/A Requesting Data...3415747369</v>
         <stp/>
         <stp>BDP|13615906068526188051</stp>
         <tr r="G101" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2190318939</v>
+        <v>#N/A Requesting Data...4247325692</v>
         <stp/>
         <stp>BDP|10912677687245148127</stp>
         <tr r="G106" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1280301803</v>
+        <v>#N/A Requesting Data...3444800029</v>
         <stp/>
         <stp>BDP|16221541486007837625</stp>
         <tr r="G58" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2281158124</v>
+        <v>#N/A Requesting Data...2871368196</v>
         <stp/>
         <stp>BDP|14989839765876665645</stp>
         <tr r="C81" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3291580075</v>
+        <v>#N/A Requesting Data...3897785055</v>
         <stp/>
         <stp>BDP|16792452589360294083</stp>
         <tr r="E11" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3282485542</v>
+        <v>#N/A Requesting Data...2815873736</v>
         <stp/>
         <stp>BDP|16409240184993364568</stp>
         <tr r="E54" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2991655323</v>
+        <v>#N/A Requesting Data...3477816444</v>
         <stp/>
         <stp>BDP|12376141866138693768</stp>
         <tr r="C88" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2534845178</v>
+        <v>#N/A Requesting Data...3532471041</v>
         <stp/>
         <stp>BDP|13146963289471890960</stp>
         <tr r="C18" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3321695672</v>
+        <v>#N/A Requesting Data...2752980938</v>
         <stp/>
         <stp>BDP|10167725043130019931</stp>
         <tr r="C110" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1389474271</v>
+        <v>#N/A Requesting Data...3415553964</v>
         <stp/>
         <stp>BDP|10589422899161895655</stp>
         <tr r="G76" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...802018258</v>
+        <v>#N/A Requesting Data...3921218378</v>
         <stp/>
         <stp>BDP|15228795190517586693</stp>
         <tr r="E84" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1569896394</v>
+        <v>#N/A Requesting Data...3862396385</v>
         <stp/>
         <stp>BDP|10096201946458505444</stp>
         <tr r="G97" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1857433059</v>
+        <v>#N/A Requesting Data...4071916570</v>
         <stp/>
         <stp>BDP|18253401034836307331</stp>
         <tr r="F99" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3676881851</v>
+        <v>#N/A Requesting Data...2857464855</v>
         <stp/>
         <stp>BDP|10867273920449518201</stp>
         <tr r="G71" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2557369291</v>
+        <v>#N/A Requesting Data...3975568440</v>
         <stp/>
         <stp>BDP|14811872563886412749</stp>
         <tr r="E114" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...762284618</v>
+        <v>#N/A Requesting Data...3826187803</v>
         <stp/>
         <stp>BDP|15237334583701669483</stp>
         <tr r="C112" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3509488155</v>
+        <v>#N/A Requesting Data...3413778382</v>
         <stp/>
         <stp>BDP|14006145231309322495</stp>
         <tr r="C65" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1584714792</v>
+        <v>#N/A Requesting Data...3096508782</v>
         <stp/>
         <stp>BDP|14761213634019822741</stp>
         <tr r="G2" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2474911944</v>
+        <v>#N/A Requesting Data...2923010925</v>
         <stp/>
         <stp>BDP|15399231330039360601</stp>
         <tr r="E42" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2929906347</v>
+        <v>#N/A Requesting Data...3754607053</v>
         <stp/>
         <stp>BDP|11120752607359953480</stp>
         <tr r="G61" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3548035795</v>
+        <v>#N/A Requesting Data...2910576014</v>
         <stp/>
         <stp>BDP|15939978441203902037</stp>
         <tr r="C26" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2772966588</v>
+        <v>#N/A Requesting Data...3323887298</v>
         <stp/>
         <stp>BDP|18066043829836356791</stp>
         <tr r="G78" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1167331241</v>
+        <v>#N/A Requesting Data...3319137471</v>
         <stp/>
         <stp>BDP|14168806967588813989</stp>
         <tr r="F77" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2262806649</v>
+        <v>#N/A Requesting Data...4034318730</v>
         <stp/>
         <stp>BDP|18397803367339867766</stp>
         <tr r="F101" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3394163086</v>
+        <v>#N/A Requesting Data...3762330008</v>
         <stp/>
         <stp>BDP|15895803206017416271</stp>
         <tr r="C33" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2787318579</v>
+        <v>#N/A Requesting Data...3939846505</v>
         <stp/>
         <stp>BDP|14908732543227691836</stp>
         <tr r="E94" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3208314582</v>
+        <v>#N/A Requesting Data...4002764499</v>
         <stp/>
         <stp>BDP|12957817799052931996</stp>
         <tr r="E120" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1878838918</v>
+        <v>#N/A Requesting Data...4181579624</v>
         <stp/>
         <stp>BDP|16275205432289392600</stp>
         <tr r="E101" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1170960444</v>
+        <v>#N/A Requesting Data...3791290922</v>
         <stp/>
         <stp>BDP|10407655300028223605</stp>
         <tr r="F47" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3712458942</v>
+        <v>#N/A Requesting Data...3217139057</v>
         <stp/>
         <stp>BDP|14031612538318230186</stp>
         <tr r="C136" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1207156183</v>
+        <v>#N/A Requesting Data...2982598901</v>
         <stp/>
         <stp>BDP|13840587393604095357</stp>
         <tr r="G3" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2827354773</v>
+        <v>#N/A Requesting Data...3010194101</v>
         <stp/>
         <stp>BDP|18397555740376217727</stp>
         <tr r="F17" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3785788442</v>
+        <v>#N/A Requesting Data...3663879244</v>
         <stp/>
         <stp>BDP|15886108592084595196</stp>
         <tr r="F19" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3313793692</v>
+        <v>#N/A Requesting Data...2821146643</v>
         <stp/>
         <stp>BDP|12574943311804341655</stp>
         <tr r="C58" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3435445995</v>
+        <v>#N/A Requesting Data...3515045440</v>
         <stp/>
         <stp>BDP|15276164033266227932</stp>
         <tr r="C121" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2799197514</v>
+        <v>#N/A Requesting Data...3820255812</v>
         <stp/>
         <stp>BDP|11413915902765857449</stp>
         <tr r="C135" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3127246163</v>
+        <v>#N/A Requesting Data...2956951133</v>
         <stp/>
         <stp>BDP|10888161880627674738</stp>
         <tr r="G74" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1701006661</v>
+        <v>#N/A Requesting Data...4066336386</v>
         <stp/>
         <stp>BDP|18252264749434830399</stp>
         <tr r="E91" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2776621519</v>
+        <v>#N/A Requesting Data...3860793368</v>
         <stp/>
         <stp>BDP|16230814927561165496</stp>
         <tr r="C25" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1837621096</v>
+        <v>#N/A Requesting Data...3090564398</v>
         <stp/>
         <stp>BDP|11669407615485914850</stp>
         <tr r="E28" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3184069362</v>
+        <v>#N/A Requesting Data...3388685810</v>
         <stp/>
         <stp>BDP|15385895124225473341</stp>
         <tr r="F89" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1073077122</v>
+        <v>#N/A Requesting Data...3276375672</v>
         <stp/>
         <stp>BDP|16215575297831427265</stp>
         <tr r="G19" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1457582627</v>
+        <v>#N/A Requesting Data...4232904491</v>
         <stp/>
         <stp>BDP|15664489079057139842</stp>
         <tr r="C50" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3358140717</v>
+        <v>#N/A Requesting Data...4246721084</v>
         <stp/>
         <stp>BDP|13556466380534139208</stp>
         <tr r="C63" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3878905229</v>
+        <v>#N/A Requesting Data...3376041502</v>
         <stp/>
         <stp>BDP|12426034393664290636</stp>
         <tr r="G70" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...503387570</v>
+        <v>#N/A Requesting Data...3180365275</v>
         <stp/>
         <stp>BDP|11206974657257798316</stp>
         <tr r="G5" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1371457682</v>
+        <v>#N/A Requesting Data...3192198335</v>
         <stp/>
         <stp>BDP|15687672872765725835</stp>
         <tr r="G133" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4156172873</v>
+        <v>#N/A Requesting Data...3247180735</v>
         <stp/>
         <stp>BDP|10646340980557108540</stp>
         <tr r="G83" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3731788715</v>
+        <v>#N/A Requesting Data...3259840774</v>
         <stp/>
         <stp>BDP|13932387258969800286</stp>
         <tr r="G30" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3815902941</v>
+        <v>#N/A Requesting Data...3143603435</v>
         <stp/>
         <stp>BDP|14685689793557045247</stp>
         <tr r="G11" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1303460890</v>
+        <v>#N/A Requesting Data...3562854848</v>
         <stp/>
         <stp>BDP|11792528289940283264</stp>
         <tr r="G39" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2017370435</v>
+        <v>#N/A Requesting Data...3563042370</v>
         <stp/>
         <stp>BDP|14038814629908297802</stp>
         <tr r="E14" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3361837077</v>
+        <v>#N/A Requesting Data...3093063234</v>
         <stp/>
         <stp>BDP|17960836852555549100</stp>
         <tr r="F79" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3121777466</v>
+        <v>#N/A Requesting Data...4011781052</v>
         <stp/>
         <stp>BDP|12258786923690042954</stp>
         <tr r="G82" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3259998277</v>
+        <v>#N/A Requesting Data...2928859117</v>
         <stp/>
         <stp>BDP|11831892951331348329</stp>
         <tr r="C35" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3162529413</v>
+        <v>#N/A Requesting Data...2816163740</v>
         <stp/>
         <stp>BDP|12634554786653062247</stp>
         <tr r="F34" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1012669930</v>
+        <v>#N/A Requesting Data...2836464449</v>
         <stp/>
         <stp>BDP|10304787173197381988</stp>
         <tr r="G53" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1749506975</v>
+        <v>#N/A Requesting Data...4190046560</v>
         <stp/>
         <stp>BDP|15772343051115104818</stp>
         <tr r="C127" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1660206629</v>
+        <v>#N/A Requesting Data...3939486405</v>
         <stp/>
         <stp>BDP|13619322587163510542</stp>
         <tr r="C45" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1747990127</v>
+        <v>#N/A Requesting Data...3999939583</v>
         <stp/>
         <stp>BDP|13709828003397613269</stp>
         <tr r="C54" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3607852767</v>
+        <v>#N/A Requesting Data...2906689535</v>
         <stp/>
         <stp>BDP|11596891797659679653</stp>
         <tr r="C89" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1483074579</v>
+        <v>#N/A Requesting Data...3786349852</v>
         <stp/>
         <stp>BDP|18339290641951108002</stp>
         <tr r="E17" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3846379806</v>
+        <v>#N/A Requesting Data...3941902385</v>
         <stp/>
         <stp>BDP|10418265688390464525</stp>
         <tr r="E18" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1118672302</v>
+        <v>#N/A Requesting Data...3956039544</v>
         <stp/>
         <stp>BDP|14859691791600738447</stp>
         <tr r="F45" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3191517874</v>
+        <v>#N/A Requesting Data...2818578487</v>
         <stp/>
         <stp>BDP|18255708956124343152</stp>
         <tr r="E26" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2962769239</v>
+        <v>#N/A Requesting Data...3735647976</v>
         <stp/>
         <stp>BDP|16855823919014233436</stp>
         <tr r="F30" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1436410056</v>
+        <v>#N/A Requesting Data...4245777978</v>
         <stp/>
         <stp>BDP|12821872971201299383</stp>
         <tr r="G124" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3454449464</v>
+        <v>#N/A Requesting Data...2819088141</v>
         <stp/>
         <stp>BDP|11466185903217969815</stp>
         <tr r="F33" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4153861783</v>
+        <v>#N/A Requesting Data...3383365178</v>
         <stp/>
         <stp>BDP|13711300257260836914</stp>
         <tr r="C102" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4236355901</v>
+        <v>#N/A Requesting Data...3773537080</v>
         <stp/>
         <stp>BDP|11622318103537999967</stp>
         <tr r="F15" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1459584173</v>
+        <v>#N/A Requesting Data...4259437884</v>
         <stp/>
         <stp>BDP|10597445640754361898</stp>
         <tr r="F50" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1059002892</v>
+        <v>#N/A Requesting Data...3492351927</v>
         <stp/>
         <stp>BDP|13987588094432951117</stp>
         <tr r="E127" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1642178506</v>
+        <v>#N/A Requesting Data...3379090880</v>
         <stp/>
         <stp>BDP|11655961067423868102</stp>
         <tr r="G104" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3039541095</v>
+        <v>#N/A Requesting Data...3885354248</v>
         <stp/>
         <stp>BDP|12468839190466923900</stp>
         <tr r="C20" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1670756863</v>
+        <v>#N/A Requesting Data...2876959041</v>
         <stp/>
         <stp>BDP|18411047804853597705</stp>
         <tr r="C67" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2543208507</v>
+        <v>#N/A Requesting Data...3788542110</v>
         <stp/>
         <stp>BDP|18331339124097518219</stp>
         <tr r="F66" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...931586932</v>
+        <v>#N/A Requesting Data...3156494521</v>
         <stp/>
         <stp>BDP|14983531083496973331</stp>
         <tr r="G132" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2464608095</v>
+        <v>#N/A Requesting Data...3689978251</v>
         <stp/>
         <stp>BDP|14115869171127460078</stp>
         <tr r="G37" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2691967196</v>
+        <v>#N/A Requesting Data...3802898741</v>
         <stp/>
         <stp>BDP|16963038037211063893</stp>
         <tr r="C13" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...733555754</v>
+        <v>#N/A Requesting Data...3013156018</v>
         <stp/>
         <stp>BDP|13900268704084418991</stp>
         <tr r="E37" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2564141710</v>
+        <v>#N/A Requesting Data...3138083324</v>
         <stp/>
         <stp>BDP|16311230542528118454</stp>
         <tr r="E9" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...818461321</v>
+        <v>#N/A Requesting Data...4040829898</v>
         <stp/>
         <stp>BDP|12403550728001134908</stp>
         <tr r="G38" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3577817020</v>
+        <v>#N/A Requesting Data...3319490089</v>
         <stp/>
         <stp>BDP|10528694388950747396</stp>
         <tr r="F80" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3462870917</v>
+        <v>#N/A Requesting Data...2996484203</v>
         <stp/>
         <stp>BDP|17962073596443790028</stp>
         <tr r="F23" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3433140974</v>
+        <v>#N/A Requesting Data...3133802233</v>
         <stp/>
         <stp>BDP|11322749828038387103</stp>
         <tr r="E122" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1893436700</v>
+        <v>#N/A Requesting Data...4002452249</v>
         <stp/>
         <stp>BDP|14872467854648029062</stp>
         <tr r="C75" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2179592472</v>
+        <v>#N/A Requesting Data...4150298252</v>
         <stp/>
         <stp>BDP|14951668809329151689</stp>
         <tr r="E56" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1214829725</v>
+        <v>#N/A Requesting Data...3233027446</v>
         <stp/>
         <stp>BDP|14211231849266296941</stp>
         <tr r="G103" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...786205641</v>
+        <v>#N/A Requesting Data...3110478502</v>
         <stp/>
         <stp>BDP|15282935006718574931</stp>
         <tr r="E92" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2042873640</v>
+        <v>#N/A Requesting Data...3375661308</v>
         <stp/>
         <stp>BDP|16389940868391785591</stp>
         <tr r="C120" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4224485094</v>
+        <v>#N/A Requesting Data...3075968681</v>
         <stp/>
         <stp>BDP|10830300668358540045</stp>
         <tr r="C115" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1050533426</v>
+        <v>#N/A Requesting Data...3909493355</v>
         <stp/>
         <stp>BDP|15417892931237679498</stp>
         <tr r="F8" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2674341264</v>
+        <v>#N/A Requesting Data...3647338079</v>
         <stp/>
         <stp>BDP|13776760394691002167</stp>
         <tr r="C4" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2382557114</v>
+        <v>#N/A Requesting Data...4242600319</v>
         <stp/>
         <stp>BDP|12950924085148446689</stp>
         <tr r="E121" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1236128874</v>
+        <v>#N/A Requesting Data...3107739492</v>
         <stp/>
         <stp>BDP|11202744698684518690</stp>
         <tr r="G111" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2976688885</v>
+        <v>#N/A Requesting Data...4267024094</v>
         <stp/>
         <stp>BDP|11005719894013994183</stp>
         <tr r="C3" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2501659359</v>
+        <v>#N/A Requesting Data...3141276551</v>
         <stp/>
         <stp>BDP|17061881470574956177</stp>
         <tr r="C69" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4006309743</v>
+        <v>#N/A Requesting Data...3593348451</v>
         <stp/>
         <stp>BDP|10195299258766033392</stp>
         <tr r="E90" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2753041888</v>
+        <v>#N/A Requesting Data...3300668784</v>
         <stp/>
         <stp>BDP|17559180385128709479</stp>
         <tr r="E15" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1243850635</v>
+        <v>#N/A Requesting Data...3861692323</v>
         <stp/>
         <stp>BDP|10477087317801173223</stp>
         <tr r="F125" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4094783320</v>
+        <v>#N/A Requesting Data...3628460517</v>
         <stp/>
         <stp>BDP|10431478218456128129</stp>
         <tr r="G32" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3409683099</v>
+        <v>#N/A Requesting Data...3970745357</v>
         <stp/>
         <stp>BDP|12817533695869473568</stp>
         <tr r="C82" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2229016864</v>
+        <v>#N/A Requesting Data...3470837373</v>
         <stp/>
         <stp>BDP|16722436137983528090</stp>
         <tr r="F127" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3260889302</v>
+        <v>#N/A Requesting Data...3255553430</v>
         <stp/>
         <stp>BDP|14949322880769358496</stp>
         <tr r="G16" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1404786241</v>
+        <v>#N/A Requesting Data...3187242500</v>
         <stp/>
         <stp>BDP|12620594347341901004</stp>
         <tr r="C76" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1450782809</v>
+        <v>#N/A Requesting Data...4012962888</v>
         <stp/>
         <stp>BDP|12047021516217693612</stp>
         <tr r="E126" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1585734847</v>
+        <v>#N/A Requesting Data...3072435057</v>
         <stp/>
         <stp>BDP|13612225533853005354</stp>
         <tr r="F102" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3220350261</v>
+        <v>#N/A Requesting Data...2902811659</v>
         <stp/>
         <stp>BDP|11536436753390219250</stp>
         <tr r="F129" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3868495510</v>
+        <v>#N/A Requesting Data...4249202340</v>
         <stp/>
         <stp>BDP|12946334758336119017</stp>
         <tr r="E72" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...929939509</v>
+        <v>#N/A Requesting Data...3933356524</v>
         <stp/>
         <stp>BDP|17733998071078953332</stp>
         <tr r="C23" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2759974875</v>
+        <v>#N/A Requesting Data...3454534798</v>
         <stp/>
         <stp>BDP|16362559715466602618</stp>
         <tr r="F68" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1260071379</v>
+        <v>#N/A Requesting Data...4209082666</v>
         <stp/>
         <stp>BDP|16070475881909673177</stp>
         <tr r="E112" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4149285303</v>
+        <v>#N/A Requesting Data...4038256577</v>
         <stp/>
         <stp>BDP|17590878194950224438</stp>
         <tr r="G87" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2513603988</v>
+        <v>#N/A Requesting Data...4159713325</v>
         <stp/>
         <stp>BDP|12427007793358727164</stp>
         <tr r="F100" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4101415419</v>
+        <v>#N/A Requesting Data...3427904631</v>
         <stp/>
         <stp>BDP|15601293270144483737</stp>
         <tr r="G15" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2177398823</v>
+        <v>#N/A Requesting Data...3210233234</v>
         <stp/>
         <stp>BDP|13723200346810339697</stp>
         <tr r="C38" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2253547025</v>
+        <v>#N/A Requesting Data...3422141446</v>
         <stp/>
         <stp>BDP|18086118189074176643</stp>
         <tr r="E88" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...886130094</v>
+        <v>#N/A Requesting Data...3184897849</v>
         <stp/>
         <stp>BDP|15679917748483251829</stp>
         <tr r="E6" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2510287358</v>
+        <v>#N/A Requesting Data...3564461410</v>
         <stp/>
         <stp>BDP|13421293548936861023</stp>
         <tr r="G66" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4116093787</v>
+        <v>#N/A Requesting Data...4122251898</v>
         <stp/>
         <stp>BDP|10594946509929542325</stp>
         <tr r="F5" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1606588796</v>
+        <v>#N/A Requesting Data...4290174979</v>
         <stp/>
         <stp>BDP|10668212108445960480</stp>
         <tr r="G57" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1488733058</v>
+        <v>#N/A Requesting Data...2992697103</v>
         <stp/>
         <stp>BDP|10103273213286136651</stp>
         <tr r="C6" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2015787689</v>
+        <v>#N/A Requesting Data...3673564600</v>
         <stp/>
         <stp>BDP|11259721862376480554</stp>
         <tr r="G69" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3867433897</v>
+        <v>#N/A Requesting Data...2895943437</v>
         <stp/>
         <stp>BDP|14885566279524266176</stp>
         <tr r="E30" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...789410965</v>
+        <v>#N/A Requesting Data...3425083770</v>
         <stp/>
         <stp>BDP|14519079130534129014</stp>
         <tr r="C49" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2424556266</v>
+        <v>#N/A Requesting Data...4285835930</v>
         <stp/>
         <stp>BDP|14873136635550817546</stp>
         <tr r="G130" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2290211675</v>
+        <v>#N/A Requesting Data...4233084838</v>
         <stp/>
         <stp>BDP|16641457892301341972</stp>
         <tr r="F130" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2734710752</v>
+        <v>#N/A Requesting Data...3906385456</v>
         <stp/>
         <stp>BDP|13231746637163726724</stp>
         <tr r="E7" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1649949747</v>
+        <v>#N/A Requesting Data...3748137646</v>
         <stp/>
         <stp>BDP|12945735048800380256</stp>
         <tr r="G118" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2926127580</v>
+        <v>#N/A Requesting Data...3424349519</v>
         <stp/>
         <stp>BDP|11265248170961260631</stp>
         <tr r="E47" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...820339038</v>
+        <v>#N/A Requesting Data...3673330270</v>
         <stp/>
         <stp>BDP|16351851074029385080</stp>
         <tr r="G35" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1838918113</v>
+        <v>#N/A Requesting Data...3755280555</v>
         <stp/>
         <stp>BDP|11944358991052271970</stp>
         <tr r="C103" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1612516393</v>
+        <v>#N/A Requesting Data...3358106653</v>
         <stp/>
         <stp>BDP|18410981990650283866</stp>
         <tr r="C99" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2218487944</v>
+        <v>#N/A Requesting Data...3560174233</v>
         <stp/>
         <stp>BDP|14383773052580838655</stp>
         <tr r="F104" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3369478515</v>
+        <v>#N/A Requesting Data...4199415284</v>
         <stp/>
         <stp>BDP|10871340643964419300</stp>
         <tr r="F95" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1840230434</v>
+        <v>#N/A Requesting Data...3674658209</v>
         <stp/>
         <stp>BDP|14690280185656044816</stp>
         <tr r="C94" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2178095358</v>
+        <v>#N/A Requesting Data...4009751490</v>
         <stp/>
         <stp>BDP|18305693996456795112</stp>
         <tr r="G80" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2642890408</v>
+        <v>#N/A Requesting Data...3401430470</v>
         <stp/>
         <stp>BDP|16273225567973824127</stp>
         <tr r="C79" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4201411901</v>
+        <v>#N/A Requesting Data...3137138059</v>
         <stp/>
         <stp>BDP|13313129291618997350</stp>
         <tr r="C43" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3185351005</v>
+        <v>#N/A Requesting Data...3444569174</v>
         <stp/>
         <stp>BDP|15444947284180871401</stp>
         <tr r="G27" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1792449690</v>
+        <v>#N/A Requesting Data...4276480859</v>
         <stp/>
         <stp>BDP|12935317504846234704</stp>
         <tr r="F98" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4262631996</v>
+        <v>#N/A Requesting Data...3458005679</v>
         <stp/>
         <stp>BDP|13057895365605005829</stp>
         <tr r="C138" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1400510134</v>
+        <v>#N/A Requesting Data...3853752619</v>
         <stp/>
         <stp>BDP|16160321537943284588</stp>
         <tr r="E76" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3407504857</v>
+        <v>#N/A Requesting Data...3884399975</v>
         <stp/>
         <stp>BDP|10621599828921836610</stp>
         <tr r="C12" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1609971585</v>
+        <v>#N/A Requesting Data...3804319181</v>
         <stp/>
         <stp>BDP|14881076967673386157</stp>
         <tr r="F122" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4244789896</v>
+        <v>#N/A Requesting Data...3641419643</v>
         <stp/>
         <stp>BDP|17321553610055816607</stp>
         <tr r="F96" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1215170446</v>
+        <v>#N/A Requesting Data...3027819076</v>
         <stp/>
         <stp>BDP|12793555755147383546</stp>
         <tr r="F42" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1072925730</v>
+        <v>#N/A Requesting Data...4003255085</v>
         <stp/>
         <stp>BDP|10194327202093986081</stp>
         <tr r="F132" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2497613595</v>
+        <v>#N/A Requesting Data...2994269397</v>
         <stp/>
         <stp>BDP|12798194599768683232</stp>
         <tr r="C42" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1129732024</v>
+        <v>#N/A Requesting Data...3766315349</v>
         <stp/>
         <stp>BDP|15675203172551734114</stp>
         <tr r="F12" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1693336900</v>
+        <v>#N/A Requesting Data...3941831554</v>
         <stp/>
         <stp>BDP|17779010845097021465</stp>
         <tr r="G23" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...815107798</v>
+        <v>#N/A Requesting Data...3620148295</v>
         <stp/>
         <stp>BDP|14698661432127374654</stp>
         <tr r="E53" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3873374339</v>
+        <v>#N/A Requesting Data...3369992649</v>
         <stp/>
         <stp>BDP|16055018629402477686</stp>
         <tr r="F18" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2097125028</v>
+        <v>#N/A Requesting Data...3577471122</v>
         <stp/>
         <stp>BDP|14191015466523343124</stp>
         <tr r="G42" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1285784491</v>
+        <v>#N/A Requesting Data...3886412513</v>
         <stp/>
         <stp>BDP|16690545673604064064</stp>
         <tr r="G6" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2530356064</v>
+        <v>#N/A Requesting Data...4002376798</v>
         <stp/>
         <stp>BDP|11057556593645206836</stp>
         <tr r="E116" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1931289579</v>
+        <v>#N/A Requesting Data...4171684340</v>
         <stp/>
         <stp>BDP|14753168038796700174</stp>
         <tr r="E131" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1123981030</v>
+        <v>#N/A Requesting Data...3218271267</v>
         <stp/>
         <stp>BDP|18400936140157917378</stp>
         <tr r="G108" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4107569244</v>
+        <v>#N/A Requesting Data...3963218670</v>
         <stp/>
         <stp>BDP|11308062409311166143</stp>
         <tr r="F138" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2165782506</v>
+        <v>#N/A Requesting Data...3708847371</v>
         <stp/>
         <stp>BDP|14929251921187622207</stp>
         <tr r="G120" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2233660972</v>
+        <v>#N/A Requesting Data...3184355720</v>
         <stp/>
         <stp>BDP|13312546151322475095</stp>
         <tr r="C117" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2677887888</v>
+        <v>#N/A Requesting Data...4273087646</v>
         <stp/>
         <stp>BDP|10370784365528062849</stp>
         <tr r="G51" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...865460929</v>
+        <v>#N/A Requesting Data...3284634339</v>
         <stp/>
         <stp>BDP|17808503947101138629</stp>
         <tr r="F128" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1828435451</v>
+        <v>#N/A Requesting Data...4207758219</v>
         <stp/>
         <stp>BDP|17640270888515662931</stp>
         <tr r="E20" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1734735328</v>
+        <v>#N/A Requesting Data...3353205682</v>
         <stp/>
         <stp>BDP|17853766030844520642</stp>
         <tr r="F65" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...784949662</v>
+        <v>#N/A Requesting Data...2938932041</v>
         <stp/>
         <stp>BDP|17345319339237647129</stp>
         <tr r="C10" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2667662498</v>
+        <v>#N/A Requesting Data...3524886946</v>
         <stp/>
         <stp>BDP|18428163184190295050</stp>
         <tr r="C48" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2337065076</v>
+        <v>#N/A Requesting Data...3425953225</v>
         <stp/>
         <stp>BDP|11469771160883398201</stp>
         <tr r="G20" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3183573758</v>
+        <v>#N/A Requesting Data...4231267459</v>
         <stp/>
         <stp>BDP|12945229628891094206</stp>
         <tr r="F36" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3772741407</v>
+        <v>#N/A Requesting Data...2977381332</v>
         <stp/>
         <stp>BDP|13088969316699575369</stp>
         <tr r="G17" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3523072682</v>
+        <v>#N/A Requesting Data...3551369882</v>
         <stp/>
         <stp>BDP|14386928546318260068</stp>
         <tr r="C78" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3647320543</v>
+        <v>#N/A Requesting Data...3148716516</v>
         <stp/>
         <stp>BDP|16250000632946565269</stp>
         <tr r="F32" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1999441671</v>
+        <v>#N/A Requesting Data...4056754640</v>
         <stp/>
         <stp>BDP|10062445544650347114</stp>
         <tr r="E69" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A N/A</v>
+        <v>#N/A Requesting Data...3047375884</v>
         <stp/>
         <stp>BDP|16445974490524697317</stp>
         <tr r="F140" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1408220706</v>
+        <v>#N/A Requesting Data...3844070358</v>
         <stp/>
         <stp>BDP|18056984346180923430</stp>
         <tr r="F67" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2274418682</v>
+        <v>#N/A Requesting Data...4129449627</v>
         <stp/>
         <stp>BDP|13607419850307697457</stp>
         <tr r="G55" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3915070250</v>
+        <v>#N/A Requesting Data...3660346219</v>
         <stp/>
         <stp>BDP|17151526894293450943</stp>
         <tr r="E34" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3221859879</v>
+        <v>#N/A Requesting Data...3373058215</v>
         <stp/>
         <stp>BDP|14769233272840536059</stp>
         <tr r="F48" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1772038875</v>
+        <v>#N/A Requesting Data...3264641920</v>
         <stp/>
         <stp>BDP|16347078018142331376</stp>
         <tr r="E59" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2775869243</v>
+        <v>#N/A Requesting Data...3397009438</v>
         <stp/>
         <stp>BDP|12157937398585487157</stp>
         <tr r="F69" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3450845366</v>
+        <v>#N/A Requesting Data...4054936395</v>
         <stp/>
         <stp>BDP|10450024654077121490</stp>
         <tr r="G29" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1968387828</v>
+        <v>#N/A Requesting Data...3901838700</v>
         <stp/>
         <stp>BDP|12405274734177384298</stp>
         <tr r="G109" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2545328806</v>
+        <v>#N/A Requesting Data...3628659570</v>
         <stp/>
         <stp>BDP|11693290023110245727</stp>
         <tr r="F93" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2404597129</v>
+        <v>#N/A Requesting Data...3797485826</v>
         <stp/>
         <stp>BDP|16857915317939051104</stp>
         <tr r="E4" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3842909688</v>
+        <v>#N/A Requesting Data...3743170959</v>
         <stp/>
         <stp>BDP|13092630751014311204</stp>
         <tr r="C29" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3000192752</v>
+        <v>#N/A Requesting Data...4025161196</v>
         <stp/>
         <stp>BDP|16560165422091315234</stp>
         <tr r="E74" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4196404766</v>
+        <v>#N/A Requesting Data...4141186032</v>
         <stp/>
         <stp>BDP|15578620992514708823</stp>
         <tr r="C74" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2667998084</v>
+        <v>#N/A Requesting Data...3089556592</v>
         <stp/>
         <stp>BDP|16311826266949112751</stp>
         <tr r="E137" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2992969174</v>
+        <v>#N/A Requesting Data...4200569805</v>
         <stp/>
         <stp>BDP|12423551309476829732</stp>
         <tr r="E29" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3199490161</v>
+        <v>#N/A Requesting Data...3025282191</v>
         <stp/>
         <stp>BDP|15334425393507822980</stp>
         <tr r="C71" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4009317134</v>
+        <v>#N/A Requesting Data...3969206831</v>
         <stp/>
         <stp>BDP|14187404668490888034</stp>
         <tr r="E115" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...983205183</v>
+        <v>#N/A Requesting Data...3647849666</v>
         <stp/>
         <stp>BDP|14038301256494491076</stp>
         <tr r="E12" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2945250430</v>
+        <v>#N/A Requesting Data...4203518602</v>
         <stp/>
         <stp>BDP|12212063840830333025</stp>
         <tr r="E132" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4147170793</v>
+        <v>#N/A Requesting Data...4293826431</v>
         <stp/>
         <stp>BDP|12411228970299104833</stp>
         <tr r="E40" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1937545442</v>
+        <v>#N/A Requesting Data...4128209380</v>
         <stp/>
         <stp>BDP|11324255971734653659</stp>
         <tr r="G93" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...923444276</v>
+        <v>#N/A Requesting Data...3756592731</v>
         <stp/>
         <stp>BDP|15080702944965265524</stp>
         <tr r="E5" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1863246818</v>
+        <v>#N/A Requesting Data...3104182181</v>
         <stp/>
         <stp>BDP|12709330545317601409</stp>
         <tr r="F78" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2003989593</v>
+        <v>#N/A Requesting Data...3705713049</v>
         <stp/>
         <stp>BDP|17558583635766924170</stp>
         <tr r="C139" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3368278043</v>
+        <v>#N/A Requesting Data...3827967286</v>
         <stp/>
         <stp>BDP|14043797868641345244</stp>
         <tr r="G127" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2821920190</v>
+        <v>#N/A Requesting Data...3142811642</v>
         <stp/>
         <stp>BDP|11097146762171726091</stp>
         <tr r="C125" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2346385945</v>
+        <v>#N/A Requesting Data...3496123262</v>
         <stp/>
         <stp>BDP|10083242995488903402</stp>
         <tr r="E22" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1973534664</v>
+        <v>#N/A Requesting Data...3171076113</v>
         <stp/>
         <stp>BDP|14104003677163905777</stp>
         <tr r="G89" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1417872037</v>
+        <v>#N/A Requesting Data...3353961891</v>
         <stp/>
         <stp>BDP|10493155251505330684</stp>
         <tr r="F113" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2109775885</v>
+        <v>#N/A Requesting Data...3604488617</v>
         <stp/>
         <stp>BDP|17307159600861837050</stp>
         <tr r="C28" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3337612575</v>
+        <v>#N/A Requesting Data...3096415670</v>
         <stp/>
         <stp>BDP|11974207352247436657</stp>
         <tr r="G84" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4044932811</v>
+        <v>#N/A Requesting Data...3447499766</v>
         <stp/>
         <stp>BDP|12417029733397010193</stp>
         <tr r="G129" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1616245422</v>
+        <v>#N/A Requesting Data...3394741485</v>
         <stp/>
         <stp>BDP|13696428749777505366</stp>
         <tr r="C128" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1732287721</v>
+        <v>#N/A Requesting Data...3195538684</v>
         <stp/>
         <stp>BDP|10265435339313984301</stp>
         <tr r="F136" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1590202008</v>
+        <v>#N/A Requesting Data...4113424714</v>
         <stp/>
         <stp>BDP|16742662035804692035</stp>
         <tr r="E24" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4003227884</v>
+        <v>#N/A Requesting Data...3819318945</v>
         <stp/>
         <stp>BDP|13311072247345018521</stp>
         <tr r="E129" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2172624229</v>
+        <v>#N/A Requesting Data...3980152121</v>
         <stp/>
         <stp>BDP|14635385909938704819</stp>
         <tr r="E106" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2469301612</v>
+        <v>#N/A Requesting Data...3777560235</v>
         <stp/>
         <stp>BDP|17965266240553639582</stp>
         <tr r="E10" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2445012252</v>
+        <v>#N/A Requesting Data...3297010256</v>
         <stp/>
         <stp>BDP|14559650107303581628</stp>
         <tr r="C72" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1174662566</v>
+        <v>#N/A Requesting Data...4112226720</v>
         <stp/>
         <stp>BDP|12078771150016496119</stp>
         <tr r="G102" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4069299378</v>
+        <v>#N/A Requesting Data...3364161578</v>
         <stp/>
         <stp>BDP|13437131854538783812</stp>
         <tr r="G22" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2382110685</v>
+        <v>#N/A Requesting Data...4021731269</v>
         <stp/>
         <stp>BDP|11816803688615161347</stp>
         <tr r="E51" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3950912559</v>
+        <v>#N/A Requesting Data...3240857903</v>
         <stp/>
         <stp>BDP|11136233214231371414</stp>
         <tr r="G139" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1745042404</v>
+        <v>#N/A Requesting Data...3640915959</v>
         <stp/>
         <stp>BDP|16387121100332435221</stp>
         <tr r="G96" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2705630820</v>
+        <v>#N/A Requesting Data...3499756445</v>
         <stp/>
         <stp>BDP|10044993787394494110</stp>
         <tr r="C113" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...982662432</v>
+        <v>#N/A Requesting Data...4237929204</v>
         <stp/>
         <stp>BDP|16851432539276999316</stp>
         <tr r="E44" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3867532259</v>
+        <v>#N/A Requesting Data...3415189358</v>
         <stp/>
         <stp>BDP|17514330731974993734</stp>
         <tr r="E65" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1019695791</v>
+        <v>#N/A Requesting Data...4237177959</v>
         <stp/>
         <stp>BDP|13397290692205579908</stp>
         <tr r="G128" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2636015311</v>
+        <v>#N/A Requesting Data...3293709413</v>
         <stp/>
         <stp>BDP|11770519860203890508</stp>
         <tr r="F106" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1474495217</v>
+        <v>#N/A Requesting Data...3472789856</v>
         <stp/>
         <stp>BDP|11828615722360397168</stp>
         <tr r="E71" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2458220676</v>
+        <v>#N/A Requesting Data...3853668383</v>
         <stp/>
         <stp>BDP|12429929188915695292</stp>
         <tr r="F109" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4112057914</v>
+        <v>#N/A Requesting Data...3876277490</v>
         <stp/>
         <stp>BDP|14807781952773549162</stp>
         <tr r="G33" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3814046755</v>
+        <v>#N/A Requesting Data...3570172028</v>
         <stp/>
         <stp>BDP|14141528956866623622</stp>
         <tr r="C134" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1848116892</v>
+        <v>#N/A Requesting Data...4128407288</v>
         <stp/>
         <stp>BDP|11925450918217650729</stp>
         <tr r="F86" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1837900561</v>
+        <v>#N/A Requesting Data...4220073621</v>
         <stp/>
         <stp>BDP|10075353521710450506</stp>
         <tr r="C109" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1624881164</v>
+        <v>#N/A Requesting Data...3336098588</v>
         <stp/>
         <stp>BDP|14507687284196916837</stp>
         <tr r="F6" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3736635479</v>
+        <v>#N/A Requesting Data...3164070915</v>
         <stp/>
         <stp>BDP|17592946715913980887</stp>
         <tr r="F7" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2501564230</v>
+        <v>#N/A Requesting Data...4216606435</v>
         <stp/>
         <stp>BDP|12670343566891576248</stp>
         <tr r="G36" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...734745559</v>
+        <v>#N/A Requesting Data...3068463115</v>
         <stp/>
         <stp>BDP|16059776447550017157</stp>
         <tr r="F63" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...721339064</v>
+        <v>#N/A Requesting Data...3218542173</v>
         <stp/>
         <stp>BDP|13709786759646324310</stp>
         <tr r="F46" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1412980980</v>
+        <v>#N/A Requesting Data...3786470116</v>
         <stp/>
         <stp>BDP|17680007951225535344</stp>
         <tr r="C93" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...838872620</v>
+        <v>#N/A Requesting Data...4255464065</v>
         <stp/>
         <stp>BDP|14249466628496635139</stp>
         <tr r="F26" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3110690599</v>
+        <v>#N/A Requesting Data...3083595684</v>
         <stp/>
         <stp>BDP|12616286245214000526</stp>
         <tr r="C114" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4067734432</v>
+        <v>#N/A Requesting Data...3605316619</v>
         <stp/>
         <stp>BDP|13229487552560837780</stp>
         <tr r="E139" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2370996999</v>
+        <v>#N/A Requesting Data...3830483153</v>
         <stp/>
         <stp>BDP|18412208651713792994</stp>
         <tr r="F118" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1829856501</v>
+        <v>#N/A Requesting Data...3174247234</v>
         <stp/>
         <stp>BDP|16919456577607807790</stp>
         <tr r="G56" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2602766238</v>
+        <v>#N/A Requesting Data...4281524874</v>
         <stp/>
         <stp>BDP|14958917677776306912</stp>
         <tr r="E124" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1007329525</v>
+        <v>#N/A Requesting Data...4095537979</v>
         <stp/>
         <stp>BDP|16906362551851442479</stp>
         <tr r="F14" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...846132354</v>
+        <v>#N/A Requesting Data...4080075873</v>
         <stp/>
         <stp>BDP|13303498173634341154</stp>
         <tr r="G72" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2793440464</v>
+        <v>#N/A Requesting Data...3125073998</v>
         <stp/>
         <stp>BDP|11394026073756494578</stp>
         <tr r="F4" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3552590034</v>
+        <v>#N/A Requesting Data...3429957104</v>
         <stp/>
         <stp>BDP|12821707660430898618</stp>
         <tr r="C40" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3517907464</v>
+        <v>#N/A Requesting Data...3800139377</v>
         <stp/>
         <stp>BDP|12207042919767891145</stp>
         <tr r="G131" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1079518061</v>
+        <v>#N/A Requesting Data...4031016283</v>
         <stp/>
         <stp>BDP|17617562141366516571</stp>
         <tr r="F24" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3260258468</v>
+        <v>#N/A Requesting Data...4252486565</v>
         <stp/>
         <stp>BDP|13776066979946925741</stp>
         <tr r="C90" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4069297517</v>
+        <v>#N/A Requesting Data...3060259867</v>
         <stp/>
         <stp>BDP|15429465971742273156</stp>
         <tr r="E67" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3659029421</v>
+        <v>#N/A Requesting Data...4046111018</v>
         <stp/>
         <stp>BDP|13319017160191784122</stp>
         <tr r="E43" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1763276761</v>
+        <v>#N/A Requesting Data...3594795096</v>
         <stp/>
         <stp>BDP|17197570677470339052</stp>
         <tr r="E33" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3828931645</v>
+        <v>#N/A Requesting Data...3897190449</v>
         <stp/>
         <stp>BDP|18198100188843948773</stp>
         <tr r="G60" s="1"/>
@@ -2739,1801 +2739,1801 @@
     </main>
     <main first="bofaddin.rtdserver">
       <tp t="s">
-        <v>#N/A Requesting Data...3850857810</v>
+        <v>#N/A Requesting Data...3630897453</v>
         <stp/>
         <stp>BDP|3930904544763426134</stp>
         <tr r="C55" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3840038934</v>
+        <v>#N/A Requesting Data...4233020119</v>
         <stp/>
         <stp>BDP|7103625188072362707</stp>
         <tr r="E98" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1388759354</v>
+        <v>#N/A Requesting Data...3533242134</v>
         <stp/>
         <stp>BDP|9365312653090978315</stp>
         <tr r="G136" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1656475012</v>
+        <v>#N/A Requesting Data...3883352046</v>
         <stp/>
         <stp>BDP|6412151529379694002</stp>
         <tr r="F110" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1422556765</v>
+        <v>#N/A Requesting Data...3552376981</v>
         <stp/>
         <stp>BDP|6245426297947871034</stp>
         <tr r="C80" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3859937569</v>
+        <v>#N/A Requesting Data...3236430324</v>
         <stp/>
         <stp>BDP|2350385774053258906</stp>
         <tr r="F72" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3573570986</v>
+        <v>#N/A Requesting Data...4069882377</v>
         <stp/>
         <stp>BDP|8530657130876609747</stp>
         <tr r="C44" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1339043229</v>
+        <v>#N/A Requesting Data...3505795335</v>
         <stp/>
         <stp>BDP|7198979431090342164</stp>
         <tr r="E50" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1722508955</v>
+        <v>#N/A Requesting Data...3350202382</v>
         <stp/>
         <stp>BDP|9075300299347332881</stp>
         <tr r="G79" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2548627137</v>
+        <v>#N/A Requesting Data...3782297636</v>
         <stp/>
         <stp>BDP|5029740995104753357</stp>
         <tr r="C111" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1827813879</v>
+        <v>#N/A Requesting Data...3935535303</v>
         <stp/>
         <stp>BDP|8128743572863334748</stp>
         <tr r="C47" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2223087047</v>
+        <v>#N/A Requesting Data...3858466168</v>
         <stp/>
         <stp>BDP|6339719327836450907</stp>
         <tr r="C98" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2469111295</v>
+        <v>#N/A Requesting Data...3555527629</v>
         <stp/>
         <stp>BDP|4200580269163222863</stp>
         <tr r="E25" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4096192954</v>
+        <v>#N/A Requesting Data...3464329028</v>
         <stp/>
         <stp>BDP|5989352249668473659</stp>
         <tr r="G50" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1806556720</v>
+        <v>#N/A Requesting Data...3778275139</v>
         <stp/>
         <stp>BDP|2484433252649720677</stp>
         <tr r="G68" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1241414605</v>
+        <v>#N/A Requesting Data...3618156854</v>
         <stp/>
         <stp>BDP|6249870436562567333</stp>
         <tr r="E49" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1190487284</v>
+        <v>#N/A Requesting Data...4097272010</v>
         <stp/>
         <stp>BDP|9572192910556051262</stp>
         <tr r="E134" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3700882917</v>
+        <v>#N/A Requesting Data...3992427768</v>
         <stp/>
         <stp>BDP|7540551159163224910</stp>
         <tr r="F51" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3658410159</v>
+        <v>#N/A Requesting Data...3279600786</v>
         <stp/>
         <stp>BDP|8451204331587951367</stp>
         <tr r="F52" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2801672410</v>
+        <v>#N/A Requesting Data...3366487196</v>
         <stp/>
         <stp>BDP|3109256470563958869</stp>
         <tr r="C52" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2444939005</v>
+        <v>#N/A Requesting Data...4234686115</v>
         <stp/>
         <stp>BDP|3590543194827878545</stp>
         <tr r="F59" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1188735601</v>
+        <v>#N/A Requesting Data...4003465645</v>
         <stp/>
         <stp>BDP|3009997314886390075</stp>
         <tr r="G100" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3745215257</v>
+        <v>#N/A Requesting Data...3540840546</v>
         <stp/>
         <stp>BDP|4777106988391072114</stp>
         <tr r="F103" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3973868701</v>
+        <v>#N/A Requesting Data...4233755007</v>
         <stp/>
         <stp>BDP|4303401897634933024</stp>
         <tr r="E93" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1979890649</v>
+        <v>#N/A Requesting Data...3418800059</v>
         <stp/>
         <stp>BDP|9055938583773500695</stp>
         <tr r="C34" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3757163502</v>
+        <v>#N/A Requesting Data...3131636593</v>
         <stp/>
         <stp>BDP|1573317174439842142</stp>
         <tr r="E133" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2879471438</v>
+        <v>#N/A Requesting Data...3799667598</v>
         <stp/>
         <stp>BDP|7180318607099335068</stp>
         <tr r="C9" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4084744174</v>
+        <v>#N/A Requesting Data...3787272980</v>
         <stp/>
         <stp>BDP|8371873502449565411</stp>
         <tr r="C62" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2802451141</v>
+        <v>#N/A Requesting Data...3450831367</v>
         <stp/>
         <stp>BDP|9300723062997279226</stp>
         <tr r="C124" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1764868100</v>
+        <v>#N/A Requesting Data...3980505806</v>
         <stp/>
         <stp>BDP|5492561896244379063</stp>
         <tr r="F70" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3061775916</v>
+        <v>#N/A Requesting Data...3817850931</v>
         <stp/>
         <stp>BDP|8460669760190400504</stp>
         <tr r="C27" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2431591848</v>
+        <v>#N/A Requesting Data...3513883699</v>
         <stp/>
         <stp>BDP|7634975275120208406</stp>
         <tr r="C31" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1668716456</v>
+        <v>#N/A Requesting Data...4179530371</v>
         <stp/>
         <stp>BDP|4040591290066838371</stp>
         <tr r="E13" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1930496584</v>
+        <v>#N/A Requesting Data...3626516292</v>
         <stp/>
         <stp>BDP|9247766641156585153</stp>
         <tr r="G94" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1701672238</v>
+        <v>#N/A Requesting Data...3356802582</v>
         <stp/>
         <stp>BDP|7940113982976758589</stp>
         <tr r="E95" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1715920813</v>
+        <v>#N/A Requesting Data...4117806693</v>
         <stp/>
         <stp>BDP|9093620553903200797</stp>
         <tr r="C105" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2857710250</v>
+        <v>#N/A Requesting Data...3341568941</v>
         <stp/>
         <stp>BDP|2405932012622401695</stp>
         <tr r="G77" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2945886548</v>
+        <v>#N/A Requesting Data...3588568089</v>
         <stp/>
         <stp>BDP|9175353808212225665</stp>
         <tr r="C66" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2495424685</v>
+        <v>#N/A Requesting Data...3238001216</v>
         <stp/>
         <stp>BDP|1414608591110891051</stp>
         <tr r="F9" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...809212008</v>
+        <v>#N/A Requesting Data...3147778087</v>
         <stp/>
         <stp>BDP|3649732806419915339</stp>
         <tr r="G14" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3458855116</v>
+        <v>#N/A Requesting Data...3204920747</v>
         <stp/>
         <stp>BDP|7006257261095505888</stp>
         <tr r="F54" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3229185616</v>
+        <v>#N/A Requesting Data...3547868879</v>
         <stp/>
         <stp>BDP|9781989741438009272</stp>
         <tr r="C39" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3563253576</v>
+        <v>#N/A Requesting Data...3676962190</v>
         <stp/>
         <stp>BDP|7532189862547338936</stp>
         <tr r="F58" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3618929613</v>
+        <v>#N/A Requesting Data...4018725262</v>
         <stp/>
         <stp>BDP|4286027170164748985</stp>
         <tr r="G113" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1847841285</v>
+        <v>#N/A Requesting Data...3465617992</v>
         <stp/>
         <stp>BDP|4691882821088256816</stp>
         <tr r="F126" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3886490395</v>
+        <v>#N/A Requesting Data...3269575976</v>
         <stp/>
         <stp>BDP|4974055815239706225</stp>
         <tr r="G110" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2173408838</v>
+        <v>#N/A Requesting Data...3891944623</v>
         <stp/>
         <stp>BDP|5916130291376545539</stp>
         <tr r="F73" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3363748330</v>
+        <v>#N/A Requesting Data...3216385225</v>
         <stp/>
         <stp>BDP|9535646277681935723</stp>
         <tr r="E60" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1784209331</v>
+        <v>#N/A Requesting Data...3440543391</v>
         <stp/>
         <stp>BDP|3472420329653378814</stp>
         <tr r="G4" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1958007647</v>
+        <v>#N/A Requesting Data...3584266284</v>
         <stp/>
         <stp>BDP|9676580711333862054</stp>
         <tr r="E135" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1534071596</v>
+        <v>#N/A Requesting Data...4089781646</v>
         <stp/>
         <stp>BDP|8651287802994649096</stp>
         <tr r="E77" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1456143147</v>
+        <v>#N/A Requesting Data...3752189155</v>
         <stp/>
         <stp>BDP|5552297197720045083</stp>
         <tr r="E118" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3996748132</v>
+        <v>#N/A Requesting Data...3135436078</v>
         <stp/>
         <stp>BDP|6195991527552839107</stp>
         <tr r="C61" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1020712784</v>
+        <v>#N/A Requesting Data...3427493599</v>
         <stp/>
         <stp>BDP|2785537291931900199</stp>
         <tr r="G91" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1867597406</v>
+        <v>#N/A Requesting Data...3159997030</v>
         <stp/>
         <stp>BDP|9875435960971965593</stp>
         <tr r="C11" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A N/A</v>
+        <v>#N/A Requesting Data...3973890212</v>
         <stp/>
         <stp>BDP|5969741853480600831</stp>
         <tr r="E140" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2688645981</v>
+        <v>#N/A Requesting Data...3338765911</v>
         <stp/>
         <stp>BDP|7662972721973338089</stp>
         <tr r="F107" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2641994697</v>
+        <v>#N/A Requesting Data...3334190764</v>
         <stp/>
         <stp>BDP|4282903616430488389</stp>
         <tr r="G9" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1456911352</v>
+        <v>#N/A Requesting Data...3776055708</v>
         <stp/>
         <stp>BDP|6606398548307737925</stp>
         <tr r="C70" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3771140410</v>
+        <v>#N/A Requesting Data...3857952183</v>
         <stp/>
         <stp>BDP|2310021551041423963</stp>
         <tr r="F123" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3522025354</v>
+        <v>#N/A Requesting Data...3795486345</v>
         <stp/>
         <stp>BDP|1666950877162018261</stp>
         <tr r="E87" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3061400763</v>
+        <v>#N/A Requesting Data...3786871715</v>
         <stp/>
         <stp>BDP|6280569068792932854</stp>
         <tr r="C46" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1749681525</v>
+        <v>#N/A Requesting Data...4151898341</v>
         <stp/>
         <stp>BDP|9635152443296662577</stp>
         <tr r="C16" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3166443068</v>
+        <v>#N/A Requesting Data...3499792371</v>
         <stp/>
         <stp>BDP|5935740968278021330</stp>
         <tr r="C96" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3805962936</v>
+        <v>#N/A Requesting Data...3497295690</v>
         <stp/>
         <stp>BDP|8225387168083679130</stp>
         <tr r="E57" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2444643324</v>
+        <v>#N/A Requesting Data...4097612619</v>
         <stp/>
         <stp>BDP|8741792397660502982</stp>
         <tr r="G24" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1827678087</v>
+        <v>#N/A Requesting Data...3555993712</v>
         <stp/>
         <stp>BDP|1988621838892198978</stp>
         <tr r="F82" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4005314878</v>
+        <v>#N/A Requesting Data...3914469917</v>
         <stp/>
         <stp>BDP|5160947801244572083</stp>
         <tr r="C97" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3015630725</v>
+        <v>#N/A Requesting Data...3844292740</v>
         <stp/>
         <stp>BDP|8781684350665372626</stp>
         <tr r="G64" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2364846878</v>
+        <v>#N/A Requesting Data...4202350163</v>
         <stp/>
         <stp>BDP|8866465832365619258</stp>
         <tr r="F120" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3282035768</v>
+        <v>#N/A Requesting Data...3585899944</v>
         <stp/>
         <stp>BDP|1231973558974048121</stp>
         <tr r="E123" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1282592653</v>
+        <v>#N/A Requesting Data...3942309829</v>
         <stp/>
         <stp>BDP|9011959145835954962</stp>
         <tr r="E102" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3055012476</v>
+        <v>#N/A Requesting Data...4172751941</v>
         <stp/>
         <stp>BDP|7048111723254898858</stp>
         <tr r="E70" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2706477691</v>
+        <v>#N/A Requesting Data...3990426416</v>
         <stp/>
         <stp>BDP|7514426398370500271</stp>
         <tr r="F84" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2912707837</v>
+        <v>#N/A Requesting Data...4219320518</v>
         <stp/>
         <stp>BDP|2286847884578687294</stp>
         <tr r="C64" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3383613311</v>
+        <v>#N/A Requesting Data...3246614486</v>
         <stp/>
         <stp>BDP|8581359335587083771</stp>
         <tr r="G40" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3057584243</v>
+        <v>#N/A Requesting Data...4038112478</v>
         <stp/>
         <stp>BDP|9176352611073152053</stp>
         <tr r="G52" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1607815042</v>
+        <v>#N/A Requesting Data...3202812828</v>
         <stp/>
         <stp>BDP|3761613276703138977</stp>
         <tr r="C22" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2684974837</v>
+        <v>#N/A Requesting Data...3258799934</v>
         <stp/>
         <stp>BDP|2402283480247992710</stp>
         <tr r="G65" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1711933552</v>
+        <v>#N/A Requesting Data...3690066133</v>
         <stp/>
         <stp>BDP|2496054182730824314</stp>
         <tr r="F108" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3760375771</v>
+        <v>#N/A Requesting Data...3688004674</v>
         <stp/>
         <stp>BDP|1156198294412416234</stp>
         <tr r="G48" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3090064044</v>
+        <v>#N/A Requesting Data...4107133867</v>
         <stp/>
         <stp>BDP|1935863512592400318</stp>
         <tr r="G99" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1520524639</v>
+        <v>#N/A Requesting Data...3663141797</v>
         <stp/>
         <stp>BDP|1182070188629538920</stp>
         <tr r="F85" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2925929779</v>
+        <v>#N/A Requesting Data...3651679020</v>
         <stp/>
         <stp>BDP|9924697901094165296</stp>
         <tr r="E38" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2975857228</v>
+        <v>#N/A Requesting Data...3260696187</v>
         <stp/>
         <stp>BDP|6412137247758825261</stp>
         <tr r="G10" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4155990218</v>
+        <v>#N/A Requesting Data...3408849884</v>
         <stp/>
         <stp>BDP|6277108296426856136</stp>
         <tr r="G122" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...885960325</v>
+        <v>#N/A Requesting Data...4246105616</v>
         <stp/>
         <stp>BDP|2351176324921816947</stp>
         <tr r="E117" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1271039753</v>
+        <v>#N/A Requesting Data...3719930543</v>
         <stp/>
         <stp>BDP|6406207188846485346</stp>
         <tr r="C37" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4005841240</v>
+        <v>#N/A Requesting Data...3476803725</v>
         <stp/>
         <stp>BDP|8112280367483097628</stp>
         <tr r="F16" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2048804741</v>
+        <v>#N/A Requesting Data...3640520984</v>
         <stp/>
         <stp>BDP|6484624822372932905</stp>
         <tr r="C108" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...943375044</v>
+        <v>#N/A Requesting Data...4066676364</v>
         <stp/>
         <stp>BDP|8605875253514357834</stp>
         <tr r="C116" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2693908349</v>
+        <v>#N/A Requesting Data...3543958993</v>
         <stp/>
         <stp>BDP|2842991807747556512</stp>
         <tr r="E110" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1510681133</v>
+        <v>#N/A Requesting Data...3842211271</v>
         <stp/>
         <stp>BDP|1377759003508711718</stp>
         <tr r="E55" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2374925903</v>
+        <v>#N/A Requesting Data...3389974686</v>
         <stp/>
         <stp>BDP|1711361391887412536</stp>
         <tr r="G47" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2948989596</v>
+        <v>#N/A Requesting Data...4246189069</v>
         <stp/>
         <stp>BDP|4564815655442574234</stp>
         <tr r="F114" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1752702899</v>
+        <v>#N/A Requesting Data...4150523836</v>
         <stp/>
         <stp>BDP|6557751567646791843</stp>
         <tr r="C85" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2637631557</v>
+        <v>#N/A Requesting Data...3340966700</v>
         <stp/>
         <stp>BDP|5018226780961297742</stp>
         <tr r="E138" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3509800840</v>
+        <v>#N/A Requesting Data...4176520765</v>
         <stp/>
         <stp>BDP|7190582290036507495</stp>
         <tr r="E48" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1075507266</v>
+        <v>#N/A Requesting Data...3420544531</v>
         <stp/>
         <stp>BDP|7268732641219205478</stp>
         <tr r="F111" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3696721765</v>
+        <v>#N/A Requesting Data...3630334258</v>
         <stp/>
         <stp>BDP|5085458293997400582</stp>
         <tr r="C30" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2894195234</v>
+        <v>#N/A Requesting Data...4158494191</v>
         <stp/>
         <stp>BDP|2916061605678582044</stp>
         <tr r="E27" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...873557922</v>
+        <v>#N/A Requesting Data...3293480919</v>
         <stp/>
         <stp>BDP|5645196194854205325</stp>
         <tr r="E19" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1245764625</v>
+        <v>#N/A Requesting Data...3756680230</v>
         <stp/>
         <stp>BDP|8929421222763426766</stp>
         <tr r="F112" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2068505916</v>
+        <v>#N/A Requesting Data...3615571542</v>
         <stp/>
         <stp>BDP|2815946348173965667</stp>
         <tr r="C137" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3908828213</v>
+        <v>#N/A Requesting Data...3415736151</v>
         <stp/>
         <stp>BDP|6645611732949919042</stp>
         <tr r="G95" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1755901299</v>
+        <v>#N/A Requesting Data...4090051918</v>
         <stp/>
         <stp>BDP|8744658502964028082</stp>
         <tr r="F139" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1984985695</v>
+        <v>#N/A Requesting Data...4290151944</v>
         <stp/>
         <stp>BDP|4077907452745230782</stp>
         <tr r="C130" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1766206147</v>
+        <v>#N/A Requesting Data...3857031093</v>
         <stp/>
         <stp>BDP|8975856381415089739</stp>
         <tr r="E75" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1764133455</v>
+        <v>#N/A Requesting Data...4213380402</v>
         <stp/>
         <stp>BDP|5738611839292209825</stp>
         <tr r="G107" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2367795726</v>
+        <v>#N/A Requesting Data...3983588128</v>
         <stp/>
         <stp>BDP|4996818111432201578</stp>
         <tr r="G134" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1814994336</v>
+        <v>#N/A Requesting Data...3207187924</v>
         <stp/>
         <stp>BDP|5458032582021895609</stp>
         <tr r="E89" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4263993066</v>
+        <v>#N/A Requesting Data...4192195537</v>
         <stp/>
         <stp>BDP|2612461303954522846</stp>
         <tr r="F21" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3004267743</v>
+        <v>#N/A Requesting Data...3237145465</v>
         <stp/>
         <stp>BDP|5852840000806674187</stp>
         <tr r="F75" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3815707830</v>
+        <v>#N/A Requesting Data...4176359506</v>
         <stp/>
         <stp>BDP|7947641811679527399</stp>
         <tr r="G13" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2344847530</v>
+        <v>#N/A Requesting Data...3772657207</v>
         <stp/>
         <stp>BDP|8407769428857900025</stp>
         <tr r="C132" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3319638468</v>
+        <v>#N/A Requesting Data...4030345872</v>
         <stp/>
         <stp>BDP|1313714864639868399</stp>
         <tr r="F87" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2131904760</v>
+        <v>#N/A Requesting Data...3632059038</v>
         <stp/>
         <stp>BDP|2531298252748844733</stp>
         <tr r="F115" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3104546847</v>
+        <v>#N/A Requesting Data...3346527458</v>
         <stp/>
         <stp>BDP|8965389266391509672</stp>
         <tr r="C41" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2081606004</v>
+        <v>#N/A Requesting Data...3409104821</v>
         <stp/>
         <stp>BDP|9146373380128430189</stp>
         <tr r="F60" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2681722967</v>
+        <v>#N/A Requesting Data...3741730065</v>
         <stp/>
         <stp>BDP|8769626454200391097</stp>
         <tr r="G85" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3810025657</v>
+        <v>#N/A Requesting Data...4031285097</v>
         <stp/>
         <stp>BDP|7701346097304455298</stp>
         <tr r="C73" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1817145433</v>
+        <v>#N/A Requesting Data...4137131917</v>
         <stp/>
         <stp>BDP|1201589979318261083</stp>
         <tr r="G123" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3347766849</v>
+        <v>#N/A Requesting Data...3291538683</v>
         <stp/>
         <stp>BDP|9994425762708075853</stp>
         <tr r="G88" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4061502689</v>
+        <v>#N/A Requesting Data...3225093032</v>
         <stp/>
         <stp>BDP|8238868892513701135</stp>
         <tr r="G137" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2282656091</v>
+        <v>#N/A Requesting Data...3409069615</v>
         <stp/>
         <stp>BDP|3321556007464177923</stp>
         <tr r="E109" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4158125882</v>
+        <v>#N/A Requesting Data...3684763288</v>
         <stp/>
         <stp>BDP|8367368187378355023</stp>
         <tr r="F64" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3915728486</v>
+        <v>#N/A Requesting Data...3489321112</v>
         <stp/>
         <stp>BDP|9054142235387080711</stp>
         <tr r="F11" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1624640732</v>
+        <v>#N/A Requesting Data...4227478973</v>
         <stp/>
         <stp>BDP|4797724273716399932</stp>
         <tr r="C5" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4057517051</v>
+        <v>#N/A Requesting Data...3782343521</v>
         <stp/>
         <stp>BDP|3084971212582403246</stp>
         <tr r="F121" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1312127835</v>
+        <v>#N/A Requesting Data...3238703716</v>
         <stp/>
         <stp>BDP|6948762204713990690</stp>
         <tr r="G90" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3029217342</v>
+        <v>#N/A Requesting Data...3412065323</v>
         <stp/>
         <stp>BDP|1832764578595986067</stp>
         <tr r="G119" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4038191518</v>
+        <v>#N/A Requesting Data...3262849731</v>
         <stp/>
         <stp>BDP|4156639623951685595</stp>
         <tr r="F13" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4102794281</v>
+        <v>#N/A Requesting Data...3244817518</v>
         <stp/>
         <stp>BDP|5919761437851372455</stp>
         <tr r="C2" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1358497038</v>
+        <v>#N/A Requesting Data...4284619977</v>
         <stp/>
         <stp>BDP|1551339666687413790</stp>
         <tr r="F40" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2670256419</v>
+        <v>#N/A Requesting Data...3716121150</v>
         <stp/>
         <stp>BDP|6420437202397070174</stp>
         <tr r="C8" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1270340641</v>
+        <v>#N/A Requesting Data...3559414181</v>
         <stp/>
         <stp>BDP|1708381902825815365</stp>
         <tr r="C101" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3598803370</v>
+        <v>#N/A Requesting Data...4082658979</v>
         <stp/>
         <stp>BDP|4945796250777738578</stp>
         <tr r="G21" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3677289348</v>
+        <v>#N/A Requesting Data...3995490738</v>
         <stp/>
         <stp>BDP|6746841414412327938</stp>
         <tr r="G75" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3616959773</v>
+        <v>#N/A Requesting Data...4025998094</v>
         <stp/>
         <stp>BDP|1709445403856801620</stp>
         <tr r="E85" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3174812154</v>
+        <v>#N/A Requesting Data...4095637098</v>
         <stp/>
         <stp>BDP|9398823419477440265</stp>
         <tr r="G125" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1320066910</v>
+        <v>#N/A Requesting Data...3974309575</v>
         <stp/>
         <stp>BDP|3430878723724827801</stp>
         <tr r="G41" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2910428025</v>
+        <v>#N/A Requesting Data...3304953062</v>
         <stp/>
         <stp>BDP|9698422803149077198</stp>
         <tr r="C100" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1483107005</v>
+        <v>#N/A Requesting Data...4170341103</v>
         <stp/>
         <stp>BDP|2887002514665714363</stp>
         <tr r="G59" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1086310647</v>
+        <v>#N/A Requesting Data...3736143860</v>
         <stp/>
         <stp>BDP|2668814054578766269</stp>
         <tr r="E31" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1301896798</v>
+        <v>#N/A Requesting Data...3773285658</v>
         <stp/>
         <stp>BDP|8894702939828266110</stp>
         <tr r="C7" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1459666417</v>
+        <v>#N/A Requesting Data...3891388398</v>
         <stp/>
         <stp>BDP|3410885660260666884</stp>
         <tr r="E64" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1425345845</v>
+        <v>#N/A Requesting Data...3723155621</v>
         <stp/>
         <stp>BDP|3658713905400418152</stp>
         <tr r="E35" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3998841534</v>
+        <v>#N/A Requesting Data...3312451464</v>
         <stp/>
         <stp>BDP|7570300716478486864</stp>
         <tr r="E32" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2494179008</v>
+        <v>#N/A Requesting Data...3871377564</v>
         <stp/>
         <stp>BDP|7851492951527237434</stp>
         <tr r="E52" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3165015246</v>
+        <v>#N/A Requesting Data...3698115123</v>
         <stp/>
         <stp>BDP|7352242467910007671</stp>
         <tr r="F124" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2295407790</v>
+        <v>#N/A Requesting Data...3785016217</v>
         <stp/>
         <stp>BDP|5657563513753480721</stp>
         <tr r="E80" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3425980426</v>
+        <v>#N/A Requesting Data...3306849545</v>
         <stp/>
         <stp>BDP|5976587264538865878</stp>
         <tr r="E62" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3040842551</v>
+        <v>#N/A Requesting Data...3934918342</v>
         <stp/>
         <stp>BDP|7151318027339523982</stp>
         <tr r="F91" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2067863983</v>
+        <v>#N/A Requesting Data...4081925213</v>
         <stp/>
         <stp>BDP|1896477110772260049</stp>
         <tr r="C91" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3395888376</v>
+        <v>#N/A Requesting Data...3325062206</v>
         <stp/>
         <stp>BDP|4252725967471187287</stp>
         <tr r="F44" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4191973330</v>
+        <v>#N/A Requesting Data...4260136553</v>
         <stp/>
         <stp>BDP|6943451920864586278</stp>
         <tr r="C118" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3188764126</v>
+        <v>#N/A Requesting Data...4111671994</v>
         <stp/>
         <stp>BDP|5838113265174067025</stp>
         <tr r="F39" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1144095221</v>
+        <v>#N/A Requesting Data...4119192350</v>
         <stp/>
         <stp>BDP|3456718228377624745</stp>
         <tr r="E111" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2651678235</v>
+        <v>#N/A Requesting Data...3910835342</v>
         <stp/>
         <stp>BDP|5917425194519245724</stp>
         <tr r="E79" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3081932147</v>
+        <v>#N/A Requesting Data...3648487553</v>
         <stp/>
         <stp>BDP|6787533358407016713</stp>
         <tr r="F135" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1282679593</v>
+        <v>#N/A Requesting Data...3296096067</v>
         <stp/>
         <stp>BDP|5576451913756991076</stp>
         <tr r="E16" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2263949882</v>
+        <v>#N/A Requesting Data...3285822119</v>
         <stp/>
         <stp>BDP|5284390591628042184</stp>
         <tr r="C24" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2450691228</v>
+        <v>#N/A Requesting Data...4167064057</v>
         <stp/>
         <stp>BDP|5412037028917536689</stp>
         <tr r="G115" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3231309567</v>
+        <v>#N/A Requesting Data...3356613014</v>
         <stp/>
         <stp>BDP|8966942938724477029</stp>
         <tr r="C15" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2781431614</v>
+        <v>#N/A Requesting Data...3384455864</v>
         <stp/>
         <stp>BDP|2938144706552859709</stp>
         <tr r="G81" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1097446561</v>
+        <v>#N/A Requesting Data...3993963850</v>
         <stp/>
         <stp>BDP|3632949480676633244</stp>
         <tr r="F31" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1494195449</v>
+        <v>#N/A Requesting Data...3541687821</v>
         <stp/>
         <stp>BDP|3513418606797579639</stp>
         <tr r="F90" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1207117214</v>
+        <v>#N/A Requesting Data...3524047675</v>
         <stp/>
         <stp>BDP|1733520919261908213</stp>
         <tr r="G73" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3843936070</v>
+        <v>#N/A Requesting Data...3757900769</v>
         <stp/>
         <stp>BDP|8368969127023380651</stp>
         <tr r="F28" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3138415599</v>
+        <v>#N/A Requesting Data...3948297376</v>
         <stp/>
         <stp>BDP|7172716621593553717</stp>
         <tr r="F53" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2530182526</v>
+        <v>#N/A Requesting Data...3990154127</v>
         <stp/>
         <stp>BDP|2954250373819174944</stp>
         <tr r="F119" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1211631174</v>
+        <v>#N/A Requesting Data...3374555653</v>
         <stp/>
         <stp>BDP|4728287753511799518</stp>
         <tr r="F3" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3805354439</v>
+        <v>#N/A Requesting Data...4240486062</v>
         <stp/>
         <stp>BDP|6348617969513327227</stp>
         <tr r="E104" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2272394103</v>
+        <v>#N/A Requesting Data...3444468144</v>
         <stp/>
         <stp>BDP|7694099704858685831</stp>
         <tr r="C107" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3889924940</v>
+        <v>#N/A Requesting Data...3719811261</v>
         <stp/>
         <stp>BDP|4106834752526835861</stp>
         <tr r="F55" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3117517842</v>
+        <v>#N/A Requesting Data...3912447448</v>
         <stp/>
         <stp>BDP|7951337561756108354</stp>
         <tr r="G112" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1455830185</v>
+        <v>#N/A Requesting Data...3963940489</v>
         <stp/>
         <stp>BDP|5468867501418549294</stp>
         <tr r="E86" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3341686779</v>
+        <v>#N/A Requesting Data...3329359168</v>
         <stp/>
         <stp>BDP|4546740053823447251</stp>
         <tr r="C32" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3505825017</v>
+        <v>#N/A Requesting Data...3695732783</v>
         <stp/>
         <stp>BDP|7484527599745538990</stp>
         <tr r="F76" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2301857210</v>
+        <v>#N/A Requesting Data...3323741885</v>
         <stp/>
         <stp>BDP|5578475423865159117</stp>
         <tr r="E61" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4097924273</v>
+        <v>#N/A Requesting Data...3961498392</v>
         <stp/>
         <stp>BDP|6158107237024797760</stp>
         <tr r="E45" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2638158749</v>
+        <v>#N/A Requesting Data...3870086719</v>
         <stp/>
         <stp>BDP|4143076943390197735</stp>
         <tr r="F97" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1242675291</v>
+        <v>#N/A Requesting Data...4159766675</v>
         <stp/>
         <stp>BDP|1762196091349932721</stp>
         <tr r="E82" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3482660034</v>
+        <v>#N/A Requesting Data...3962206144</v>
         <stp/>
         <stp>BDP|4189169184528349241</stp>
         <tr r="F137" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1240918565</v>
+        <v>#N/A Requesting Data...4014482094</v>
         <stp/>
         <stp>BDP|9103140635044368872</stp>
         <tr r="F29" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2979363983</v>
+        <v>#N/A Requesting Data...3508900283</v>
         <stp/>
         <stp>BDP|5519603296584718917</stp>
         <tr r="G54" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3607224321</v>
+        <v>#N/A Requesting Data...3343128970</v>
         <stp/>
         <stp>BDP|1156250824766982737</stp>
         <tr r="G44" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3643064057</v>
+        <v>#N/A Requesting Data...4066598687</v>
         <stp/>
         <stp>BDP|6031605254431729496</stp>
         <tr r="G86" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2227040547</v>
+        <v>#N/A Requesting Data...3747447311</v>
         <stp/>
         <stp>BDP|2649489454114394728</stp>
         <tr r="C14" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2554160395</v>
+        <v>#N/A Requesting Data...4244937468</v>
         <stp/>
         <stp>BDP|8999377595616850481</stp>
         <tr r="E108" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3636534756</v>
+        <v>#N/A Requesting Data...3840422711</v>
         <stp/>
         <stp>BDP|8988928209665280487</stp>
         <tr r="F71" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2079920517</v>
+        <v>#N/A Requesting Data...3996049805</v>
         <stp/>
         <stp>BDP|8368023487691952119</stp>
         <tr r="F88" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4060178811</v>
+        <v>#N/A Requesting Data...3427276886</v>
         <stp/>
         <stp>BDP|5199287207907438042</stp>
         <tr r="E66" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3313275961</v>
+        <v>#N/A Requesting Data...3617180605</v>
         <stp/>
         <stp>BDP|7460099446995728631</stp>
         <tr r="F134" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2312576859</v>
+        <v>#N/A Requesting Data...3659228875</v>
         <stp/>
         <stp>BDP|6160638673325976246</stp>
         <tr r="C104" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1853080294</v>
+        <v>#N/A Requesting Data...3527844676</v>
         <stp/>
         <stp>BDP|5660731962530222490</stp>
         <tr r="E128" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2841630111</v>
+        <v>#N/A Requesting Data...4287872777</v>
         <stp/>
         <stp>BDP|3355023726294311595</stp>
         <tr r="G114" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2920637192</v>
+        <v>#N/A Requesting Data...4022211714</v>
         <stp/>
         <stp>BDP|5604474461391860653</stp>
         <tr r="E130" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2857206261</v>
+        <v>#N/A Requesting Data...4013368080</v>
         <stp/>
         <stp>BDP|3542140114402066179</stp>
         <tr r="E78" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4081039713</v>
+        <v>#N/A Requesting Data...3867359588</v>
         <stp/>
         <stp>BDP|2942496252996870592</stp>
         <tr r="G121" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2533566179</v>
+        <v>#N/A Requesting Data...4107259145</v>
         <stp/>
         <stp>BDP|1823820926283534897</stp>
         <tr r="G18" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3996444994</v>
+        <v>#N/A Requesting Data...4032337224</v>
         <stp/>
         <stp>BDP|3716189405712826043</stp>
         <tr r="G92" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A N/A</v>
+        <v>#N/A Requesting Data...3470983927</v>
         <stp/>
         <stp>BDP|3228146609442097080</stp>
         <tr r="C140" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3457981722</v>
+        <v>#N/A Requesting Data...3894476568</v>
         <stp/>
         <stp>BDP|9344147089140006098</stp>
         <tr r="E83" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4167042075</v>
+        <v>#N/A Requesting Data...4203792947</v>
         <stp/>
         <stp>BDP|6993061706081965773</stp>
         <tr r="F81" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2949027126</v>
+        <v>#N/A Requesting Data...4040723902</v>
         <stp/>
         <stp>BDP|6176792116871092198</stp>
         <tr r="C68" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3521126179</v>
+        <v>#N/A Requesting Data...3780628298</v>
         <stp/>
         <stp>BDP|7185432584822399912</stp>
         <tr r="F131" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3455908174</v>
+        <v>#N/A Requesting Data...3932798986</v>
         <stp/>
         <stp>BDP|8280856169194643320</stp>
         <tr r="G49" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2923300990</v>
+        <v>#N/A Requesting Data...4097649655</v>
         <stp/>
         <stp>BDP|9399109618929306123</stp>
         <tr r="F37" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3077051607</v>
+        <v>#N/A Requesting Data...3586656742</v>
         <stp/>
         <stp>BDP|6669663699409638145</stp>
         <tr r="C123" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2158535965</v>
+        <v>#N/A Requesting Data...3492167884</v>
         <stp/>
         <stp>BDP|6175693122901836298</stp>
         <tr r="C36" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1198607382</v>
+        <v>#N/A Requesting Data...4195095585</v>
         <stp/>
         <stp>BDP|8135075327118072391</stp>
         <tr r="C17" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2179139113</v>
+        <v>#N/A Requesting Data...3854711385</v>
         <stp/>
         <stp>BDP|5726291712345411206</stp>
         <tr r="G28" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4239908784</v>
+        <v>#N/A Requesting Data...4131006111</v>
         <stp/>
         <stp>BDP|8698973352783506690</stp>
         <tr r="F25" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2318547612</v>
+        <v>#N/A Requesting Data...3592905464</v>
         <stp/>
         <stp>BDP|5493604681742158862</stp>
         <tr r="G63" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1246532595</v>
+        <v>#N/A Requesting Data...3372211764</v>
         <stp/>
         <stp>BDP|3239104742287612040</stp>
         <tr r="E39" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4072869786</v>
+        <v>#N/A Requesting Data...3382001044</v>
         <stp/>
         <stp>BDP|3381147726641663059</stp>
         <tr r="C122" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3802330131</v>
+        <v>#N/A Requesting Data...3536280642</v>
         <stp/>
         <stp>BDP|6625906764329795167</stp>
         <tr r="F56" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3418195065</v>
+        <v>#N/A Requesting Data...3488951099</v>
         <stp/>
         <stp>BDP|3325218238213801010</stp>
         <tr r="F57" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2758475650</v>
+        <v>#N/A Requesting Data...4059144489</v>
         <stp/>
         <stp>BDP|1313137390988032037</stp>
         <tr r="C83" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1875467233</v>
+        <v>#N/A Requesting Data...3467129993</v>
         <stp/>
         <stp>BDP|3702733300853619616</stp>
         <tr r="G34" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1105296424</v>
+        <v>#N/A Requesting Data...4186265653</v>
         <stp/>
         <stp>BDP|8558611930018338475</stp>
         <tr r="F35" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4255201935</v>
+        <v>#N/A Requesting Data...3411262565</v>
         <stp/>
         <stp>BDP|5387098906493173798</stp>
         <tr r="G62" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3789769220</v>
+        <v>#N/A Requesting Data...3441188077</v>
         <stp/>
         <stp>BDP|1951038018907673608</stp>
         <tr r="C126" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2009334446</v>
+        <v>#N/A Requesting Data...3705705585</v>
         <stp/>
         <stp>BDP|9253802402770546012</stp>
         <tr r="F74" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3695275716</v>
+        <v>#N/A Requesting Data...3746057017</v>
         <stp/>
         <stp>BDP|1884505914021260664</stp>
         <tr r="E96" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2679831280</v>
+        <v>#N/A Requesting Data...3813817363</v>
         <stp/>
         <stp>BDP|3540127028674193608</stp>
         <tr r="F94" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2628704940</v>
+        <v>#N/A Requesting Data...3874855901</v>
         <stp/>
         <stp>BDP|5372375359741187031</stp>
         <tr r="F27" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1194205678</v>
+        <v>#N/A Requesting Data...3406236356</v>
         <stp/>
         <stp>BDP|5121625602631825066</stp>
         <tr r="E81" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1903778350</v>
+        <v>#N/A Requesting Data...3410624760</v>
         <stp/>
         <stp>BDP|5282708515920897138</stp>
         <tr r="F43" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1853388977</v>
+        <v>#N/A Requesting Data...3700949023</v>
         <stp/>
         <stp>BDP|1250299291741371958</stp>
         <tr r="G31" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2883616175</v>
+        <v>#N/A Requesting Data...3761898525</v>
         <stp/>
         <stp>BDP|4253176148933327033</stp>
         <tr r="C133" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1728374499</v>
+        <v>#N/A Requesting Data...3897069578</v>
         <stp/>
         <stp>BDP|9704751602229087502</stp>
         <tr r="F49" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3761824224</v>
+        <v>#N/A Requesting Data...4276460625</v>
         <stp/>
         <stp>BDP|6775233901286469015</stp>
         <tr r="E125" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2339955902</v>
+        <v>#N/A Requesting Data...4231627636</v>
         <stp/>
         <stp>BDP|7918289416910309647</stp>
         <tr r="C56" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3501091081</v>
+        <v>#N/A Requesting Data...3430201572</v>
         <stp/>
         <stp>BDP|3731272815900600241</stp>
         <tr r="C53" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3421836247</v>
+        <v>#N/A Requesting Data...4196786209</v>
         <stp/>
         <stp>BDP|1685459166489439868</stp>
         <tr r="F133" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3203319780</v>
+        <v>#N/A Requesting Data...4129067630</v>
         <stp/>
         <stp>BDP|2506644172580171154</stp>
         <tr r="C119" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1392842394</v>
+        <v>#N/A Requesting Data...3734698182</v>
         <stp/>
         <stp>BDP|1995353227627490580</stp>
         <tr r="E119" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3300623214</v>
+        <v>#N/A Requesting Data...3968931675</v>
         <stp/>
         <stp>BDP|9173868178561206592</stp>
         <tr r="C77" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1149555560</v>
+        <v>#N/A Requesting Data...3968647508</v>
         <stp/>
         <stp>BDP|4008096672221657096</stp>
         <tr r="G43" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1498338613</v>
+        <v>#N/A Requesting Data...4229522405</v>
         <stp/>
         <stp>BDP|5434663182001395869</stp>
         <tr r="E107" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4257408197</v>
+        <v>#N/A Requesting Data...4102354705</v>
         <stp/>
         <stp>BDP|8686279502629263146</stp>
         <tr r="C129" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2322562648</v>
+        <v>#N/A Requesting Data...4078756585</v>
         <stp/>
         <stp>BDP|4576300957588172984</stp>
         <tr r="E63" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1113118131</v>
+        <v>#N/A Requesting Data...3936207456</v>
         <stp/>
         <stp>BDP|7469671678835895086</stp>
         <tr r="E2" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2104394279</v>
+        <v>#N/A Requesting Data...3932190795</v>
         <stp/>
         <stp>BDP|5444751401066968714</stp>
         <tr r="E73" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4286367257</v>
+        <v>#N/A Requesting Data...3762270595</v>
         <stp/>
         <stp>BDP|2824124077350027748</stp>
         <tr r="E136" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2494334552</v>
+        <v>#N/A Requesting Data...3400754951</v>
         <stp/>
         <stp>BDP|3708851985886704699</stp>
         <tr r="C19" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1635770335</v>
+        <v>#N/A Requesting Data...4199193167</v>
         <stp/>
         <stp>BDP|1006071828475585561</stp>
         <tr r="F116" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3531987168</v>
+        <v>#N/A Requesting Data...3647293100</v>
         <stp/>
         <stp>BDP|1086712249007771639</stp>
         <tr r="G26" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4074378601</v>
+        <v>#N/A Requesting Data...3925901306</v>
         <stp/>
         <stp>BDP|6634730869724168016</stp>
         <tr r="E103" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2457924617</v>
+        <v>#N/A Requesting Data...3625466746</v>
         <stp/>
         <stp>BDP|3520366017777816505</stp>
         <tr r="E97" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1070287254</v>
+        <v>#N/A Requesting Data...4091657438</v>
         <stp/>
         <stp>BDP|2995135217932647367</stp>
         <tr r="F105" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3458541308</v>
+        <v>#N/A Requesting Data...4275910114</v>
         <stp/>
         <stp>BDP|3565057922625094707</stp>
         <tr r="G45" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1637723018</v>
+        <v>#N/A Requesting Data...3939252163</v>
         <stp/>
         <stp>BDP|1485569542807651461</stp>
         <tr r="C86" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2581743270</v>
+        <v>#N/A Requesting Data...3582669017</v>
         <stp/>
         <stp>BDP|1159006460850353421</stp>
         <tr r="E46" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1468506262</v>
+        <v>#N/A Requesting Data...4154209838</v>
         <stp/>
         <stp>BDP|5113311422502283510</stp>
         <tr r="C84" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2887735648</v>
+        <v>#N/A Requesting Data...3985529281</v>
         <stp/>
         <stp>BDP|4420649803735408460</stp>
         <tr r="F117" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1132838510</v>
+        <v>#N/A Requesting Data...4263321647</v>
         <stp/>
         <stp>BDP|9873235984695079585</stp>
         <tr r="C60" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2291847032</v>
+        <v>#N/A Requesting Data...3802492820</v>
         <stp/>
         <stp>BDP|4726106605717010168</stp>
         <tr r="G46" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3644448675</v>
+        <v>#N/A Requesting Data...4000574625</v>
         <stp/>
         <stp>BDP|97453184744598227</stp>
         <tr r="G135" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3995124466</v>
+        <v>#N/A Requesting Data...3522916377</v>
         <stp/>
         <stp>BDP|71129432364790944</stp>
         <tr r="E105" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2277765017</v>
+        <v>#N/A Requesting Data...3975674632</v>
         <stp/>
         <stp>BDP|13870968378316918</stp>
         <tr r="F38" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1550402552</v>
+        <v>#N/A Requesting Data...3745667598</v>
         <stp/>
         <stp>BDP|545017254499479967</stp>
         <tr r="E23" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1126631800</v>
+        <v>#N/A Requesting Data...4116184235</v>
         <stp/>
         <stp>BDP|562457211792430265</stp>
         <tr r="G116" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2958597565</v>
+        <v>#N/A Requesting Data...3430198192</v>
         <stp/>
         <stp>BDP|752318736222262646</stp>
         <tr r="F83" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1210056363</v>
+        <v>#N/A Requesting Data...3940459850</v>
         <stp/>
         <stp>BDP|926433161397617222</stp>
         <tr r="F10" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1077243446</v>
+        <v>#N/A Requesting Data...3868982850</v>
         <stp/>
         <stp>BDP|455507803480864317</stp>
         <tr r="C51" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1253044260</v>
+        <v>#N/A Requesting Data...3465689972</v>
         <stp/>
         <stp>BDP|738430784972633891</stp>
         <tr r="F41" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1222853957</v>
+        <v>#N/A Requesting Data...3535506534</v>
         <stp/>
         <stp>BDP|226270545351892196</stp>
         <tr r="F61" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2647917022</v>
+        <v>#N/A Requesting Data...4077106971</v>
         <stp/>
         <stp>BDP|478534605105814154</stp>
         <tr r="G12" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3633834868</v>
+        <v>#N/A Requesting Data...3728609545</v>
         <stp/>
         <stp>BDP|292697057297288557</stp>
         <tr r="C106" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1105510249</v>
+        <v>#N/A Requesting Data...4034100476</v>
         <stp/>
         <stp>BDP|449489448517477649</stp>
         <tr r="E99" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4135670200</v>
+        <v>#N/A Requesting Data...4195463525</v>
         <stp/>
         <stp>BDP|477239144286521179</stp>
         <tr r="G138" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2022772395</v>
+        <v>#N/A Requesting Data...3980828019</v>
         <stp/>
         <stp>BDP|136361134742057301</stp>
         <tr r="C57" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2556838060</v>
+        <v>#N/A Requesting Data...4021388650</v>
         <stp/>
         <stp>BDP|282958180978155995</stp>
         <tr r="C59" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2329102317</v>
+        <v>#N/A Requesting Data...4176049266</v>
         <stp/>
         <stp>BDP|991366924295531418</stp>
         <tr r="F2" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2027401332</v>
+        <v>#N/A Requesting Data...3873494235</v>
         <stp/>
         <stp>BDP|934073235795196633</stp>
         <tr r="F62" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3530671686</v>
+        <v>#N/A Requesting Data...3871479426</v>
         <stp/>
         <stp>BDP|266608211912165570</stp>
         <tr r="E113" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3113665726</v>
+        <v>#N/A Requesting Data...3929019725</v>
         <stp/>
         <stp>BDP|910156400954699593</stp>
         <tr r="G8" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3974993112</v>
+        <v>#N/A Requesting Data...3972015169</v>
         <stp/>
         <stp>BDP|794293317440269040</stp>
         <tr r="E100" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4077776812</v>
+        <v>#N/A Requesting Data...4293887052</v>
         <stp/>
         <stp>BDP|206766873121157269</stp>
         <tr r="E41" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4081095894</v>
+        <v>#N/A Requesting Data...4244196410</v>
         <stp/>
         <stp>BDP|315261912951356153</stp>
         <tr r="E21" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4029829725</v>
+        <v>#N/A Requesting Data...3441553482</v>
         <stp/>
         <stp>BDP|169080827246056602</stp>
         <tr r="G126" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3787822754</v>
+        <v>#N/A Requesting Data...4144842789</v>
         <stp/>
         <stp>BDP|454779781439338455</stp>
         <tr r="E36" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4207164293</v>
+        <v>#N/A Requesting Data...3819542564</v>
         <stp/>
         <stp>BDP|198524097739196711</stp>
         <tr r="F92" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1339984719</v>
+        <v>#N/A Requesting Data...3540774733</v>
         <stp/>
         <stp>BDP|618726407191106421</stp>
         <tr r="C92" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1964109500</v>
+        <v>#N/A Requesting Data...4101795691</v>
         <stp/>
         <stp>BDP|442808307356626303</stp>
         <tr r="F20" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A N/A</v>
+        <v>#N/A Requesting Data...3481883073</v>
         <stp/>
         <stp>BDP|624014897144495064</stp>
         <tr r="G140" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2417705575</v>
+        <v>#N/A Requesting Data...4124007044</v>
         <stp/>
         <stp>BDP|304889655090792147</stp>
         <tr r="E58" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2198712958</v>
+        <v>#N/A Requesting Data...3685881379</v>
         <stp/>
         <stp>BDP|427627592191043219</stp>
         <tr r="C87" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2078385749</v>
+        <v>#N/A Requesting Data...3481819126</v>
         <stp/>
         <stp>BDP|768711067038142524</stp>
         <tr r="G25" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3144113388</v>
+        <v>#N/A Requesting Data...3628296959</v>
         <stp/>
         <stp>BDP|447365482187669383</stp>
         <tr r="C95" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3489956823</v>
+        <v>#N/A Requesting Data...3999580787</v>
         <stp/>
         <stp>BDP|901925773788783965</stp>
         <tr r="G67" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3317480784</v>
+        <v>#N/A Requesting Data...4021460504</v>
         <stp/>
         <stp>BDP|511429594874391764</stp>
         <tr r="G117" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4071104396</v>
+        <v>#N/A Requesting Data...3598432217</v>
         <stp/>
         <stp>BDP|544620567958067604</stp>
         <tr r="C131" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2770898833</v>
+        <v>#N/A Requesting Data...3470177714</v>
         <stp/>
         <stp>BDP|945569483354328027</stp>
         <tr r="C21" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4015290613</v>
+        <v>#N/A Requesting Data...3515393032</v>
         <stp/>
         <stp>BDP|691281527639744142</stp>
         <tr r="E8" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3627187458</v>
+        <v>#N/A Requesting Data...3791515676</v>
         <stp/>
         <stp>BDP|968314719543295935</stp>
         <tr r="E68" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3908949143</v>
+        <v>#N/A Requesting Data...3948807595</v>
         <stp/>
         <stp>BDP|760426044168153386</stp>
         <tr r="G7" s="1"/>
@@ -4843,7 +4843,7 @@
   <dimension ref="A1:E140"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A113" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:E140"/>
+      <selection activeCell="H117" sqref="H117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>